<commit_message>
Q3 2022 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\0. IAD activities\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2022\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of November 2022\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4CC732-4401-43C7-A9CE-DA833AA5F0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FCD235-A6B5-4813-B08D-DEFC58E4D815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3195" yWindow="3195" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="PCE_Per_Anl">#REF!</definedName>
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CM$202</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CN$202</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="61">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -220,13 +220,13 @@
     <t>2021 - 2022</t>
   </si>
   <si>
-    <t>As of August 2022</t>
+    <t>Q1 2000 to Q3 2022</t>
   </si>
   <si>
-    <t>Q1 2000 to Q2 2022</t>
+    <t>Q1 2001 to Q3 2022</t>
   </si>
   <si>
-    <t>Q1 2001 to Q2 2022</t>
+    <t>As of November 2022</t>
   </si>
 </sst>
 </file>
@@ -234,10 +234,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -310,11 +310,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -332,39 +332,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -702,174 +699,173 @@
   </sheetPr>
   <dimension ref="A1:EW202"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="CA2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="CA66" sqref="CA66"/>
       <selection pane="topRight" activeCell="CA66" sqref="CA66"/>
       <selection pane="bottomLeft" activeCell="CA66" sqref="CA66"/>
-      <selection pane="bottomRight" activeCell="CB31" sqref="CB31"/>
+      <selection pane="bottomRight" activeCell="CH1" sqref="CH1:CN1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.90625" style="1" customWidth="1"/>
-    <col min="2" max="56" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="58" max="60" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="64" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="79" max="81" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="86" max="91" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="92" max="16384" width="7.81640625" style="1"/>
+    <col min="1" max="1" width="38.88671875" style="1" customWidth="1"/>
+    <col min="2" max="56" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="60" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="64" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="79" max="81" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="92" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="93" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="35">
+      <c r="B9" s="33">
         <v>2000</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33">
         <v>2001</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35">
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33">
         <v>2002</v>
       </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35">
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33">
         <v>2003</v>
       </c>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35">
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33">
         <v>2004</v>
       </c>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35">
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33">
         <v>2005</v>
       </c>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="35">
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
+      <c r="Z9" s="33">
         <v>2006</v>
       </c>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="35"/>
-      <c r="AD9" s="35">
+      <c r="AA9" s="33"/>
+      <c r="AB9" s="33"/>
+      <c r="AC9" s="33"/>
+      <c r="AD9" s="33">
         <v>2007</v>
       </c>
-      <c r="AE9" s="35"/>
-      <c r="AF9" s="35"/>
-      <c r="AG9" s="35"/>
-      <c r="AH9" s="35">
+      <c r="AE9" s="33"/>
+      <c r="AF9" s="33"/>
+      <c r="AG9" s="33"/>
+      <c r="AH9" s="33">
         <v>2008</v>
       </c>
-      <c r="AI9" s="35"/>
-      <c r="AJ9" s="35"/>
-      <c r="AK9" s="35"/>
-      <c r="AL9" s="35">
+      <c r="AI9" s="33"/>
+      <c r="AJ9" s="33"/>
+      <c r="AK9" s="33"/>
+      <c r="AL9" s="33">
         <v>2009</v>
       </c>
-      <c r="AM9" s="35"/>
-      <c r="AN9" s="35"/>
-      <c r="AO9" s="35"/>
-      <c r="AP9" s="35">
+      <c r="AM9" s="33"/>
+      <c r="AN9" s="33"/>
+      <c r="AO9" s="33"/>
+      <c r="AP9" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="35"/>
-      <c r="AR9" s="35"/>
-      <c r="AS9" s="35"/>
-      <c r="AT9" s="35">
+      <c r="AQ9" s="33"/>
+      <c r="AR9" s="33"/>
+      <c r="AS9" s="33"/>
+      <c r="AT9" s="33">
         <v>2011</v>
       </c>
-      <c r="AU9" s="35"/>
-      <c r="AV9" s="35"/>
-      <c r="AW9" s="35"/>
-      <c r="AX9" s="35">
+      <c r="AU9" s="33"/>
+      <c r="AV9" s="33"/>
+      <c r="AW9" s="33"/>
+      <c r="AX9" s="33">
         <v>2012</v>
       </c>
-      <c r="AY9" s="35"/>
-      <c r="AZ9" s="35"/>
-      <c r="BA9" s="35"/>
-      <c r="BB9" s="35">
+      <c r="AY9" s="33"/>
+      <c r="AZ9" s="33"/>
+      <c r="BA9" s="33"/>
+      <c r="BB9" s="33">
         <v>2013</v>
       </c>
-      <c r="BC9" s="35"/>
-      <c r="BD9" s="35"/>
-      <c r="BE9" s="35"/>
-      <c r="BF9" s="35">
+      <c r="BC9" s="33"/>
+      <c r="BD9" s="33"/>
+      <c r="BE9" s="33"/>
+      <c r="BF9" s="33">
         <v>2014</v>
       </c>
-      <c r="BG9" s="35"/>
-      <c r="BH9" s="35"/>
-      <c r="BI9" s="35"/>
-      <c r="BJ9" s="35">
+      <c r="BG9" s="33"/>
+      <c r="BH9" s="33"/>
+      <c r="BI9" s="33"/>
+      <c r="BJ9" s="33">
         <v>2015</v>
       </c>
-      <c r="BK9" s="35"/>
-      <c r="BL9" s="35"/>
-      <c r="BM9" s="35"/>
-      <c r="BN9" s="35">
+      <c r="BK9" s="33"/>
+      <c r="BL9" s="33"/>
+      <c r="BM9" s="33"/>
+      <c r="BN9" s="33">
         <v>2016</v>
       </c>
-      <c r="BO9" s="35"/>
-      <c r="BP9" s="35"/>
-      <c r="BQ9" s="35"/>
+      <c r="BO9" s="33"/>
+      <c r="BP9" s="33"/>
+      <c r="BQ9" s="33"/>
       <c r="BR9" s="34">
         <v>2017</v>
       </c>
@@ -904,8 +900,9 @@
         <v>2022</v>
       </c>
       <c r="CM9" s="34"/>
+      <c r="CN9" s="34"/>
     </row>
-    <row r="10" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
@@ -1179,11 +1176,14 @@
       <c r="CM10" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="CN10" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:153" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
     </row>
-    <row r="12" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1455,9 +1455,11 @@
         <v>1384611.9383681593</v>
       </c>
       <c r="CM12" s="10">
-        <v>1566848.5961453628</v>
-      </c>
-      <c r="CN12" s="11"/>
+        <v>1566368.7437218034</v>
+      </c>
+      <c r="CN12" s="10">
+        <v>1447422.0423746321</v>
+      </c>
       <c r="CO12" s="11"/>
       <c r="CP12" s="11"/>
       <c r="CQ12" s="11"/>
@@ -1520,7 +1522,7 @@
       <c r="EV12" s="11"/>
       <c r="EW12" s="11"/>
     </row>
-    <row r="13" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1792,9 +1794,11 @@
         <v>70230.878218037135</v>
       </c>
       <c r="CM13" s="10">
-        <v>74442.309405138949</v>
-      </c>
-      <c r="CN13" s="11"/>
+        <v>74860.089917473437</v>
+      </c>
+      <c r="CN13" s="10">
+        <v>74795.7906436333</v>
+      </c>
       <c r="CO13" s="11"/>
       <c r="CP13" s="11"/>
       <c r="CQ13" s="11"/>
@@ -1857,7 +1861,7 @@
       <c r="EV13" s="11"/>
       <c r="EW13" s="11"/>
     </row>
-    <row r="14" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2131,7 +2135,9 @@
       <c r="CM14" s="10">
         <v>64914.406063883871</v>
       </c>
-      <c r="CN14" s="11"/>
+      <c r="CN14" s="10">
+        <v>67943.680306057722</v>
+      </c>
       <c r="CO14" s="11"/>
       <c r="CP14" s="11"/>
       <c r="CQ14" s="11"/>
@@ -2194,7 +2200,7 @@
       <c r="EV14" s="11"/>
       <c r="EW14" s="11"/>
     </row>
-    <row r="15" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -2466,9 +2472,11 @@
         <v>445782.86298792978</v>
       </c>
       <c r="CM15" s="10">
-        <v>575337.08921437419</v>
-      </c>
-      <c r="CN15" s="11"/>
+        <v>574802.88069589285</v>
+      </c>
+      <c r="CN15" s="10">
+        <v>523179.3209197055</v>
+      </c>
       <c r="CO15" s="11"/>
       <c r="CP15" s="11"/>
       <c r="CQ15" s="11"/>
@@ -2531,7 +2539,7 @@
       <c r="EV15" s="11"/>
       <c r="EW15" s="11"/>
     </row>
-    <row r="16" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>8</v>
       </c>
@@ -2803,9 +2811,11 @@
         <v>106137.49800889417</v>
       </c>
       <c r="CM16" s="10">
-        <v>104482.69146951211</v>
-      </c>
-      <c r="CN16" s="11"/>
+        <v>103093.70168045604</v>
+      </c>
+      <c r="CN16" s="10">
+        <v>124232.08946906852</v>
+      </c>
       <c r="CO16" s="11"/>
       <c r="CP16" s="11"/>
       <c r="CQ16" s="11"/>
@@ -2868,7 +2878,7 @@
       <c r="EV16" s="11"/>
       <c r="EW16" s="11"/>
     </row>
-    <row r="17" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3140,9 +3150,11 @@
         <v>163582.39680684087</v>
       </c>
       <c r="CM17" s="10">
-        <v>138241.59289105353</v>
-      </c>
-      <c r="CN17" s="11"/>
+        <v>138209.36175477973</v>
+      </c>
+      <c r="CN17" s="10">
+        <v>222442.30928271718</v>
+      </c>
       <c r="CO17" s="11"/>
       <c r="CP17" s="11"/>
       <c r="CQ17" s="11"/>
@@ -3205,7 +3217,7 @@
       <c r="EV17" s="11"/>
       <c r="EW17" s="11"/>
     </row>
-    <row r="18" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3477,9 +3489,11 @@
         <v>381175.32430561678</v>
       </c>
       <c r="CM18" s="10">
-        <v>297267.53453825763</v>
-      </c>
-      <c r="CN18" s="11"/>
+        <v>295969.14642522112</v>
+      </c>
+      <c r="CN18" s="10">
+        <v>465531.09190673259</v>
+      </c>
       <c r="CO18" s="11"/>
       <c r="CP18" s="11"/>
       <c r="CQ18" s="11"/>
@@ -3542,7 +3556,7 @@
       <c r="EV18" s="11"/>
       <c r="EW18" s="11"/>
     </row>
-    <row r="19" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -3814,9 +3828,11 @@
         <v>121612.14168047598</v>
       </c>
       <c r="CM19" s="10">
-        <v>127983.13537798337</v>
-      </c>
-      <c r="CN19" s="11"/>
+        <v>127268.98601639032</v>
+      </c>
+      <c r="CN19" s="10">
+        <v>96958.131594522769</v>
+      </c>
       <c r="CO19" s="11"/>
       <c r="CP19" s="11"/>
       <c r="CQ19" s="11"/>
@@ -3879,7 +3895,7 @@
       <c r="EV19" s="11"/>
       <c r="EW19" s="11"/>
     </row>
-    <row r="20" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -4151,9 +4167,11 @@
         <v>56265.310122822433</v>
       </c>
       <c r="CM20" s="10">
-        <v>41080.396687636669</v>
-      </c>
-      <c r="CN20" s="11"/>
+        <v>41983.761192967853</v>
+      </c>
+      <c r="CN20" s="10">
+        <v>53161.871137265283</v>
+      </c>
       <c r="CO20" s="11"/>
       <c r="CP20" s="11"/>
       <c r="CQ20" s="11"/>
@@ -4216,7 +4234,7 @@
       <c r="EV20" s="11"/>
       <c r="EW20" s="11"/>
     </row>
-    <row r="21" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -4488,9 +4506,11 @@
         <v>205911.95644780132</v>
       </c>
       <c r="CM21" s="10">
-        <v>186679.2048021091</v>
-      </c>
-      <c r="CN21" s="11"/>
+        <v>187158.10532078435</v>
+      </c>
+      <c r="CN21" s="10">
+        <v>219511.8826930408</v>
+      </c>
       <c r="CO21" s="11"/>
       <c r="CP21" s="11"/>
       <c r="CQ21" s="11"/>
@@ -4553,7 +4573,7 @@
       <c r="EV21" s="11"/>
       <c r="EW21" s="11"/>
     </row>
-    <row r="22" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -4825,9 +4845,11 @@
         <v>316266.57631519978</v>
       </c>
       <c r="CM22" s="10">
-        <v>181099.29772127935</v>
-      </c>
-      <c r="CN22" s="11"/>
+        <v>182344.68526335541</v>
+      </c>
+      <c r="CN22" s="10">
+        <v>287705.19347809529</v>
+      </c>
       <c r="CO22" s="11"/>
       <c r="CP22" s="11"/>
       <c r="CQ22" s="11"/>
@@ -4890,7 +4912,7 @@
       <c r="EV22" s="11"/>
       <c r="EW22" s="11"/>
     </row>
-    <row r="23" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -5162,9 +5184,11 @@
         <v>544500.70931277948</v>
       </c>
       <c r="CM23" s="10">
-        <v>522949.58713426144</v>
-      </c>
-      <c r="CN23" s="11"/>
+        <v>521463.04467852885</v>
+      </c>
+      <c r="CN23" s="10">
+        <v>545733.85762884712</v>
+      </c>
       <c r="CO23" s="11"/>
       <c r="CP23" s="11"/>
       <c r="CQ23" s="11"/>
@@ -5227,7 +5251,7 @@
       <c r="EV23" s="11"/>
       <c r="EW23" s="11"/>
     </row>
-    <row r="24" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -5381,7 +5405,7 @@
       <c r="EV24" s="11"/>
       <c r="EW24" s="11"/>
     </row>
-    <row r="25" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>18</v>
       </c>
@@ -5637,25 +5661,27 @@
       <c r="CG25" s="15">
         <v>3801007.5529332561</v>
       </c>
-      <c r="CH25" s="31">
+      <c r="CH25" s="30">
         <v>3397554.7518358915</v>
       </c>
-      <c r="CI25" s="31">
+      <c r="CI25" s="30">
         <v>3396198.6721503939</v>
       </c>
-      <c r="CJ25" s="31">
+      <c r="CJ25" s="30">
         <v>3582435.6457165424</v>
       </c>
-      <c r="CK25" s="31">
+      <c r="CK25" s="30">
         <v>4233960.1057822816</v>
       </c>
-      <c r="CL25" s="31">
+      <c r="CL25" s="30">
         <v>3853894.6766090612</v>
       </c>
-      <c r="CM25" s="31">
-        <v>3881325.8414508533</v>
-      </c>
-      <c r="CN25" s="11"/>
+      <c r="CM25" s="30">
+        <v>3878436.9127315367</v>
+      </c>
+      <c r="CN25" s="30">
+        <v>4128617.261434318</v>
+      </c>
       <c r="CO25" s="11"/>
       <c r="CP25" s="11"/>
       <c r="CQ25" s="11"/>
@@ -5718,7 +5744,7 @@
       <c r="EV25" s="11"/>
       <c r="EW25" s="11"/>
     </row>
-    <row r="26" spans="1:153" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:153" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -5810,13 +5836,14 @@
       <c r="CK26" s="16"/>
       <c r="CL26" s="16"/>
       <c r="CM26" s="16"/>
+      <c r="CN26" s="16"/>
     </row>
-    <row r="27" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -5901,13 +5928,13 @@
       <c r="CE28" s="21"/>
       <c r="CF28" s="21"/>
       <c r="CG28" s="21"/>
-      <c r="CH28" s="32"/>
-      <c r="CI28" s="32"/>
-      <c r="CJ28" s="32"/>
-      <c r="CK28" s="32"/>
-      <c r="CL28" s="32"/>
-      <c r="CM28" s="32"/>
-      <c r="CN28" s="11"/>
+      <c r="CH28" s="31"/>
+      <c r="CI28" s="31"/>
+      <c r="CJ28" s="31"/>
+      <c r="CK28" s="31"/>
+      <c r="CL28" s="31"/>
+      <c r="CM28" s="31"/>
+      <c r="CN28" s="31"/>
       <c r="CO28" s="11"/>
       <c r="CP28" s="11"/>
       <c r="CQ28" s="11"/>
@@ -5970,7 +5997,7 @@
       <c r="EV28" s="11"/>
       <c r="EW28" s="11"/>
     </row>
-    <row r="29" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="22"/>
       <c r="C29" s="23"/>
       <c r="D29" s="23"/>
@@ -6055,13 +6082,13 @@
       <c r="CE29" s="24"/>
       <c r="CF29" s="24"/>
       <c r="CG29" s="24"/>
-      <c r="CH29" s="33"/>
-      <c r="CI29" s="33"/>
-      <c r="CJ29" s="33"/>
-      <c r="CK29" s="33"/>
-      <c r="CL29" s="33"/>
-      <c r="CM29" s="33"/>
-      <c r="CN29" s="11"/>
+      <c r="CH29" s="32"/>
+      <c r="CI29" s="32"/>
+      <c r="CJ29" s="32"/>
+      <c r="CK29" s="32"/>
+      <c r="CL29" s="32"/>
+      <c r="CM29" s="32"/>
+      <c r="CN29" s="32"/>
       <c r="CO29" s="11"/>
       <c r="CP29" s="11"/>
       <c r="CQ29" s="11"/>
@@ -6124,140 +6151,140 @@
       <c r="EV29" s="11"/>
       <c r="EW29" s="11"/>
     </row>
-    <row r="30" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="35">
+      <c r="B38" s="33">
         <v>2000</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35">
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33">
         <v>2001</v>
       </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35">
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33">
         <v>2002</v>
       </c>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35">
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33">
         <v>2003</v>
       </c>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="35">
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="33">
         <v>2004</v>
       </c>
-      <c r="S38" s="35"/>
-      <c r="T38" s="35"/>
-      <c r="U38" s="35"/>
-      <c r="V38" s="35">
+      <c r="S38" s="33"/>
+      <c r="T38" s="33"/>
+      <c r="U38" s="33"/>
+      <c r="V38" s="33">
         <v>2005</v>
       </c>
-      <c r="W38" s="35"/>
-      <c r="X38" s="35"/>
-      <c r="Y38" s="35"/>
-      <c r="Z38" s="35">
+      <c r="W38" s="33"/>
+      <c r="X38" s="33"/>
+      <c r="Y38" s="33"/>
+      <c r="Z38" s="33">
         <v>2006</v>
       </c>
-      <c r="AA38" s="35"/>
-      <c r="AB38" s="35"/>
-      <c r="AC38" s="35"/>
-      <c r="AD38" s="35">
+      <c r="AA38" s="33"/>
+      <c r="AB38" s="33"/>
+      <c r="AC38" s="33"/>
+      <c r="AD38" s="33">
         <v>2007</v>
       </c>
-      <c r="AE38" s="35"/>
-      <c r="AF38" s="35"/>
-      <c r="AG38" s="35"/>
-      <c r="AH38" s="35">
+      <c r="AE38" s="33"/>
+      <c r="AF38" s="33"/>
+      <c r="AG38" s="33"/>
+      <c r="AH38" s="33">
         <v>2008</v>
       </c>
-      <c r="AI38" s="35"/>
-      <c r="AJ38" s="35"/>
-      <c r="AK38" s="35"/>
-      <c r="AL38" s="35">
+      <c r="AI38" s="33"/>
+      <c r="AJ38" s="33"/>
+      <c r="AK38" s="33"/>
+      <c r="AL38" s="33">
         <v>2009</v>
       </c>
-      <c r="AM38" s="35"/>
-      <c r="AN38" s="35"/>
-      <c r="AO38" s="35"/>
-      <c r="AP38" s="35">
+      <c r="AM38" s="33"/>
+      <c r="AN38" s="33"/>
+      <c r="AO38" s="33"/>
+      <c r="AP38" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ38" s="35"/>
-      <c r="AR38" s="35"/>
-      <c r="AS38" s="35"/>
-      <c r="AT38" s="35">
+      <c r="AQ38" s="33"/>
+      <c r="AR38" s="33"/>
+      <c r="AS38" s="33"/>
+      <c r="AT38" s="33">
         <v>2011</v>
       </c>
-      <c r="AU38" s="35"/>
-      <c r="AV38" s="35"/>
-      <c r="AW38" s="35"/>
-      <c r="AX38" s="35">
+      <c r="AU38" s="33"/>
+      <c r="AV38" s="33"/>
+      <c r="AW38" s="33"/>
+      <c r="AX38" s="33">
         <v>2012</v>
       </c>
-      <c r="AY38" s="35"/>
-      <c r="AZ38" s="35"/>
-      <c r="BA38" s="35"/>
-      <c r="BB38" s="35">
+      <c r="AY38" s="33"/>
+      <c r="AZ38" s="33"/>
+      <c r="BA38" s="33"/>
+      <c r="BB38" s="33">
         <v>2013</v>
       </c>
-      <c r="BC38" s="35"/>
-      <c r="BD38" s="35"/>
-      <c r="BE38" s="35"/>
-      <c r="BF38" s="35">
+      <c r="BC38" s="33"/>
+      <c r="BD38" s="33"/>
+      <c r="BE38" s="33"/>
+      <c r="BF38" s="33">
         <v>2014</v>
       </c>
-      <c r="BG38" s="35"/>
-      <c r="BH38" s="35"/>
-      <c r="BI38" s="35"/>
-      <c r="BJ38" s="35">
+      <c r="BG38" s="33"/>
+      <c r="BH38" s="33"/>
+      <c r="BI38" s="33"/>
+      <c r="BJ38" s="33">
         <v>2015</v>
       </c>
-      <c r="BK38" s="35"/>
-      <c r="BL38" s="35"/>
-      <c r="BM38" s="35"/>
-      <c r="BN38" s="35">
+      <c r="BK38" s="33"/>
+      <c r="BL38" s="33"/>
+      <c r="BM38" s="33"/>
+      <c r="BN38" s="33">
         <v>2016</v>
       </c>
-      <c r="BO38" s="35"/>
-      <c r="BP38" s="35"/>
-      <c r="BQ38" s="35"/>
+      <c r="BO38" s="33"/>
+      <c r="BP38" s="33"/>
+      <c r="BQ38" s="33"/>
       <c r="BR38" s="34">
         <v>2017</v>
       </c>
@@ -6292,8 +6319,9 @@
         <v>2022</v>
       </c>
       <c r="CM38" s="34"/>
+      <c r="CN38" s="34"/>
     </row>
-    <row r="39" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
@@ -6567,11 +6595,14 @@
       <c r="CM39" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="CN39" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="40" spans="1:153" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
@@ -6843,9 +6874,11 @@
         <v>1257238.1072275483</v>
       </c>
       <c r="CM41" s="10">
-        <v>1359793.6379108157</v>
-      </c>
-      <c r="CN41" s="11"/>
+        <v>1359377.1967343693</v>
+      </c>
+      <c r="CN41" s="10">
+        <v>1223797.3567871188</v>
+      </c>
       <c r="CO41" s="11"/>
       <c r="CP41" s="11"/>
       <c r="CQ41" s="11"/>
@@ -6908,7 +6941,7 @@
       <c r="EV41" s="11"/>
       <c r="EW41" s="11"/>
     </row>
-    <row r="42" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
@@ -7180,9 +7213,11 @@
         <v>50198.981533964208</v>
       </c>
       <c r="CM42" s="10">
-        <v>47912.342705809031</v>
-      </c>
-      <c r="CN42" s="11"/>
+        <v>48181.233384278457</v>
+      </c>
+      <c r="CN42" s="10">
+        <v>44607.164360110328</v>
+      </c>
       <c r="CO42" s="11"/>
       <c r="CP42" s="11"/>
       <c r="CQ42" s="11"/>
@@ -7245,7 +7280,7 @@
       <c r="EV42" s="11"/>
       <c r="EW42" s="11"/>
     </row>
-    <row r="43" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -7517,9 +7552,11 @@
         <v>54639.266418910112</v>
       </c>
       <c r="CM43" s="10">
-        <v>55970.074684183688</v>
-      </c>
-      <c r="CN43" s="11"/>
+        <v>55970.074684183695</v>
+      </c>
+      <c r="CN43" s="10">
+        <v>63680.949954978059</v>
+      </c>
       <c r="CO43" s="11"/>
       <c r="CP43" s="11"/>
       <c r="CQ43" s="11"/>
@@ -7582,7 +7619,7 @@
       <c r="EV43" s="11"/>
       <c r="EW43" s="11"/>
     </row>
-    <row r="44" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -7854,9 +7891,11 @@
         <v>427214.04576726747</v>
       </c>
       <c r="CM44" s="10">
-        <v>521578.42713518749</v>
-      </c>
-      <c r="CN44" s="11"/>
+        <v>521094.13428486529</v>
+      </c>
+      <c r="CN44" s="10">
+        <v>440204.03601303318</v>
+      </c>
       <c r="CO44" s="11"/>
       <c r="CP44" s="11"/>
       <c r="CQ44" s="11"/>
@@ -7919,7 +7958,7 @@
       <c r="EV44" s="11"/>
       <c r="EW44" s="11"/>
     </row>
-    <row r="45" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>8</v>
       </c>
@@ -8191,9 +8230,11 @@
         <v>94846.2622091511</v>
       </c>
       <c r="CM45" s="10">
-        <v>93256.232517505254</v>
-      </c>
-      <c r="CN45" s="11"/>
+        <v>92016.486939449867</v>
+      </c>
+      <c r="CN45" s="10">
+        <v>108355.21511056753</v>
+      </c>
       <c r="CO45" s="11"/>
       <c r="CP45" s="11"/>
       <c r="CQ45" s="11"/>
@@ -8256,7 +8297,7 @@
       <c r="EV45" s="11"/>
       <c r="EW45" s="11"/>
     </row>
-    <row r="46" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -8528,9 +8569,11 @@
         <v>150621.16349268309</v>
       </c>
       <c r="CM46" s="10">
-        <v>126639.21500560004</v>
-      </c>
-      <c r="CN46" s="11"/>
+        <v>126609.68897286928</v>
+      </c>
+      <c r="CN46" s="10">
+        <v>194356.15373197355</v>
+      </c>
       <c r="CO46" s="11"/>
       <c r="CP46" s="11"/>
       <c r="CQ46" s="11"/>
@@ -8593,7 +8636,7 @@
       <c r="EV46" s="11"/>
       <c r="EW46" s="11"/>
     </row>
-    <row r="47" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
@@ -8865,9 +8908,11 @@
         <v>312055.43731491663</v>
       </c>
       <c r="CM47" s="10">
-        <v>238129.69216395734</v>
-      </c>
-      <c r="CN47" s="11"/>
+        <v>237089.60293205726</v>
+      </c>
+      <c r="CN47" s="10">
+        <v>327756.35641066451</v>
+      </c>
       <c r="CO47" s="11"/>
       <c r="CP47" s="11"/>
       <c r="CQ47" s="11"/>
@@ -8930,7 +8975,7 @@
       <c r="EV47" s="11"/>
       <c r="EW47" s="11"/>
     </row>
-    <row r="48" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -9202,9 +9247,11 @@
         <v>115909.90445148885</v>
       </c>
       <c r="CM48" s="10">
-        <v>125381.5631915612</v>
-      </c>
-      <c r="CN48" s="11"/>
+        <v>124681.93067322711</v>
+      </c>
+      <c r="CN48" s="10">
+        <v>96723.354802973481</v>
+      </c>
       <c r="CO48" s="11"/>
       <c r="CP48" s="11"/>
       <c r="CQ48" s="11"/>
@@ -9267,7 +9314,7 @@
       <c r="EV48" s="11"/>
       <c r="EW48" s="11"/>
     </row>
-    <row r="49" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -9539,9 +9586,11 @@
         <v>53886.224246606071</v>
       </c>
       <c r="CM49" s="10">
-        <v>39799.817325731965</v>
-      </c>
-      <c r="CN49" s="11"/>
+        <v>40675.021685712061</v>
+      </c>
+      <c r="CN49" s="10">
+        <v>51283.064171945523</v>
+      </c>
       <c r="CO49" s="11"/>
       <c r="CP49" s="11"/>
       <c r="CQ49" s="11"/>
@@ -9604,7 +9653,7 @@
       <c r="EV49" s="11"/>
       <c r="EW49" s="11"/>
     </row>
-    <row r="50" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -9876,9 +9925,11 @@
         <v>197356.69930389794</v>
       </c>
       <c r="CM50" s="10">
-        <v>175132.12224164006</v>
-      </c>
-      <c r="CN50" s="11"/>
+        <v>175581.40026522669</v>
+      </c>
+      <c r="CN50" s="10">
+        <v>201819.05369660654</v>
+      </c>
       <c r="CO50" s="11"/>
       <c r="CP50" s="11"/>
       <c r="CQ50" s="11"/>
@@ -9941,7 +9992,7 @@
       <c r="EV50" s="11"/>
       <c r="EW50" s="11"/>
     </row>
-    <row r="51" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -10213,9 +10264,11 @@
         <v>282708.60999129753</v>
       </c>
       <c r="CM51" s="10">
-        <v>166923.42037536853</v>
-      </c>
-      <c r="CN51" s="11"/>
+        <v>168071.32293949748</v>
+      </c>
+      <c r="CN51" s="10">
+        <v>242385.99179231143</v>
+      </c>
       <c r="CO51" s="11"/>
       <c r="CP51" s="11"/>
       <c r="CQ51" s="11"/>
@@ -10278,7 +10331,7 @@
       <c r="EV51" s="11"/>
       <c r="EW51" s="11"/>
     </row>
-    <row r="52" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
@@ -10550,9 +10603,11 @@
         <v>476676.3395911071</v>
       </c>
       <c r="CM52" s="10">
-        <v>451000.60114325891</v>
-      </c>
-      <c r="CN52" s="11"/>
+        <v>449718.58169500902</v>
+      </c>
+      <c r="CN52" s="10">
+        <v>509520.5050821944</v>
+      </c>
       <c r="CO52" s="11"/>
       <c r="CP52" s="11"/>
       <c r="CQ52" s="11"/>
@@ -10615,7 +10670,7 @@
       <c r="EV52" s="11"/>
       <c r="EW52" s="11"/>
     </row>
-    <row r="53" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
@@ -10769,7 +10824,7 @@
       <c r="EV53" s="11"/>
       <c r="EW53" s="11"/>
     </row>
-    <row r="54" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>18</v>
       </c>
@@ -11025,25 +11080,27 @@
       <c r="CG54" s="15">
         <v>3648921.6749099772</v>
       </c>
-      <c r="CH54" s="31">
+      <c r="CH54" s="30">
         <v>3156671.4757222617</v>
       </c>
-      <c r="CI54" s="31">
+      <c r="CI54" s="30">
         <v>3131017.1444008318</v>
       </c>
-      <c r="CJ54" s="31">
+      <c r="CJ54" s="30">
         <v>3244927.2295096582</v>
       </c>
-      <c r="CK54" s="31">
+      <c r="CK54" s="30">
         <v>3923915.6638969723</v>
       </c>
-      <c r="CL54" s="31">
+      <c r="CL54" s="30">
         <v>3473351.0415488388</v>
       </c>
-      <c r="CM54" s="31">
-        <v>3401517.1464006188</v>
-      </c>
-      <c r="CN54" s="11"/>
+      <c r="CM54" s="30">
+        <v>3399066.6751907454</v>
+      </c>
+      <c r="CN54" s="30">
+        <v>3504489.2019144772</v>
+      </c>
       <c r="CO54" s="11"/>
       <c r="CP54" s="11"/>
       <c r="CQ54" s="11"/>
@@ -11106,7 +11163,7 @@
       <c r="EV54" s="11"/>
       <c r="EW54" s="11"/>
     </row>
-    <row r="55" spans="1:153" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:153" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="16"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -11198,13 +11255,14 @@
       <c r="CK55" s="16"/>
       <c r="CL55" s="16"/>
       <c r="CM55" s="16"/>
+      <c r="CN55" s="16"/>
     </row>
-    <row r="56" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
@@ -11358,7 +11416,7 @@
       <c r="EV57" s="11"/>
       <c r="EW57" s="11"/>
     </row>
-    <row r="58" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="23"/>
       <c r="C58" s="23"/>
       <c r="D58" s="23"/>
@@ -11443,13 +11501,13 @@
       <c r="CE58" s="24"/>
       <c r="CF58" s="24"/>
       <c r="CG58" s="24"/>
-      <c r="CH58" s="33"/>
-      <c r="CI58" s="33"/>
-      <c r="CJ58" s="33"/>
-      <c r="CK58" s="33"/>
-      <c r="CL58" s="33"/>
-      <c r="CM58" s="33"/>
-      <c r="CN58" s="11"/>
+      <c r="CH58" s="32"/>
+      <c r="CI58" s="32"/>
+      <c r="CJ58" s="32"/>
+      <c r="CK58" s="32"/>
+      <c r="CL58" s="32"/>
+      <c r="CM58" s="32"/>
+      <c r="CN58" s="32"/>
       <c r="CO58" s="11"/>
       <c r="CP58" s="11"/>
       <c r="CQ58" s="11"/>
@@ -11512,140 +11570,140 @@
       <c r="EV58" s="11"/>
       <c r="EW58" s="11"/>
     </row>
-    <row r="59" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35" t="s">
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35" t="s">
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K67" s="35"/>
-      <c r="L67" s="35"/>
-      <c r="M67" s="35"/>
-      <c r="N67" s="35" t="s">
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="O67" s="35"/>
-      <c r="P67" s="35"/>
-      <c r="Q67" s="35"/>
-      <c r="R67" s="35" t="s">
+      <c r="O67" s="33"/>
+      <c r="P67" s="33"/>
+      <c r="Q67" s="33"/>
+      <c r="R67" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="S67" s="35"/>
-      <c r="T67" s="35"/>
-      <c r="U67" s="35"/>
-      <c r="V67" s="35" t="s">
+      <c r="S67" s="33"/>
+      <c r="T67" s="33"/>
+      <c r="U67" s="33"/>
+      <c r="V67" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="W67" s="35"/>
-      <c r="X67" s="35"/>
-      <c r="Y67" s="35"/>
-      <c r="Z67" s="35" t="s">
+      <c r="W67" s="33"/>
+      <c r="X67" s="33"/>
+      <c r="Y67" s="33"/>
+      <c r="Z67" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AA67" s="35"/>
-      <c r="AB67" s="35"/>
-      <c r="AC67" s="35"/>
-      <c r="AD67" s="35" t="s">
+      <c r="AA67" s="33"/>
+      <c r="AB67" s="33"/>
+      <c r="AC67" s="33"/>
+      <c r="AD67" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="AE67" s="35"/>
-      <c r="AF67" s="35"/>
-      <c r="AG67" s="35"/>
-      <c r="AH67" s="35" t="s">
+      <c r="AE67" s="33"/>
+      <c r="AF67" s="33"/>
+      <c r="AG67" s="33"/>
+      <c r="AH67" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="AI67" s="35"/>
-      <c r="AJ67" s="35"/>
-      <c r="AK67" s="35"/>
-      <c r="AL67" s="35" t="s">
+      <c r="AI67" s="33"/>
+      <c r="AJ67" s="33"/>
+      <c r="AK67" s="33"/>
+      <c r="AL67" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="AM67" s="35"/>
-      <c r="AN67" s="35"/>
-      <c r="AO67" s="35"/>
-      <c r="AP67" s="35" t="s">
+      <c r="AM67" s="33"/>
+      <c r="AN67" s="33"/>
+      <c r="AO67" s="33"/>
+      <c r="AP67" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="AQ67" s="35"/>
-      <c r="AR67" s="35"/>
-      <c r="AS67" s="35"/>
-      <c r="AT67" s="35" t="s">
+      <c r="AQ67" s="33"/>
+      <c r="AR67" s="33"/>
+      <c r="AS67" s="33"/>
+      <c r="AT67" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AU67" s="35"/>
-      <c r="AV67" s="35"/>
-      <c r="AW67" s="35"/>
-      <c r="AX67" s="35" t="s">
+      <c r="AU67" s="33"/>
+      <c r="AV67" s="33"/>
+      <c r="AW67" s="33"/>
+      <c r="AX67" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="AY67" s="35"/>
-      <c r="AZ67" s="35"/>
-      <c r="BA67" s="35"/>
-      <c r="BB67" s="35" t="s">
+      <c r="AY67" s="33"/>
+      <c r="AZ67" s="33"/>
+      <c r="BA67" s="33"/>
+      <c r="BB67" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="BC67" s="35"/>
-      <c r="BD67" s="35"/>
-      <c r="BE67" s="35"/>
-      <c r="BF67" s="35" t="s">
+      <c r="BC67" s="33"/>
+      <c r="BD67" s="33"/>
+      <c r="BE67" s="33"/>
+      <c r="BF67" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="BG67" s="35"/>
-      <c r="BH67" s="35"/>
-      <c r="BI67" s="35"/>
-      <c r="BJ67" s="35" t="s">
+      <c r="BG67" s="33"/>
+      <c r="BH67" s="33"/>
+      <c r="BI67" s="33"/>
+      <c r="BJ67" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="BK67" s="35"/>
-      <c r="BL67" s="35"/>
-      <c r="BM67" s="35"/>
-      <c r="BN67" s="35" t="s">
+      <c r="BK67" s="33"/>
+      <c r="BL67" s="33"/>
+      <c r="BM67" s="33"/>
+      <c r="BN67" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="BO67" s="35"/>
-      <c r="BP67" s="35"/>
-      <c r="BQ67" s="35"/>
+      <c r="BO67" s="33"/>
+      <c r="BP67" s="33"/>
+      <c r="BQ67" s="33"/>
       <c r="BR67" s="34" t="s">
         <v>34</v>
       </c>
@@ -11674,12 +11732,13 @@
         <v>57</v>
       </c>
       <c r="CI67" s="34"/>
-      <c r="CJ67" s="4"/>
+      <c r="CJ67" s="34"/>
       <c r="CK67" s="4"/>
-      <c r="CL67" s="30"/>
-      <c r="CM67" s="4"/>
+      <c r="CL67" s="34"/>
+      <c r="CM67" s="34"/>
+      <c r="CN67" s="4"/>
     </row>
-    <row r="68" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>37</v>
       </c>
@@ -11941,15 +12000,18 @@
       <c r="CI68" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CJ68" s="7"/>
+      <c r="CJ68" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="CK68" s="7"/>
       <c r="CL68" s="7"/>
       <c r="CM68" s="7"/>
+      <c r="CN68" s="7"/>
     </row>
-    <row r="69" spans="1:149" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
     </row>
-    <row r="70" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
@@ -12209,13 +12271,15 @@
         <v>11.950152669019531</v>
       </c>
       <c r="CI70" s="26">
-        <v>11.774689710196995</v>
-      </c>
-      <c r="CJ70" s="26"/>
+        <v>11.740458351862841</v>
+      </c>
+      <c r="CJ70" s="26">
+        <v>11.151227845362868</v>
+      </c>
       <c r="CK70" s="26"/>
       <c r="CL70" s="26"/>
-      <c r="CM70" s="11"/>
-      <c r="CN70" s="11"/>
+      <c r="CM70" s="26"/>
+      <c r="CN70" s="26"/>
       <c r="CO70" s="11"/>
       <c r="CP70" s="11"/>
       <c r="CQ70" s="11"/>
@@ -12274,7 +12338,7 @@
       <c r="ER70" s="11"/>
       <c r="ES70" s="11"/>
     </row>
-    <row r="71" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
@@ -12534,13 +12598,15 @@
         <v>11.853475217909363</v>
       </c>
       <c r="CI71" s="26">
-        <v>9.6345039267237524</v>
-      </c>
-      <c r="CJ71" s="26"/>
+        <v>10.249787890722899</v>
+      </c>
+      <c r="CJ71" s="26">
+        <v>-1.7502827870363404</v>
+      </c>
       <c r="CK71" s="26"/>
       <c r="CL71" s="26"/>
-      <c r="CM71" s="11"/>
-      <c r="CN71" s="11"/>
+      <c r="CM71" s="26"/>
+      <c r="CN71" s="26"/>
       <c r="CO71" s="11"/>
       <c r="CP71" s="11"/>
       <c r="CQ71" s="11"/>
@@ -12599,7 +12665,7 @@
       <c r="ER71" s="11"/>
       <c r="ES71" s="11"/>
     </row>
-    <row r="72" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
@@ -12861,11 +12927,13 @@
       <c r="CI72" s="26">
         <v>7.1613224771094792</v>
       </c>
-      <c r="CJ72" s="26"/>
+      <c r="CJ72" s="26">
+        <v>-2.9400297906872623</v>
+      </c>
       <c r="CK72" s="26"/>
       <c r="CL72" s="26"/>
-      <c r="CM72" s="11"/>
-      <c r="CN72" s="11"/>
+      <c r="CM72" s="26"/>
+      <c r="CN72" s="26"/>
       <c r="CO72" s="11"/>
       <c r="CP72" s="11"/>
       <c r="CQ72" s="11"/>
@@ -12924,7 +12992,7 @@
       <c r="ER72" s="11"/>
       <c r="ES72" s="11"/>
     </row>
-    <row r="73" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>9</v>
       </c>
@@ -13184,13 +13252,15 @@
         <v>11.407602824630359</v>
       </c>
       <c r="CI73" s="26">
-        <v>14.097769382171307</v>
-      </c>
-      <c r="CJ73" s="26"/>
+        <v>13.99182801060617</v>
+      </c>
+      <c r="CJ73" s="26">
+        <v>9.1587849685091527</v>
+      </c>
       <c r="CK73" s="26"/>
       <c r="CL73" s="26"/>
-      <c r="CM73" s="11"/>
-      <c r="CN73" s="11"/>
+      <c r="CM73" s="26"/>
+      <c r="CN73" s="26"/>
       <c r="CO73" s="11"/>
       <c r="CP73" s="11"/>
       <c r="CQ73" s="11"/>
@@ -13249,7 +13319,7 @@
       <c r="ER73" s="11"/>
       <c r="ES73" s="11"/>
     </row>
-    <row r="74" spans="1:149" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:149" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
         <v>8</v>
       </c>
@@ -13509,13 +13579,15 @@
         <v>11.072394012374389</v>
       </c>
       <c r="CI74" s="26">
-        <v>11.357262448822226</v>
-      </c>
-      <c r="CJ74" s="26"/>
+        <v>9.8768823178817229</v>
+      </c>
+      <c r="CJ74" s="26">
+        <v>13.128951967603626</v>
+      </c>
       <c r="CK74" s="26"/>
       <c r="CL74" s="26"/>
-      <c r="CM74" s="11"/>
-      <c r="CN74" s="11"/>
+      <c r="CM74" s="26"/>
+      <c r="CN74" s="26"/>
       <c r="CO74" s="11"/>
       <c r="CP74" s="11"/>
       <c r="CQ74" s="11"/>
@@ -13574,7 +13646,7 @@
       <c r="ER74" s="11"/>
       <c r="ES74" s="11"/>
     </row>
-    <row r="75" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
@@ -13834,13 +13906,15 @@
         <v>3.8539330160627827</v>
       </c>
       <c r="CI75" s="26">
-        <v>-3.2490572877989621E-2</v>
-      </c>
-      <c r="CJ75" s="26"/>
+        <v>-5.5798076444133926E-2</v>
+      </c>
+      <c r="CJ75" s="26">
+        <v>9.5001212693810828</v>
+      </c>
       <c r="CK75" s="26"/>
       <c r="CL75" s="26"/>
-      <c r="CM75" s="11"/>
-      <c r="CN75" s="11"/>
+      <c r="CM75" s="26"/>
+      <c r="CN75" s="26"/>
       <c r="CO75" s="11"/>
       <c r="CP75" s="11"/>
       <c r="CQ75" s="11"/>
@@ -13899,7 +13973,7 @@
       <c r="ER75" s="11"/>
       <c r="ES75" s="11"/>
     </row>
-    <row r="76" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -14159,13 +14233,15 @@
         <v>26.071426339240304</v>
       </c>
       <c r="CI76" s="26">
-        <v>44.461671434839133</v>
-      </c>
-      <c r="CJ76" s="26"/>
+        <v>43.830700019572674</v>
+      </c>
+      <c r="CJ76" s="26">
+        <v>39.405611281779471</v>
+      </c>
       <c r="CK76" s="26"/>
       <c r="CL76" s="26"/>
-      <c r="CM76" s="11"/>
-      <c r="CN76" s="11"/>
+      <c r="CM76" s="26"/>
+      <c r="CN76" s="26"/>
       <c r="CO76" s="11"/>
       <c r="CP76" s="11"/>
       <c r="CQ76" s="11"/>
@@ -14224,7 +14300,7 @@
       <c r="ER76" s="11"/>
       <c r="ES76" s="11"/>
     </row>
-    <row r="77" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -14484,13 +14560,15 @@
         <v>7.7006334235734499</v>
       </c>
       <c r="CI77" s="26">
-        <v>10.939979233635015</v>
-      </c>
-      <c r="CJ77" s="26"/>
+        <v>10.320931144909437</v>
+      </c>
+      <c r="CJ77" s="26">
+        <v>7.780031501783796</v>
+      </c>
       <c r="CK77" s="26"/>
       <c r="CL77" s="26"/>
-      <c r="CM77" s="11"/>
-      <c r="CN77" s="11"/>
+      <c r="CM77" s="26"/>
+      <c r="CN77" s="26"/>
       <c r="CO77" s="11"/>
       <c r="CP77" s="11"/>
       <c r="CQ77" s="11"/>
@@ -14549,7 +14627,7 @@
       <c r="ER77" s="11"/>
       <c r="ES77" s="11"/>
     </row>
-    <row r="78" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
@@ -14809,13 +14887,15 @@
         <v>18.08872700967035</v>
       </c>
       <c r="CI78" s="26">
-        <v>37.318151602676693</v>
-      </c>
-      <c r="CJ78" s="26"/>
+        <v>40.337799758432624</v>
+      </c>
+      <c r="CJ78" s="26">
+        <v>49.490424187724415</v>
+      </c>
       <c r="CK78" s="26"/>
       <c r="CL78" s="26"/>
-      <c r="CM78" s="11"/>
-      <c r="CN78" s="11"/>
+      <c r="CM78" s="26"/>
+      <c r="CN78" s="26"/>
       <c r="CO78" s="11"/>
       <c r="CP78" s="11"/>
       <c r="CQ78" s="11"/>
@@ -14874,7 +14954,7 @@
       <c r="ER78" s="11"/>
       <c r="ES78" s="11"/>
     </row>
-    <row r="79" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>3</v>
       </c>
@@ -15134,13 +15214,15 @@
         <v>12.108892270262899</v>
       </c>
       <c r="CI79" s="26">
-        <v>7.8475707414959288</v>
-      </c>
-      <c r="CJ79" s="26"/>
+        <v>8.1242392521675839</v>
+      </c>
+      <c r="CJ79" s="26">
+        <v>8.453074846232127</v>
+      </c>
       <c r="CK79" s="26"/>
       <c r="CL79" s="26"/>
-      <c r="CM79" s="11"/>
-      <c r="CN79" s="11"/>
+      <c r="CM79" s="26"/>
+      <c r="CN79" s="26"/>
       <c r="CO79" s="11"/>
       <c r="CP79" s="11"/>
       <c r="CQ79" s="11"/>
@@ -15199,7 +15281,7 @@
       <c r="ER79" s="11"/>
       <c r="ES79" s="11"/>
     </row>
-    <row r="80" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
@@ -15459,13 +15541,15 @@
         <v>23.295892172965438</v>
       </c>
       <c r="CI80" s="26">
-        <v>36.05248457268965</v>
-      </c>
-      <c r="CJ80" s="26"/>
+        <v>36.98809322212847</v>
+      </c>
+      <c r="CJ80" s="26">
+        <v>44.461553239018315</v>
+      </c>
       <c r="CK80" s="26"/>
       <c r="CL80" s="26"/>
-      <c r="CM80" s="11"/>
-      <c r="CN80" s="11"/>
+      <c r="CM80" s="26"/>
+      <c r="CN80" s="26"/>
       <c r="CO80" s="11"/>
       <c r="CP80" s="11"/>
       <c r="CQ80" s="11"/>
@@ -15524,7 +15608,7 @@
       <c r="ER80" s="11"/>
       <c r="ES80" s="11"/>
     </row>
-    <row r="81" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
@@ -15784,13 +15868,15 @@
         <v>11.327847732547809</v>
       </c>
       <c r="CI81" s="26">
-        <v>10.722249790118951</v>
-      </c>
-      <c r="CJ81" s="26"/>
+        <v>10.40750946111477</v>
+      </c>
+      <c r="CJ81" s="26">
+        <v>13.497300320640363</v>
+      </c>
       <c r="CK81" s="26"/>
       <c r="CL81" s="26"/>
-      <c r="CM81" s="11"/>
-      <c r="CN81" s="11"/>
+      <c r="CM81" s="26"/>
+      <c r="CN81" s="26"/>
       <c r="CO81" s="11"/>
       <c r="CP81" s="11"/>
       <c r="CQ81" s="11"/>
@@ -15849,7 +15935,7 @@
       <c r="ER81" s="11"/>
       <c r="ES81" s="11"/>
     </row>
-    <row r="82" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
@@ -15999,7 +16085,7 @@
       <c r="ER82" s="11"/>
       <c r="ES82" s="11"/>
     </row>
-    <row r="83" spans="1:149" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:149" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12" t="s">
         <v>18</v>
       </c>
@@ -16259,13 +16345,15 @@
         <v>13.431422246443077</v>
       </c>
       <c r="CI83" s="26">
-        <v>14.284416670868325</v>
-      </c>
-      <c r="CJ83" s="26"/>
+        <v>14.1993530748247</v>
+      </c>
+      <c r="CJ83" s="26">
+        <v>15.24609706166909</v>
+      </c>
       <c r="CK83" s="26"/>
       <c r="CL83" s="26"/>
-      <c r="CM83" s="11"/>
-      <c r="CN83" s="11"/>
+      <c r="CM83" s="26"/>
+      <c r="CN83" s="26"/>
       <c r="CO83" s="11"/>
       <c r="CP83" s="11"/>
       <c r="CQ83" s="11"/>
@@ -16324,7 +16412,7 @@
       <c r="ER83" s="11"/>
       <c r="ES83" s="11"/>
     </row>
-    <row r="84" spans="1:149" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:149" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -16416,13 +16504,14 @@
       <c r="CK84" s="16"/>
       <c r="CL84" s="16"/>
       <c r="CM84" s="16"/>
+      <c r="CN84" s="16"/>
     </row>
-    <row r="85" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
@@ -16572,7 +16661,7 @@
       <c r="ER86" s="11"/>
       <c r="ES86" s="11"/>
     </row>
-    <row r="87" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
@@ -16722,140 +16811,140 @@
       <c r="ER87" s="11"/>
       <c r="ES87" s="11"/>
     </row>
-    <row r="88" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
-      <c r="B96" s="35" t="s">
+      <c r="B96" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C96" s="35"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="35" t="s">
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G96" s="35"/>
-      <c r="H96" s="35"/>
-      <c r="I96" s="35"/>
-      <c r="J96" s="35" t="s">
+      <c r="G96" s="33"/>
+      <c r="H96" s="33"/>
+      <c r="I96" s="33"/>
+      <c r="J96" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K96" s="35"/>
-      <c r="L96" s="35"/>
-      <c r="M96" s="35"/>
-      <c r="N96" s="35" t="s">
+      <c r="K96" s="33"/>
+      <c r="L96" s="33"/>
+      <c r="M96" s="33"/>
+      <c r="N96" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="O96" s="35"/>
-      <c r="P96" s="35"/>
-      <c r="Q96" s="35"/>
-      <c r="R96" s="35" t="s">
+      <c r="O96" s="33"/>
+      <c r="P96" s="33"/>
+      <c r="Q96" s="33"/>
+      <c r="R96" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="S96" s="35"/>
-      <c r="T96" s="35"/>
-      <c r="U96" s="35"/>
-      <c r="V96" s="35" t="s">
+      <c r="S96" s="33"/>
+      <c r="T96" s="33"/>
+      <c r="U96" s="33"/>
+      <c r="V96" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="W96" s="35"/>
-      <c r="X96" s="35"/>
-      <c r="Y96" s="35"/>
-      <c r="Z96" s="35" t="s">
+      <c r="W96" s="33"/>
+      <c r="X96" s="33"/>
+      <c r="Y96" s="33"/>
+      <c r="Z96" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AA96" s="35"/>
-      <c r="AB96" s="35"/>
-      <c r="AC96" s="35"/>
-      <c r="AD96" s="35" t="s">
+      <c r="AA96" s="33"/>
+      <c r="AB96" s="33"/>
+      <c r="AC96" s="33"/>
+      <c r="AD96" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="AE96" s="35"/>
-      <c r="AF96" s="35"/>
-      <c r="AG96" s="35"/>
-      <c r="AH96" s="35" t="s">
+      <c r="AE96" s="33"/>
+      <c r="AF96" s="33"/>
+      <c r="AG96" s="33"/>
+      <c r="AH96" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="AI96" s="35"/>
-      <c r="AJ96" s="35"/>
-      <c r="AK96" s="35"/>
-      <c r="AL96" s="35" t="s">
+      <c r="AI96" s="33"/>
+      <c r="AJ96" s="33"/>
+      <c r="AK96" s="33"/>
+      <c r="AL96" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="AM96" s="35"/>
-      <c r="AN96" s="35"/>
-      <c r="AO96" s="35"/>
-      <c r="AP96" s="35" t="s">
+      <c r="AM96" s="33"/>
+      <c r="AN96" s="33"/>
+      <c r="AO96" s="33"/>
+      <c r="AP96" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="AQ96" s="35"/>
-      <c r="AR96" s="35"/>
-      <c r="AS96" s="35"/>
-      <c r="AT96" s="35" t="s">
+      <c r="AQ96" s="33"/>
+      <c r="AR96" s="33"/>
+      <c r="AS96" s="33"/>
+      <c r="AT96" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AU96" s="35"/>
-      <c r="AV96" s="35"/>
-      <c r="AW96" s="35"/>
-      <c r="AX96" s="35" t="s">
+      <c r="AU96" s="33"/>
+      <c r="AV96" s="33"/>
+      <c r="AW96" s="33"/>
+      <c r="AX96" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="AY96" s="35"/>
-      <c r="AZ96" s="35"/>
-      <c r="BA96" s="35"/>
-      <c r="BB96" s="35" t="s">
+      <c r="AY96" s="33"/>
+      <c r="AZ96" s="33"/>
+      <c r="BA96" s="33"/>
+      <c r="BB96" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="BC96" s="35"/>
-      <c r="BD96" s="35"/>
-      <c r="BE96" s="35"/>
-      <c r="BF96" s="35" t="s">
+      <c r="BC96" s="33"/>
+      <c r="BD96" s="33"/>
+      <c r="BE96" s="33"/>
+      <c r="BF96" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="BG96" s="35"/>
-      <c r="BH96" s="35"/>
-      <c r="BI96" s="35"/>
-      <c r="BJ96" s="35" t="s">
+      <c r="BG96" s="33"/>
+      <c r="BH96" s="33"/>
+      <c r="BI96" s="33"/>
+      <c r="BJ96" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="BK96" s="35"/>
-      <c r="BL96" s="35"/>
-      <c r="BM96" s="35"/>
-      <c r="BN96" s="35" t="s">
+      <c r="BK96" s="33"/>
+      <c r="BL96" s="33"/>
+      <c r="BM96" s="33"/>
+      <c r="BN96" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="BO96" s="35"/>
-      <c r="BP96" s="35"/>
-      <c r="BQ96" s="35"/>
+      <c r="BO96" s="33"/>
+      <c r="BP96" s="33"/>
+      <c r="BQ96" s="33"/>
       <c r="BR96" s="34" t="s">
         <v>34</v>
       </c>
@@ -16884,12 +16973,13 @@
         <v>57</v>
       </c>
       <c r="CI96" s="34"/>
-      <c r="CJ96" s="4"/>
+      <c r="CJ96" s="34"/>
       <c r="CK96" s="4"/>
-      <c r="CL96" s="30"/>
-      <c r="CM96" s="30"/>
+      <c r="CL96" s="34"/>
+      <c r="CM96" s="34"/>
+      <c r="CN96" s="4"/>
     </row>
-    <row r="97" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>37</v>
       </c>
@@ -17151,15 +17241,18 @@
       <c r="CI97" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CJ97" s="7"/>
+      <c r="CJ97" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="CK97" s="7"/>
       <c r="CL97" s="7"/>
       <c r="CM97" s="7"/>
+      <c r="CN97" s="7"/>
     </row>
-    <row r="98" spans="1:149" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
     </row>
-    <row r="99" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
@@ -17419,13 +17512,15 @@
         <v>9.9504476496265113</v>
       </c>
       <c r="CI99" s="26">
-        <v>5.7624797140016568</v>
-      </c>
-      <c r="CJ99" s="26"/>
+        <v>5.7300896143217699</v>
+      </c>
+      <c r="CJ99" s="26">
+        <v>3.8964820872820098</v>
+      </c>
       <c r="CK99" s="26"/>
       <c r="CL99" s="26"/>
-      <c r="CM99" s="11"/>
-      <c r="CN99" s="11"/>
+      <c r="CM99" s="26"/>
+      <c r="CN99" s="26"/>
       <c r="CO99" s="11"/>
       <c r="CP99" s="11"/>
       <c r="CQ99" s="11"/>
@@ -17484,7 +17579,7 @@
       <c r="ER99" s="11"/>
       <c r="ES99" s="11"/>
     </row>
-    <row r="100" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>11</v>
       </c>
@@ -17744,13 +17839,15 @@
         <v>6.4955304652266221</v>
       </c>
       <c r="CI100" s="26">
-        <v>2.1587446497476321</v>
-      </c>
-      <c r="CJ100" s="26"/>
+        <v>2.7320736211386532</v>
+      </c>
+      <c r="CJ100" s="26">
+        <v>-10.039445224275696</v>
+      </c>
       <c r="CK100" s="26"/>
       <c r="CL100" s="26"/>
-      <c r="CM100" s="11"/>
-      <c r="CN100" s="11"/>
+      <c r="CM100" s="26"/>
+      <c r="CN100" s="26"/>
       <c r="CO100" s="11"/>
       <c r="CP100" s="11"/>
       <c r="CQ100" s="11"/>
@@ -17809,7 +17906,7 @@
       <c r="ER100" s="11"/>
       <c r="ES100" s="11"/>
     </row>
-    <row r="101" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -18071,11 +18168,13 @@
       <c r="CI101" s="26">
         <v>4.464427553075339</v>
       </c>
-      <c r="CJ101" s="26"/>
+      <c r="CJ101" s="26">
+        <v>-5.5243799808292948</v>
+      </c>
       <c r="CK101" s="26"/>
       <c r="CL101" s="26"/>
-      <c r="CM101" s="11"/>
-      <c r="CN101" s="11"/>
+      <c r="CM101" s="26"/>
+      <c r="CN101" s="26"/>
       <c r="CO101" s="11"/>
       <c r="CP101" s="11"/>
       <c r="CQ101" s="11"/>
@@ -18134,7 +18233,7 @@
       <c r="ER101" s="11"/>
       <c r="ES101" s="11"/>
     </row>
-    <row r="102" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>9</v>
       </c>
@@ -18394,13 +18493,15 @@
         <v>5.9185421015190087</v>
       </c>
       <c r="CI102" s="26">
-        <v>6.9794309341492777</v>
-      </c>
-      <c r="CJ102" s="26"/>
+        <v>6.8800990391981998</v>
+      </c>
+      <c r="CJ102" s="26">
+        <v>1.3308625699598053</v>
+      </c>
       <c r="CK102" s="26"/>
       <c r="CL102" s="26"/>
-      <c r="CM102" s="11"/>
-      <c r="CN102" s="11"/>
+      <c r="CM102" s="26"/>
+      <c r="CN102" s="26"/>
       <c r="CO102" s="11"/>
       <c r="CP102" s="11"/>
       <c r="CQ102" s="11"/>
@@ -18459,7 +18560,7 @@
       <c r="ER102" s="11"/>
       <c r="ES102" s="11"/>
     </row>
-    <row r="103" spans="1:149" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:149" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
         <v>8</v>
       </c>
@@ -18719,13 +18820,15 @@
         <v>8.4182139981645747</v>
       </c>
       <c r="CI103" s="26">
-        <v>8.4848195662191159</v>
-      </c>
-      <c r="CJ103" s="26"/>
+        <v>7.042625605422856</v>
+      </c>
+      <c r="CJ103" s="26">
+        <v>9.4731394077255118</v>
+      </c>
       <c r="CK103" s="26"/>
       <c r="CL103" s="26"/>
-      <c r="CM103" s="11"/>
-      <c r="CN103" s="11"/>
+      <c r="CM103" s="26"/>
+      <c r="CN103" s="26"/>
       <c r="CO103" s="11"/>
       <c r="CP103" s="11"/>
       <c r="CQ103" s="11"/>
@@ -18784,7 +18887,7 @@
       <c r="ER103" s="11"/>
       <c r="ES103" s="11"/>
     </row>
-    <row r="104" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>7</v>
       </c>
@@ -19044,13 +19147,15 @@
         <v>1.0585667675321559</v>
       </c>
       <c r="CI104" s="26">
-        <v>-2.4473052650931066</v>
-      </c>
-      <c r="CJ104" s="26"/>
+        <v>-2.4700497527116454</v>
+      </c>
+      <c r="CJ104" s="26">
+        <v>6.9095240552757389</v>
+      </c>
       <c r="CK104" s="26"/>
       <c r="CL104" s="26"/>
-      <c r="CM104" s="11"/>
-      <c r="CN104" s="11"/>
+      <c r="CM104" s="26"/>
+      <c r="CN104" s="26"/>
       <c r="CO104" s="11"/>
       <c r="CP104" s="11"/>
       <c r="CQ104" s="11"/>
@@ -19109,7 +19214,7 @@
       <c r="ER104" s="11"/>
       <c r="ES104" s="11"/>
     </row>
-    <row r="105" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -19369,13 +19474,15 @@
         <v>15.960257541421257</v>
       </c>
       <c r="CI105" s="26">
-        <v>25.725384716907243</v>
-      </c>
-      <c r="CJ105" s="26"/>
+        <v>25.17624858175229</v>
+      </c>
+      <c r="CJ105" s="26">
+        <v>20.460381599681469</v>
+      </c>
       <c r="CK105" s="26"/>
       <c r="CL105" s="26"/>
-      <c r="CM105" s="11"/>
-      <c r="CN105" s="11"/>
+      <c r="CM105" s="26"/>
+      <c r="CN105" s="26"/>
       <c r="CO105" s="11"/>
       <c r="CP105" s="11"/>
       <c r="CQ105" s="11"/>
@@ -19434,7 +19541,7 @@
       <c r="ER105" s="11"/>
       <c r="ES105" s="11"/>
     </row>
-    <row r="106" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -19694,13 +19801,15 @@
         <v>6.9962473318561536</v>
       </c>
       <c r="CI106" s="26">
-        <v>10.251136225321574</v>
-      </c>
-      <c r="CJ106" s="26"/>
+        <v>9.6359318992384146</v>
+      </c>
+      <c r="CJ106" s="26">
+        <v>7.287242330972262</v>
+      </c>
       <c r="CK106" s="26"/>
       <c r="CL106" s="26"/>
-      <c r="CM106" s="11"/>
-      <c r="CN106" s="11"/>
+      <c r="CM106" s="26"/>
+      <c r="CN106" s="26"/>
       <c r="CO106" s="11"/>
       <c r="CP106" s="11"/>
       <c r="CQ106" s="11"/>
@@ -19759,7 +19868,7 @@
       <c r="ER106" s="11"/>
       <c r="ES106" s="11"/>
     </row>
-    <row r="107" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>4</v>
       </c>
@@ -20019,13 +20128,15 @@
         <v>16.267402608199205</v>
       </c>
       <c r="CI107" s="26">
-        <v>34.952821712871753</v>
-      </c>
-      <c r="CJ107" s="26"/>
+        <v>37.920455885362259</v>
+      </c>
+      <c r="CJ107" s="26">
+        <v>45.96864110084681</v>
+      </c>
       <c r="CK107" s="26"/>
       <c r="CL107" s="26"/>
-      <c r="CM107" s="11"/>
-      <c r="CN107" s="11"/>
+      <c r="CM107" s="26"/>
+      <c r="CN107" s="26"/>
       <c r="CO107" s="11"/>
       <c r="CP107" s="11"/>
       <c r="CQ107" s="11"/>
@@ -20084,7 +20195,7 @@
       <c r="ER107" s="11"/>
       <c r="ES107" s="11"/>
     </row>
-    <row r="108" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
@@ -20344,13 +20455,15 @@
         <v>11.482001912740486</v>
       </c>
       <c r="CI108" s="26">
-        <v>7.2445088361380812</v>
-      </c>
-      <c r="CJ108" s="26"/>
+        <v>7.5196302721927282</v>
+      </c>
+      <c r="CJ108" s="26">
+        <v>5.4235924203911594</v>
+      </c>
       <c r="CK108" s="26"/>
       <c r="CL108" s="26"/>
-      <c r="CM108" s="11"/>
-      <c r="CN108" s="11"/>
+      <c r="CM108" s="26"/>
+      <c r="CN108" s="26"/>
       <c r="CO108" s="11"/>
       <c r="CP108" s="11"/>
       <c r="CQ108" s="11"/>
@@ -20409,7 +20522,7 @@
       <c r="ER108" s="11"/>
       <c r="ES108" s="11"/>
     </row>
-    <row r="109" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>2</v>
       </c>
@@ -20669,13 +20782,15 @@
         <v>19.780553110410892</v>
       </c>
       <c r="CI109" s="26">
-        <v>32.338292115512388</v>
-      </c>
-      <c r="CJ109" s="26"/>
+        <v>33.248358926450209</v>
+      </c>
+      <c r="CJ109" s="26">
+        <v>38.234942116316432</v>
+      </c>
       <c r="CK109" s="26"/>
       <c r="CL109" s="26"/>
-      <c r="CM109" s="11"/>
-      <c r="CN109" s="11"/>
+      <c r="CM109" s="26"/>
+      <c r="CN109" s="26"/>
       <c r="CO109" s="11"/>
       <c r="CP109" s="11"/>
       <c r="CQ109" s="11"/>
@@ -20734,7 +20849,7 @@
       <c r="ER109" s="11"/>
       <c r="ES109" s="11"/>
     </row>
-    <row r="110" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>1</v>
       </c>
@@ -20994,13 +21109,15 @@
         <v>8.6439596750421401</v>
       </c>
       <c r="CI110" s="26">
-        <v>7.5219911348847006</v>
-      </c>
-      <c r="CJ110" s="26"/>
+        <v>7.216347897602887</v>
+      </c>
+      <c r="CJ110" s="26">
+        <v>8.2502579963249332</v>
+      </c>
       <c r="CK110" s="26"/>
       <c r="CL110" s="26"/>
-      <c r="CM110" s="11"/>
-      <c r="CN110" s="11"/>
+      <c r="CM110" s="26"/>
+      <c r="CN110" s="26"/>
       <c r="CO110" s="11"/>
       <c r="CP110" s="11"/>
       <c r="CQ110" s="11"/>
@@ -21059,7 +21176,7 @@
       <c r="ER110" s="11"/>
       <c r="ES110" s="11"/>
     </row>
-    <row r="111" spans="1:149" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="13"/>
       <c r="C111" s="13"/>
       <c r="D111" s="13"/>
@@ -21209,7 +21326,7 @@
       <c r="ER111" s="11"/>
       <c r="ES111" s="11"/>
     </row>
-    <row r="112" spans="1:149" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:149" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
         <v>18</v>
       </c>
@@ -21469,13 +21586,15 @@
         <v>10.032072335120617</v>
       </c>
       <c r="CI112" s="26">
-        <v>8.6393650856725515</v>
-      </c>
-      <c r="CJ112" s="26"/>
+        <v>8.5611007039442057</v>
+      </c>
+      <c r="CJ112" s="26">
+        <v>7.9990074983604842</v>
+      </c>
       <c r="CK112" s="26"/>
       <c r="CL112" s="26"/>
-      <c r="CM112" s="11"/>
-      <c r="CN112" s="11"/>
+      <c r="CM112" s="26"/>
+      <c r="CN112" s="26"/>
       <c r="CO112" s="11"/>
       <c r="CP112" s="11"/>
       <c r="CQ112" s="11"/>
@@ -21534,7 +21653,7 @@
       <c r="ER112" s="11"/>
       <c r="ES112" s="11"/>
     </row>
-    <row r="113" spans="1:153" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:153" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="16"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
@@ -21626,13 +21745,14 @@
       <c r="CK113" s="16"/>
       <c r="CL113" s="16"/>
       <c r="CM113" s="16"/>
+      <c r="CN113" s="16"/>
     </row>
-    <row r="114" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
       <c r="D115" s="13"/>
@@ -21782,7 +21902,7 @@
       <c r="ER115" s="11"/>
       <c r="ES115" s="11"/>
     </row>
-    <row r="116" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
@@ -21932,135 +22052,135 @@
       <c r="ER116" s="11"/>
       <c r="ES116" s="11"/>
     </row>
-    <row r="117" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
-      <c r="B124" s="35">
+      <c r="B124" s="33">
         <v>2000</v>
       </c>
-      <c r="C124" s="35"/>
-      <c r="D124" s="35"/>
-      <c r="E124" s="35"/>
-      <c r="F124" s="35">
+      <c r="C124" s="33"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="33"/>
+      <c r="F124" s="33">
         <v>2001</v>
       </c>
-      <c r="G124" s="35"/>
-      <c r="H124" s="35"/>
-      <c r="I124" s="35"/>
-      <c r="J124" s="35">
+      <c r="G124" s="33"/>
+      <c r="H124" s="33"/>
+      <c r="I124" s="33"/>
+      <c r="J124" s="33">
         <v>2002</v>
       </c>
-      <c r="K124" s="35"/>
-      <c r="L124" s="35"/>
-      <c r="M124" s="35"/>
-      <c r="N124" s="35">
+      <c r="K124" s="33"/>
+      <c r="L124" s="33"/>
+      <c r="M124" s="33"/>
+      <c r="N124" s="33">
         <v>2003</v>
       </c>
-      <c r="O124" s="35"/>
-      <c r="P124" s="35"/>
-      <c r="Q124" s="35"/>
-      <c r="R124" s="35">
+      <c r="O124" s="33"/>
+      <c r="P124" s="33"/>
+      <c r="Q124" s="33"/>
+      <c r="R124" s="33">
         <v>2004</v>
       </c>
-      <c r="S124" s="35"/>
-      <c r="T124" s="35"/>
-      <c r="U124" s="35"/>
-      <c r="V124" s="35">
+      <c r="S124" s="33"/>
+      <c r="T124" s="33"/>
+      <c r="U124" s="33"/>
+      <c r="V124" s="33">
         <v>2005</v>
       </c>
-      <c r="W124" s="35"/>
-      <c r="X124" s="35"/>
-      <c r="Y124" s="35"/>
-      <c r="Z124" s="35">
+      <c r="W124" s="33"/>
+      <c r="X124" s="33"/>
+      <c r="Y124" s="33"/>
+      <c r="Z124" s="33">
         <v>2006</v>
       </c>
-      <c r="AA124" s="35"/>
-      <c r="AB124" s="35"/>
-      <c r="AC124" s="35"/>
-      <c r="AD124" s="35">
+      <c r="AA124" s="33"/>
+      <c r="AB124" s="33"/>
+      <c r="AC124" s="33"/>
+      <c r="AD124" s="33">
         <v>2007</v>
       </c>
-      <c r="AE124" s="35"/>
-      <c r="AF124" s="35"/>
-      <c r="AG124" s="35"/>
-      <c r="AH124" s="35">
+      <c r="AE124" s="33"/>
+      <c r="AF124" s="33"/>
+      <c r="AG124" s="33"/>
+      <c r="AH124" s="33">
         <v>2008</v>
       </c>
-      <c r="AI124" s="35"/>
-      <c r="AJ124" s="35"/>
-      <c r="AK124" s="35"/>
-      <c r="AL124" s="35">
+      <c r="AI124" s="33"/>
+      <c r="AJ124" s="33"/>
+      <c r="AK124" s="33"/>
+      <c r="AL124" s="33">
         <v>2009</v>
       </c>
-      <c r="AM124" s="35"/>
-      <c r="AN124" s="35"/>
-      <c r="AO124" s="35"/>
-      <c r="AP124" s="35">
+      <c r="AM124" s="33"/>
+      <c r="AN124" s="33"/>
+      <c r="AO124" s="33"/>
+      <c r="AP124" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ124" s="35"/>
-      <c r="AR124" s="35"/>
-      <c r="AS124" s="35"/>
-      <c r="AT124" s="35">
+      <c r="AQ124" s="33"/>
+      <c r="AR124" s="33"/>
+      <c r="AS124" s="33"/>
+      <c r="AT124" s="33">
         <v>2011</v>
       </c>
-      <c r="AU124" s="35"/>
-      <c r="AV124" s="35"/>
-      <c r="AW124" s="35"/>
-      <c r="AX124" s="35">
+      <c r="AU124" s="33"/>
+      <c r="AV124" s="33"/>
+      <c r="AW124" s="33"/>
+      <c r="AX124" s="33">
         <v>2012</v>
       </c>
-      <c r="AY124" s="35"/>
-      <c r="AZ124" s="35"/>
-      <c r="BA124" s="35"/>
-      <c r="BB124" s="35">
+      <c r="AY124" s="33"/>
+      <c r="AZ124" s="33"/>
+      <c r="BA124" s="33"/>
+      <c r="BB124" s="33">
         <v>2013</v>
       </c>
-      <c r="BC124" s="35"/>
-      <c r="BD124" s="35"/>
-      <c r="BE124" s="35"/>
-      <c r="BF124" s="35">
+      <c r="BC124" s="33"/>
+      <c r="BD124" s="33"/>
+      <c r="BE124" s="33"/>
+      <c r="BF124" s="33">
         <v>2014</v>
       </c>
-      <c r="BG124" s="35"/>
-      <c r="BH124" s="35"/>
-      <c r="BI124" s="35"/>
-      <c r="BJ124" s="35">
+      <c r="BG124" s="33"/>
+      <c r="BH124" s="33"/>
+      <c r="BI124" s="33"/>
+      <c r="BJ124" s="33">
         <v>2015</v>
       </c>
-      <c r="BK124" s="35"/>
-      <c r="BL124" s="35"/>
-      <c r="BM124" s="35"/>
-      <c r="BN124" s="35">
+      <c r="BK124" s="33"/>
+      <c r="BL124" s="33"/>
+      <c r="BM124" s="33"/>
+      <c r="BN124" s="33">
         <v>2016</v>
       </c>
-      <c r="BO124" s="35"/>
-      <c r="BP124" s="35"/>
-      <c r="BQ124" s="35"/>
+      <c r="BO124" s="33"/>
+      <c r="BP124" s="33"/>
+      <c r="BQ124" s="33"/>
       <c r="BR124" s="34">
         <v>2017</v>
       </c>
@@ -22095,8 +22215,9 @@
         <v>2022</v>
       </c>
       <c r="CM124" s="34"/>
+      <c r="CN124" s="34"/>
     </row>
-    <row r="125" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>37</v>
       </c>
@@ -22370,11 +22491,14 @@
       <c r="CM125" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="CN125" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="126" spans="1:153" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="8"/>
     </row>
-    <row r="127" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>12</v>
       </c>
@@ -22648,7 +22772,9 @@
       <c r="CM127" s="26">
         <v>115.22693976952753</v>
       </c>
-      <c r="CN127" s="11"/>
+      <c r="CN127" s="26">
+        <v>118.27301589983847</v>
+      </c>
       <c r="CO127" s="11"/>
       <c r="CP127" s="11"/>
       <c r="CQ127" s="11"/>
@@ -22711,7 +22837,7 @@
       <c r="EV127" s="11"/>
       <c r="EW127" s="11"/>
     </row>
-    <row r="128" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>11</v>
       </c>
@@ -22985,7 +23111,9 @@
       <c r="CM128" s="26">
         <v>155.37188373824463</v>
       </c>
-      <c r="CN128" s="11"/>
+      <c r="CN128" s="26">
+        <v>167.67663158279336</v>
+      </c>
       <c r="CO128" s="11"/>
       <c r="CP128" s="11"/>
       <c r="CQ128" s="11"/>
@@ -23048,7 +23176,7 @@
       <c r="EV128" s="11"/>
       <c r="EW128" s="11"/>
     </row>
-    <row r="129" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -23322,7 +23450,9 @@
       <c r="CM129" s="26">
         <v>115.98056002277895</v>
       </c>
-      <c r="CN129" s="11"/>
+      <c r="CN129" s="26">
+        <v>106.69388624713258</v>
+      </c>
       <c r="CO129" s="11"/>
       <c r="CP129" s="11"/>
       <c r="CQ129" s="11"/>
@@ -23385,7 +23515,7 @@
       <c r="EV129" s="11"/>
       <c r="EW129" s="11"/>
     </row>
-    <row r="130" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>9</v>
       </c>
@@ -23659,7 +23789,9 @@
       <c r="CM130" s="26">
         <v>110.30691824707179</v>
       </c>
-      <c r="CN130" s="11"/>
+      <c r="CN130" s="26">
+        <v>118.84927854323799</v>
+      </c>
       <c r="CO130" s="11"/>
       <c r="CP130" s="11"/>
       <c r="CQ130" s="11"/>
@@ -23722,7 +23854,7 @@
       <c r="EV130" s="11"/>
       <c r="EW130" s="11"/>
     </row>
-    <row r="131" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="12" t="s">
         <v>8</v>
       </c>
@@ -23996,7 +24128,9 @@
       <c r="CM131" s="26">
         <v>112.03829347266363</v>
       </c>
-      <c r="CN131" s="11"/>
+      <c r="CN131" s="26">
+        <v>114.65261671281807</v>
+      </c>
       <c r="CO131" s="11"/>
       <c r="CP131" s="11"/>
       <c r="CQ131" s="11"/>
@@ -24059,7 +24193,7 @@
       <c r="EV131" s="11"/>
       <c r="EW131" s="11"/>
     </row>
-    <row r="132" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>7</v>
       </c>
@@ -24333,7 +24467,9 @@
       <c r="CM132" s="26">
         <v>109.16175758428417</v>
       </c>
-      <c r="CN132" s="11"/>
+      <c r="CN132" s="26">
+        <v>114.45087022532654</v>
+      </c>
       <c r="CO132" s="11"/>
       <c r="CP132" s="11"/>
       <c r="CQ132" s="11"/>
@@ -24396,7 +24532,7 @@
       <c r="EV132" s="11"/>
       <c r="EW132" s="11"/>
     </row>
-    <row r="133" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>6</v>
       </c>
@@ -24670,7 +24806,9 @@
       <c r="CM133" s="26">
         <v>124.83430009794101</v>
       </c>
-      <c r="CN133" s="11"/>
+      <c r="CN133" s="26">
+        <v>142.03571732517136</v>
+      </c>
       <c r="CO133" s="11"/>
       <c r="CP133" s="11"/>
       <c r="CQ133" s="11"/>
@@ -24733,7 +24871,7 @@
       <c r="EV133" s="11"/>
       <c r="EW133" s="11"/>
     </row>
-    <row r="134" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -25007,7 +25145,9 @@
       <c r="CM134" s="26">
         <v>102.0749240320504</v>
       </c>
-      <c r="CN134" s="11"/>
+      <c r="CN134" s="26">
+        <v>100.24273019895509</v>
+      </c>
       <c r="CO134" s="11"/>
       <c r="CP134" s="11"/>
       <c r="CQ134" s="11"/>
@@ -25070,7 +25210,7 @@
       <c r="EV134" s="11"/>
       <c r="EW134" s="11"/>
     </row>
-    <row r="135" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>4</v>
       </c>
@@ -25344,7 +25484,9 @@
       <c r="CM135" s="26">
         <v>103.21755085312103</v>
       </c>
-      <c r="CN135" s="11"/>
+      <c r="CN135" s="26">
+        <v>103.66360122129279</v>
+      </c>
       <c r="CO135" s="11"/>
       <c r="CP135" s="11"/>
       <c r="CQ135" s="11"/>
@@ -25407,7 +25549,7 @@
       <c r="EV135" s="11"/>
       <c r="EW135" s="11"/>
     </row>
-    <row r="136" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>3</v>
       </c>
@@ -25681,7 +25823,9 @@
       <c r="CM136" s="26">
         <v>106.59335501258693</v>
       </c>
-      <c r="CN136" s="11"/>
+      <c r="CN136" s="26">
+        <v>108.76667919721386</v>
+      </c>
       <c r="CO136" s="11"/>
       <c r="CP136" s="11"/>
       <c r="CQ136" s="11"/>
@@ -25744,7 +25888,7 @@
       <c r="EV136" s="11"/>
       <c r="EW136" s="11"/>
     </row>
-    <row r="137" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>2</v>
       </c>
@@ -26018,7 +26162,9 @@
       <c r="CM137" s="26">
         <v>108.49244360919089</v>
       </c>
-      <c r="CN137" s="11"/>
+      <c r="CN137" s="26">
+        <v>118.69712079921501</v>
+      </c>
       <c r="CO137" s="11"/>
       <c r="CP137" s="11"/>
       <c r="CQ137" s="11"/>
@@ -26081,7 +26227,7 @@
       <c r="EV137" s="11"/>
       <c r="EW137" s="11"/>
     </row>
-    <row r="138" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
@@ -26355,7 +26501,9 @@
       <c r="CM138" s="26">
         <v>115.95319070720001</v>
       </c>
-      <c r="CN138" s="11"/>
+      <c r="CN138" s="26">
+        <v>107.10733958406853</v>
+      </c>
       <c r="CO138" s="11"/>
       <c r="CP138" s="11"/>
       <c r="CQ138" s="11"/>
@@ -26418,7 +26566,7 @@
       <c r="EV138" s="11"/>
       <c r="EW138" s="11"/>
     </row>
-    <row r="139" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
       <c r="D139" s="13"/>
@@ -26572,7 +26720,7 @@
       <c r="EV139" s="11"/>
       <c r="EW139" s="11"/>
     </row>
-    <row r="140" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="s">
         <v>18</v>
       </c>
@@ -26844,9 +26992,11 @@
         <v>110.95609486366602</v>
       </c>
       <c r="CM140" s="26">
-        <v>114.10572619214791</v>
-      </c>
-      <c r="CN140" s="11"/>
+        <v>114.10299600886442</v>
+      </c>
+      <c r="CN140" s="26">
+        <v>117.80938743309251</v>
+      </c>
       <c r="CO140" s="11"/>
       <c r="CP140" s="11"/>
       <c r="CQ140" s="11"/>
@@ -26909,7 +27059,7 @@
       <c r="EV140" s="11"/>
       <c r="EW140" s="11"/>
     </row>
-    <row r="141" spans="1:153" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:153" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="16"/>
       <c r="B141" s="17"/>
       <c r="C141" s="17"/>
@@ -27001,146 +27151,147 @@
       <c r="CK141" s="16"/>
       <c r="CL141" s="16"/>
       <c r="CM141" s="16"/>
+      <c r="CN141" s="16"/>
     </row>
-    <row r="142" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="149" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="151" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="153" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
-      <c r="B153" s="35">
+      <c r="B153" s="33">
         <v>2000</v>
       </c>
-      <c r="C153" s="35"/>
-      <c r="D153" s="35"/>
-      <c r="E153" s="35"/>
-      <c r="F153" s="35">
+      <c r="C153" s="33"/>
+      <c r="D153" s="33"/>
+      <c r="E153" s="33"/>
+      <c r="F153" s="33">
         <v>2001</v>
       </c>
-      <c r="G153" s="35"/>
-      <c r="H153" s="35"/>
-      <c r="I153" s="35"/>
-      <c r="J153" s="35">
+      <c r="G153" s="33"/>
+      <c r="H153" s="33"/>
+      <c r="I153" s="33"/>
+      <c r="J153" s="33">
         <v>2002</v>
       </c>
-      <c r="K153" s="35"/>
-      <c r="L153" s="35"/>
-      <c r="M153" s="35"/>
-      <c r="N153" s="35">
+      <c r="K153" s="33"/>
+      <c r="L153" s="33"/>
+      <c r="M153" s="33"/>
+      <c r="N153" s="33">
         <v>2003</v>
       </c>
-      <c r="O153" s="35"/>
-      <c r="P153" s="35"/>
-      <c r="Q153" s="35"/>
-      <c r="R153" s="35">
+      <c r="O153" s="33"/>
+      <c r="P153" s="33"/>
+      <c r="Q153" s="33"/>
+      <c r="R153" s="33">
         <v>2004</v>
       </c>
-      <c r="S153" s="35"/>
-      <c r="T153" s="35"/>
-      <c r="U153" s="35"/>
-      <c r="V153" s="35">
+      <c r="S153" s="33"/>
+      <c r="T153" s="33"/>
+      <c r="U153" s="33"/>
+      <c r="V153" s="33">
         <v>2005</v>
       </c>
-      <c r="W153" s="35"/>
-      <c r="X153" s="35"/>
-      <c r="Y153" s="35"/>
-      <c r="Z153" s="35">
+      <c r="W153" s="33"/>
+      <c r="X153" s="33"/>
+      <c r="Y153" s="33"/>
+      <c r="Z153" s="33">
         <v>2006</v>
       </c>
-      <c r="AA153" s="35"/>
-      <c r="AB153" s="35"/>
-      <c r="AC153" s="35"/>
-      <c r="AD153" s="35">
+      <c r="AA153" s="33"/>
+      <c r="AB153" s="33"/>
+      <c r="AC153" s="33"/>
+      <c r="AD153" s="33">
         <v>2007</v>
       </c>
-      <c r="AE153" s="35"/>
-      <c r="AF153" s="35"/>
-      <c r="AG153" s="35"/>
-      <c r="AH153" s="35">
+      <c r="AE153" s="33"/>
+      <c r="AF153" s="33"/>
+      <c r="AG153" s="33"/>
+      <c r="AH153" s="33">
         <v>2008</v>
       </c>
-      <c r="AI153" s="35"/>
-      <c r="AJ153" s="35"/>
-      <c r="AK153" s="35"/>
-      <c r="AL153" s="35">
+      <c r="AI153" s="33"/>
+      <c r="AJ153" s="33"/>
+      <c r="AK153" s="33"/>
+      <c r="AL153" s="33">
         <v>2009</v>
       </c>
-      <c r="AM153" s="35"/>
-      <c r="AN153" s="35"/>
-      <c r="AO153" s="35"/>
-      <c r="AP153" s="35">
+      <c r="AM153" s="33"/>
+      <c r="AN153" s="33"/>
+      <c r="AO153" s="33"/>
+      <c r="AP153" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ153" s="35"/>
-      <c r="AR153" s="35"/>
-      <c r="AS153" s="35"/>
-      <c r="AT153" s="35">
+      <c r="AQ153" s="33"/>
+      <c r="AR153" s="33"/>
+      <c r="AS153" s="33"/>
+      <c r="AT153" s="33">
         <v>2011</v>
       </c>
-      <c r="AU153" s="35"/>
-      <c r="AV153" s="35"/>
-      <c r="AW153" s="35"/>
-      <c r="AX153" s="35">
+      <c r="AU153" s="33"/>
+      <c r="AV153" s="33"/>
+      <c r="AW153" s="33"/>
+      <c r="AX153" s="33">
         <v>2012</v>
       </c>
-      <c r="AY153" s="35"/>
-      <c r="AZ153" s="35"/>
-      <c r="BA153" s="35"/>
-      <c r="BB153" s="35">
+      <c r="AY153" s="33"/>
+      <c r="AZ153" s="33"/>
+      <c r="BA153" s="33"/>
+      <c r="BB153" s="33">
         <v>2013</v>
       </c>
-      <c r="BC153" s="35"/>
-      <c r="BD153" s="35"/>
-      <c r="BE153" s="35"/>
-      <c r="BF153" s="35">
+      <c r="BC153" s="33"/>
+      <c r="BD153" s="33"/>
+      <c r="BE153" s="33"/>
+      <c r="BF153" s="33">
         <v>2014</v>
       </c>
-      <c r="BG153" s="35"/>
-      <c r="BH153" s="35"/>
-      <c r="BI153" s="35"/>
-      <c r="BJ153" s="35">
+      <c r="BG153" s="33"/>
+      <c r="BH153" s="33"/>
+      <c r="BI153" s="33"/>
+      <c r="BJ153" s="33">
         <v>2015</v>
       </c>
-      <c r="BK153" s="35"/>
-      <c r="BL153" s="35"/>
-      <c r="BM153" s="35"/>
-      <c r="BN153" s="35">
+      <c r="BK153" s="33"/>
+      <c r="BL153" s="33"/>
+      <c r="BM153" s="33"/>
+      <c r="BN153" s="33">
         <v>2016</v>
       </c>
-      <c r="BO153" s="35"/>
-      <c r="BP153" s="35"/>
-      <c r="BQ153" s="35"/>
+      <c r="BO153" s="33"/>
+      <c r="BP153" s="33"/>
+      <c r="BQ153" s="33"/>
       <c r="BR153" s="34">
         <v>2017</v>
       </c>
@@ -27175,8 +27326,9 @@
         <v>2022</v>
       </c>
       <c r="CM153" s="34"/>
+      <c r="CN153" s="34"/>
     </row>
-    <row r="154" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
         <v>37</v>
       </c>
@@ -27450,11 +27602,14 @@
       <c r="CM154" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="CN154" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="155" spans="1:153" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="8"/>
     </row>
-    <row r="156" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>12</v>
       </c>
@@ -27726,9 +27881,11 @@
         <v>35.927601934011399</v>
       </c>
       <c r="CM156" s="26">
-        <v>40.36890125049819</v>
-      </c>
-      <c r="CN156" s="11"/>
+        <v>40.386598492293864</v>
+      </c>
+      <c r="CN156" s="26">
+        <v>35.058276190798679</v>
+      </c>
       <c r="CO156" s="11"/>
       <c r="CP156" s="11"/>
       <c r="CQ156" s="11"/>
@@ -27791,7 +27948,7 @@
       <c r="EV156" s="11"/>
       <c r="EW156" s="11"/>
     </row>
-    <row r="157" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>11</v>
       </c>
@@ -28063,9 +28220,11 @@
         <v>1.8223351728914243</v>
       </c>
       <c r="CM157" s="26">
-        <v>1.917960832098347</v>
-      </c>
-      <c r="CN157" s="11"/>
+        <v>1.9301613408157867</v>
+      </c>
+      <c r="CN157" s="26">
+        <v>1.811642637410487</v>
+      </c>
       <c r="CO157" s="11"/>
       <c r="CP157" s="11"/>
       <c r="CQ157" s="11"/>
@@ -28128,7 +28287,7 @@
       <c r="EV157" s="11"/>
       <c r="EW157" s="11"/>
     </row>
-    <row r="158" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>10</v>
       </c>
@@ -28400,9 +28559,11 @@
         <v>1.5002248085662859</v>
       </c>
       <c r="CM158" s="26">
-        <v>1.6724801966025775</v>
-      </c>
-      <c r="CN158" s="11"/>
+        <v>1.6737259758123908</v>
+      </c>
+      <c r="CN158" s="26">
+        <v>1.6456764094052518</v>
+      </c>
       <c r="CO158" s="11"/>
       <c r="CP158" s="11"/>
       <c r="CQ158" s="11"/>
@@ -28465,7 +28626,7 @@
       <c r="EV158" s="11"/>
       <c r="EW158" s="11"/>
     </row>
-    <row r="159" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>9</v>
       </c>
@@ -28737,9 +28898,11 @@
         <v>11.567074359701033</v>
       </c>
       <c r="CM159" s="26">
-        <v>14.823210230638898</v>
-      </c>
-      <c r="CN159" s="11"/>
+        <v>14.820477775699233</v>
+      </c>
+      <c r="CN159" s="26">
+        <v>12.672022805474306</v>
+      </c>
       <c r="CO159" s="11"/>
       <c r="CP159" s="11"/>
       <c r="CQ159" s="11"/>
@@ -28802,7 +28965,7 @@
       <c r="EV159" s="11"/>
       <c r="EW159" s="11"/>
     </row>
-    <row r="160" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="12" t="s">
         <v>8</v>
       </c>
@@ -29074,9 +29237,11 @@
         <v>2.7540321393080136</v>
       </c>
       <c r="CM160" s="26">
-        <v>2.6919330078831032</v>
-      </c>
-      <c r="CN160" s="11"/>
+        <v>2.658125012734792</v>
+      </c>
+      <c r="CN160" s="26">
+        <v>3.0090483472403351</v>
+      </c>
       <c r="CO160" s="11"/>
       <c r="CP160" s="11"/>
       <c r="CQ160" s="11"/>
@@ -29139,7 +29304,7 @@
       <c r="EV160" s="11"/>
       <c r="EW160" s="11"/>
     </row>
-    <row r="161" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>7</v>
       </c>
@@ -29411,9 +29576,11 @@
         <v>4.2445995683196163</v>
       </c>
       <c r="CM161" s="26">
-        <v>3.5617105736059083</v>
-      </c>
-      <c r="CN161" s="11"/>
+        <v>3.5635325484111213</v>
+      </c>
+      <c r="CN161" s="26">
+        <v>5.387816191163207</v>
+      </c>
       <c r="CO161" s="11"/>
       <c r="CP161" s="11"/>
       <c r="CQ161" s="11"/>
@@ -29476,7 +29643,7 @@
       <c r="EV161" s="11"/>
       <c r="EW161" s="11"/>
     </row>
-    <row r="162" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>6</v>
       </c>
@@ -29748,9 +29915,11 @@
         <v>9.8906523475883557</v>
       </c>
       <c r="CM162" s="26">
-        <v>7.6589172535727625</v>
-      </c>
-      <c r="CN162" s="11"/>
+        <v>7.6311450485028924</v>
+      </c>
+      <c r="CN162" s="26">
+        <v>11.27571442030456</v>
+      </c>
       <c r="CO162" s="11"/>
       <c r="CP162" s="11"/>
       <c r="CQ162" s="11"/>
@@ -29813,7 +29982,7 @@
       <c r="EV162" s="11"/>
       <c r="EW162" s="11"/>
     </row>
-    <row r="163" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>5</v>
       </c>
@@ -30085,9 +30254,11 @@
         <v>3.155564743857485</v>
       </c>
       <c r="CM163" s="26">
-        <v>3.2974076541366295</v>
-      </c>
-      <c r="CN163" s="11"/>
+        <v>3.281450462649302</v>
+      </c>
+      <c r="CN163" s="26">
+        <v>2.3484407842842439</v>
+      </c>
       <c r="CO163" s="11"/>
       <c r="CP163" s="11"/>
       <c r="CQ163" s="11"/>
@@ -30150,7 +30321,7 @@
       <c r="EV163" s="11"/>
       <c r="EW163" s="11"/>
     </row>
-    <row r="164" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>4</v>
       </c>
@@ -30422,9 +30593,11 @@
         <v>1.4599597250106682</v>
       </c>
       <c r="CM164" s="26">
-        <v>1.058411438919044</v>
-      </c>
-      <c r="CN164" s="11"/>
+        <v>1.0824917908333125</v>
+      </c>
+      <c r="CN164" s="26">
+        <v>1.287643483784602</v>
+      </c>
       <c r="CO164" s="11"/>
       <c r="CP164" s="11"/>
       <c r="CQ164" s="11"/>
@@ -30487,7 +30660,7 @@
       <c r="EV164" s="11"/>
       <c r="EW164" s="11"/>
     </row>
-    <row r="165" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>3</v>
       </c>
@@ -30759,9 +30932,11 @@
         <v>5.3429575462341834</v>
       </c>
       <c r="CM165" s="26">
-        <v>4.8096761886996777</v>
-      </c>
-      <c r="CN165" s="11"/>
+        <v>4.8256065402639523</v>
+      </c>
+      <c r="CN165" s="26">
+        <v>5.3168377883684093</v>
+      </c>
       <c r="CO165" s="11"/>
       <c r="CP165" s="11"/>
       <c r="CQ165" s="11"/>
@@ -30824,7 +30999,7 @@
       <c r="EV165" s="11"/>
       <c r="EW165" s="11"/>
     </row>
-    <row r="166" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>2</v>
       </c>
@@ -31096,9 +31271,11 @@
         <v>8.2064146234913267</v>
       </c>
       <c r="CM166" s="26">
-        <v>4.6659132760052886</v>
-      </c>
-      <c r="CN166" s="11"/>
+        <v>4.7014993247610217</v>
+      </c>
+      <c r="CN166" s="26">
+        <v>6.9685605436369258</v>
+      </c>
       <c r="CO166" s="11"/>
       <c r="CP166" s="11"/>
       <c r="CQ166" s="11"/>
@@ -31161,7 +31338,7 @@
       <c r="EV166" s="11"/>
       <c r="EW166" s="11"/>
     </row>
-    <row r="167" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>1</v>
       </c>
@@ -31433,9 +31610,11 @@
         <v>14.128583031020222</v>
       </c>
       <c r="CM167" s="26">
-        <v>13.473478097339569</v>
-      </c>
-      <c r="CN167" s="11"/>
+        <v>13.445185687222347</v>
+      </c>
+      <c r="CN167" s="26">
+        <v>13.218320398128993</v>
+      </c>
       <c r="CO167" s="11"/>
       <c r="CP167" s="11"/>
       <c r="CQ167" s="11"/>
@@ -31498,7 +31677,7 @@
       <c r="EV167" s="11"/>
       <c r="EW167" s="11"/>
     </row>
-    <row r="168" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="13"/>
       <c r="C168" s="13"/>
       <c r="D168" s="13"/>
@@ -31652,7 +31831,7 @@
       <c r="EV168" s="11"/>
       <c r="EW168" s="11"/>
     </row>
-    <row r="169" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="12" t="s">
         <v>18</v>
       </c>
@@ -31926,7 +32105,9 @@
       <c r="CM169" s="26">
         <v>100</v>
       </c>
-      <c r="CN169" s="11"/>
+      <c r="CN169" s="26">
+        <v>100</v>
+      </c>
       <c r="CO169" s="11"/>
       <c r="CP169" s="11"/>
       <c r="CQ169" s="11"/>
@@ -31989,7 +32170,7 @@
       <c r="EV169" s="11"/>
       <c r="EW169" s="11"/>
     </row>
-    <row r="170" spans="1:153" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:153" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="16"/>
       <c r="B170" s="17"/>
       <c r="C170" s="17"/>
@@ -32081,13 +32262,14 @@
       <c r="CK170" s="16"/>
       <c r="CL170" s="16"/>
       <c r="CM170" s="16"/>
+      <c r="CN170" s="16"/>
     </row>
-    <row r="171" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
       <c r="D172" s="13"/>
@@ -32241,7 +32423,7 @@
       <c r="EV172" s="11"/>
       <c r="EW172" s="11"/>
     </row>
-    <row r="173" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="13"/>
       <c r="C173" s="13"/>
       <c r="D173" s="13"/>
@@ -32395,140 +32577,140 @@
       <c r="EV173" s="11"/>
       <c r="EW173" s="11"/>
     </row>
-    <row r="174" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="178" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="180" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A182" s="4"/>
-      <c r="B182" s="35">
+      <c r="B182" s="33">
         <v>2000</v>
       </c>
-      <c r="C182" s="35"/>
-      <c r="D182" s="35"/>
-      <c r="E182" s="35"/>
-      <c r="F182" s="35">
+      <c r="C182" s="33"/>
+      <c r="D182" s="33"/>
+      <c r="E182" s="33"/>
+      <c r="F182" s="33">
         <v>2001</v>
       </c>
-      <c r="G182" s="35"/>
-      <c r="H182" s="35"/>
-      <c r="I182" s="35"/>
-      <c r="J182" s="35">
+      <c r="G182" s="33"/>
+      <c r="H182" s="33"/>
+      <c r="I182" s="33"/>
+      <c r="J182" s="33">
         <v>2002</v>
       </c>
-      <c r="K182" s="35"/>
-      <c r="L182" s="35"/>
-      <c r="M182" s="35"/>
-      <c r="N182" s="35">
+      <c r="K182" s="33"/>
+      <c r="L182" s="33"/>
+      <c r="M182" s="33"/>
+      <c r="N182" s="33">
         <v>2003</v>
       </c>
-      <c r="O182" s="35"/>
-      <c r="P182" s="35"/>
-      <c r="Q182" s="35"/>
-      <c r="R182" s="35">
+      <c r="O182" s="33"/>
+      <c r="P182" s="33"/>
+      <c r="Q182" s="33"/>
+      <c r="R182" s="33">
         <v>2004</v>
       </c>
-      <c r="S182" s="35"/>
-      <c r="T182" s="35"/>
-      <c r="U182" s="35"/>
-      <c r="V182" s="35">
+      <c r="S182" s="33"/>
+      <c r="T182" s="33"/>
+      <c r="U182" s="33"/>
+      <c r="V182" s="33">
         <v>2005</v>
       </c>
-      <c r="W182" s="35"/>
-      <c r="X182" s="35"/>
-      <c r="Y182" s="35"/>
-      <c r="Z182" s="35">
+      <c r="W182" s="33"/>
+      <c r="X182" s="33"/>
+      <c r="Y182" s="33"/>
+      <c r="Z182" s="33">
         <v>2006</v>
       </c>
-      <c r="AA182" s="35"/>
-      <c r="AB182" s="35"/>
-      <c r="AC182" s="35"/>
-      <c r="AD182" s="35">
+      <c r="AA182" s="33"/>
+      <c r="AB182" s="33"/>
+      <c r="AC182" s="33"/>
+      <c r="AD182" s="33">
         <v>2007</v>
       </c>
-      <c r="AE182" s="35"/>
-      <c r="AF182" s="35"/>
-      <c r="AG182" s="35"/>
-      <c r="AH182" s="35">
+      <c r="AE182" s="33"/>
+      <c r="AF182" s="33"/>
+      <c r="AG182" s="33"/>
+      <c r="AH182" s="33">
         <v>2008</v>
       </c>
-      <c r="AI182" s="35"/>
-      <c r="AJ182" s="35"/>
-      <c r="AK182" s="35"/>
-      <c r="AL182" s="35">
+      <c r="AI182" s="33"/>
+      <c r="AJ182" s="33"/>
+      <c r="AK182" s="33"/>
+      <c r="AL182" s="33">
         <v>2009</v>
       </c>
-      <c r="AM182" s="35"/>
-      <c r="AN182" s="35"/>
-      <c r="AO182" s="35"/>
-      <c r="AP182" s="35">
+      <c r="AM182" s="33"/>
+      <c r="AN182" s="33"/>
+      <c r="AO182" s="33"/>
+      <c r="AP182" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ182" s="35"/>
-      <c r="AR182" s="35"/>
-      <c r="AS182" s="35"/>
-      <c r="AT182" s="35">
+      <c r="AQ182" s="33"/>
+      <c r="AR182" s="33"/>
+      <c r="AS182" s="33"/>
+      <c r="AT182" s="33">
         <v>2011</v>
       </c>
-      <c r="AU182" s="35"/>
-      <c r="AV182" s="35"/>
-      <c r="AW182" s="35"/>
-      <c r="AX182" s="35">
+      <c r="AU182" s="33"/>
+      <c r="AV182" s="33"/>
+      <c r="AW182" s="33"/>
+      <c r="AX182" s="33">
         <v>2012</v>
       </c>
-      <c r="AY182" s="35"/>
-      <c r="AZ182" s="35"/>
-      <c r="BA182" s="35"/>
-      <c r="BB182" s="35">
+      <c r="AY182" s="33"/>
+      <c r="AZ182" s="33"/>
+      <c r="BA182" s="33"/>
+      <c r="BB182" s="33">
         <v>2013</v>
       </c>
-      <c r="BC182" s="35"/>
-      <c r="BD182" s="35"/>
-      <c r="BE182" s="35"/>
-      <c r="BF182" s="35">
+      <c r="BC182" s="33"/>
+      <c r="BD182" s="33"/>
+      <c r="BE182" s="33"/>
+      <c r="BF182" s="33">
         <v>2014</v>
       </c>
-      <c r="BG182" s="35"/>
-      <c r="BH182" s="35"/>
-      <c r="BI182" s="35"/>
-      <c r="BJ182" s="35">
+      <c r="BG182" s="33"/>
+      <c r="BH182" s="33"/>
+      <c r="BI182" s="33"/>
+      <c r="BJ182" s="33">
         <v>2015</v>
       </c>
-      <c r="BK182" s="35"/>
-      <c r="BL182" s="35"/>
-      <c r="BM182" s="35"/>
-      <c r="BN182" s="35">
+      <c r="BK182" s="33"/>
+      <c r="BL182" s="33"/>
+      <c r="BM182" s="33"/>
+      <c r="BN182" s="33">
         <v>2016</v>
       </c>
-      <c r="BO182" s="35"/>
-      <c r="BP182" s="35"/>
-      <c r="BQ182" s="35"/>
+      <c r="BO182" s="33"/>
+      <c r="BP182" s="33"/>
+      <c r="BQ182" s="33"/>
       <c r="BR182" s="34">
         <v>2017</v>
       </c>
@@ -32563,8 +32745,9 @@
         <v>2022</v>
       </c>
       <c r="CM182" s="34"/>
+      <c r="CN182" s="34"/>
     </row>
-    <row r="183" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
         <v>37</v>
       </c>
@@ -32838,11 +33021,14 @@
       <c r="CM183" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="CN183" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="184" spans="1:153" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="8"/>
     </row>
-    <row r="185" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>12</v>
       </c>
@@ -33114,9 +33300,11 @@
         <v>36.196689945480429</v>
       </c>
       <c r="CM185" s="26">
-        <v>39.976092413636891</v>
-      </c>
-      <c r="CN185" s="11"/>
+        <v>39.992660534029831</v>
+      </c>
+      <c r="CN185" s="26">
+        <v>34.920848268517055</v>
+      </c>
       <c r="CO185" s="11"/>
       <c r="CP185" s="11"/>
       <c r="CQ185" s="11"/>
@@ -33179,7 +33367,7 @@
       <c r="EV185" s="11"/>
       <c r="EW185" s="11"/>
     </row>
-    <row r="186" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>11</v>
       </c>
@@ -33451,9 +33639,11 @@
         <v>1.4452608139366023</v>
       </c>
       <c r="CM186" s="26">
-        <v>1.4085580240719469</v>
-      </c>
-      <c r="CN186" s="11"/>
+        <v>1.4174842092962083</v>
+      </c>
+      <c r="CN186" s="26">
+        <v>1.272857805803532</v>
+      </c>
       <c r="CO186" s="11"/>
       <c r="CP186" s="11"/>
       <c r="CQ186" s="11"/>
@@ -33516,7 +33706,7 @@
       <c r="EV186" s="11"/>
       <c r="EW186" s="11"/>
     </row>
-    <row r="187" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>10</v>
       </c>
@@ -33788,9 +33978,11 @@
         <v>1.5730994582841051</v>
       </c>
       <c r="CM187" s="26">
-        <v>1.6454444377388928</v>
-      </c>
-      <c r="CN187" s="11"/>
+        <v>1.6466306793185461</v>
+      </c>
+      <c r="CN187" s="26">
+        <v>1.8171250155426251</v>
+      </c>
       <c r="CO187" s="11"/>
       <c r="CP187" s="11"/>
       <c r="CQ187" s="11"/>
@@ -33853,7 +34045,7 @@
       <c r="EV187" s="11"/>
       <c r="EW187" s="11"/>
     </row>
-    <row r="188" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>9</v>
       </c>
@@ -34125,9 +34317,11 @@
         <v>12.299765864632096</v>
       </c>
       <c r="CM188" s="26">
-        <v>15.33369977826235</v>
-      </c>
-      <c r="CN188" s="11"/>
+        <v>15.330506403073811</v>
+      </c>
+      <c r="CN188" s="26">
+        <v>12.561146879053098</v>
+      </c>
       <c r="CO188" s="11"/>
       <c r="CP188" s="11"/>
       <c r="CQ188" s="11"/>
@@ -34190,7 +34384,7 @@
       <c r="EV188" s="11"/>
       <c r="EW188" s="11"/>
     </row>
-    <row r="189" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:153" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="12" t="s">
         <v>8</v>
       </c>
@@ -34462,9 +34656,11 @@
         <v>2.7306846061507564</v>
       </c>
       <c r="CM189" s="26">
-        <v>2.7416070095717773</v>
-      </c>
-      <c r="CN189" s="11"/>
+        <v>2.7071103844788857</v>
+      </c>
+      <c r="CN189" s="26">
+        <v>3.0918975310688319</v>
+      </c>
       <c r="CO189" s="11"/>
       <c r="CP189" s="11"/>
       <c r="CQ189" s="11"/>
@@ -34527,7 +34723,7 @@
       <c r="EV189" s="11"/>
       <c r="EW189" s="11"/>
     </row>
-    <row r="190" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>7</v>
       </c>
@@ -34799,9 +34995,11 @@
         <v>4.3364797191797235</v>
       </c>
       <c r="CM190" s="26">
-        <v>3.7230215093757728</v>
-      </c>
-      <c r="CN190" s="11"/>
+        <v>3.7248368764571036</v>
+      </c>
+      <c r="CN190" s="26">
+        <v>5.5459196057958513</v>
+      </c>
       <c r="CO190" s="11"/>
       <c r="CP190" s="11"/>
       <c r="CQ190" s="11"/>
@@ -34864,7 +35062,7 @@
       <c r="EV190" s="11"/>
       <c r="EW190" s="11"/>
     </row>
-    <row r="191" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>6</v>
       </c>
@@ -35136,9 +35334,11 @@
         <v>8.9842758069096487</v>
       </c>
       <c r="CM191" s="26">
-        <v>7.0006906305305234</v>
-      </c>
-      <c r="CN191" s="11"/>
+        <v>6.9751383420200934</v>
+      </c>
+      <c r="CN191" s="26">
+        <v>9.3524715736494084</v>
+      </c>
       <c r="CO191" s="11"/>
       <c r="CP191" s="11"/>
       <c r="CQ191" s="11"/>
@@ -35201,7 +35401,7 @@
       <c r="EV191" s="11"/>
       <c r="EW191" s="11"/>
     </row>
-    <row r="192" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>5</v>
       </c>
@@ -35473,9 +35673,11 @@
         <v>3.3371203504901774</v>
       </c>
       <c r="CM192" s="26">
-        <v>3.6860482483304877</v>
-      </c>
-      <c r="CN192" s="11"/>
+        <v>3.6681225344374964</v>
+      </c>
+      <c r="CN192" s="26">
+        <v>2.7599843866014542</v>
+      </c>
       <c r="CO192" s="11"/>
       <c r="CP192" s="11"/>
       <c r="CQ192" s="11"/>
@@ -35538,7 +35740,7 @@
       <c r="EV192" s="11"/>
       <c r="EW192" s="11"/>
     </row>
-    <row r="193" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>4</v>
       </c>
@@ -35810,9 +36012,11 @@
         <v>1.5514188920730885</v>
       </c>
       <c r="CM193" s="26">
-        <v>1.1700607585602474</v>
-      </c>
-      <c r="CN193" s="11"/>
+        <v>1.1966526571129854</v>
+      </c>
+      <c r="CN193" s="26">
+        <v>1.4633534651477869</v>
+      </c>
       <c r="CO193" s="11"/>
       <c r="CP193" s="11"/>
       <c r="CQ193" s="11"/>
@@ -35875,7 +36079,7 @@
       <c r="EV193" s="11"/>
       <c r="EW193" s="11"/>
     </row>
-    <row r="194" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>3</v>
       </c>
@@ -36147,9 +36351,11 @@
         <v>5.6820257135855901</v>
       </c>
       <c r="CM194" s="26">
-        <v>5.1486473448166947</v>
-      </c>
-      <c r="CN194" s="11"/>
+        <v>5.1655768198596341</v>
+      </c>
+      <c r="CN194" s="26">
+        <v>5.7588721798986926</v>
+      </c>
       <c r="CO194" s="11"/>
       <c r="CP194" s="11"/>
       <c r="CQ194" s="11"/>
@@ -36212,7 +36418,7 @@
       <c r="EV194" s="11"/>
       <c r="EW194" s="11"/>
     </row>
-    <row r="195" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>2</v>
       </c>
@@ -36484,9 +36690,11 @@
         <v>8.1393618614844048</v>
       </c>
       <c r="CM195" s="26">
-        <v>4.9073226207900129</v>
-      </c>
-      <c r="CN195" s="11"/>
+        <v>4.9446315415412032</v>
+      </c>
+      <c r="CN195" s="26">
+        <v>6.9164428202517421</v>
+      </c>
       <c r="CO195" s="11"/>
       <c r="CP195" s="11"/>
       <c r="CQ195" s="11"/>
@@ -36549,7 +36757,7 @@
       <c r="EV195" s="11"/>
       <c r="EW195" s="11"/>
     </row>
-    <row r="196" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>1</v>
       </c>
@@ -36821,9 +37029,11 @@
         <v>13.723816967793365</v>
       </c>
       <c r="CM196" s="26">
-        <v>13.25880722431442</v>
-      </c>
-      <c r="CN196" s="11"/>
+        <v>13.230649018374201</v>
+      </c>
+      <c r="CN196" s="26">
+        <v>14.53908046866993</v>
+      </c>
       <c r="CO196" s="11"/>
       <c r="CP196" s="11"/>
       <c r="CQ196" s="11"/>
@@ -36886,7 +37096,7 @@
       <c r="EV196" s="11"/>
       <c r="EW196" s="11"/>
     </row>
-    <row r="197" spans="1:153" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="13"/>
       <c r="C197" s="13"/>
       <c r="D197" s="13"/>
@@ -37040,7 +37250,7 @@
       <c r="EV197" s="11"/>
       <c r="EW197" s="11"/>
     </row>
-    <row r="198" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:153" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="12" t="s">
         <v>18</v>
       </c>
@@ -37314,7 +37524,9 @@
       <c r="CM198" s="26">
         <v>100</v>
       </c>
-      <c r="CN198" s="11"/>
+      <c r="CN198" s="26">
+        <v>100</v>
+      </c>
       <c r="CO198" s="11"/>
       <c r="CP198" s="11"/>
       <c r="CQ198" s="11"/>
@@ -37377,7 +37589,7 @@
       <c r="EV198" s="11"/>
       <c r="EW198" s="11"/>
     </row>
-    <row r="199" spans="1:153" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:153" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="16"/>
       <c r="B199" s="17"/>
       <c r="C199" s="17"/>
@@ -37469,13 +37681,14 @@
       <c r="CK199" s="16"/>
       <c r="CL199" s="16"/>
       <c r="CM199" s="16"/>
+      <c r="CN199" s="16"/>
     </row>
-    <row r="200" spans="1:153" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:153" s="29" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:153" s="29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" s="27"/>
       <c r="C201" s="27"/>
@@ -37567,7 +37780,7 @@
       <c r="CK201" s="1"/>
       <c r="CL201" s="1"/>
       <c r="CM201" s="1"/>
-      <c r="CN201" s="28"/>
+      <c r="CN201" s="1"/>
       <c r="CO201" s="28"/>
       <c r="CP201" s="28"/>
       <c r="CQ201" s="28"/>
@@ -37630,7 +37843,7 @@
       <c r="EV201" s="28"/>
       <c r="EW201" s="28"/>
     </row>
-    <row r="202" spans="1:153" s="29" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:153" s="29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="B202" s="27"/>
       <c r="C202" s="27"/>
@@ -37722,7 +37935,7 @@
       <c r="CK202" s="1"/>
       <c r="CL202" s="1"/>
       <c r="CM202" s="1"/>
-      <c r="CN202" s="28"/>
+      <c r="CN202" s="1"/>
       <c r="CO202" s="28"/>
       <c r="CP202" s="28"/>
       <c r="CQ202" s="28"/>
@@ -37786,41 +37999,110 @@
       <c r="EW202" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="159">
-    <mergeCell ref="B182:E182"/>
-    <mergeCell ref="F182:I182"/>
-    <mergeCell ref="J182:M182"/>
-    <mergeCell ref="N182:Q182"/>
-    <mergeCell ref="R182:U182"/>
-    <mergeCell ref="V182:Y182"/>
-    <mergeCell ref="Z182:AC182"/>
-    <mergeCell ref="AD182:AG182"/>
-    <mergeCell ref="AH182:AK182"/>
-    <mergeCell ref="B124:E124"/>
-    <mergeCell ref="F124:I124"/>
-    <mergeCell ref="J124:M124"/>
-    <mergeCell ref="N124:Q124"/>
-    <mergeCell ref="R124:U124"/>
-    <mergeCell ref="V124:Y124"/>
-    <mergeCell ref="Z124:AC124"/>
-    <mergeCell ref="AD124:AG124"/>
-    <mergeCell ref="F153:I153"/>
-    <mergeCell ref="J153:M153"/>
-    <mergeCell ref="N153:Q153"/>
-    <mergeCell ref="R153:U153"/>
-    <mergeCell ref="V153:Y153"/>
-    <mergeCell ref="Z153:AC153"/>
-    <mergeCell ref="AD153:AG153"/>
-    <mergeCell ref="B153:E153"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="J96:M96"/>
-    <mergeCell ref="N96:Q96"/>
-    <mergeCell ref="R96:U96"/>
-    <mergeCell ref="V96:Y96"/>
-    <mergeCell ref="Z96:AC96"/>
-    <mergeCell ref="AD96:AG96"/>
-    <mergeCell ref="AH96:AK96"/>
+  <mergeCells count="161">
+    <mergeCell ref="CH9:CK9"/>
+    <mergeCell ref="CH38:CK38"/>
+    <mergeCell ref="CL9:CN9"/>
+    <mergeCell ref="CL38:CN38"/>
+    <mergeCell ref="CH67:CJ67"/>
+    <mergeCell ref="CL67:CM67"/>
+    <mergeCell ref="CH96:CJ96"/>
+    <mergeCell ref="CL96:CM96"/>
+    <mergeCell ref="CL124:CN124"/>
+    <mergeCell ref="CL153:CN153"/>
+    <mergeCell ref="CL182:CN182"/>
+    <mergeCell ref="CH124:CK124"/>
+    <mergeCell ref="CH153:CK153"/>
+    <mergeCell ref="CH182:CK182"/>
+    <mergeCell ref="AH124:AK124"/>
+    <mergeCell ref="BR182:BU182"/>
+    <mergeCell ref="BV182:BY182"/>
+    <mergeCell ref="BZ124:CC124"/>
+    <mergeCell ref="BR124:BU124"/>
+    <mergeCell ref="BV124:BY124"/>
+    <mergeCell ref="BR153:BU153"/>
+    <mergeCell ref="BV153:BY153"/>
+    <mergeCell ref="BZ153:CC153"/>
+    <mergeCell ref="AH153:AK153"/>
+    <mergeCell ref="BN182:BQ182"/>
+    <mergeCell ref="BB153:BE153"/>
+    <mergeCell ref="BF153:BI153"/>
+    <mergeCell ref="BJ153:BM153"/>
+    <mergeCell ref="BN153:BQ153"/>
+    <mergeCell ref="AP153:AS153"/>
+    <mergeCell ref="AT153:AW153"/>
+    <mergeCell ref="AX153:BA153"/>
+    <mergeCell ref="AX182:BA182"/>
+    <mergeCell ref="BB182:BE182"/>
+    <mergeCell ref="BZ182:CC182"/>
+    <mergeCell ref="BV38:BY38"/>
+    <mergeCell ref="BZ67:CC67"/>
+    <mergeCell ref="BZ96:CC96"/>
+    <mergeCell ref="BJ96:BM96"/>
+    <mergeCell ref="BB38:BE38"/>
+    <mergeCell ref="CD9:CG9"/>
+    <mergeCell ref="CD38:CG38"/>
+    <mergeCell ref="CD124:CG124"/>
+    <mergeCell ref="CD153:CG153"/>
+    <mergeCell ref="CD182:CG182"/>
+    <mergeCell ref="BV9:BY9"/>
+    <mergeCell ref="BZ9:CC9"/>
+    <mergeCell ref="BR9:BU9"/>
+    <mergeCell ref="BR67:BU67"/>
+    <mergeCell ref="BV67:BY67"/>
+    <mergeCell ref="BR96:BU96"/>
+    <mergeCell ref="BV96:BY96"/>
+    <mergeCell ref="BZ38:CC38"/>
+    <mergeCell ref="CD67:CG67"/>
+    <mergeCell ref="CD96:CG96"/>
+    <mergeCell ref="AL182:AO182"/>
+    <mergeCell ref="AP182:AS182"/>
+    <mergeCell ref="AT182:AW182"/>
+    <mergeCell ref="BF124:BI124"/>
+    <mergeCell ref="BJ124:BM124"/>
+    <mergeCell ref="BN124:BQ124"/>
+    <mergeCell ref="BJ9:BM9"/>
+    <mergeCell ref="BN9:BQ9"/>
+    <mergeCell ref="AL153:AO153"/>
+    <mergeCell ref="AL124:AO124"/>
+    <mergeCell ref="AP124:AS124"/>
+    <mergeCell ref="AT124:AW124"/>
+    <mergeCell ref="AX124:BA124"/>
+    <mergeCell ref="BB124:BE124"/>
+    <mergeCell ref="BF182:BI182"/>
+    <mergeCell ref="BJ182:BM182"/>
+    <mergeCell ref="BN38:BQ38"/>
+    <mergeCell ref="BN96:BQ96"/>
+    <mergeCell ref="AL96:AO96"/>
+    <mergeCell ref="AP96:AS96"/>
+    <mergeCell ref="AT96:AW96"/>
+    <mergeCell ref="AX96:BA96"/>
+    <mergeCell ref="BB96:BE96"/>
+    <mergeCell ref="BF96:BI96"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="BJ38:BM38"/>
+    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="BB9:BE9"/>
+    <mergeCell ref="BF9:BI9"/>
+    <mergeCell ref="Z38:AC38"/>
+    <mergeCell ref="AD38:AG38"/>
+    <mergeCell ref="AH38:AK38"/>
+    <mergeCell ref="AL38:AO38"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="AD9:AG9"/>
+    <mergeCell ref="BF38:BI38"/>
+    <mergeCell ref="AP38:AS38"/>
+    <mergeCell ref="AT38:AW38"/>
+    <mergeCell ref="AX38:BA38"/>
     <mergeCell ref="B67:E67"/>
     <mergeCell ref="F67:I67"/>
     <mergeCell ref="J67:M67"/>
@@ -37845,115 +38127,48 @@
     <mergeCell ref="N38:Q38"/>
     <mergeCell ref="R38:U38"/>
     <mergeCell ref="V38:Y38"/>
-    <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="AP9:AS9"/>
-    <mergeCell ref="BJ38:BM38"/>
-    <mergeCell ref="AT9:AW9"/>
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="BB9:BE9"/>
-    <mergeCell ref="BF9:BI9"/>
-    <mergeCell ref="Z38:AC38"/>
-    <mergeCell ref="AD38:AG38"/>
-    <mergeCell ref="AH38:AK38"/>
-    <mergeCell ref="AL38:AO38"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="AD9:AG9"/>
-    <mergeCell ref="BF38:BI38"/>
-    <mergeCell ref="AP38:AS38"/>
-    <mergeCell ref="AT38:AW38"/>
-    <mergeCell ref="AX38:BA38"/>
-    <mergeCell ref="AL182:AO182"/>
-    <mergeCell ref="AP182:AS182"/>
-    <mergeCell ref="AT182:AW182"/>
-    <mergeCell ref="BF124:BI124"/>
-    <mergeCell ref="BJ124:BM124"/>
-    <mergeCell ref="BN124:BQ124"/>
-    <mergeCell ref="BJ9:BM9"/>
-    <mergeCell ref="BN9:BQ9"/>
-    <mergeCell ref="AL153:AO153"/>
-    <mergeCell ref="AL124:AO124"/>
-    <mergeCell ref="AP124:AS124"/>
-    <mergeCell ref="AT124:AW124"/>
-    <mergeCell ref="AX124:BA124"/>
-    <mergeCell ref="BB124:BE124"/>
-    <mergeCell ref="BF182:BI182"/>
-    <mergeCell ref="BJ182:BM182"/>
-    <mergeCell ref="BN38:BQ38"/>
-    <mergeCell ref="BN96:BQ96"/>
-    <mergeCell ref="AL96:AO96"/>
-    <mergeCell ref="AP96:AS96"/>
-    <mergeCell ref="AT96:AW96"/>
-    <mergeCell ref="AX96:BA96"/>
-    <mergeCell ref="BB96:BE96"/>
-    <mergeCell ref="BF96:BI96"/>
-    <mergeCell ref="BB182:BE182"/>
-    <mergeCell ref="BZ182:CC182"/>
-    <mergeCell ref="BV38:BY38"/>
-    <mergeCell ref="BZ67:CC67"/>
-    <mergeCell ref="BZ96:CC96"/>
-    <mergeCell ref="BJ96:BM96"/>
-    <mergeCell ref="BB38:BE38"/>
-    <mergeCell ref="CD9:CG9"/>
-    <mergeCell ref="CD38:CG38"/>
-    <mergeCell ref="CD124:CG124"/>
-    <mergeCell ref="CD153:CG153"/>
-    <mergeCell ref="CD182:CG182"/>
-    <mergeCell ref="BV9:BY9"/>
-    <mergeCell ref="BZ9:CC9"/>
-    <mergeCell ref="BR9:BU9"/>
-    <mergeCell ref="BR67:BU67"/>
-    <mergeCell ref="BV67:BY67"/>
-    <mergeCell ref="BR96:BU96"/>
-    <mergeCell ref="BV96:BY96"/>
-    <mergeCell ref="BZ38:CC38"/>
-    <mergeCell ref="CD67:CG67"/>
-    <mergeCell ref="CD96:CG96"/>
-    <mergeCell ref="CH124:CK124"/>
-    <mergeCell ref="CH153:CK153"/>
-    <mergeCell ref="CH182:CK182"/>
-    <mergeCell ref="AH124:AK124"/>
-    <mergeCell ref="BR182:BU182"/>
-    <mergeCell ref="BV182:BY182"/>
-    <mergeCell ref="BZ124:CC124"/>
-    <mergeCell ref="BR124:BU124"/>
-    <mergeCell ref="BV124:BY124"/>
-    <mergeCell ref="BR153:BU153"/>
-    <mergeCell ref="BV153:BY153"/>
-    <mergeCell ref="BZ153:CC153"/>
-    <mergeCell ref="AH153:AK153"/>
-    <mergeCell ref="BN182:BQ182"/>
-    <mergeCell ref="BB153:BE153"/>
-    <mergeCell ref="BF153:BI153"/>
-    <mergeCell ref="BJ153:BM153"/>
-    <mergeCell ref="BN153:BQ153"/>
-    <mergeCell ref="AP153:AS153"/>
-    <mergeCell ref="AT153:AW153"/>
-    <mergeCell ref="AX153:BA153"/>
-    <mergeCell ref="AX182:BA182"/>
-    <mergeCell ref="CL9:CM9"/>
-    <mergeCell ref="CL38:CM38"/>
-    <mergeCell ref="CH67:CI67"/>
-    <mergeCell ref="CH96:CI96"/>
-    <mergeCell ref="CL124:CM124"/>
-    <mergeCell ref="CL153:CM153"/>
-    <mergeCell ref="CL182:CM182"/>
-    <mergeCell ref="CH9:CK9"/>
-    <mergeCell ref="CH38:CK38"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="J96:M96"/>
+    <mergeCell ref="N96:Q96"/>
+    <mergeCell ref="R96:U96"/>
+    <mergeCell ref="V96:Y96"/>
+    <mergeCell ref="Z96:AC96"/>
+    <mergeCell ref="AD96:AG96"/>
+    <mergeCell ref="AH96:AK96"/>
+    <mergeCell ref="B124:E124"/>
+    <mergeCell ref="F124:I124"/>
+    <mergeCell ref="J124:M124"/>
+    <mergeCell ref="N124:Q124"/>
+    <mergeCell ref="R124:U124"/>
+    <mergeCell ref="V124:Y124"/>
+    <mergeCell ref="Z124:AC124"/>
+    <mergeCell ref="AD124:AG124"/>
+    <mergeCell ref="F153:I153"/>
+    <mergeCell ref="J153:M153"/>
+    <mergeCell ref="N153:Q153"/>
+    <mergeCell ref="R153:U153"/>
+    <mergeCell ref="V153:Y153"/>
+    <mergeCell ref="Z153:AC153"/>
+    <mergeCell ref="AD153:AG153"/>
+    <mergeCell ref="B153:E153"/>
+    <mergeCell ref="B182:E182"/>
+    <mergeCell ref="F182:I182"/>
+    <mergeCell ref="J182:M182"/>
+    <mergeCell ref="N182:Q182"/>
+    <mergeCell ref="R182:U182"/>
+    <mergeCell ref="V182:Y182"/>
+    <mergeCell ref="Z182:AC182"/>
+    <mergeCell ref="AD182:AG182"/>
+    <mergeCell ref="AH182:AK182"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="58" max="90" man="1"/>
-    <brk id="116" max="90" man="1"/>
-    <brk id="144" max="90" man="1"/>
+    <brk id="58" max="91" man="1"/>
+    <brk id="116" max="91" man="1"/>
+    <brk id="144" max="91" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q4 2022 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of November 2022\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2023\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FCD235-A6B5-4813-B08D-DEFC58E4D815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0E0DAA-4166-49BD-B8E5-A458BC768054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3195" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13650" yWindow="1395" windowWidth="13830" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="PCE_Per_Anl">#REF!</definedName>
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CN$202</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CO$202</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="61">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -220,13 +220,13 @@
     <t>2021 - 2022</t>
   </si>
   <si>
-    <t>Q1 2000 to Q3 2022</t>
+    <t>As of January 2023</t>
   </si>
   <si>
-    <t>Q1 2001 to Q3 2022</t>
+    <t>Q1 2000 to Q4 2022</t>
   </si>
   <si>
-    <t>As of November 2022</t>
+    <t>Q1 2001 to Q4 2022</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -355,13 +355,10 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -385,7 +382,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="HFCE"/>
@@ -686,7 +683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,11 +697,11 @@
   <dimension ref="A1:EW202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CA2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CH2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="CA66" sqref="CA66"/>
       <selection pane="topRight" activeCell="CA66" sqref="CA66"/>
       <selection pane="bottomLeft" activeCell="CA66" sqref="CA66"/>
-      <selection pane="bottomRight" activeCell="CH1" sqref="CH1:CN1048576"/>
+      <selection pane="bottomRight" activeCell="CP10" sqref="CP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -728,8 +725,12 @@
     <col min="78" max="78" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="79" max="81" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="92" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="93" max="16384" width="7.77734375" style="1"/>
+    <col min="83" max="85" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="87" max="89" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="91" max="93" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="94" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:153" x14ac:dyDescent="0.2">
@@ -744,7 +745,7 @@
     </row>
     <row r="3" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:153" x14ac:dyDescent="0.2">
@@ -754,7 +755,7 @@
     </row>
     <row r="6" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:153" x14ac:dyDescent="0.2">
@@ -764,143 +765,144 @@
     </row>
     <row r="9" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="33">
+      <c r="B9" s="31">
         <v>2000</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31">
         <v>2001</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33">
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31">
         <v>2002</v>
       </c>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33">
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31">
         <v>2003</v>
       </c>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33">
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31">
         <v>2004</v>
       </c>
-      <c r="S9" s="33"/>
-      <c r="T9" s="33"/>
-      <c r="U9" s="33"/>
-      <c r="V9" s="33">
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31">
         <v>2005</v>
       </c>
-      <c r="W9" s="33"/>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="33"/>
-      <c r="Z9" s="33">
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="31">
         <v>2006</v>
       </c>
-      <c r="AA9" s="33"/>
-      <c r="AB9" s="33"/>
-      <c r="AC9" s="33"/>
-      <c r="AD9" s="33">
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="31"/>
+      <c r="AC9" s="31"/>
+      <c r="AD9" s="31">
         <v>2007</v>
       </c>
-      <c r="AE9" s="33"/>
-      <c r="AF9" s="33"/>
-      <c r="AG9" s="33"/>
-      <c r="AH9" s="33">
+      <c r="AE9" s="31"/>
+      <c r="AF9" s="31"/>
+      <c r="AG9" s="31"/>
+      <c r="AH9" s="31">
         <v>2008</v>
       </c>
-      <c r="AI9" s="33"/>
-      <c r="AJ9" s="33"/>
-      <c r="AK9" s="33"/>
-      <c r="AL9" s="33">
+      <c r="AI9" s="31"/>
+      <c r="AJ9" s="31"/>
+      <c r="AK9" s="31"/>
+      <c r="AL9" s="31">
         <v>2009</v>
       </c>
-      <c r="AM9" s="33"/>
-      <c r="AN9" s="33"/>
-      <c r="AO9" s="33"/>
-      <c r="AP9" s="33">
+      <c r="AM9" s="31"/>
+      <c r="AN9" s="31"/>
+      <c r="AO9" s="31"/>
+      <c r="AP9" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="33"/>
-      <c r="AR9" s="33"/>
-      <c r="AS9" s="33"/>
-      <c r="AT9" s="33">
+      <c r="AQ9" s="31"/>
+      <c r="AR9" s="31"/>
+      <c r="AS9" s="31"/>
+      <c r="AT9" s="31">
         <v>2011</v>
       </c>
-      <c r="AU9" s="33"/>
-      <c r="AV9" s="33"/>
-      <c r="AW9" s="33"/>
-      <c r="AX9" s="33">
+      <c r="AU9" s="31"/>
+      <c r="AV9" s="31"/>
+      <c r="AW9" s="31"/>
+      <c r="AX9" s="31">
         <v>2012</v>
       </c>
-      <c r="AY9" s="33"/>
-      <c r="AZ9" s="33"/>
-      <c r="BA9" s="33"/>
-      <c r="BB9" s="33">
+      <c r="AY9" s="31"/>
+      <c r="AZ9" s="31"/>
+      <c r="BA9" s="31"/>
+      <c r="BB9" s="31">
         <v>2013</v>
       </c>
-      <c r="BC9" s="33"/>
-      <c r="BD9" s="33"/>
-      <c r="BE9" s="33"/>
-      <c r="BF9" s="33">
+      <c r="BC9" s="31"/>
+      <c r="BD9" s="31"/>
+      <c r="BE9" s="31"/>
+      <c r="BF9" s="31">
         <v>2014</v>
       </c>
-      <c r="BG9" s="33"/>
-      <c r="BH9" s="33"/>
-      <c r="BI9" s="33"/>
-      <c r="BJ9" s="33">
+      <c r="BG9" s="31"/>
+      <c r="BH9" s="31"/>
+      <c r="BI9" s="31"/>
+      <c r="BJ9" s="31">
         <v>2015</v>
       </c>
-      <c r="BK9" s="33"/>
-      <c r="BL9" s="33"/>
-      <c r="BM9" s="33"/>
-      <c r="BN9" s="33">
+      <c r="BK9" s="31"/>
+      <c r="BL9" s="31"/>
+      <c r="BM9" s="31"/>
+      <c r="BN9" s="31">
         <v>2016</v>
       </c>
-      <c r="BO9" s="33"/>
-      <c r="BP9" s="33"/>
-      <c r="BQ9" s="33"/>
-      <c r="BR9" s="34">
+      <c r="BO9" s="31"/>
+      <c r="BP9" s="31"/>
+      <c r="BQ9" s="31"/>
+      <c r="BR9" s="30">
         <v>2017</v>
       </c>
-      <c r="BS9" s="34"/>
-      <c r="BT9" s="34"/>
-      <c r="BU9" s="34"/>
-      <c r="BV9" s="34">
+      <c r="BS9" s="30"/>
+      <c r="BT9" s="30"/>
+      <c r="BU9" s="30"/>
+      <c r="BV9" s="30">
         <v>2018</v>
       </c>
-      <c r="BW9" s="34"/>
-      <c r="BX9" s="34"/>
-      <c r="BY9" s="34"/>
-      <c r="BZ9" s="34">
+      <c r="BW9" s="30"/>
+      <c r="BX9" s="30"/>
+      <c r="BY9" s="30"/>
+      <c r="BZ9" s="30">
         <v>2019</v>
       </c>
-      <c r="CA9" s="34"/>
-      <c r="CB9" s="34"/>
-      <c r="CC9" s="34"/>
-      <c r="CD9" s="34">
+      <c r="CA9" s="30"/>
+      <c r="CB9" s="30"/>
+      <c r="CC9" s="30"/>
+      <c r="CD9" s="30">
         <v>2020</v>
       </c>
-      <c r="CE9" s="34"/>
-      <c r="CF9" s="34"/>
-      <c r="CG9" s="34"/>
-      <c r="CH9" s="34">
+      <c r="CE9" s="30"/>
+      <c r="CF9" s="30"/>
+      <c r="CG9" s="30"/>
+      <c r="CH9" s="30">
         <v>2021</v>
       </c>
-      <c r="CI9" s="34"/>
-      <c r="CJ9" s="34"/>
-      <c r="CK9" s="34"/>
-      <c r="CL9" s="34">
+      <c r="CI9" s="30"/>
+      <c r="CJ9" s="30"/>
+      <c r="CK9" s="30"/>
+      <c r="CL9" s="30">
         <v>2022</v>
       </c>
-      <c r="CM9" s="34"/>
-      <c r="CN9" s="34"/>
+      <c r="CM9" s="30"/>
+      <c r="CN9" s="30"/>
+      <c r="CO9" s="30"/>
     </row>
     <row r="10" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -1178,6 +1180,9 @@
       </c>
       <c r="CN10" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="CO10" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1458,9 +1463,11 @@
         <v>1566368.7437218034</v>
       </c>
       <c r="CN12" s="10">
-        <v>1447422.0423746321</v>
-      </c>
-      <c r="CO12" s="11"/>
+        <v>1451685.7820223121</v>
+      </c>
+      <c r="CO12" s="10">
+        <v>1932064.3672458061</v>
+      </c>
       <c r="CP12" s="11"/>
       <c r="CQ12" s="11"/>
       <c r="CR12" s="11"/>
@@ -1797,9 +1804,11 @@
         <v>74860.089917473437</v>
       </c>
       <c r="CN13" s="10">
-        <v>74795.7906436333</v>
-      </c>
-      <c r="CO13" s="11"/>
+        <v>74289.792089048482</v>
+      </c>
+      <c r="CO13" s="10">
+        <v>109142.10559779602</v>
+      </c>
       <c r="CP13" s="11"/>
       <c r="CQ13" s="11"/>
       <c r="CR13" s="11"/>
@@ -2136,9 +2145,11 @@
         <v>64914.406063883871</v>
       </c>
       <c r="CN14" s="10">
-        <v>67943.680306057722</v>
-      </c>
-      <c r="CO14" s="11"/>
+        <v>69554.021923991808</v>
+      </c>
+      <c r="CO14" s="10">
+        <v>86470.527163922685</v>
+      </c>
       <c r="CP14" s="11"/>
       <c r="CQ14" s="11"/>
       <c r="CR14" s="11"/>
@@ -2475,9 +2486,11 @@
         <v>574802.88069589285</v>
       </c>
       <c r="CN15" s="10">
-        <v>523179.3209197055</v>
-      </c>
-      <c r="CO15" s="11"/>
+        <v>523580.72850303527</v>
+      </c>
+      <c r="CO15" s="10">
+        <v>541263.00036780431</v>
+      </c>
       <c r="CP15" s="11"/>
       <c r="CQ15" s="11"/>
       <c r="CR15" s="11"/>
@@ -2814,9 +2827,11 @@
         <v>103093.70168045604</v>
       </c>
       <c r="CN16" s="10">
-        <v>124232.08946906852</v>
-      </c>
-      <c r="CO16" s="11"/>
+        <v>123408.34211154476</v>
+      </c>
+      <c r="CO16" s="10">
+        <v>131795.65122189542</v>
+      </c>
       <c r="CP16" s="11"/>
       <c r="CQ16" s="11"/>
       <c r="CR16" s="11"/>
@@ -3153,9 +3168,11 @@
         <v>138209.36175477973</v>
       </c>
       <c r="CN17" s="10">
-        <v>222442.30928271718</v>
-      </c>
-      <c r="CO17" s="11"/>
+        <v>219136.25766281766</v>
+      </c>
+      <c r="CO17" s="10">
+        <v>195136.01074342543</v>
+      </c>
       <c r="CP17" s="11"/>
       <c r="CQ17" s="11"/>
       <c r="CR17" s="11"/>
@@ -3492,9 +3509,11 @@
         <v>295969.14642522112</v>
       </c>
       <c r="CN18" s="10">
-        <v>465531.09190673259</v>
-      </c>
-      <c r="CO18" s="11"/>
+        <v>462616.28316767089</v>
+      </c>
+      <c r="CO18" s="10">
+        <v>376555.80258819682</v>
+      </c>
       <c r="CP18" s="11"/>
       <c r="CQ18" s="11"/>
       <c r="CR18" s="11"/>
@@ -3831,9 +3850,11 @@
         <v>127268.98601639032</v>
       </c>
       <c r="CN19" s="10">
-        <v>96958.131594522769</v>
-      </c>
-      <c r="CO19" s="11"/>
+        <v>96871.982373834515</v>
+      </c>
+      <c r="CO19" s="10">
+        <v>126614.50894329554</v>
+      </c>
       <c r="CP19" s="11"/>
       <c r="CQ19" s="11"/>
       <c r="CR19" s="11"/>
@@ -4170,9 +4191,11 @@
         <v>41983.761192967853</v>
       </c>
       <c r="CN20" s="10">
-        <v>53161.871137265283</v>
-      </c>
-      <c r="CO20" s="11"/>
+        <v>53214.762708552298</v>
+      </c>
+      <c r="CO20" s="10">
+        <v>84458.758774137357</v>
+      </c>
       <c r="CP20" s="11"/>
       <c r="CQ20" s="11"/>
       <c r="CR20" s="11"/>
@@ -4509,9 +4532,11 @@
         <v>187158.10532078435</v>
       </c>
       <c r="CN21" s="10">
-        <v>219511.8826930408</v>
-      </c>
-      <c r="CO21" s="11"/>
+        <v>219402.41345024187</v>
+      </c>
+      <c r="CO21" s="10">
+        <v>222839.41359088762</v>
+      </c>
       <c r="CP21" s="11"/>
       <c r="CQ21" s="11"/>
       <c r="CR21" s="11"/>
@@ -4848,9 +4873,11 @@
         <v>182344.68526335541</v>
       </c>
       <c r="CN22" s="10">
-        <v>287705.19347809529</v>
-      </c>
-      <c r="CO22" s="11"/>
+        <v>289764.55945846002</v>
+      </c>
+      <c r="CO22" s="10">
+        <v>372766.13837253017</v>
+      </c>
       <c r="CP22" s="11"/>
       <c r="CQ22" s="11"/>
       <c r="CR22" s="11"/>
@@ -5187,9 +5214,11 @@
         <v>521463.04467852885</v>
       </c>
       <c r="CN23" s="10">
-        <v>545733.85762884712</v>
-      </c>
-      <c r="CO23" s="11"/>
+        <v>546303.19141846139</v>
+      </c>
+      <c r="CO23" s="10">
+        <v>685788.67666286661</v>
+      </c>
       <c r="CP23" s="11"/>
       <c r="CQ23" s="11"/>
       <c r="CR23" s="11"/>
@@ -5661,28 +5690,30 @@
       <c r="CG25" s="15">
         <v>3801007.5529332561</v>
       </c>
-      <c r="CH25" s="30">
+      <c r="CH25" s="15">
         <v>3397554.7518358915</v>
       </c>
-      <c r="CI25" s="30">
+      <c r="CI25" s="15">
         <v>3396198.6721503939</v>
       </c>
-      <c r="CJ25" s="30">
+      <c r="CJ25" s="15">
         <v>3582435.6457165424</v>
       </c>
-      <c r="CK25" s="30">
+      <c r="CK25" s="15">
         <v>4233960.1057822816</v>
       </c>
-      <c r="CL25" s="30">
+      <c r="CL25" s="15">
         <v>3853894.6766090612</v>
       </c>
-      <c r="CM25" s="30">
+      <c r="CM25" s="15">
         <v>3878436.9127315367</v>
       </c>
-      <c r="CN25" s="30">
-        <v>4128617.261434318</v>
-      </c>
-      <c r="CO25" s="11"/>
+      <c r="CN25" s="15">
+        <v>4129828.1168899718</v>
+      </c>
+      <c r="CO25" s="15">
+        <v>4864894.9612725647</v>
+      </c>
       <c r="CP25" s="11"/>
       <c r="CQ25" s="11"/>
       <c r="CR25" s="11"/>
@@ -5837,6 +5868,7 @@
       <c r="CL26" s="16"/>
       <c r="CM26" s="16"/>
       <c r="CN26" s="16"/>
+      <c r="CO26" s="16"/>
     </row>
     <row r="27" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -5928,14 +5960,14 @@
       <c r="CE28" s="21"/>
       <c r="CF28" s="21"/>
       <c r="CG28" s="21"/>
-      <c r="CH28" s="31"/>
-      <c r="CI28" s="31"/>
-      <c r="CJ28" s="31"/>
-      <c r="CK28" s="31"/>
-      <c r="CL28" s="31"/>
-      <c r="CM28" s="31"/>
-      <c r="CN28" s="31"/>
-      <c r="CO28" s="11"/>
+      <c r="CH28" s="21"/>
+      <c r="CI28" s="21"/>
+      <c r="CJ28" s="21"/>
+      <c r="CK28" s="21"/>
+      <c r="CL28" s="21"/>
+      <c r="CM28" s="21"/>
+      <c r="CN28" s="21"/>
+      <c r="CO28" s="21"/>
       <c r="CP28" s="11"/>
       <c r="CQ28" s="11"/>
       <c r="CR28" s="11"/>
@@ -6082,14 +6114,14 @@
       <c r="CE29" s="24"/>
       <c r="CF29" s="24"/>
       <c r="CG29" s="24"/>
-      <c r="CH29" s="32"/>
-      <c r="CI29" s="32"/>
-      <c r="CJ29" s="32"/>
-      <c r="CK29" s="32"/>
-      <c r="CL29" s="32"/>
-      <c r="CM29" s="32"/>
-      <c r="CN29" s="32"/>
-      <c r="CO29" s="11"/>
+      <c r="CH29" s="24"/>
+      <c r="CI29" s="24"/>
+      <c r="CJ29" s="24"/>
+      <c r="CK29" s="24"/>
+      <c r="CL29" s="24"/>
+      <c r="CM29" s="24"/>
+      <c r="CN29" s="24"/>
+      <c r="CO29" s="24"/>
       <c r="CP29" s="11"/>
       <c r="CQ29" s="11"/>
       <c r="CR29" s="11"/>
@@ -6163,7 +6195,7 @@
     </row>
     <row r="32" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:153" x14ac:dyDescent="0.2">
@@ -6173,7 +6205,7 @@
     </row>
     <row r="35" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:153" x14ac:dyDescent="0.2">
@@ -6183,143 +6215,144 @@
     </row>
     <row r="38" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="33">
+      <c r="B38" s="31">
         <v>2000</v>
       </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33">
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31">
         <v>2001</v>
       </c>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33">
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31">
         <v>2002</v>
       </c>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33">
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31">
         <v>2003</v>
       </c>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
-      <c r="Q38" s="33"/>
-      <c r="R38" s="33">
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31">
         <v>2004</v>
       </c>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="33"/>
-      <c r="V38" s="33">
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31">
         <v>2005</v>
       </c>
-      <c r="W38" s="33"/>
-      <c r="X38" s="33"/>
-      <c r="Y38" s="33"/>
-      <c r="Z38" s="33">
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
+      <c r="Z38" s="31">
         <v>2006</v>
       </c>
-      <c r="AA38" s="33"/>
-      <c r="AB38" s="33"/>
-      <c r="AC38" s="33"/>
-      <c r="AD38" s="33">
+      <c r="AA38" s="31"/>
+      <c r="AB38" s="31"/>
+      <c r="AC38" s="31"/>
+      <c r="AD38" s="31">
         <v>2007</v>
       </c>
-      <c r="AE38" s="33"/>
-      <c r="AF38" s="33"/>
-      <c r="AG38" s="33"/>
-      <c r="AH38" s="33">
+      <c r="AE38" s="31"/>
+      <c r="AF38" s="31"/>
+      <c r="AG38" s="31"/>
+      <c r="AH38" s="31">
         <v>2008</v>
       </c>
-      <c r="AI38" s="33"/>
-      <c r="AJ38" s="33"/>
-      <c r="AK38" s="33"/>
-      <c r="AL38" s="33">
+      <c r="AI38" s="31"/>
+      <c r="AJ38" s="31"/>
+      <c r="AK38" s="31"/>
+      <c r="AL38" s="31">
         <v>2009</v>
       </c>
-      <c r="AM38" s="33"/>
-      <c r="AN38" s="33"/>
-      <c r="AO38" s="33"/>
-      <c r="AP38" s="33">
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+      <c r="AO38" s="31"/>
+      <c r="AP38" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ38" s="33"/>
-      <c r="AR38" s="33"/>
-      <c r="AS38" s="33"/>
-      <c r="AT38" s="33">
+      <c r="AQ38" s="31"/>
+      <c r="AR38" s="31"/>
+      <c r="AS38" s="31"/>
+      <c r="AT38" s="31">
         <v>2011</v>
       </c>
-      <c r="AU38" s="33"/>
-      <c r="AV38" s="33"/>
-      <c r="AW38" s="33"/>
-      <c r="AX38" s="33">
+      <c r="AU38" s="31"/>
+      <c r="AV38" s="31"/>
+      <c r="AW38" s="31"/>
+      <c r="AX38" s="31">
         <v>2012</v>
       </c>
-      <c r="AY38" s="33"/>
-      <c r="AZ38" s="33"/>
-      <c r="BA38" s="33"/>
-      <c r="BB38" s="33">
+      <c r="AY38" s="31"/>
+      <c r="AZ38" s="31"/>
+      <c r="BA38" s="31"/>
+      <c r="BB38" s="31">
         <v>2013</v>
       </c>
-      <c r="BC38" s="33"/>
-      <c r="BD38" s="33"/>
-      <c r="BE38" s="33"/>
-      <c r="BF38" s="33">
+      <c r="BC38" s="31"/>
+      <c r="BD38" s="31"/>
+      <c r="BE38" s="31"/>
+      <c r="BF38" s="31">
         <v>2014</v>
       </c>
-      <c r="BG38" s="33"/>
-      <c r="BH38" s="33"/>
-      <c r="BI38" s="33"/>
-      <c r="BJ38" s="33">
+      <c r="BG38" s="31"/>
+      <c r="BH38" s="31"/>
+      <c r="BI38" s="31"/>
+      <c r="BJ38" s="31">
         <v>2015</v>
       </c>
-      <c r="BK38" s="33"/>
-      <c r="BL38" s="33"/>
-      <c r="BM38" s="33"/>
-      <c r="BN38" s="33">
+      <c r="BK38" s="31"/>
+      <c r="BL38" s="31"/>
+      <c r="BM38" s="31"/>
+      <c r="BN38" s="31">
         <v>2016</v>
       </c>
-      <c r="BO38" s="33"/>
-      <c r="BP38" s="33"/>
-      <c r="BQ38" s="33"/>
-      <c r="BR38" s="34">
+      <c r="BO38" s="31"/>
+      <c r="BP38" s="31"/>
+      <c r="BQ38" s="31"/>
+      <c r="BR38" s="30">
         <v>2017</v>
       </c>
-      <c r="BS38" s="34"/>
-      <c r="BT38" s="34"/>
-      <c r="BU38" s="34"/>
-      <c r="BV38" s="34">
+      <c r="BS38" s="30"/>
+      <c r="BT38" s="30"/>
+      <c r="BU38" s="30"/>
+      <c r="BV38" s="30">
         <v>2018</v>
       </c>
-      <c r="BW38" s="34"/>
-      <c r="BX38" s="34"/>
-      <c r="BY38" s="34"/>
-      <c r="BZ38" s="34">
+      <c r="BW38" s="30"/>
+      <c r="BX38" s="30"/>
+      <c r="BY38" s="30"/>
+      <c r="BZ38" s="30">
         <v>2019</v>
       </c>
-      <c r="CA38" s="34"/>
-      <c r="CB38" s="34"/>
-      <c r="CC38" s="34"/>
-      <c r="CD38" s="34">
+      <c r="CA38" s="30"/>
+      <c r="CB38" s="30"/>
+      <c r="CC38" s="30"/>
+      <c r="CD38" s="30">
         <v>2020</v>
       </c>
-      <c r="CE38" s="34"/>
-      <c r="CF38" s="34"/>
-      <c r="CG38" s="34"/>
-      <c r="CH38" s="34">
+      <c r="CE38" s="30"/>
+      <c r="CF38" s="30"/>
+      <c r="CG38" s="30"/>
+      <c r="CH38" s="30">
         <v>2021</v>
       </c>
-      <c r="CI38" s="34"/>
-      <c r="CJ38" s="34"/>
-      <c r="CK38" s="34"/>
-      <c r="CL38" s="34">
+      <c r="CI38" s="30"/>
+      <c r="CJ38" s="30"/>
+      <c r="CK38" s="30"/>
+      <c r="CL38" s="30">
         <v>2022</v>
       </c>
-      <c r="CM38" s="34"/>
-      <c r="CN38" s="34"/>
+      <c r="CM38" s="30"/>
+      <c r="CN38" s="30"/>
+      <c r="CO38" s="30"/>
     </row>
     <row r="39" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -6597,6 +6630,9 @@
       </c>
       <c r="CN39" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="CO39" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -6877,9 +6913,11 @@
         <v>1359377.1967343693</v>
       </c>
       <c r="CN41" s="10">
-        <v>1223797.3567871188</v>
-      </c>
-      <c r="CO41" s="11"/>
+        <v>1227402.3546095223</v>
+      </c>
+      <c r="CO41" s="10">
+        <v>1614965.4573629305</v>
+      </c>
       <c r="CP41" s="11"/>
       <c r="CQ41" s="11"/>
       <c r="CR41" s="11"/>
@@ -7216,9 +7254,11 @@
         <v>48181.233384278457</v>
       </c>
       <c r="CN42" s="10">
-        <v>44607.164360110328</v>
-      </c>
-      <c r="CO42" s="11"/>
+        <v>44305.393892867272</v>
+      </c>
+      <c r="CO42" s="10">
+        <v>69139.808603506113</v>
+      </c>
       <c r="CP42" s="11"/>
       <c r="CQ42" s="11"/>
       <c r="CR42" s="11"/>
@@ -7555,9 +7595,11 @@
         <v>55970.074684183695</v>
       </c>
       <c r="CN43" s="10">
-        <v>63680.949954978059</v>
-      </c>
-      <c r="CO43" s="11"/>
+        <v>65190.260070652439</v>
+      </c>
+      <c r="CO43" s="10">
+        <v>80147.35175470839</v>
+      </c>
       <c r="CP43" s="11"/>
       <c r="CQ43" s="11"/>
       <c r="CR43" s="11"/>
@@ -7894,9 +7936,11 @@
         <v>521094.13428486529</v>
       </c>
       <c r="CN44" s="10">
-        <v>440204.03601303318</v>
-      </c>
-      <c r="CO44" s="11"/>
+        <v>440541.78108666756</v>
+      </c>
+      <c r="CO44" s="10">
+        <v>462151.73480429081</v>
+      </c>
       <c r="CP44" s="11"/>
       <c r="CQ44" s="11"/>
       <c r="CR44" s="11"/>
@@ -8233,9 +8277,11 @@
         <v>92016.486939449867</v>
       </c>
       <c r="CN45" s="10">
-        <v>108355.21511056753</v>
-      </c>
-      <c r="CO45" s="11"/>
+        <v>107636.74275368526</v>
+      </c>
+      <c r="CO45" s="10">
+        <v>117842.51314579241</v>
+      </c>
       <c r="CP45" s="11"/>
       <c r="CQ45" s="11"/>
       <c r="CR45" s="11"/>
@@ -8572,9 +8618,11 @@
         <v>126609.68897286928</v>
       </c>
       <c r="CN46" s="10">
-        <v>194356.15373197355</v>
-      </c>
-      <c r="CO46" s="11"/>
+        <v>191467.53295225321</v>
+      </c>
+      <c r="CO46" s="10">
+        <v>170677.12725855637</v>
+      </c>
       <c r="CP46" s="11"/>
       <c r="CQ46" s="11"/>
       <c r="CR46" s="11"/>
@@ -8911,9 +8959,11 @@
         <v>237089.60293205726</v>
       </c>
       <c r="CN47" s="10">
-        <v>327756.35641066451</v>
-      </c>
-      <c r="CO47" s="11"/>
+        <v>325704.19038232067</v>
+      </c>
+      <c r="CO47" s="10">
+        <v>297786.34651382209</v>
+      </c>
       <c r="CP47" s="11"/>
       <c r="CQ47" s="11"/>
       <c r="CR47" s="11"/>
@@ -9250,9 +9300,11 @@
         <v>124681.93067322711</v>
       </c>
       <c r="CN48" s="10">
-        <v>96723.354802973481</v>
-      </c>
-      <c r="CO48" s="11"/>
+        <v>96637.414186115508</v>
+      </c>
+      <c r="CO48" s="10">
+        <v>129501.23148380035</v>
+      </c>
       <c r="CP48" s="11"/>
       <c r="CQ48" s="11"/>
       <c r="CR48" s="11"/>
@@ -9589,9 +9641,11 @@
         <v>40675.021685712061</v>
       </c>
       <c r="CN49" s="10">
-        <v>51283.064171945523</v>
-      </c>
-      <c r="CO49" s="11"/>
+        <v>51334.086489001733</v>
+      </c>
+      <c r="CO49" s="10">
+        <v>78626.137610299207</v>
+      </c>
       <c r="CP49" s="11"/>
       <c r="CQ49" s="11"/>
       <c r="CR49" s="11"/>
@@ -9928,9 +9982,11 @@
         <v>175581.40026522669</v>
       </c>
       <c r="CN50" s="10">
-        <v>201819.05369660654</v>
-      </c>
-      <c r="CO50" s="11"/>
+        <v>201718.40776017922</v>
+      </c>
+      <c r="CO50" s="10">
+        <v>217284.99806181726</v>
+      </c>
       <c r="CP50" s="11"/>
       <c r="CQ50" s="11"/>
       <c r="CR50" s="11"/>
@@ -10267,9 +10323,11 @@
         <v>168071.32293949748</v>
       </c>
       <c r="CN51" s="10">
-        <v>242385.99179231143</v>
-      </c>
-      <c r="CO51" s="11"/>
+        <v>244120.96730519543</v>
+      </c>
+      <c r="CO51" s="10">
+        <v>320767.81728373282</v>
+      </c>
       <c r="CP51" s="11"/>
       <c r="CQ51" s="11"/>
       <c r="CR51" s="11"/>
@@ -10606,9 +10664,11 @@
         <v>449718.58169500902</v>
       </c>
       <c r="CN52" s="10">
-        <v>509520.5050821944</v>
-      </c>
-      <c r="CO52" s="11"/>
+        <v>510052.05949464196</v>
+      </c>
+      <c r="CO52" s="10">
+        <v>640928.01680368162</v>
+      </c>
       <c r="CP52" s="11"/>
       <c r="CQ52" s="11"/>
       <c r="CR52" s="11"/>
@@ -11080,28 +11140,30 @@
       <c r="CG54" s="15">
         <v>3648921.6749099772</v>
       </c>
-      <c r="CH54" s="30">
+      <c r="CH54" s="15">
         <v>3156671.4757222617</v>
       </c>
-      <c r="CI54" s="30">
+      <c r="CI54" s="15">
         <v>3131017.1444008318</v>
       </c>
-      <c r="CJ54" s="30">
+      <c r="CJ54" s="15">
         <v>3244927.2295096582</v>
       </c>
-      <c r="CK54" s="30">
+      <c r="CK54" s="15">
         <v>3923915.6638969723</v>
       </c>
-      <c r="CL54" s="30">
+      <c r="CL54" s="15">
         <v>3473351.0415488388</v>
       </c>
-      <c r="CM54" s="30">
+      <c r="CM54" s="15">
         <v>3399066.6751907454</v>
       </c>
-      <c r="CN54" s="30">
-        <v>3504489.2019144772</v>
-      </c>
-      <c r="CO54" s="11"/>
+      <c r="CN54" s="15">
+        <v>3506111.1909831027</v>
+      </c>
+      <c r="CO54" s="15">
+        <v>4199818.540686938</v>
+      </c>
       <c r="CP54" s="11"/>
       <c r="CQ54" s="11"/>
       <c r="CR54" s="11"/>
@@ -11256,6 +11318,7 @@
       <c r="CL55" s="16"/>
       <c r="CM55" s="16"/>
       <c r="CN55" s="16"/>
+      <c r="CO55" s="16"/>
     </row>
     <row r="56" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
@@ -11501,14 +11564,14 @@
       <c r="CE58" s="24"/>
       <c r="CF58" s="24"/>
       <c r="CG58" s="24"/>
-      <c r="CH58" s="32"/>
-      <c r="CI58" s="32"/>
-      <c r="CJ58" s="32"/>
-      <c r="CK58" s="32"/>
-      <c r="CL58" s="32"/>
-      <c r="CM58" s="32"/>
-      <c r="CN58" s="32"/>
-      <c r="CO58" s="11"/>
+      <c r="CH58" s="24"/>
+      <c r="CI58" s="24"/>
+      <c r="CJ58" s="24"/>
+      <c r="CK58" s="24"/>
+      <c r="CL58" s="24"/>
+      <c r="CM58" s="24"/>
+      <c r="CN58" s="24"/>
+      <c r="CO58" s="24"/>
       <c r="CP58" s="11"/>
       <c r="CQ58" s="11"/>
       <c r="CR58" s="11"/>
@@ -11582,7 +11645,7 @@
     </row>
     <row r="61" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:153" x14ac:dyDescent="0.2">
@@ -11592,7 +11655,7 @@
     </row>
     <row r="64" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:149" x14ac:dyDescent="0.2">
@@ -11602,141 +11665,142 @@
     </row>
     <row r="67" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="33"/>
-      <c r="F67" s="33" t="s">
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G67" s="33"/>
-      <c r="H67" s="33"/>
-      <c r="I67" s="33"/>
-      <c r="J67" s="33" t="s">
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K67" s="33"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="33"/>
-      <c r="N67" s="33" t="s">
+      <c r="K67" s="31"/>
+      <c r="L67" s="31"/>
+      <c r="M67" s="31"/>
+      <c r="N67" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="O67" s="33"/>
-      <c r="P67" s="33"/>
-      <c r="Q67" s="33"/>
-      <c r="R67" s="33" t="s">
+      <c r="O67" s="31"/>
+      <c r="P67" s="31"/>
+      <c r="Q67" s="31"/>
+      <c r="R67" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="S67" s="33"/>
-      <c r="T67" s="33"/>
-      <c r="U67" s="33"/>
-      <c r="V67" s="33" t="s">
+      <c r="S67" s="31"/>
+      <c r="T67" s="31"/>
+      <c r="U67" s="31"/>
+      <c r="V67" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="W67" s="33"/>
-      <c r="X67" s="33"/>
-      <c r="Y67" s="33"/>
-      <c r="Z67" s="33" t="s">
+      <c r="W67" s="31"/>
+      <c r="X67" s="31"/>
+      <c r="Y67" s="31"/>
+      <c r="Z67" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="AA67" s="33"/>
-      <c r="AB67" s="33"/>
-      <c r="AC67" s="33"/>
-      <c r="AD67" s="33" t="s">
+      <c r="AA67" s="31"/>
+      <c r="AB67" s="31"/>
+      <c r="AC67" s="31"/>
+      <c r="AD67" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="AE67" s="33"/>
-      <c r="AF67" s="33"/>
-      <c r="AG67" s="33"/>
-      <c r="AH67" s="33" t="s">
+      <c r="AE67" s="31"/>
+      <c r="AF67" s="31"/>
+      <c r="AG67" s="31"/>
+      <c r="AH67" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="AI67" s="33"/>
-      <c r="AJ67" s="33"/>
-      <c r="AK67" s="33"/>
-      <c r="AL67" s="33" t="s">
+      <c r="AI67" s="31"/>
+      <c r="AJ67" s="31"/>
+      <c r="AK67" s="31"/>
+      <c r="AL67" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="AM67" s="33"/>
-      <c r="AN67" s="33"/>
-      <c r="AO67" s="33"/>
-      <c r="AP67" s="33" t="s">
+      <c r="AM67" s="31"/>
+      <c r="AN67" s="31"/>
+      <c r="AO67" s="31"/>
+      <c r="AP67" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="AQ67" s="33"/>
-      <c r="AR67" s="33"/>
-      <c r="AS67" s="33"/>
-      <c r="AT67" s="33" t="s">
+      <c r="AQ67" s="31"/>
+      <c r="AR67" s="31"/>
+      <c r="AS67" s="31"/>
+      <c r="AT67" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="AU67" s="33"/>
-      <c r="AV67" s="33"/>
-      <c r="AW67" s="33"/>
-      <c r="AX67" s="33" t="s">
+      <c r="AU67" s="31"/>
+      <c r="AV67" s="31"/>
+      <c r="AW67" s="31"/>
+      <c r="AX67" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="AY67" s="33"/>
-      <c r="AZ67" s="33"/>
-      <c r="BA67" s="33"/>
-      <c r="BB67" s="33" t="s">
+      <c r="AY67" s="31"/>
+      <c r="AZ67" s="31"/>
+      <c r="BA67" s="31"/>
+      <c r="BB67" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="BC67" s="33"/>
-      <c r="BD67" s="33"/>
-      <c r="BE67" s="33"/>
-      <c r="BF67" s="33" t="s">
+      <c r="BC67" s="31"/>
+      <c r="BD67" s="31"/>
+      <c r="BE67" s="31"/>
+      <c r="BF67" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="BG67" s="33"/>
-      <c r="BH67" s="33"/>
-      <c r="BI67" s="33"/>
-      <c r="BJ67" s="33" t="s">
+      <c r="BG67" s="31"/>
+      <c r="BH67" s="31"/>
+      <c r="BI67" s="31"/>
+      <c r="BJ67" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="BK67" s="33"/>
-      <c r="BL67" s="33"/>
-      <c r="BM67" s="33"/>
-      <c r="BN67" s="33" t="s">
+      <c r="BK67" s="31"/>
+      <c r="BL67" s="31"/>
+      <c r="BM67" s="31"/>
+      <c r="BN67" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="BO67" s="33"/>
-      <c r="BP67" s="33"/>
-      <c r="BQ67" s="33"/>
-      <c r="BR67" s="34" t="s">
+      <c r="BO67" s="31"/>
+      <c r="BP67" s="31"/>
+      <c r="BQ67" s="31"/>
+      <c r="BR67" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="BS67" s="34"/>
-      <c r="BT67" s="34"/>
-      <c r="BU67" s="34"/>
-      <c r="BV67" s="34" t="s">
+      <c r="BS67" s="30"/>
+      <c r="BT67" s="30"/>
+      <c r="BU67" s="30"/>
+      <c r="BV67" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="BW67" s="34"/>
-      <c r="BX67" s="34"/>
-      <c r="BY67" s="34"/>
-      <c r="BZ67" s="34" t="s">
+      <c r="BW67" s="30"/>
+      <c r="BX67" s="30"/>
+      <c r="BY67" s="30"/>
+      <c r="BZ67" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="CA67" s="34"/>
-      <c r="CB67" s="34"/>
-      <c r="CC67" s="34"/>
-      <c r="CD67" s="34" t="s">
+      <c r="CA67" s="30"/>
+      <c r="CB67" s="30"/>
+      <c r="CC67" s="30"/>
+      <c r="CD67" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="CE67" s="34"/>
-      <c r="CF67" s="34"/>
-      <c r="CG67" s="34"/>
-      <c r="CH67" s="34" t="s">
+      <c r="CE67" s="30"/>
+      <c r="CF67" s="30"/>
+      <c r="CG67" s="30"/>
+      <c r="CH67" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="CI67" s="34"/>
-      <c r="CJ67" s="34"/>
-      <c r="CK67" s="4"/>
-      <c r="CL67" s="34"/>
-      <c r="CM67" s="34"/>
-      <c r="CN67" s="4"/>
+      <c r="CI67" s="30"/>
+      <c r="CJ67" s="30"/>
+      <c r="CK67" s="30"/>
+      <c r="CL67" s="30"/>
+      <c r="CM67" s="30"/>
+      <c r="CN67" s="30"/>
+      <c r="CO67" s="30"/>
     </row>
     <row r="68" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
@@ -12003,10 +12067,13 @@
       <c r="CJ68" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="CK68" s="7"/>
+      <c r="CK68" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="CL68" s="7"/>
       <c r="CM68" s="7"/>
       <c r="CN68" s="7"/>
+      <c r="CO68" s="7"/>
     </row>
     <row r="69" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
@@ -12274,13 +12341,15 @@
         <v>11.740458351862841</v>
       </c>
       <c r="CJ70" s="26">
-        <v>11.151227845362868</v>
-      </c>
-      <c r="CK70" s="26"/>
+        <v>11.478651280392967</v>
+      </c>
+      <c r="CK70" s="26">
+        <v>14.084808546536507</v>
+      </c>
       <c r="CL70" s="26"/>
       <c r="CM70" s="26"/>
       <c r="CN70" s="26"/>
-      <c r="CO70" s="11"/>
+      <c r="CO70" s="26"/>
       <c r="CP70" s="11"/>
       <c r="CQ70" s="11"/>
       <c r="CR70" s="11"/>
@@ -12601,13 +12670,15 @@
         <v>10.249787890722899</v>
       </c>
       <c r="CJ71" s="26">
-        <v>-1.7502827870363404</v>
-      </c>
-      <c r="CK71" s="26"/>
+        <v>-2.4149487324100818</v>
+      </c>
+      <c r="CK71" s="26">
+        <v>14.382122600044795</v>
+      </c>
       <c r="CL71" s="26"/>
       <c r="CM71" s="26"/>
       <c r="CN71" s="26"/>
-      <c r="CO71" s="11"/>
+      <c r="CO71" s="26"/>
       <c r="CP71" s="11"/>
       <c r="CQ71" s="11"/>
       <c r="CR71" s="11"/>
@@ -12928,13 +12999,15 @@
         <v>7.1613224771094792</v>
       </c>
       <c r="CJ72" s="26">
-        <v>-2.9400297906872623</v>
-      </c>
-      <c r="CK72" s="26"/>
+        <v>-0.63959936420117458</v>
+      </c>
+      <c r="CK72" s="26">
+        <v>13.655243123508228</v>
+      </c>
       <c r="CL72" s="26"/>
       <c r="CM72" s="26"/>
       <c r="CN72" s="26"/>
-      <c r="CO72" s="11"/>
+      <c r="CO72" s="26"/>
       <c r="CP72" s="11"/>
       <c r="CQ72" s="11"/>
       <c r="CR72" s="11"/>
@@ -13255,13 +13328,15 @@
         <v>13.99182801060617</v>
       </c>
       <c r="CJ73" s="26">
-        <v>9.1587849685091527</v>
-      </c>
-      <c r="CK73" s="26"/>
+        <v>9.2425366810126093</v>
+      </c>
+      <c r="CK73" s="26">
+        <v>11.678280109053674</v>
+      </c>
       <c r="CL73" s="26"/>
       <c r="CM73" s="26"/>
       <c r="CN73" s="26"/>
-      <c r="CO73" s="11"/>
+      <c r="CO73" s="26"/>
       <c r="CP73" s="11"/>
       <c r="CQ73" s="11"/>
       <c r="CR73" s="11"/>
@@ -13582,13 +13657,15 @@
         <v>9.8768823178817229</v>
       </c>
       <c r="CJ74" s="26">
-        <v>13.128951967603626</v>
-      </c>
-      <c r="CK74" s="26"/>
+        <v>12.378826330652544</v>
+      </c>
+      <c r="CK74" s="26">
+        <v>14.599393058568893</v>
+      </c>
       <c r="CL74" s="26"/>
       <c r="CM74" s="26"/>
       <c r="CN74" s="26"/>
-      <c r="CO74" s="11"/>
+      <c r="CO74" s="26"/>
       <c r="CP74" s="11"/>
       <c r="CQ74" s="11"/>
       <c r="CR74" s="11"/>
@@ -13909,13 +13986,15 @@
         <v>-5.5798076444133926E-2</v>
       </c>
       <c r="CJ75" s="26">
-        <v>9.5001212693810828</v>
-      </c>
-      <c r="CK75" s="26"/>
+        <v>7.872674339571887</v>
+      </c>
+      <c r="CK75" s="26">
+        <v>8.5927491333481782</v>
+      </c>
       <c r="CL75" s="26"/>
       <c r="CM75" s="26"/>
       <c r="CN75" s="26"/>
-      <c r="CO75" s="11"/>
+      <c r="CO75" s="26"/>
       <c r="CP75" s="11"/>
       <c r="CQ75" s="11"/>
       <c r="CR75" s="11"/>
@@ -14236,13 +14315,15 @@
         <v>43.830700019572674</v>
       </c>
       <c r="CJ76" s="26">
-        <v>39.405611281779471</v>
-      </c>
-      <c r="CK76" s="26"/>
+        <v>38.532757242376732</v>
+      </c>
+      <c r="CK76" s="26">
+        <v>21.192184051873369</v>
+      </c>
       <c r="CL76" s="26"/>
       <c r="CM76" s="26"/>
       <c r="CN76" s="26"/>
-      <c r="CO76" s="11"/>
+      <c r="CO76" s="26"/>
       <c r="CP76" s="11"/>
       <c r="CQ76" s="11"/>
       <c r="CR76" s="11"/>
@@ -14563,13 +14644,15 @@
         <v>10.320931144909437</v>
       </c>
       <c r="CJ77" s="26">
-        <v>7.780031501783796</v>
-      </c>
-      <c r="CK77" s="26"/>
+        <v>7.6842668086432013</v>
+      </c>
+      <c r="CK77" s="26">
+        <v>6.3247396980613786</v>
+      </c>
       <c r="CL77" s="26"/>
       <c r="CM77" s="26"/>
       <c r="CN77" s="26"/>
-      <c r="CO77" s="11"/>
+      <c r="CO77" s="26"/>
       <c r="CP77" s="11"/>
       <c r="CQ77" s="11"/>
       <c r="CR77" s="11"/>
@@ -14890,13 +14973,15 @@
         <v>40.337799758432624</v>
       </c>
       <c r="CJ78" s="26">
-        <v>49.490424187724415</v>
-      </c>
-      <c r="CK78" s="26"/>
+        <v>49.639154532584485</v>
+      </c>
+      <c r="CK78" s="26">
+        <v>19.169117113990779</v>
+      </c>
       <c r="CL78" s="26"/>
       <c r="CM78" s="26"/>
       <c r="CN78" s="26"/>
-      <c r="CO78" s="11"/>
+      <c r="CO78" s="26"/>
       <c r="CP78" s="11"/>
       <c r="CQ78" s="11"/>
       <c r="CR78" s="11"/>
@@ -15217,13 +15302,15 @@
         <v>8.1242392521675839</v>
       </c>
       <c r="CJ79" s="26">
-        <v>8.453074846232127</v>
-      </c>
-      <c r="CK79" s="26"/>
+        <v>8.3989899564440123</v>
+      </c>
+      <c r="CK79" s="26">
+        <v>15.506097686573156</v>
+      </c>
       <c r="CL79" s="26"/>
       <c r="CM79" s="26"/>
       <c r="CN79" s="26"/>
-      <c r="CO79" s="11"/>
+      <c r="CO79" s="26"/>
       <c r="CP79" s="11"/>
       <c r="CQ79" s="11"/>
       <c r="CR79" s="11"/>
@@ -15544,13 +15631,15 @@
         <v>36.98809322212847</v>
       </c>
       <c r="CJ80" s="26">
-        <v>44.461553239018315</v>
-      </c>
-      <c r="CK80" s="26"/>
+        <v>45.495595080997532</v>
+      </c>
+      <c r="CK80" s="26">
+        <v>32.737421254601742</v>
+      </c>
       <c r="CL80" s="26"/>
       <c r="CM80" s="26"/>
       <c r="CN80" s="26"/>
-      <c r="CO80" s="11"/>
+      <c r="CO80" s="26"/>
       <c r="CP80" s="11"/>
       <c r="CQ80" s="11"/>
       <c r="CR80" s="11"/>
@@ -15871,13 +15960,15 @@
         <v>10.40750946111477</v>
       </c>
       <c r="CJ81" s="26">
-        <v>13.497300320640363</v>
-      </c>
-      <c r="CK81" s="26"/>
+        <v>13.615705743355562</v>
+      </c>
+      <c r="CK81" s="26">
+        <v>11.484379082457494</v>
+      </c>
       <c r="CL81" s="26"/>
       <c r="CM81" s="26"/>
       <c r="CN81" s="26"/>
-      <c r="CO81" s="11"/>
+      <c r="CO81" s="26"/>
       <c r="CP81" s="11"/>
       <c r="CQ81" s="11"/>
       <c r="CR81" s="11"/>
@@ -16348,13 +16439,15 @@
         <v>14.1993530748247</v>
       </c>
       <c r="CJ83" s="26">
-        <v>15.24609706166909</v>
-      </c>
-      <c r="CK83" s="26"/>
+        <v>15.27989684414672</v>
+      </c>
+      <c r="CK83" s="26">
+        <v>14.901766661160096</v>
+      </c>
       <c r="CL83" s="26"/>
       <c r="CM83" s="26"/>
       <c r="CN83" s="26"/>
-      <c r="CO83" s="11"/>
+      <c r="CO83" s="26"/>
       <c r="CP83" s="11"/>
       <c r="CQ83" s="11"/>
       <c r="CR83" s="11"/>
@@ -16505,6 +16598,7 @@
       <c r="CL84" s="16"/>
       <c r="CM84" s="16"/>
       <c r="CN84" s="16"/>
+      <c r="CO84" s="16"/>
     </row>
     <row r="85" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
@@ -16823,7 +16917,7 @@
     </row>
     <row r="90" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:149" x14ac:dyDescent="0.2">
@@ -16833,7 +16927,7 @@
     </row>
     <row r="93" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:149" x14ac:dyDescent="0.2">
@@ -16843,141 +16937,142 @@
     </row>
     <row r="96" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
-      <c r="B96" s="33" t="s">
+      <c r="B96" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C96" s="33"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="33"/>
-      <c r="F96" s="33" t="s">
+      <c r="C96" s="31"/>
+      <c r="D96" s="31"/>
+      <c r="E96" s="31"/>
+      <c r="F96" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G96" s="33"/>
-      <c r="H96" s="33"/>
-      <c r="I96" s="33"/>
-      <c r="J96" s="33" t="s">
+      <c r="G96" s="31"/>
+      <c r="H96" s="31"/>
+      <c r="I96" s="31"/>
+      <c r="J96" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K96" s="33"/>
-      <c r="L96" s="33"/>
-      <c r="M96" s="33"/>
-      <c r="N96" s="33" t="s">
+      <c r="K96" s="31"/>
+      <c r="L96" s="31"/>
+      <c r="M96" s="31"/>
+      <c r="N96" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="O96" s="33"/>
-      <c r="P96" s="33"/>
-      <c r="Q96" s="33"/>
-      <c r="R96" s="33" t="s">
+      <c r="O96" s="31"/>
+      <c r="P96" s="31"/>
+      <c r="Q96" s="31"/>
+      <c r="R96" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="S96" s="33"/>
-      <c r="T96" s="33"/>
-      <c r="U96" s="33"/>
-      <c r="V96" s="33" t="s">
+      <c r="S96" s="31"/>
+      <c r="T96" s="31"/>
+      <c r="U96" s="31"/>
+      <c r="V96" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="W96" s="33"/>
-      <c r="X96" s="33"/>
-      <c r="Y96" s="33"/>
-      <c r="Z96" s="33" t="s">
+      <c r="W96" s="31"/>
+      <c r="X96" s="31"/>
+      <c r="Y96" s="31"/>
+      <c r="Z96" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="AA96" s="33"/>
-      <c r="AB96" s="33"/>
-      <c r="AC96" s="33"/>
-      <c r="AD96" s="33" t="s">
+      <c r="AA96" s="31"/>
+      <c r="AB96" s="31"/>
+      <c r="AC96" s="31"/>
+      <c r="AD96" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="AE96" s="33"/>
-      <c r="AF96" s="33"/>
-      <c r="AG96" s="33"/>
-      <c r="AH96" s="33" t="s">
+      <c r="AE96" s="31"/>
+      <c r="AF96" s="31"/>
+      <c r="AG96" s="31"/>
+      <c r="AH96" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="AI96" s="33"/>
-      <c r="AJ96" s="33"/>
-      <c r="AK96" s="33"/>
-      <c r="AL96" s="33" t="s">
+      <c r="AI96" s="31"/>
+      <c r="AJ96" s="31"/>
+      <c r="AK96" s="31"/>
+      <c r="AL96" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="AM96" s="33"/>
-      <c r="AN96" s="33"/>
-      <c r="AO96" s="33"/>
-      <c r="AP96" s="33" t="s">
+      <c r="AM96" s="31"/>
+      <c r="AN96" s="31"/>
+      <c r="AO96" s="31"/>
+      <c r="AP96" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="AQ96" s="33"/>
-      <c r="AR96" s="33"/>
-      <c r="AS96" s="33"/>
-      <c r="AT96" s="33" t="s">
+      <c r="AQ96" s="31"/>
+      <c r="AR96" s="31"/>
+      <c r="AS96" s="31"/>
+      <c r="AT96" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="AU96" s="33"/>
-      <c r="AV96" s="33"/>
-      <c r="AW96" s="33"/>
-      <c r="AX96" s="33" t="s">
+      <c r="AU96" s="31"/>
+      <c r="AV96" s="31"/>
+      <c r="AW96" s="31"/>
+      <c r="AX96" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="AY96" s="33"/>
-      <c r="AZ96" s="33"/>
-      <c r="BA96" s="33"/>
-      <c r="BB96" s="33" t="s">
+      <c r="AY96" s="31"/>
+      <c r="AZ96" s="31"/>
+      <c r="BA96" s="31"/>
+      <c r="BB96" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="BC96" s="33"/>
-      <c r="BD96" s="33"/>
-      <c r="BE96" s="33"/>
-      <c r="BF96" s="33" t="s">
+      <c r="BC96" s="31"/>
+      <c r="BD96" s="31"/>
+      <c r="BE96" s="31"/>
+      <c r="BF96" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="BG96" s="33"/>
-      <c r="BH96" s="33"/>
-      <c r="BI96" s="33"/>
-      <c r="BJ96" s="33" t="s">
+      <c r="BG96" s="31"/>
+      <c r="BH96" s="31"/>
+      <c r="BI96" s="31"/>
+      <c r="BJ96" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="BK96" s="33"/>
-      <c r="BL96" s="33"/>
-      <c r="BM96" s="33"/>
-      <c r="BN96" s="33" t="s">
+      <c r="BK96" s="31"/>
+      <c r="BL96" s="31"/>
+      <c r="BM96" s="31"/>
+      <c r="BN96" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="BO96" s="33"/>
-      <c r="BP96" s="33"/>
-      <c r="BQ96" s="33"/>
-      <c r="BR96" s="34" t="s">
+      <c r="BO96" s="31"/>
+      <c r="BP96" s="31"/>
+      <c r="BQ96" s="31"/>
+      <c r="BR96" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="BS96" s="34"/>
-      <c r="BT96" s="34"/>
-      <c r="BU96" s="34"/>
-      <c r="BV96" s="34" t="s">
+      <c r="BS96" s="30"/>
+      <c r="BT96" s="30"/>
+      <c r="BU96" s="30"/>
+      <c r="BV96" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="BW96" s="34"/>
-      <c r="BX96" s="34"/>
-      <c r="BY96" s="34"/>
-      <c r="BZ96" s="34" t="s">
+      <c r="BW96" s="30"/>
+      <c r="BX96" s="30"/>
+      <c r="BY96" s="30"/>
+      <c r="BZ96" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="CA96" s="34"/>
-      <c r="CB96" s="34"/>
-      <c r="CC96" s="34"/>
-      <c r="CD96" s="34" t="s">
+      <c r="CA96" s="30"/>
+      <c r="CB96" s="30"/>
+      <c r="CC96" s="30"/>
+      <c r="CD96" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="CE96" s="34"/>
-      <c r="CF96" s="34"/>
-      <c r="CG96" s="34"/>
-      <c r="CH96" s="34" t="s">
+      <c r="CE96" s="30"/>
+      <c r="CF96" s="30"/>
+      <c r="CG96" s="30"/>
+      <c r="CH96" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="CI96" s="34"/>
-      <c r="CJ96" s="34"/>
-      <c r="CK96" s="4"/>
-      <c r="CL96" s="34"/>
-      <c r="CM96" s="34"/>
-      <c r="CN96" s="4"/>
+      <c r="CI96" s="30"/>
+      <c r="CJ96" s="30"/>
+      <c r="CK96" s="30"/>
+      <c r="CL96" s="30"/>
+      <c r="CM96" s="30"/>
+      <c r="CN96" s="30"/>
+      <c r="CO96" s="30"/>
     </row>
     <row r="97" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
@@ -17244,10 +17339,13 @@
       <c r="CJ97" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="CK97" s="7"/>
+      <c r="CK97" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="CL97" s="7"/>
       <c r="CM97" s="7"/>
       <c r="CN97" s="7"/>
+      <c r="CO97" s="7"/>
     </row>
     <row r="98" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
@@ -17515,13 +17613,15 @@
         <v>5.7300896143217699</v>
       </c>
       <c r="CJ99" s="26">
-        <v>3.8964820872820098</v>
-      </c>
-      <c r="CK99" s="26"/>
+        <v>4.2025348742101869</v>
+      </c>
+      <c r="CK99" s="26">
+        <v>3.8460218945411242</v>
+      </c>
       <c r="CL99" s="26"/>
       <c r="CM99" s="26"/>
       <c r="CN99" s="26"/>
-      <c r="CO99" s="11"/>
+      <c r="CO99" s="26"/>
       <c r="CP99" s="11"/>
       <c r="CQ99" s="11"/>
       <c r="CR99" s="11"/>
@@ -17842,13 +17942,15 @@
         <v>2.7320736211386532</v>
       </c>
       <c r="CJ100" s="26">
-        <v>-10.039445224275696</v>
-      </c>
-      <c r="CK100" s="26"/>
+        <v>-10.648034428219603</v>
+      </c>
+      <c r="CK100" s="26">
+        <v>3.4645925427717827</v>
+      </c>
       <c r="CL100" s="26"/>
       <c r="CM100" s="26"/>
       <c r="CN100" s="26"/>
-      <c r="CO100" s="11"/>
+      <c r="CO100" s="26"/>
       <c r="CP100" s="11"/>
       <c r="CQ100" s="11"/>
       <c r="CR100" s="11"/>
@@ -18169,13 +18271,15 @@
         <v>4.464427553075339</v>
       </c>
       <c r="CJ101" s="26">
-        <v>-5.5243799808292948</v>
-      </c>
-      <c r="CK101" s="26"/>
+        <v>-3.2852015596475326</v>
+      </c>
+      <c r="CK101" s="26">
+        <v>9.7783138248607173</v>
+      </c>
       <c r="CL101" s="26"/>
       <c r="CM101" s="26"/>
       <c r="CN101" s="26"/>
-      <c r="CO101" s="11"/>
+      <c r="CO101" s="26"/>
       <c r="CP101" s="11"/>
       <c r="CQ101" s="11"/>
       <c r="CR101" s="11"/>
@@ -18496,13 +18600,15 @@
         <v>6.8800990391981998</v>
       </c>
       <c r="CJ102" s="26">
-        <v>1.3308625699598053</v>
-      </c>
-      <c r="CK102" s="26"/>
+        <v>1.4086083351965328</v>
+      </c>
+      <c r="CK102" s="26">
+        <v>4.2695681318162002</v>
+      </c>
       <c r="CL102" s="26"/>
       <c r="CM102" s="26"/>
       <c r="CN102" s="26"/>
-      <c r="CO102" s="11"/>
+      <c r="CO102" s="26"/>
       <c r="CP102" s="11"/>
       <c r="CQ102" s="11"/>
       <c r="CR102" s="11"/>
@@ -18823,13 +18929,15 @@
         <v>7.042625605422856</v>
       </c>
       <c r="CJ103" s="26">
-        <v>9.4731394077255118</v>
-      </c>
-      <c r="CK103" s="26"/>
+        <v>8.7472544154313425</v>
+      </c>
+      <c r="CK103" s="26">
+        <v>9.8090647313618007</v>
+      </c>
       <c r="CL103" s="26"/>
       <c r="CM103" s="26"/>
       <c r="CN103" s="26"/>
-      <c r="CO103" s="11"/>
+      <c r="CO103" s="26"/>
       <c r="CP103" s="11"/>
       <c r="CQ103" s="11"/>
       <c r="CR103" s="11"/>
@@ -19150,13 +19258,15 @@
         <v>-2.4700497527116454</v>
       </c>
       <c r="CJ104" s="26">
-        <v>6.9095240552757389</v>
-      </c>
-      <c r="CK104" s="26"/>
+        <v>5.3205799091492452</v>
+      </c>
+      <c r="CK104" s="26">
+        <v>5.6090903134278847</v>
+      </c>
       <c r="CL104" s="26"/>
       <c r="CM104" s="26"/>
       <c r="CN104" s="26"/>
-      <c r="CO104" s="11"/>
+      <c r="CO104" s="26"/>
       <c r="CP104" s="11"/>
       <c r="CQ104" s="11"/>
       <c r="CR104" s="11"/>
@@ -19477,13 +19587,15 @@
         <v>25.17624858175229</v>
       </c>
       <c r="CJ105" s="26">
-        <v>20.460381599681469</v>
-      </c>
-      <c r="CK105" s="26"/>
+        <v>19.706148468744217</v>
+      </c>
+      <c r="CK105" s="26">
+        <v>8.0726393139359374</v>
+      </c>
       <c r="CL105" s="26"/>
       <c r="CM105" s="26"/>
       <c r="CN105" s="26"/>
-      <c r="CO105" s="11"/>
+      <c r="CO105" s="26"/>
       <c r="CP105" s="11"/>
       <c r="CQ105" s="11"/>
       <c r="CR105" s="11"/>
@@ -19804,13 +19916,15 @@
         <v>9.6359318992384146</v>
       </c>
       <c r="CJ106" s="26">
-        <v>7.287242330972262</v>
-      </c>
-      <c r="CK106" s="26"/>
+        <v>7.1919154907722316</v>
+      </c>
+      <c r="CK106" s="26">
+        <v>5.6669181238955701</v>
+      </c>
       <c r="CL106" s="26"/>
       <c r="CM106" s="26"/>
       <c r="CN106" s="26"/>
-      <c r="CO106" s="11"/>
+      <c r="CO106" s="26"/>
       <c r="CP106" s="11"/>
       <c r="CQ106" s="11"/>
       <c r="CR106" s="11"/>
@@ -20131,13 +20245,15 @@
         <v>37.920455885362259</v>
       </c>
       <c r="CJ107" s="26">
-        <v>45.96864110084681</v>
-      </c>
-      <c r="CK107" s="26"/>
+        <v>46.113867569014559</v>
+      </c>
+      <c r="CK107" s="26">
+        <v>15.233256365271814</v>
+      </c>
       <c r="CL107" s="26"/>
       <c r="CM107" s="26"/>
       <c r="CN107" s="26"/>
-      <c r="CO107" s="11"/>
+      <c r="CO107" s="26"/>
       <c r="CP107" s="11"/>
       <c r="CQ107" s="11"/>
       <c r="CR107" s="11"/>
@@ -20458,13 +20574,15 @@
         <v>7.5196302721927282</v>
       </c>
       <c r="CJ108" s="26">
-        <v>5.4235924203911594</v>
-      </c>
-      <c r="CK108" s="26"/>
+        <v>5.3710183150907227</v>
+      </c>
+      <c r="CK108" s="26">
+        <v>11.555394075331236</v>
+      </c>
       <c r="CL108" s="26"/>
       <c r="CM108" s="26"/>
       <c r="CN108" s="26"/>
-      <c r="CO108" s="11"/>
+      <c r="CO108" s="26"/>
       <c r="CP108" s="11"/>
       <c r="CQ108" s="11"/>
       <c r="CR108" s="11"/>
@@ -20785,13 +20903,15 @@
         <v>33.248358926450209</v>
       </c>
       <c r="CJ109" s="26">
-        <v>38.234942116316432</v>
-      </c>
-      <c r="CK109" s="26"/>
+        <v>39.224414477418264</v>
+      </c>
+      <c r="CK109" s="26">
+        <v>24.747548084250923</v>
+      </c>
       <c r="CL109" s="26"/>
       <c r="CM109" s="26"/>
       <c r="CN109" s="26"/>
-      <c r="CO109" s="11"/>
+      <c r="CO109" s="26"/>
       <c r="CP109" s="11"/>
       <c r="CQ109" s="11"/>
       <c r="CR109" s="11"/>
@@ -21112,13 +21232,15 @@
         <v>7.216347897602887</v>
       </c>
       <c r="CJ110" s="26">
-        <v>8.2502579963249332</v>
-      </c>
-      <c r="CK110" s="26"/>
+        <v>8.3631894715307169</v>
+      </c>
+      <c r="CK110" s="26">
+        <v>7.0835590822963894</v>
+      </c>
       <c r="CL110" s="26"/>
       <c r="CM110" s="26"/>
       <c r="CN110" s="26"/>
-      <c r="CO110" s="11"/>
+      <c r="CO110" s="26"/>
       <c r="CP110" s="11"/>
       <c r="CQ110" s="11"/>
       <c r="CR110" s="11"/>
@@ -21589,13 +21711,15 @@
         <v>8.5611007039442057</v>
       </c>
       <c r="CJ112" s="26">
-        <v>7.9990074983604842</v>
-      </c>
-      <c r="CK112" s="26"/>
+        <v>8.0489928741148447</v>
+      </c>
+      <c r="CK112" s="26">
+        <v>7.0313151561457659</v>
+      </c>
       <c r="CL112" s="26"/>
       <c r="CM112" s="26"/>
       <c r="CN112" s="26"/>
-      <c r="CO112" s="11"/>
+      <c r="CO112" s="26"/>
       <c r="CP112" s="11"/>
       <c r="CQ112" s="11"/>
       <c r="CR112" s="11"/>
@@ -21746,6 +21870,7 @@
       <c r="CL113" s="16"/>
       <c r="CM113" s="16"/>
       <c r="CN113" s="16"/>
+      <c r="CO113" s="16"/>
     </row>
     <row r="114" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
@@ -22059,7 +22184,7 @@
     </row>
     <row r="118" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="120" spans="1:153" x14ac:dyDescent="0.2">
@@ -22069,7 +22194,7 @@
     </row>
     <row r="121" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="122" spans="1:153" x14ac:dyDescent="0.2">
@@ -22079,143 +22204,144 @@
     </row>
     <row r="124" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
-      <c r="B124" s="33">
+      <c r="B124" s="31">
         <v>2000</v>
       </c>
-      <c r="C124" s="33"/>
-      <c r="D124" s="33"/>
-      <c r="E124" s="33"/>
-      <c r="F124" s="33">
+      <c r="C124" s="31"/>
+      <c r="D124" s="31"/>
+      <c r="E124" s="31"/>
+      <c r="F124" s="31">
         <v>2001</v>
       </c>
-      <c r="G124" s="33"/>
-      <c r="H124" s="33"/>
-      <c r="I124" s="33"/>
-      <c r="J124" s="33">
+      <c r="G124" s="31"/>
+      <c r="H124" s="31"/>
+      <c r="I124" s="31"/>
+      <c r="J124" s="31">
         <v>2002</v>
       </c>
-      <c r="K124" s="33"/>
-      <c r="L124" s="33"/>
-      <c r="M124" s="33"/>
-      <c r="N124" s="33">
+      <c r="K124" s="31"/>
+      <c r="L124" s="31"/>
+      <c r="M124" s="31"/>
+      <c r="N124" s="31">
         <v>2003</v>
       </c>
-      <c r="O124" s="33"/>
-      <c r="P124" s="33"/>
-      <c r="Q124" s="33"/>
-      <c r="R124" s="33">
+      <c r="O124" s="31"/>
+      <c r="P124" s="31"/>
+      <c r="Q124" s="31"/>
+      <c r="R124" s="31">
         <v>2004</v>
       </c>
-      <c r="S124" s="33"/>
-      <c r="T124" s="33"/>
-      <c r="U124" s="33"/>
-      <c r="V124" s="33">
+      <c r="S124" s="31"/>
+      <c r="T124" s="31"/>
+      <c r="U124" s="31"/>
+      <c r="V124" s="31">
         <v>2005</v>
       </c>
-      <c r="W124" s="33"/>
-      <c r="X124" s="33"/>
-      <c r="Y124" s="33"/>
-      <c r="Z124" s="33">
+      <c r="W124" s="31"/>
+      <c r="X124" s="31"/>
+      <c r="Y124" s="31"/>
+      <c r="Z124" s="31">
         <v>2006</v>
       </c>
-      <c r="AA124" s="33"/>
-      <c r="AB124" s="33"/>
-      <c r="AC124" s="33"/>
-      <c r="AD124" s="33">
+      <c r="AA124" s="31"/>
+      <c r="AB124" s="31"/>
+      <c r="AC124" s="31"/>
+      <c r="AD124" s="31">
         <v>2007</v>
       </c>
-      <c r="AE124" s="33"/>
-      <c r="AF124" s="33"/>
-      <c r="AG124" s="33"/>
-      <c r="AH124" s="33">
+      <c r="AE124" s="31"/>
+      <c r="AF124" s="31"/>
+      <c r="AG124" s="31"/>
+      <c r="AH124" s="31">
         <v>2008</v>
       </c>
-      <c r="AI124" s="33"/>
-      <c r="AJ124" s="33"/>
-      <c r="AK124" s="33"/>
-      <c r="AL124" s="33">
+      <c r="AI124" s="31"/>
+      <c r="AJ124" s="31"/>
+      <c r="AK124" s="31"/>
+      <c r="AL124" s="31">
         <v>2009</v>
       </c>
-      <c r="AM124" s="33"/>
-      <c r="AN124" s="33"/>
-      <c r="AO124" s="33"/>
-      <c r="AP124" s="33">
+      <c r="AM124" s="31"/>
+      <c r="AN124" s="31"/>
+      <c r="AO124" s="31"/>
+      <c r="AP124" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ124" s="33"/>
-      <c r="AR124" s="33"/>
-      <c r="AS124" s="33"/>
-      <c r="AT124" s="33">
+      <c r="AQ124" s="31"/>
+      <c r="AR124" s="31"/>
+      <c r="AS124" s="31"/>
+      <c r="AT124" s="31">
         <v>2011</v>
       </c>
-      <c r="AU124" s="33"/>
-      <c r="AV124" s="33"/>
-      <c r="AW124" s="33"/>
-      <c r="AX124" s="33">
+      <c r="AU124" s="31"/>
+      <c r="AV124" s="31"/>
+      <c r="AW124" s="31"/>
+      <c r="AX124" s="31">
         <v>2012</v>
       </c>
-      <c r="AY124" s="33"/>
-      <c r="AZ124" s="33"/>
-      <c r="BA124" s="33"/>
-      <c r="BB124" s="33">
+      <c r="AY124" s="31"/>
+      <c r="AZ124" s="31"/>
+      <c r="BA124" s="31"/>
+      <c r="BB124" s="31">
         <v>2013</v>
       </c>
-      <c r="BC124" s="33"/>
-      <c r="BD124" s="33"/>
-      <c r="BE124" s="33"/>
-      <c r="BF124" s="33">
+      <c r="BC124" s="31"/>
+      <c r="BD124" s="31"/>
+      <c r="BE124" s="31"/>
+      <c r="BF124" s="31">
         <v>2014</v>
       </c>
-      <c r="BG124" s="33"/>
-      <c r="BH124" s="33"/>
-      <c r="BI124" s="33"/>
-      <c r="BJ124" s="33">
+      <c r="BG124" s="31"/>
+      <c r="BH124" s="31"/>
+      <c r="BI124" s="31"/>
+      <c r="BJ124" s="31">
         <v>2015</v>
       </c>
-      <c r="BK124" s="33"/>
-      <c r="BL124" s="33"/>
-      <c r="BM124" s="33"/>
-      <c r="BN124" s="33">
+      <c r="BK124" s="31"/>
+      <c r="BL124" s="31"/>
+      <c r="BM124" s="31"/>
+      <c r="BN124" s="31">
         <v>2016</v>
       </c>
-      <c r="BO124" s="33"/>
-      <c r="BP124" s="33"/>
-      <c r="BQ124" s="33"/>
-      <c r="BR124" s="34">
+      <c r="BO124" s="31"/>
+      <c r="BP124" s="31"/>
+      <c r="BQ124" s="31"/>
+      <c r="BR124" s="30">
         <v>2017</v>
       </c>
-      <c r="BS124" s="34"/>
-      <c r="BT124" s="34"/>
-      <c r="BU124" s="34"/>
-      <c r="BV124" s="34">
+      <c r="BS124" s="30"/>
+      <c r="BT124" s="30"/>
+      <c r="BU124" s="30"/>
+      <c r="BV124" s="30">
         <v>2018</v>
       </c>
-      <c r="BW124" s="34"/>
-      <c r="BX124" s="34"/>
-      <c r="BY124" s="34"/>
-      <c r="BZ124" s="34">
+      <c r="BW124" s="30"/>
+      <c r="BX124" s="30"/>
+      <c r="BY124" s="30"/>
+      <c r="BZ124" s="30">
         <v>2019</v>
       </c>
-      <c r="CA124" s="34"/>
-      <c r="CB124" s="34"/>
-      <c r="CC124" s="34"/>
-      <c r="CD124" s="34">
+      <c r="CA124" s="30"/>
+      <c r="CB124" s="30"/>
+      <c r="CC124" s="30"/>
+      <c r="CD124" s="30">
         <v>2020</v>
       </c>
-      <c r="CE124" s="34"/>
-      <c r="CF124" s="34"/>
-      <c r="CG124" s="34"/>
-      <c r="CH124" s="34">
+      <c r="CE124" s="30"/>
+      <c r="CF124" s="30"/>
+      <c r="CG124" s="30"/>
+      <c r="CH124" s="30">
         <v>2021</v>
       </c>
-      <c r="CI124" s="34"/>
-      <c r="CJ124" s="34"/>
-      <c r="CK124" s="34"/>
-      <c r="CL124" s="34">
+      <c r="CI124" s="30"/>
+      <c r="CJ124" s="30"/>
+      <c r="CK124" s="30"/>
+      <c r="CL124" s="30">
         <v>2022</v>
       </c>
-      <c r="CM124" s="34"/>
-      <c r="CN124" s="34"/>
+      <c r="CM124" s="30"/>
+      <c r="CN124" s="30"/>
+      <c r="CO124" s="30"/>
     </row>
     <row r="125" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
@@ -22493,6 +22619,9 @@
       </c>
       <c r="CN125" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="CO125" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="126" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -22775,7 +22904,9 @@
       <c r="CN127" s="26">
         <v>118.27301589983847</v>
       </c>
-      <c r="CO127" s="11"/>
+      <c r="CO127" s="26">
+        <v>119.63502738941952</v>
+      </c>
       <c r="CP127" s="11"/>
       <c r="CQ127" s="11"/>
       <c r="CR127" s="11"/>
@@ -23114,7 +23245,9 @@
       <c r="CN128" s="26">
         <v>167.67663158279336</v>
       </c>
-      <c r="CO128" s="11"/>
+      <c r="CO128" s="26">
+        <v>157.85711271445632</v>
+      </c>
       <c r="CP128" s="11"/>
       <c r="CQ128" s="11"/>
       <c r="CR128" s="11"/>
@@ -23453,7 +23586,9 @@
       <c r="CN129" s="26">
         <v>106.69388624713258</v>
       </c>
-      <c r="CO129" s="11"/>
+      <c r="CO129" s="26">
+        <v>107.88943773035248</v>
+      </c>
       <c r="CP129" s="11"/>
       <c r="CQ129" s="11"/>
       <c r="CR129" s="11"/>
@@ -23792,7 +23927,9 @@
       <c r="CN130" s="26">
         <v>118.84927854323799</v>
       </c>
-      <c r="CO130" s="11"/>
+      <c r="CO130" s="26">
+        <v>117.1180284754346</v>
+      </c>
       <c r="CP130" s="11"/>
       <c r="CQ130" s="11"/>
       <c r="CR130" s="11"/>
@@ -24131,7 +24268,9 @@
       <c r="CN131" s="26">
         <v>114.65261671281807</v>
       </c>
-      <c r="CO131" s="11"/>
+      <c r="CO131" s="26">
+        <v>111.84049601763029</v>
+      </c>
       <c r="CP131" s="11"/>
       <c r="CQ131" s="11"/>
       <c r="CR131" s="11"/>
@@ -24470,7 +24609,9 @@
       <c r="CN132" s="26">
         <v>114.45087022532654</v>
       </c>
-      <c r="CO132" s="11"/>
+      <c r="CO132" s="26">
+        <v>114.33049868938599</v>
+      </c>
       <c r="CP132" s="11"/>
       <c r="CQ132" s="11"/>
       <c r="CR132" s="11"/>
@@ -24809,7 +24950,9 @@
       <c r="CN133" s="26">
         <v>142.03571732517136</v>
       </c>
-      <c r="CO133" s="11"/>
+      <c r="CO133" s="26">
+        <v>126.45166811592503</v>
+      </c>
       <c r="CP133" s="11"/>
       <c r="CQ133" s="11"/>
       <c r="CR133" s="11"/>
@@ -25148,7 +25291,9 @@
       <c r="CN134" s="26">
         <v>100.24273019895509</v>
       </c>
-      <c r="CO134" s="11"/>
+      <c r="CO134" s="26">
+        <v>97.770891822858133</v>
+      </c>
       <c r="CP134" s="11"/>
       <c r="CQ134" s="11"/>
       <c r="CR134" s="11"/>
@@ -25487,7 +25632,9 @@
       <c r="CN135" s="26">
         <v>103.66360122129279</v>
       </c>
-      <c r="CO135" s="11"/>
+      <c r="CO135" s="26">
+        <v>107.41817077769586</v>
+      </c>
       <c r="CP135" s="11"/>
       <c r="CQ135" s="11"/>
       <c r="CR135" s="11"/>
@@ -25826,7 +25973,9 @@
       <c r="CN136" s="26">
         <v>108.76667919721386</v>
       </c>
-      <c r="CO136" s="11"/>
+      <c r="CO136" s="26">
+        <v>102.55628118766403</v>
+      </c>
       <c r="CP136" s="11"/>
       <c r="CQ136" s="11"/>
       <c r="CR136" s="11"/>
@@ -26165,7 +26314,9 @@
       <c r="CN137" s="26">
         <v>118.69712079921501</v>
       </c>
-      <c r="CO137" s="11"/>
+      <c r="CO137" s="26">
+        <v>116.21057920620589</v>
+      </c>
       <c r="CP137" s="11"/>
       <c r="CQ137" s="11"/>
       <c r="CR137" s="11"/>
@@ -26504,7 +26655,9 @@
       <c r="CN138" s="26">
         <v>107.10733958406853</v>
       </c>
-      <c r="CO138" s="11"/>
+      <c r="CO138" s="26">
+        <v>106.99932889233112</v>
+      </c>
       <c r="CP138" s="11"/>
       <c r="CQ138" s="11"/>
       <c r="CR138" s="11"/>
@@ -26995,9 +27148,11 @@
         <v>114.10299600886442</v>
       </c>
       <c r="CN140" s="26">
-        <v>117.80938743309251</v>
-      </c>
-      <c r="CO140" s="11"/>
+        <v>117.7894222953032</v>
+      </c>
+      <c r="CO140" s="26">
+        <v>115.83583705206568</v>
+      </c>
       <c r="CP140" s="11"/>
       <c r="CQ140" s="11"/>
       <c r="CR140" s="11"/>
@@ -27152,6 +27307,7 @@
       <c r="CL141" s="16"/>
       <c r="CM141" s="16"/>
       <c r="CN141" s="16"/>
+      <c r="CO141" s="16"/>
     </row>
     <row r="142" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
@@ -27170,7 +27326,7 @@
     </row>
     <row r="147" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="149" spans="1:153" x14ac:dyDescent="0.2">
@@ -27180,7 +27336,7 @@
     </row>
     <row r="150" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="151" spans="1:153" x14ac:dyDescent="0.2">
@@ -27190,143 +27346,144 @@
     </row>
     <row r="153" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
-      <c r="B153" s="33">
+      <c r="B153" s="31">
         <v>2000</v>
       </c>
-      <c r="C153" s="33"/>
-      <c r="D153" s="33"/>
-      <c r="E153" s="33"/>
-      <c r="F153" s="33">
+      <c r="C153" s="31"/>
+      <c r="D153" s="31"/>
+      <c r="E153" s="31"/>
+      <c r="F153" s="31">
         <v>2001</v>
       </c>
-      <c r="G153" s="33"/>
-      <c r="H153" s="33"/>
-      <c r="I153" s="33"/>
-      <c r="J153" s="33">
+      <c r="G153" s="31"/>
+      <c r="H153" s="31"/>
+      <c r="I153" s="31"/>
+      <c r="J153" s="31">
         <v>2002</v>
       </c>
-      <c r="K153" s="33"/>
-      <c r="L153" s="33"/>
-      <c r="M153" s="33"/>
-      <c r="N153" s="33">
+      <c r="K153" s="31"/>
+      <c r="L153" s="31"/>
+      <c r="M153" s="31"/>
+      <c r="N153" s="31">
         <v>2003</v>
       </c>
-      <c r="O153" s="33"/>
-      <c r="P153" s="33"/>
-      <c r="Q153" s="33"/>
-      <c r="R153" s="33">
+      <c r="O153" s="31"/>
+      <c r="P153" s="31"/>
+      <c r="Q153" s="31"/>
+      <c r="R153" s="31">
         <v>2004</v>
       </c>
-      <c r="S153" s="33"/>
-      <c r="T153" s="33"/>
-      <c r="U153" s="33"/>
-      <c r="V153" s="33">
+      <c r="S153" s="31"/>
+      <c r="T153" s="31"/>
+      <c r="U153" s="31"/>
+      <c r="V153" s="31">
         <v>2005</v>
       </c>
-      <c r="W153" s="33"/>
-      <c r="X153" s="33"/>
-      <c r="Y153" s="33"/>
-      <c r="Z153" s="33">
+      <c r="W153" s="31"/>
+      <c r="X153" s="31"/>
+      <c r="Y153" s="31"/>
+      <c r="Z153" s="31">
         <v>2006</v>
       </c>
-      <c r="AA153" s="33"/>
-      <c r="AB153" s="33"/>
-      <c r="AC153" s="33"/>
-      <c r="AD153" s="33">
+      <c r="AA153" s="31"/>
+      <c r="AB153" s="31"/>
+      <c r="AC153" s="31"/>
+      <c r="AD153" s="31">
         <v>2007</v>
       </c>
-      <c r="AE153" s="33"/>
-      <c r="AF153" s="33"/>
-      <c r="AG153" s="33"/>
-      <c r="AH153" s="33">
+      <c r="AE153" s="31"/>
+      <c r="AF153" s="31"/>
+      <c r="AG153" s="31"/>
+      <c r="AH153" s="31">
         <v>2008</v>
       </c>
-      <c r="AI153" s="33"/>
-      <c r="AJ153" s="33"/>
-      <c r="AK153" s="33"/>
-      <c r="AL153" s="33">
+      <c r="AI153" s="31"/>
+      <c r="AJ153" s="31"/>
+      <c r="AK153" s="31"/>
+      <c r="AL153" s="31">
         <v>2009</v>
       </c>
-      <c r="AM153" s="33"/>
-      <c r="AN153" s="33"/>
-      <c r="AO153" s="33"/>
-      <c r="AP153" s="33">
+      <c r="AM153" s="31"/>
+      <c r="AN153" s="31"/>
+      <c r="AO153" s="31"/>
+      <c r="AP153" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ153" s="33"/>
-      <c r="AR153" s="33"/>
-      <c r="AS153" s="33"/>
-      <c r="AT153" s="33">
+      <c r="AQ153" s="31"/>
+      <c r="AR153" s="31"/>
+      <c r="AS153" s="31"/>
+      <c r="AT153" s="31">
         <v>2011</v>
       </c>
-      <c r="AU153" s="33"/>
-      <c r="AV153" s="33"/>
-      <c r="AW153" s="33"/>
-      <c r="AX153" s="33">
+      <c r="AU153" s="31"/>
+      <c r="AV153" s="31"/>
+      <c r="AW153" s="31"/>
+      <c r="AX153" s="31">
         <v>2012</v>
       </c>
-      <c r="AY153" s="33"/>
-      <c r="AZ153" s="33"/>
-      <c r="BA153" s="33"/>
-      <c r="BB153" s="33">
+      <c r="AY153" s="31"/>
+      <c r="AZ153" s="31"/>
+      <c r="BA153" s="31"/>
+      <c r="BB153" s="31">
         <v>2013</v>
       </c>
-      <c r="BC153" s="33"/>
-      <c r="BD153" s="33"/>
-      <c r="BE153" s="33"/>
-      <c r="BF153" s="33">
+      <c r="BC153" s="31"/>
+      <c r="BD153" s="31"/>
+      <c r="BE153" s="31"/>
+      <c r="BF153" s="31">
         <v>2014</v>
       </c>
-      <c r="BG153" s="33"/>
-      <c r="BH153" s="33"/>
-      <c r="BI153" s="33"/>
-      <c r="BJ153" s="33">
+      <c r="BG153" s="31"/>
+      <c r="BH153" s="31"/>
+      <c r="BI153" s="31"/>
+      <c r="BJ153" s="31">
         <v>2015</v>
       </c>
-      <c r="BK153" s="33"/>
-      <c r="BL153" s="33"/>
-      <c r="BM153" s="33"/>
-      <c r="BN153" s="33">
+      <c r="BK153" s="31"/>
+      <c r="BL153" s="31"/>
+      <c r="BM153" s="31"/>
+      <c r="BN153" s="31">
         <v>2016</v>
       </c>
-      <c r="BO153" s="33"/>
-      <c r="BP153" s="33"/>
-      <c r="BQ153" s="33"/>
-      <c r="BR153" s="34">
+      <c r="BO153" s="31"/>
+      <c r="BP153" s="31"/>
+      <c r="BQ153" s="31"/>
+      <c r="BR153" s="30">
         <v>2017</v>
       </c>
-      <c r="BS153" s="34"/>
-      <c r="BT153" s="34"/>
-      <c r="BU153" s="34"/>
-      <c r="BV153" s="34">
+      <c r="BS153" s="30"/>
+      <c r="BT153" s="30"/>
+      <c r="BU153" s="30"/>
+      <c r="BV153" s="30">
         <v>2018</v>
       </c>
-      <c r="BW153" s="34"/>
-      <c r="BX153" s="34"/>
-      <c r="BY153" s="34"/>
-      <c r="BZ153" s="34">
+      <c r="BW153" s="30"/>
+      <c r="BX153" s="30"/>
+      <c r="BY153" s="30"/>
+      <c r="BZ153" s="30">
         <v>2019</v>
       </c>
-      <c r="CA153" s="34"/>
-      <c r="CB153" s="34"/>
-      <c r="CC153" s="34"/>
-      <c r="CD153" s="34">
+      <c r="CA153" s="30"/>
+      <c r="CB153" s="30"/>
+      <c r="CC153" s="30"/>
+      <c r="CD153" s="30">
         <v>2020</v>
       </c>
-      <c r="CE153" s="34"/>
-      <c r="CF153" s="34"/>
-      <c r="CG153" s="34"/>
-      <c r="CH153" s="34">
+      <c r="CE153" s="30"/>
+      <c r="CF153" s="30"/>
+      <c r="CG153" s="30"/>
+      <c r="CH153" s="30">
         <v>2021</v>
       </c>
-      <c r="CI153" s="34"/>
-      <c r="CJ153" s="34"/>
-      <c r="CK153" s="34"/>
-      <c r="CL153" s="34">
+      <c r="CI153" s="30"/>
+      <c r="CJ153" s="30"/>
+      <c r="CK153" s="30"/>
+      <c r="CL153" s="30">
         <v>2022</v>
       </c>
-      <c r="CM153" s="34"/>
-      <c r="CN153" s="34"/>
+      <c r="CM153" s="30"/>
+      <c r="CN153" s="30"/>
+      <c r="CO153" s="30"/>
     </row>
     <row r="154" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
@@ -27604,6 +27761,9 @@
       </c>
       <c r="CN154" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="CO154" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="155" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -27884,9 +28044,11 @@
         <v>40.386598492293864</v>
       </c>
       <c r="CN156" s="26">
-        <v>35.058276190798679</v>
-      </c>
-      <c r="CO156" s="11"/>
+        <v>35.151239735263502</v>
+      </c>
+      <c r="CO156" s="26">
+        <v>39.714410745271564</v>
+      </c>
       <c r="CP156" s="11"/>
       <c r="CQ156" s="11"/>
       <c r="CR156" s="11"/>
@@ -28223,9 +28385,11 @@
         <v>1.9301613408157867</v>
       </c>
       <c r="CN157" s="26">
-        <v>1.811642637410487</v>
-      </c>
-      <c r="CO157" s="11"/>
+        <v>1.7988591773401337</v>
+      </c>
+      <c r="CO157" s="26">
+        <v>2.2434627359199242</v>
+      </c>
       <c r="CP157" s="11"/>
       <c r="CQ157" s="11"/>
       <c r="CR157" s="11"/>
@@ -28562,9 +28726,11 @@
         <v>1.6737259758123908</v>
       </c>
       <c r="CN158" s="26">
-        <v>1.6456764094052518</v>
-      </c>
-      <c r="CO158" s="11"/>
+        <v>1.684186846409736</v>
+      </c>
+      <c r="CO158" s="26">
+        <v>1.7774387289402775</v>
+      </c>
       <c r="CP158" s="11"/>
       <c r="CQ158" s="11"/>
       <c r="CR158" s="11"/>
@@ -28901,9 +29067,11 @@
         <v>14.820477775699233</v>
       </c>
       <c r="CN159" s="26">
-        <v>12.672022805474306</v>
-      </c>
-      <c r="CO159" s="11"/>
+        <v>12.67802711598868</v>
+      </c>
+      <c r="CO159" s="26">
+        <v>11.125892844071194</v>
+      </c>
       <c r="CP159" s="11"/>
       <c r="CQ159" s="11"/>
       <c r="CR159" s="11"/>
@@ -29240,9 +29408,11 @@
         <v>2.658125012734792</v>
       </c>
       <c r="CN160" s="26">
-        <v>3.0090483472403351</v>
-      </c>
-      <c r="CO160" s="11"/>
+        <v>2.9882198149321342</v>
+      </c>
+      <c r="CO160" s="26">
+        <v>2.7091160707695972</v>
+      </c>
       <c r="CP160" s="11"/>
       <c r="CQ160" s="11"/>
       <c r="CR160" s="11"/>
@@ -29579,9 +29749,11 @@
         <v>3.5635325484111213</v>
       </c>
       <c r="CN161" s="26">
-        <v>5.387816191163207</v>
-      </c>
-      <c r="CO161" s="11"/>
+        <v>5.3061834890078057</v>
+      </c>
+      <c r="CO161" s="26">
+        <v>4.0111042950942055</v>
+      </c>
       <c r="CP161" s="11"/>
       <c r="CQ161" s="11"/>
       <c r="CR161" s="11"/>
@@ -29918,9 +30090,11 @@
         <v>7.6311450485028924</v>
       </c>
       <c r="CN162" s="26">
-        <v>11.27571442030456</v>
-      </c>
-      <c r="CO162" s="11"/>
+        <v>11.201828988370851</v>
+      </c>
+      <c r="CO162" s="26">
+        <v>7.7402658348392563</v>
+      </c>
       <c r="CP162" s="11"/>
       <c r="CQ162" s="11"/>
       <c r="CR162" s="11"/>
@@ -30257,9 +30431,11 @@
         <v>3.281450462649302</v>
       </c>
       <c r="CN163" s="26">
-        <v>2.3484407842842439</v>
-      </c>
-      <c r="CO163" s="11"/>
+        <v>2.3456662028536286</v>
+      </c>
+      <c r="CO163" s="26">
+        <v>2.6026154716848313</v>
+      </c>
       <c r="CP163" s="11"/>
       <c r="CQ163" s="11"/>
       <c r="CR163" s="11"/>
@@ -30596,9 +30772,11 @@
         <v>1.0824917908333125</v>
       </c>
       <c r="CN164" s="26">
-        <v>1.287643483784602</v>
-      </c>
-      <c r="CO164" s="11"/>
+        <v>1.2885466707662028</v>
+      </c>
+      <c r="CO164" s="26">
+        <v>1.7360859678673215</v>
+      </c>
       <c r="CP164" s="11"/>
       <c r="CQ164" s="11"/>
       <c r="CR164" s="11"/>
@@ -30935,9 +31113,11 @@
         <v>4.8256065402639523</v>
       </c>
       <c r="CN165" s="26">
-        <v>5.3168377883684093</v>
-      </c>
-      <c r="CO165" s="11"/>
+        <v>5.3126282072839901</v>
+      </c>
+      <c r="CO165" s="26">
+        <v>4.5805596084770768</v>
+      </c>
       <c r="CP165" s="11"/>
       <c r="CQ165" s="11"/>
       <c r="CR165" s="11"/>
@@ -31274,9 +31454,11 @@
         <v>4.7014993247610217</v>
       </c>
       <c r="CN166" s="26">
-        <v>6.9685605436369258</v>
-      </c>
-      <c r="CO166" s="11"/>
+        <v>7.0163830371873086</v>
+      </c>
+      <c r="CO166" s="26">
+        <v>7.6623676634329962</v>
+      </c>
       <c r="CP166" s="11"/>
       <c r="CQ166" s="11"/>
       <c r="CR166" s="11"/>
@@ -31613,9 +31795,11 @@
         <v>13.445185687222347</v>
       </c>
       <c r="CN167" s="26">
-        <v>13.218320398128993</v>
-      </c>
-      <c r="CO167" s="11"/>
+        <v>13.228230714596013</v>
+      </c>
+      <c r="CO167" s="26">
+        <v>14.096680033631747</v>
+      </c>
       <c r="CP167" s="11"/>
       <c r="CQ167" s="11"/>
       <c r="CR167" s="11"/>
@@ -32108,7 +32292,9 @@
       <c r="CN169" s="26">
         <v>100</v>
       </c>
-      <c r="CO169" s="11"/>
+      <c r="CO169" s="26">
+        <v>100</v>
+      </c>
       <c r="CP169" s="11"/>
       <c r="CQ169" s="11"/>
       <c r="CR169" s="11"/>
@@ -32263,6 +32449,7 @@
       <c r="CL170" s="16"/>
       <c r="CM170" s="16"/>
       <c r="CN170" s="16"/>
+      <c r="CO170" s="16"/>
     </row>
     <row r="171" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
@@ -32589,7 +32776,7 @@
     </row>
     <row r="176" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="178" spans="1:153" x14ac:dyDescent="0.2">
@@ -32599,7 +32786,7 @@
     </row>
     <row r="179" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="180" spans="1:153" x14ac:dyDescent="0.2">
@@ -32609,143 +32796,144 @@
     </row>
     <row r="182" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A182" s="4"/>
-      <c r="B182" s="33">
+      <c r="B182" s="31">
         <v>2000</v>
       </c>
-      <c r="C182" s="33"/>
-      <c r="D182" s="33"/>
-      <c r="E182" s="33"/>
-      <c r="F182" s="33">
+      <c r="C182" s="31"/>
+      <c r="D182" s="31"/>
+      <c r="E182" s="31"/>
+      <c r="F182" s="31">
         <v>2001</v>
       </c>
-      <c r="G182" s="33"/>
-      <c r="H182" s="33"/>
-      <c r="I182" s="33"/>
-      <c r="J182" s="33">
+      <c r="G182" s="31"/>
+      <c r="H182" s="31"/>
+      <c r="I182" s="31"/>
+      <c r="J182" s="31">
         <v>2002</v>
       </c>
-      <c r="K182" s="33"/>
-      <c r="L182" s="33"/>
-      <c r="M182" s="33"/>
-      <c r="N182" s="33">
+      <c r="K182" s="31"/>
+      <c r="L182" s="31"/>
+      <c r="M182" s="31"/>
+      <c r="N182" s="31">
         <v>2003</v>
       </c>
-      <c r="O182" s="33"/>
-      <c r="P182" s="33"/>
-      <c r="Q182" s="33"/>
-      <c r="R182" s="33">
+      <c r="O182" s="31"/>
+      <c r="P182" s="31"/>
+      <c r="Q182" s="31"/>
+      <c r="R182" s="31">
         <v>2004</v>
       </c>
-      <c r="S182" s="33"/>
-      <c r="T182" s="33"/>
-      <c r="U182" s="33"/>
-      <c r="V182" s="33">
+      <c r="S182" s="31"/>
+      <c r="T182" s="31"/>
+      <c r="U182" s="31"/>
+      <c r="V182" s="31">
         <v>2005</v>
       </c>
-      <c r="W182" s="33"/>
-      <c r="X182" s="33"/>
-      <c r="Y182" s="33"/>
-      <c r="Z182" s="33">
+      <c r="W182" s="31"/>
+      <c r="X182" s="31"/>
+      <c r="Y182" s="31"/>
+      <c r="Z182" s="31">
         <v>2006</v>
       </c>
-      <c r="AA182" s="33"/>
-      <c r="AB182" s="33"/>
-      <c r="AC182" s="33"/>
-      <c r="AD182" s="33">
+      <c r="AA182" s="31"/>
+      <c r="AB182" s="31"/>
+      <c r="AC182" s="31"/>
+      <c r="AD182" s="31">
         <v>2007</v>
       </c>
-      <c r="AE182" s="33"/>
-      <c r="AF182" s="33"/>
-      <c r="AG182" s="33"/>
-      <c r="AH182" s="33">
+      <c r="AE182" s="31"/>
+      <c r="AF182" s="31"/>
+      <c r="AG182" s="31"/>
+      <c r="AH182" s="31">
         <v>2008</v>
       </c>
-      <c r="AI182" s="33"/>
-      <c r="AJ182" s="33"/>
-      <c r="AK182" s="33"/>
-      <c r="AL182" s="33">
+      <c r="AI182" s="31"/>
+      <c r="AJ182" s="31"/>
+      <c r="AK182" s="31"/>
+      <c r="AL182" s="31">
         <v>2009</v>
       </c>
-      <c r="AM182" s="33"/>
-      <c r="AN182" s="33"/>
-      <c r="AO182" s="33"/>
-      <c r="AP182" s="33">
+      <c r="AM182" s="31"/>
+      <c r="AN182" s="31"/>
+      <c r="AO182" s="31"/>
+      <c r="AP182" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ182" s="33"/>
-      <c r="AR182" s="33"/>
-      <c r="AS182" s="33"/>
-      <c r="AT182" s="33">
+      <c r="AQ182" s="31"/>
+      <c r="AR182" s="31"/>
+      <c r="AS182" s="31"/>
+      <c r="AT182" s="31">
         <v>2011</v>
       </c>
-      <c r="AU182" s="33"/>
-      <c r="AV182" s="33"/>
-      <c r="AW182" s="33"/>
-      <c r="AX182" s="33">
+      <c r="AU182" s="31"/>
+      <c r="AV182" s="31"/>
+      <c r="AW182" s="31"/>
+      <c r="AX182" s="31">
         <v>2012</v>
       </c>
-      <c r="AY182" s="33"/>
-      <c r="AZ182" s="33"/>
-      <c r="BA182" s="33"/>
-      <c r="BB182" s="33">
+      <c r="AY182" s="31"/>
+      <c r="AZ182" s="31"/>
+      <c r="BA182" s="31"/>
+      <c r="BB182" s="31">
         <v>2013</v>
       </c>
-      <c r="BC182" s="33"/>
-      <c r="BD182" s="33"/>
-      <c r="BE182" s="33"/>
-      <c r="BF182" s="33">
+      <c r="BC182" s="31"/>
+      <c r="BD182" s="31"/>
+      <c r="BE182" s="31"/>
+      <c r="BF182" s="31">
         <v>2014</v>
       </c>
-      <c r="BG182" s="33"/>
-      <c r="BH182" s="33"/>
-      <c r="BI182" s="33"/>
-      <c r="BJ182" s="33">
+      <c r="BG182" s="31"/>
+      <c r="BH182" s="31"/>
+      <c r="BI182" s="31"/>
+      <c r="BJ182" s="31">
         <v>2015</v>
       </c>
-      <c r="BK182" s="33"/>
-      <c r="BL182" s="33"/>
-      <c r="BM182" s="33"/>
-      <c r="BN182" s="33">
+      <c r="BK182" s="31"/>
+      <c r="BL182" s="31"/>
+      <c r="BM182" s="31"/>
+      <c r="BN182" s="31">
         <v>2016</v>
       </c>
-      <c r="BO182" s="33"/>
-      <c r="BP182" s="33"/>
-      <c r="BQ182" s="33"/>
-      <c r="BR182" s="34">
+      <c r="BO182" s="31"/>
+      <c r="BP182" s="31"/>
+      <c r="BQ182" s="31"/>
+      <c r="BR182" s="30">
         <v>2017</v>
       </c>
-      <c r="BS182" s="34"/>
-      <c r="BT182" s="34"/>
-      <c r="BU182" s="34"/>
-      <c r="BV182" s="34">
+      <c r="BS182" s="30"/>
+      <c r="BT182" s="30"/>
+      <c r="BU182" s="30"/>
+      <c r="BV182" s="30">
         <v>2018</v>
       </c>
-      <c r="BW182" s="34"/>
-      <c r="BX182" s="34"/>
-      <c r="BY182" s="34"/>
-      <c r="BZ182" s="34">
+      <c r="BW182" s="30"/>
+      <c r="BX182" s="30"/>
+      <c r="BY182" s="30"/>
+      <c r="BZ182" s="30">
         <v>2019</v>
       </c>
-      <c r="CA182" s="34"/>
-      <c r="CB182" s="34"/>
-      <c r="CC182" s="34"/>
-      <c r="CD182" s="34">
+      <c r="CA182" s="30"/>
+      <c r="CB182" s="30"/>
+      <c r="CC182" s="30"/>
+      <c r="CD182" s="30">
         <v>2020</v>
       </c>
-      <c r="CE182" s="34"/>
-      <c r="CF182" s="34"/>
-      <c r="CG182" s="34"/>
-      <c r="CH182" s="34">
+      <c r="CE182" s="30"/>
+      <c r="CF182" s="30"/>
+      <c r="CG182" s="30"/>
+      <c r="CH182" s="30">
         <v>2021</v>
       </c>
-      <c r="CI182" s="34"/>
-      <c r="CJ182" s="34"/>
-      <c r="CK182" s="34"/>
-      <c r="CL182" s="34">
+      <c r="CI182" s="30"/>
+      <c r="CJ182" s="30"/>
+      <c r="CK182" s="30"/>
+      <c r="CL182" s="30">
         <v>2022</v>
       </c>
-      <c r="CM182" s="34"/>
-      <c r="CN182" s="34"/>
+      <c r="CM182" s="30"/>
+      <c r="CN182" s="30"/>
+      <c r="CO182" s="30"/>
     </row>
     <row r="183" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
@@ -33023,6 +33211,9 @@
       </c>
       <c r="CN183" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="CO183" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="184" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -33303,9 +33494,11 @@
         <v>39.992660534029831</v>
       </c>
       <c r="CN185" s="26">
-        <v>34.920848268517055</v>
-      </c>
-      <c r="CO185" s="11"/>
+        <v>35.00751367401336</v>
+      </c>
+      <c r="CO185" s="26">
+        <v>38.453219864560644</v>
+      </c>
       <c r="CP185" s="11"/>
       <c r="CQ185" s="11"/>
       <c r="CR185" s="11"/>
@@ -33642,9 +33835,11 @@
         <v>1.4174842092962083</v>
       </c>
       <c r="CN186" s="26">
-        <v>1.272857805803532</v>
-      </c>
-      <c r="CO186" s="11"/>
+        <v>1.263661974178411</v>
+      </c>
+      <c r="CO186" s="26">
+        <v>1.6462570450055052</v>
+      </c>
       <c r="CP186" s="11"/>
       <c r="CQ186" s="11"/>
       <c r="CR186" s="11"/>
@@ -33981,9 +34176,11 @@
         <v>1.6466306793185461</v>
       </c>
       <c r="CN187" s="26">
-        <v>1.8171250155426251</v>
-      </c>
-      <c r="CO187" s="11"/>
+        <v>1.8593323633975594</v>
+      </c>
+      <c r="CO187" s="26">
+        <v>1.9083527294871931</v>
+      </c>
       <c r="CP187" s="11"/>
       <c r="CQ187" s="11"/>
       <c r="CR187" s="11"/>
@@ -34320,9 +34517,11 @@
         <v>15.330506403073811</v>
       </c>
       <c r="CN188" s="26">
-        <v>12.561146879053098</v>
-      </c>
-      <c r="CO188" s="11"/>
+        <v>12.56496890970366</v>
+      </c>
+      <c r="CO188" s="26">
+        <v>11.004088160644663</v>
+      </c>
       <c r="CP188" s="11"/>
       <c r="CQ188" s="11"/>
       <c r="CR188" s="11"/>
@@ -34659,9 +34858,11 @@
         <v>2.7071103844788857</v>
       </c>
       <c r="CN189" s="26">
-        <v>3.0918975310688319</v>
-      </c>
-      <c r="CO189" s="11"/>
+        <v>3.0699751630952772</v>
+      </c>
+      <c r="CO189" s="26">
+        <v>2.8058953501004749</v>
+      </c>
       <c r="CP189" s="11"/>
       <c r="CQ189" s="11"/>
       <c r="CR189" s="11"/>
@@ -34998,9 +35199,11 @@
         <v>3.7248368764571036</v>
       </c>
       <c r="CN190" s="26">
-        <v>5.5459196057958513</v>
-      </c>
-      <c r="CO190" s="11"/>
+        <v>5.4609657972246541</v>
+      </c>
+      <c r="CO190" s="26">
+        <v>4.0639167050926872</v>
+      </c>
       <c r="CP190" s="11"/>
       <c r="CQ190" s="11"/>
       <c r="CR190" s="11"/>
@@ -35337,9 +35540,11 @@
         <v>6.9751383420200934</v>
       </c>
       <c r="CN191" s="26">
-        <v>9.3524715736494084</v>
-      </c>
-      <c r="CO191" s="11"/>
+        <v>9.2896138382591982</v>
+      </c>
+      <c r="CO191" s="26">
+        <v>7.0904574478380926</v>
+      </c>
       <c r="CP191" s="11"/>
       <c r="CQ191" s="11"/>
       <c r="CR191" s="11"/>
@@ -35676,9 +35881,11 @@
         <v>3.6681225344374964</v>
       </c>
       <c r="CN192" s="26">
-        <v>2.7599843866014542</v>
-      </c>
-      <c r="CO192" s="11"/>
+        <v>2.7562564026675571</v>
+      </c>
+      <c r="CO192" s="26">
+        <v>3.0834958755770114</v>
+      </c>
       <c r="CP192" s="11"/>
       <c r="CQ192" s="11"/>
       <c r="CR192" s="11"/>
@@ -36015,9 +36222,11 @@
         <v>1.1966526571129854</v>
       </c>
       <c r="CN193" s="26">
-        <v>1.4633534651477869</v>
-      </c>
-      <c r="CO193" s="11"/>
+        <v>1.4641317315041515</v>
+      </c>
+      <c r="CO193" s="26">
+        <v>1.872131780184932</v>
+      </c>
       <c r="CP193" s="11"/>
       <c r="CQ193" s="11"/>
       <c r="CR193" s="11"/>
@@ -36354,9 +36563,11 @@
         <v>5.1655768198596341</v>
       </c>
       <c r="CN194" s="26">
-        <v>5.7588721798986926</v>
-      </c>
-      <c r="CO194" s="11"/>
+        <v>5.7533374377558744</v>
+      </c>
+      <c r="CO194" s="26">
+        <v>5.1736758613927476</v>
+      </c>
       <c r="CP194" s="11"/>
       <c r="CQ194" s="11"/>
       <c r="CR194" s="11"/>
@@ -36693,9 +36904,11 @@
         <v>4.9446315415412032</v>
       </c>
       <c r="CN195" s="26">
-        <v>6.9164428202517421</v>
-      </c>
-      <c r="CO195" s="11"/>
+        <v>6.9627274780394144</v>
+      </c>
+      <c r="CO195" s="26">
+        <v>7.6376589649339186</v>
+      </c>
       <c r="CP195" s="11"/>
       <c r="CQ195" s="11"/>
       <c r="CR195" s="11"/>
@@ -37032,9 +37245,11 @@
         <v>13.230649018374201</v>
       </c>
       <c r="CN196" s="26">
-        <v>14.53908046866993</v>
-      </c>
-      <c r="CO196" s="11"/>
+        <v>14.547515230160881</v>
+      </c>
+      <c r="CO196" s="26">
+        <v>15.260850215182131</v>
+      </c>
       <c r="CP196" s="11"/>
       <c r="CQ196" s="11"/>
       <c r="CR196" s="11"/>
@@ -37527,7 +37742,9 @@
       <c r="CN198" s="26">
         <v>100</v>
       </c>
-      <c r="CO198" s="11"/>
+      <c r="CO198" s="26">
+        <v>100</v>
+      </c>
       <c r="CP198" s="11"/>
       <c r="CQ198" s="11"/>
       <c r="CR198" s="11"/>
@@ -37682,6 +37899,7 @@
       <c r="CL199" s="16"/>
       <c r="CM199" s="16"/>
       <c r="CN199" s="16"/>
+      <c r="CO199" s="16"/>
     </row>
     <row r="200" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
@@ -37781,7 +37999,7 @@
       <c r="CL201" s="1"/>
       <c r="CM201" s="1"/>
       <c r="CN201" s="1"/>
-      <c r="CO201" s="28"/>
+      <c r="CO201" s="1"/>
       <c r="CP201" s="28"/>
       <c r="CQ201" s="28"/>
       <c r="CR201" s="28"/>
@@ -37936,7 +38154,7 @@
       <c r="CL202" s="1"/>
       <c r="CM202" s="1"/>
       <c r="CN202" s="1"/>
-      <c r="CO202" s="28"/>
+      <c r="CO202" s="1"/>
       <c r="CP202" s="28"/>
       <c r="CQ202" s="28"/>
       <c r="CR202" s="28"/>
@@ -38000,62 +38218,88 @@
     </row>
   </sheetData>
   <mergeCells count="161">
-    <mergeCell ref="CH9:CK9"/>
-    <mergeCell ref="CH38:CK38"/>
-    <mergeCell ref="CL9:CN9"/>
-    <mergeCell ref="CL38:CN38"/>
-    <mergeCell ref="CH67:CJ67"/>
-    <mergeCell ref="CL67:CM67"/>
-    <mergeCell ref="CH96:CJ96"/>
-    <mergeCell ref="CL96:CM96"/>
-    <mergeCell ref="CL124:CN124"/>
-    <mergeCell ref="CL153:CN153"/>
-    <mergeCell ref="CL182:CN182"/>
-    <mergeCell ref="CH124:CK124"/>
-    <mergeCell ref="CH153:CK153"/>
-    <mergeCell ref="CH182:CK182"/>
-    <mergeCell ref="AH124:AK124"/>
-    <mergeCell ref="BR182:BU182"/>
-    <mergeCell ref="BV182:BY182"/>
-    <mergeCell ref="BZ124:CC124"/>
-    <mergeCell ref="BR124:BU124"/>
-    <mergeCell ref="BV124:BY124"/>
-    <mergeCell ref="BR153:BU153"/>
-    <mergeCell ref="BV153:BY153"/>
-    <mergeCell ref="BZ153:CC153"/>
-    <mergeCell ref="AH153:AK153"/>
-    <mergeCell ref="BN182:BQ182"/>
-    <mergeCell ref="BB153:BE153"/>
-    <mergeCell ref="BF153:BI153"/>
-    <mergeCell ref="BJ153:BM153"/>
-    <mergeCell ref="BN153:BQ153"/>
-    <mergeCell ref="AP153:AS153"/>
-    <mergeCell ref="AT153:AW153"/>
-    <mergeCell ref="AX153:BA153"/>
-    <mergeCell ref="AX182:BA182"/>
-    <mergeCell ref="BB182:BE182"/>
-    <mergeCell ref="BZ182:CC182"/>
-    <mergeCell ref="BV38:BY38"/>
-    <mergeCell ref="BZ67:CC67"/>
-    <mergeCell ref="BZ96:CC96"/>
-    <mergeCell ref="BJ96:BM96"/>
-    <mergeCell ref="BB38:BE38"/>
-    <mergeCell ref="CD9:CG9"/>
-    <mergeCell ref="CD38:CG38"/>
-    <mergeCell ref="CD124:CG124"/>
-    <mergeCell ref="CD153:CG153"/>
-    <mergeCell ref="CD182:CG182"/>
-    <mergeCell ref="BV9:BY9"/>
-    <mergeCell ref="BZ9:CC9"/>
-    <mergeCell ref="BR9:BU9"/>
-    <mergeCell ref="BR67:BU67"/>
-    <mergeCell ref="BV67:BY67"/>
-    <mergeCell ref="BR96:BU96"/>
-    <mergeCell ref="BV96:BY96"/>
-    <mergeCell ref="BZ38:CC38"/>
-    <mergeCell ref="CD67:CG67"/>
-    <mergeCell ref="CD96:CG96"/>
-    <mergeCell ref="AL182:AO182"/>
+    <mergeCell ref="CL182:CO182"/>
+    <mergeCell ref="CL67:CO67"/>
+    <mergeCell ref="CL96:CO96"/>
+    <mergeCell ref="B182:E182"/>
+    <mergeCell ref="F182:I182"/>
+    <mergeCell ref="J182:M182"/>
+    <mergeCell ref="N182:Q182"/>
+    <mergeCell ref="R182:U182"/>
+    <mergeCell ref="V182:Y182"/>
+    <mergeCell ref="Z182:AC182"/>
+    <mergeCell ref="AD182:AG182"/>
+    <mergeCell ref="AH182:AK182"/>
+    <mergeCell ref="B124:E124"/>
+    <mergeCell ref="F124:I124"/>
+    <mergeCell ref="J124:M124"/>
+    <mergeCell ref="N124:Q124"/>
+    <mergeCell ref="R124:U124"/>
+    <mergeCell ref="V124:Y124"/>
+    <mergeCell ref="Z124:AC124"/>
+    <mergeCell ref="AD124:AG124"/>
+    <mergeCell ref="F153:I153"/>
+    <mergeCell ref="J153:M153"/>
+    <mergeCell ref="N153:Q153"/>
+    <mergeCell ref="R153:U153"/>
+    <mergeCell ref="V153:Y153"/>
+    <mergeCell ref="Z153:AC153"/>
+    <mergeCell ref="AD153:AG153"/>
+    <mergeCell ref="B153:E153"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="J96:M96"/>
+    <mergeCell ref="N96:Q96"/>
+    <mergeCell ref="R96:U96"/>
+    <mergeCell ref="V96:Y96"/>
+    <mergeCell ref="Z96:AC96"/>
+    <mergeCell ref="AD96:AG96"/>
+    <mergeCell ref="AH96:AK96"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="J67:M67"/>
+    <mergeCell ref="N67:Q67"/>
+    <mergeCell ref="R67:U67"/>
+    <mergeCell ref="V67:Y67"/>
+    <mergeCell ref="Z67:AC67"/>
+    <mergeCell ref="AD67:AG67"/>
+    <mergeCell ref="AH67:AK67"/>
+    <mergeCell ref="AL67:AO67"/>
+    <mergeCell ref="AP67:AS67"/>
+    <mergeCell ref="AT67:AW67"/>
+    <mergeCell ref="AX67:BA67"/>
+    <mergeCell ref="BB67:BE67"/>
+    <mergeCell ref="BF67:BI67"/>
+    <mergeCell ref="BJ67:BM67"/>
+    <mergeCell ref="BN67:BQ67"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="R38:U38"/>
+    <mergeCell ref="V38:Y38"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="BB9:BE9"/>
+    <mergeCell ref="BF9:BI9"/>
+    <mergeCell ref="Z38:AC38"/>
+    <mergeCell ref="AD38:AG38"/>
+    <mergeCell ref="AH38:AK38"/>
+    <mergeCell ref="AL38:AO38"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="AD9:AG9"/>
+    <mergeCell ref="BF38:BI38"/>
+    <mergeCell ref="AP38:AS38"/>
+    <mergeCell ref="AT38:AW38"/>
+    <mergeCell ref="AX38:BA38"/>
     <mergeCell ref="AP182:AS182"/>
     <mergeCell ref="AT182:AW182"/>
     <mergeCell ref="BF124:BI124"/>
@@ -38079,96 +38323,70 @@
     <mergeCell ref="AX96:BA96"/>
     <mergeCell ref="BB96:BE96"/>
     <mergeCell ref="BF96:BI96"/>
-    <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:U9"/>
     <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="BV38:BY38"/>
+    <mergeCell ref="BZ67:CC67"/>
+    <mergeCell ref="BZ96:CC96"/>
+    <mergeCell ref="BJ96:BM96"/>
+    <mergeCell ref="BB38:BE38"/>
+    <mergeCell ref="CD9:CG9"/>
+    <mergeCell ref="CD38:CG38"/>
+    <mergeCell ref="CD124:CG124"/>
+    <mergeCell ref="CD153:CG153"/>
+    <mergeCell ref="BV9:BY9"/>
+    <mergeCell ref="BZ9:CC9"/>
+    <mergeCell ref="BR9:BU9"/>
+    <mergeCell ref="BR67:BU67"/>
+    <mergeCell ref="BV67:BY67"/>
+    <mergeCell ref="BR96:BU96"/>
+    <mergeCell ref="BV96:BY96"/>
+    <mergeCell ref="BZ38:CC38"/>
+    <mergeCell ref="CD67:CG67"/>
+    <mergeCell ref="CD96:CG96"/>
     <mergeCell ref="BJ38:BM38"/>
-    <mergeCell ref="AT9:AW9"/>
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="BB9:BE9"/>
-    <mergeCell ref="BF9:BI9"/>
-    <mergeCell ref="Z38:AC38"/>
-    <mergeCell ref="AD38:AG38"/>
-    <mergeCell ref="AH38:AK38"/>
-    <mergeCell ref="AL38:AO38"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="AD9:AG9"/>
-    <mergeCell ref="BF38:BI38"/>
-    <mergeCell ref="AP38:AS38"/>
-    <mergeCell ref="AT38:AW38"/>
-    <mergeCell ref="AX38:BA38"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="J67:M67"/>
-    <mergeCell ref="N67:Q67"/>
-    <mergeCell ref="R67:U67"/>
-    <mergeCell ref="V67:Y67"/>
-    <mergeCell ref="Z67:AC67"/>
-    <mergeCell ref="AD67:AG67"/>
     <mergeCell ref="BR38:BU38"/>
-    <mergeCell ref="AH67:AK67"/>
-    <mergeCell ref="AL67:AO67"/>
-    <mergeCell ref="AP67:AS67"/>
-    <mergeCell ref="AT67:AW67"/>
-    <mergeCell ref="AX67:BA67"/>
-    <mergeCell ref="BB67:BE67"/>
-    <mergeCell ref="BF67:BI67"/>
-    <mergeCell ref="BJ67:BM67"/>
-    <mergeCell ref="BN67:BQ67"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="N38:Q38"/>
-    <mergeCell ref="R38:U38"/>
-    <mergeCell ref="V38:Y38"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="J96:M96"/>
-    <mergeCell ref="N96:Q96"/>
-    <mergeCell ref="R96:U96"/>
-    <mergeCell ref="V96:Y96"/>
-    <mergeCell ref="Z96:AC96"/>
-    <mergeCell ref="AD96:AG96"/>
-    <mergeCell ref="AH96:AK96"/>
-    <mergeCell ref="B124:E124"/>
-    <mergeCell ref="F124:I124"/>
-    <mergeCell ref="J124:M124"/>
-    <mergeCell ref="N124:Q124"/>
-    <mergeCell ref="R124:U124"/>
-    <mergeCell ref="V124:Y124"/>
-    <mergeCell ref="Z124:AC124"/>
-    <mergeCell ref="AD124:AG124"/>
-    <mergeCell ref="F153:I153"/>
-    <mergeCell ref="J153:M153"/>
-    <mergeCell ref="N153:Q153"/>
-    <mergeCell ref="R153:U153"/>
-    <mergeCell ref="V153:Y153"/>
-    <mergeCell ref="Z153:AC153"/>
-    <mergeCell ref="AD153:AG153"/>
-    <mergeCell ref="B153:E153"/>
-    <mergeCell ref="B182:E182"/>
-    <mergeCell ref="F182:I182"/>
-    <mergeCell ref="J182:M182"/>
-    <mergeCell ref="N182:Q182"/>
-    <mergeCell ref="R182:U182"/>
-    <mergeCell ref="V182:Y182"/>
-    <mergeCell ref="Z182:AC182"/>
-    <mergeCell ref="AD182:AG182"/>
-    <mergeCell ref="AH182:AK182"/>
+    <mergeCell ref="CH182:CK182"/>
+    <mergeCell ref="AH124:AK124"/>
+    <mergeCell ref="BR182:BU182"/>
+    <mergeCell ref="BV182:BY182"/>
+    <mergeCell ref="BZ124:CC124"/>
+    <mergeCell ref="BR124:BU124"/>
+    <mergeCell ref="BV124:BY124"/>
+    <mergeCell ref="BR153:BU153"/>
+    <mergeCell ref="BV153:BY153"/>
+    <mergeCell ref="BZ153:CC153"/>
+    <mergeCell ref="AH153:AK153"/>
+    <mergeCell ref="BN182:BQ182"/>
+    <mergeCell ref="BB153:BE153"/>
+    <mergeCell ref="BF153:BI153"/>
+    <mergeCell ref="BJ153:BM153"/>
+    <mergeCell ref="BN153:BQ153"/>
+    <mergeCell ref="AP153:AS153"/>
+    <mergeCell ref="AT153:AW153"/>
+    <mergeCell ref="AX153:BA153"/>
+    <mergeCell ref="AX182:BA182"/>
+    <mergeCell ref="BB182:BE182"/>
+    <mergeCell ref="BZ182:CC182"/>
+    <mergeCell ref="CD182:CG182"/>
+    <mergeCell ref="AL182:AO182"/>
+    <mergeCell ref="CH9:CK9"/>
+    <mergeCell ref="CH38:CK38"/>
+    <mergeCell ref="CL9:CO9"/>
+    <mergeCell ref="CL38:CO38"/>
+    <mergeCell ref="CH67:CK67"/>
+    <mergeCell ref="CH96:CK96"/>
+    <mergeCell ref="CL124:CO124"/>
+    <mergeCell ref="CH124:CK124"/>
+    <mergeCell ref="CH153:CK153"/>
+    <mergeCell ref="CL153:CO153"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="58" max="91" man="1"/>
-    <brk id="116" max="91" man="1"/>
-    <brk id="144" max="91" man="1"/>
+    <brk id="58" max="92" man="1"/>
+    <brk id="116" max="92" man="1"/>
+    <brk id="144" max="92" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q1 2023 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of April 2023\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of May 2023\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9AF6D5-451A-4570-AB0A-82A0EF7A76B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B859DD5E-24AD-4784-9ACF-E38A8CF73368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <definedName name="PCE_Per_Anl">#REF!</definedName>
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CO$202</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CP$202</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="62">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -220,13 +220,16 @@
     <t>2021 - 2022</t>
   </si>
   <si>
-    <t>Q1 2000 to Q4 2022</t>
+    <t>2022 - 2023</t>
   </si>
   <si>
-    <t>Q1 2001 to Q4 2022</t>
+    <t>As of May 2023</t>
   </si>
   <si>
-    <t>As of April 2023</t>
+    <t>Q1 2000 to Q1 2023</t>
+  </si>
+  <si>
+    <t>Q1 2001 to Q1 2023</t>
   </si>
 </sst>
 </file>
@@ -315,7 +318,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -356,10 +359,16 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,11 +708,11 @@
   <dimension ref="A1:EW202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BX2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BX158" activePane="bottomRight" state="frozen"/>
       <selection activeCell="CA66" sqref="CA66"/>
       <selection pane="topRight" activeCell="CA66" sqref="CA66"/>
       <selection pane="bottomLeft" activeCell="CA66" sqref="CA66"/>
-      <selection pane="bottomRight" activeCell="CD1" sqref="CD1:CO1048576"/>
+      <selection pane="bottomRight" activeCell="CQ4" sqref="CQ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -725,14 +734,8 @@
     <col min="74" max="74" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="75" max="77" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="79" max="81" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="87" max="89" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="91" max="93" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="94" max="16384" width="7.77734375" style="1"/>
+    <col min="79" max="94" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="95" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:153" x14ac:dyDescent="0.2">
@@ -747,7 +750,7 @@
     </row>
     <row r="3" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:153" x14ac:dyDescent="0.2">
@@ -757,7 +760,7 @@
     </row>
     <row r="6" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:153" x14ac:dyDescent="0.2">
@@ -767,144 +770,147 @@
     </row>
     <row r="9" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="30">
+      <c r="B9" s="35">
         <v>2000</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30">
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35">
         <v>2001</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30">
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35">
         <v>2002</v>
       </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30">
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35">
         <v>2003</v>
       </c>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30">
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35">
         <v>2004</v>
       </c>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30">
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35">
         <v>2005</v>
       </c>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30">
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35">
         <v>2006</v>
       </c>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="30"/>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="30">
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="35"/>
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35">
         <v>2007</v>
       </c>
-      <c r="AE9" s="30"/>
-      <c r="AF9" s="30"/>
-      <c r="AG9" s="30"/>
-      <c r="AH9" s="30">
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="35">
         <v>2008</v>
       </c>
-      <c r="AI9" s="30"/>
-      <c r="AJ9" s="30"/>
-      <c r="AK9" s="30"/>
-      <c r="AL9" s="30">
+      <c r="AI9" s="35"/>
+      <c r="AJ9" s="35"/>
+      <c r="AK9" s="35"/>
+      <c r="AL9" s="35">
         <v>2009</v>
       </c>
-      <c r="AM9" s="30"/>
-      <c r="AN9" s="30"/>
-      <c r="AO9" s="30"/>
-      <c r="AP9" s="30">
+      <c r="AM9" s="35"/>
+      <c r="AN9" s="35"/>
+      <c r="AO9" s="35"/>
+      <c r="AP9" s="35">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="30"/>
-      <c r="AR9" s="30"/>
-      <c r="AS9" s="30"/>
-      <c r="AT9" s="30">
+      <c r="AQ9" s="35"/>
+      <c r="AR9" s="35"/>
+      <c r="AS9" s="35"/>
+      <c r="AT9" s="35">
         <v>2011</v>
       </c>
-      <c r="AU9" s="30"/>
-      <c r="AV9" s="30"/>
-      <c r="AW9" s="30"/>
-      <c r="AX9" s="30">
+      <c r="AU9" s="35"/>
+      <c r="AV9" s="35"/>
+      <c r="AW9" s="35"/>
+      <c r="AX9" s="35">
         <v>2012</v>
       </c>
-      <c r="AY9" s="30"/>
-      <c r="AZ9" s="30"/>
-      <c r="BA9" s="30"/>
-      <c r="BB9" s="30">
+      <c r="AY9" s="35"/>
+      <c r="AZ9" s="35"/>
+      <c r="BA9" s="35"/>
+      <c r="BB9" s="35">
         <v>2013</v>
       </c>
-      <c r="BC9" s="30"/>
-      <c r="BD9" s="30"/>
-      <c r="BE9" s="30"/>
-      <c r="BF9" s="30">
+      <c r="BC9" s="35"/>
+      <c r="BD9" s="35"/>
+      <c r="BE9" s="35"/>
+      <c r="BF9" s="35">
         <v>2014</v>
       </c>
-      <c r="BG9" s="30"/>
-      <c r="BH9" s="30"/>
-      <c r="BI9" s="30"/>
-      <c r="BJ9" s="30">
+      <c r="BG9" s="35"/>
+      <c r="BH9" s="35"/>
+      <c r="BI9" s="35"/>
+      <c r="BJ9" s="35">
         <v>2015</v>
       </c>
-      <c r="BK9" s="30"/>
-      <c r="BL9" s="30"/>
-      <c r="BM9" s="30"/>
-      <c r="BN9" s="30">
+      <c r="BK9" s="35"/>
+      <c r="BL9" s="35"/>
+      <c r="BM9" s="35"/>
+      <c r="BN9" s="35">
         <v>2016</v>
       </c>
-      <c r="BO9" s="30"/>
-      <c r="BP9" s="30"/>
-      <c r="BQ9" s="30"/>
-      <c r="BR9" s="31">
+      <c r="BO9" s="35"/>
+      <c r="BP9" s="35"/>
+      <c r="BQ9" s="35"/>
+      <c r="BR9" s="34">
         <v>2017</v>
       </c>
-      <c r="BS9" s="31"/>
-      <c r="BT9" s="31"/>
-      <c r="BU9" s="31"/>
-      <c r="BV9" s="31">
+      <c r="BS9" s="34"/>
+      <c r="BT9" s="34"/>
+      <c r="BU9" s="34"/>
+      <c r="BV9" s="34">
         <v>2018</v>
       </c>
-      <c r="BW9" s="31"/>
-      <c r="BX9" s="31"/>
-      <c r="BY9" s="31"/>
-      <c r="BZ9" s="31">
+      <c r="BW9" s="34"/>
+      <c r="BX9" s="34"/>
+      <c r="BY9" s="34"/>
+      <c r="BZ9" s="34">
         <v>2019</v>
       </c>
-      <c r="CA9" s="31"/>
-      <c r="CB9" s="31"/>
-      <c r="CC9" s="31"/>
-      <c r="CD9" s="31">
+      <c r="CA9" s="34"/>
+      <c r="CB9" s="34"/>
+      <c r="CC9" s="34"/>
+      <c r="CD9" s="34">
         <v>2020</v>
       </c>
-      <c r="CE9" s="31"/>
-      <c r="CF9" s="31"/>
-      <c r="CG9" s="31"/>
-      <c r="CH9" s="31">
+      <c r="CE9" s="34"/>
+      <c r="CF9" s="34"/>
+      <c r="CG9" s="34"/>
+      <c r="CH9" s="34">
         <v>2021</v>
       </c>
-      <c r="CI9" s="31"/>
-      <c r="CJ9" s="31"/>
-      <c r="CK9" s="31"/>
-      <c r="CL9" s="31">
+      <c r="CI9" s="34"/>
+      <c r="CJ9" s="34"/>
+      <c r="CK9" s="34"/>
+      <c r="CL9" s="34">
         <v>2022</v>
       </c>
-      <c r="CM9" s="31"/>
-      <c r="CN9" s="31"/>
-      <c r="CO9" s="31"/>
+      <c r="CM9" s="34"/>
+      <c r="CN9" s="34"/>
+      <c r="CO9" s="34"/>
+      <c r="CP9" s="30">
+        <v>2023</v>
+      </c>
     </row>
     <row r="10" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -1185,6 +1191,9 @@
       </c>
       <c r="CO10" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="CP10" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1470,7 +1479,9 @@
       <c r="CO12" s="10">
         <v>1931500.2484176089</v>
       </c>
-      <c r="CP12" s="11"/>
+      <c r="CP12" s="10">
+        <v>1536961.5454871436</v>
+      </c>
       <c r="CQ12" s="11"/>
       <c r="CR12" s="11"/>
       <c r="CS12" s="11"/>
@@ -1811,7 +1822,9 @@
       <c r="CO13" s="10">
         <v>109227.64524527798</v>
       </c>
-      <c r="CP13" s="11"/>
+      <c r="CP13" s="10">
+        <v>79054.108896076417</v>
+      </c>
       <c r="CQ13" s="11"/>
       <c r="CR13" s="11"/>
       <c r="CS13" s="11"/>
@@ -2152,7 +2165,9 @@
       <c r="CO14" s="10">
         <v>86797.581272444193</v>
       </c>
-      <c r="CP14" s="11"/>
+      <c r="CP14" s="10">
+        <v>58248.544076025151</v>
+      </c>
       <c r="CQ14" s="11"/>
       <c r="CR14" s="11"/>
       <c r="CS14" s="11"/>
@@ -2493,7 +2508,9 @@
       <c r="CO15" s="10">
         <v>542954.16776765871</v>
       </c>
-      <c r="CP15" s="11"/>
+      <c r="CP15" s="10">
+        <v>498433.61856295553</v>
+      </c>
       <c r="CQ15" s="11"/>
       <c r="CR15" s="11"/>
       <c r="CS15" s="11"/>
@@ -2834,7 +2851,9 @@
       <c r="CO16" s="10">
         <v>131512.8002420741</v>
       </c>
-      <c r="CP16" s="11"/>
+      <c r="CP16" s="10">
+        <v>110059.36652862828</v>
+      </c>
       <c r="CQ16" s="11"/>
       <c r="CR16" s="11"/>
       <c r="CS16" s="11"/>
@@ -3175,7 +3194,9 @@
       <c r="CO17" s="10">
         <v>195015.04490842862</v>
       </c>
-      <c r="CP17" s="11"/>
+      <c r="CP17" s="10">
+        <v>183078.28945161527</v>
+      </c>
       <c r="CQ17" s="11"/>
       <c r="CR17" s="11"/>
       <c r="CS17" s="11"/>
@@ -3516,7 +3537,9 @@
       <c r="CO18" s="10">
         <v>375843.52030543314</v>
       </c>
-      <c r="CP18" s="11"/>
+      <c r="CP18" s="10">
+        <v>473196.04520302895</v>
+      </c>
       <c r="CQ18" s="11"/>
       <c r="CR18" s="11"/>
       <c r="CS18" s="11"/>
@@ -3857,7 +3880,9 @@
       <c r="CO19" s="10">
         <v>126963.0439176754</v>
       </c>
-      <c r="CP19" s="11"/>
+      <c r="CP19" s="10">
+        <v>127762.99898698949</v>
+      </c>
       <c r="CQ19" s="11"/>
       <c r="CR19" s="11"/>
       <c r="CS19" s="11"/>
@@ -4198,7 +4223,9 @@
       <c r="CO20" s="10">
         <v>84734.360573593935</v>
       </c>
-      <c r="CP20" s="11"/>
+      <c r="CP20" s="10">
+        <v>75412.844071492102</v>
+      </c>
       <c r="CQ20" s="11"/>
       <c r="CR20" s="11"/>
       <c r="CS20" s="11"/>
@@ -4539,7 +4566,9 @@
       <c r="CO21" s="10">
         <v>220643.41206795338</v>
       </c>
-      <c r="CP21" s="11"/>
+      <c r="CP21" s="10">
+        <v>226734.34972381941</v>
+      </c>
       <c r="CQ21" s="11"/>
       <c r="CR21" s="11"/>
       <c r="CS21" s="11"/>
@@ -4880,7 +4909,9 @@
       <c r="CO22" s="10">
         <v>372256.41956097959</v>
       </c>
-      <c r="CP22" s="11"/>
+      <c r="CP22" s="10">
+        <v>423772.64912412758</v>
+      </c>
       <c r="CQ22" s="11"/>
       <c r="CR22" s="11"/>
       <c r="CS22" s="11"/>
@@ -5221,7 +5252,9 @@
       <c r="CO23" s="10">
         <v>686014.65602713195</v>
       </c>
-      <c r="CP23" s="11"/>
+      <c r="CP23" s="10">
+        <v>623675.61552757153</v>
+      </c>
       <c r="CQ23" s="11"/>
       <c r="CR23" s="11"/>
       <c r="CS23" s="11"/>
@@ -5680,43 +5713,45 @@
       <c r="CC25" s="15">
         <v>3985148.1660785396</v>
       </c>
-      <c r="CD25" s="15">
+      <c r="CD25" s="31">
         <v>3422615.4261275791</v>
       </c>
-      <c r="CE25" s="15">
+      <c r="CE25" s="31">
         <v>3042127.6382782664</v>
       </c>
-      <c r="CF25" s="15">
+      <c r="CF25" s="31">
         <v>3210324.7745829187</v>
       </c>
-      <c r="CG25" s="15">
+      <c r="CG25" s="31">
         <v>3801007.5529332561</v>
       </c>
-      <c r="CH25" s="15">
+      <c r="CH25" s="31">
         <v>3397749.5102690379</v>
       </c>
-      <c r="CI25" s="15">
+      <c r="CI25" s="31">
         <v>3395239.9625219679</v>
       </c>
-      <c r="CJ25" s="15">
+      <c r="CJ25" s="31">
         <v>3583126.8104622592</v>
       </c>
-      <c r="CK25" s="15">
+      <c r="CK25" s="31">
         <v>4232430.2197240982</v>
       </c>
-      <c r="CL25" s="15">
+      <c r="CL25" s="31">
         <v>3852962.0714052701</v>
       </c>
-      <c r="CM25" s="15">
+      <c r="CM25" s="31">
         <v>3877423.6981095998</v>
       </c>
-      <c r="CN25" s="15">
+      <c r="CN25" s="31">
         <v>4130910.5601173565</v>
       </c>
-      <c r="CO25" s="15">
+      <c r="CO25" s="31">
         <v>4863462.9003062602</v>
       </c>
-      <c r="CP25" s="11"/>
+      <c r="CP25" s="31">
+        <v>4416389.9756394727</v>
+      </c>
       <c r="CQ25" s="11"/>
       <c r="CR25" s="11"/>
       <c r="CS25" s="11"/>
@@ -5871,6 +5906,7 @@
       <c r="CM26" s="16"/>
       <c r="CN26" s="16"/>
       <c r="CO26" s="16"/>
+      <c r="CP26" s="16"/>
     </row>
     <row r="27" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -5958,19 +5994,19 @@
       <c r="CA28" s="21"/>
       <c r="CB28" s="21"/>
       <c r="CC28" s="21"/>
-      <c r="CD28" s="21"/>
-      <c r="CE28" s="21"/>
-      <c r="CF28" s="21"/>
-      <c r="CG28" s="21"/>
-      <c r="CH28" s="21"/>
-      <c r="CI28" s="21"/>
-      <c r="CJ28" s="21"/>
-      <c r="CK28" s="21"/>
-      <c r="CL28" s="21"/>
-      <c r="CM28" s="21"/>
-      <c r="CN28" s="21"/>
-      <c r="CO28" s="21"/>
-      <c r="CP28" s="11"/>
+      <c r="CD28" s="32"/>
+      <c r="CE28" s="32"/>
+      <c r="CF28" s="32"/>
+      <c r="CG28" s="32"/>
+      <c r="CH28" s="32"/>
+      <c r="CI28" s="32"/>
+      <c r="CJ28" s="32"/>
+      <c r="CK28" s="32"/>
+      <c r="CL28" s="32"/>
+      <c r="CM28" s="32"/>
+      <c r="CN28" s="32"/>
+      <c r="CO28" s="32"/>
+      <c r="CP28" s="32"/>
       <c r="CQ28" s="11"/>
       <c r="CR28" s="11"/>
       <c r="CS28" s="11"/>
@@ -6112,19 +6148,19 @@
       <c r="CA29" s="24"/>
       <c r="CB29" s="24"/>
       <c r="CC29" s="24"/>
-      <c r="CD29" s="24"/>
-      <c r="CE29" s="24"/>
-      <c r="CF29" s="24"/>
-      <c r="CG29" s="24"/>
-      <c r="CH29" s="24"/>
-      <c r="CI29" s="24"/>
-      <c r="CJ29" s="24"/>
-      <c r="CK29" s="24"/>
-      <c r="CL29" s="24"/>
-      <c r="CM29" s="24"/>
-      <c r="CN29" s="24"/>
-      <c r="CO29" s="24"/>
-      <c r="CP29" s="11"/>
+      <c r="CD29" s="33"/>
+      <c r="CE29" s="33"/>
+      <c r="CF29" s="33"/>
+      <c r="CG29" s="33"/>
+      <c r="CH29" s="33"/>
+      <c r="CI29" s="33"/>
+      <c r="CJ29" s="33"/>
+      <c r="CK29" s="33"/>
+      <c r="CL29" s="33"/>
+      <c r="CM29" s="33"/>
+      <c r="CN29" s="33"/>
+      <c r="CO29" s="33"/>
+      <c r="CP29" s="33"/>
       <c r="CQ29" s="11"/>
       <c r="CR29" s="11"/>
       <c r="CS29" s="11"/>
@@ -6197,7 +6233,7 @@
     </row>
     <row r="32" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:153" x14ac:dyDescent="0.2">
@@ -6207,7 +6243,7 @@
     </row>
     <row r="35" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:153" x14ac:dyDescent="0.2">
@@ -6217,144 +6253,147 @@
     </row>
     <row r="38" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="30">
+      <c r="B38" s="35">
         <v>2000</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30">
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35">
         <v>2001</v>
       </c>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30">
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35">
         <v>2002</v>
       </c>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30">
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35">
         <v>2003</v>
       </c>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30">
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35">
         <v>2004</v>
       </c>
-      <c r="S38" s="30"/>
-      <c r="T38" s="30"/>
-      <c r="U38" s="30"/>
-      <c r="V38" s="30">
+      <c r="S38" s="35"/>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="35">
         <v>2005</v>
       </c>
-      <c r="W38" s="30"/>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="30"/>
-      <c r="Z38" s="30">
+      <c r="W38" s="35"/>
+      <c r="X38" s="35"/>
+      <c r="Y38" s="35"/>
+      <c r="Z38" s="35">
         <v>2006</v>
       </c>
-      <c r="AA38" s="30"/>
-      <c r="AB38" s="30"/>
-      <c r="AC38" s="30"/>
-      <c r="AD38" s="30">
+      <c r="AA38" s="35"/>
+      <c r="AB38" s="35"/>
+      <c r="AC38" s="35"/>
+      <c r="AD38" s="35">
         <v>2007</v>
       </c>
-      <c r="AE38" s="30"/>
-      <c r="AF38" s="30"/>
-      <c r="AG38" s="30"/>
-      <c r="AH38" s="30">
+      <c r="AE38" s="35"/>
+      <c r="AF38" s="35"/>
+      <c r="AG38" s="35"/>
+      <c r="AH38" s="35">
         <v>2008</v>
       </c>
-      <c r="AI38" s="30"/>
-      <c r="AJ38" s="30"/>
-      <c r="AK38" s="30"/>
-      <c r="AL38" s="30">
+      <c r="AI38" s="35"/>
+      <c r="AJ38" s="35"/>
+      <c r="AK38" s="35"/>
+      <c r="AL38" s="35">
         <v>2009</v>
       </c>
-      <c r="AM38" s="30"/>
-      <c r="AN38" s="30"/>
-      <c r="AO38" s="30"/>
-      <c r="AP38" s="30">
+      <c r="AM38" s="35"/>
+      <c r="AN38" s="35"/>
+      <c r="AO38" s="35"/>
+      <c r="AP38" s="35">
         <v>2010</v>
       </c>
-      <c r="AQ38" s="30"/>
-      <c r="AR38" s="30"/>
-      <c r="AS38" s="30"/>
-      <c r="AT38" s="30">
+      <c r="AQ38" s="35"/>
+      <c r="AR38" s="35"/>
+      <c r="AS38" s="35"/>
+      <c r="AT38" s="35">
         <v>2011</v>
       </c>
-      <c r="AU38" s="30"/>
-      <c r="AV38" s="30"/>
-      <c r="AW38" s="30"/>
-      <c r="AX38" s="30">
+      <c r="AU38" s="35"/>
+      <c r="AV38" s="35"/>
+      <c r="AW38" s="35"/>
+      <c r="AX38" s="35">
         <v>2012</v>
       </c>
-      <c r="AY38" s="30"/>
-      <c r="AZ38" s="30"/>
-      <c r="BA38" s="30"/>
-      <c r="BB38" s="30">
+      <c r="AY38" s="35"/>
+      <c r="AZ38" s="35"/>
+      <c r="BA38" s="35"/>
+      <c r="BB38" s="35">
         <v>2013</v>
       </c>
-      <c r="BC38" s="30"/>
-      <c r="BD38" s="30"/>
-      <c r="BE38" s="30"/>
-      <c r="BF38" s="30">
+      <c r="BC38" s="35"/>
+      <c r="BD38" s="35"/>
+      <c r="BE38" s="35"/>
+      <c r="BF38" s="35">
         <v>2014</v>
       </c>
-      <c r="BG38" s="30"/>
-      <c r="BH38" s="30"/>
-      <c r="BI38" s="30"/>
-      <c r="BJ38" s="30">
+      <c r="BG38" s="35"/>
+      <c r="BH38" s="35"/>
+      <c r="BI38" s="35"/>
+      <c r="BJ38" s="35">
         <v>2015</v>
       </c>
-      <c r="BK38" s="30"/>
-      <c r="BL38" s="30"/>
-      <c r="BM38" s="30"/>
-      <c r="BN38" s="30">
+      <c r="BK38" s="35"/>
+      <c r="BL38" s="35"/>
+      <c r="BM38" s="35"/>
+      <c r="BN38" s="35">
         <v>2016</v>
       </c>
-      <c r="BO38" s="30"/>
-      <c r="BP38" s="30"/>
-      <c r="BQ38" s="30"/>
-      <c r="BR38" s="31">
+      <c r="BO38" s="35"/>
+      <c r="BP38" s="35"/>
+      <c r="BQ38" s="35"/>
+      <c r="BR38" s="34">
         <v>2017</v>
       </c>
-      <c r="BS38" s="31"/>
-      <c r="BT38" s="31"/>
-      <c r="BU38" s="31"/>
-      <c r="BV38" s="31">
+      <c r="BS38" s="34"/>
+      <c r="BT38" s="34"/>
+      <c r="BU38" s="34"/>
+      <c r="BV38" s="34">
         <v>2018</v>
       </c>
-      <c r="BW38" s="31"/>
-      <c r="BX38" s="31"/>
-      <c r="BY38" s="31"/>
-      <c r="BZ38" s="31">
+      <c r="BW38" s="34"/>
+      <c r="BX38" s="34"/>
+      <c r="BY38" s="34"/>
+      <c r="BZ38" s="34">
         <v>2019</v>
       </c>
-      <c r="CA38" s="31"/>
-      <c r="CB38" s="31"/>
-      <c r="CC38" s="31"/>
-      <c r="CD38" s="31">
+      <c r="CA38" s="34"/>
+      <c r="CB38" s="34"/>
+      <c r="CC38" s="34"/>
+      <c r="CD38" s="34">
         <v>2020</v>
       </c>
-      <c r="CE38" s="31"/>
-      <c r="CF38" s="31"/>
-      <c r="CG38" s="31"/>
-      <c r="CH38" s="31">
+      <c r="CE38" s="34"/>
+      <c r="CF38" s="34"/>
+      <c r="CG38" s="34"/>
+      <c r="CH38" s="34">
         <v>2021</v>
       </c>
-      <c r="CI38" s="31"/>
-      <c r="CJ38" s="31"/>
-      <c r="CK38" s="31"/>
-      <c r="CL38" s="31">
+      <c r="CI38" s="34"/>
+      <c r="CJ38" s="34"/>
+      <c r="CK38" s="34"/>
+      <c r="CL38" s="34">
         <v>2022</v>
       </c>
-      <c r="CM38" s="31"/>
-      <c r="CN38" s="31"/>
-      <c r="CO38" s="31"/>
+      <c r="CM38" s="34"/>
+      <c r="CN38" s="34"/>
+      <c r="CO38" s="34"/>
+      <c r="CP38" s="30">
+        <v>2023</v>
+      </c>
     </row>
     <row r="39" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -6635,6 +6674,9 @@
       </c>
       <c r="CO39" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="CP39" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -6920,7 +6962,9 @@
       <c r="CO41" s="10">
         <v>1614493.9242003553</v>
       </c>
-      <c r="CP41" s="11"/>
+      <c r="CP41" s="10">
+        <v>1265927.2769908078</v>
+      </c>
       <c r="CQ41" s="11"/>
       <c r="CR41" s="11"/>
       <c r="CS41" s="11"/>
@@ -7261,7 +7305,9 @@
       <c r="CO42" s="10">
         <v>69193.996625832791</v>
       </c>
-      <c r="CP42" s="11"/>
+      <c r="CP42" s="10">
+        <v>50720.805813530118</v>
+      </c>
       <c r="CQ42" s="11"/>
       <c r="CR42" s="11"/>
       <c r="CS42" s="11"/>
@@ -7602,7 +7648,9 @@
       <c r="CO43" s="10">
         <v>80450.489963046188</v>
       </c>
-      <c r="CP43" s="11"/>
+      <c r="CP43" s="10">
+        <v>52568.438469482084</v>
+      </c>
       <c r="CQ43" s="11"/>
       <c r="CR43" s="11"/>
       <c r="CS43" s="11"/>
@@ -7943,7 +7991,9 @@
       <c r="CO44" s="10">
         <v>463595.72034765157</v>
       </c>
-      <c r="CP44" s="11"/>
+      <c r="CP44" s="10">
+        <v>441299.36415666755</v>
+      </c>
       <c r="CQ44" s="11"/>
       <c r="CR44" s="11"/>
       <c r="CS44" s="11"/>
@@ -8284,7 +8334,9 @@
       <c r="CO45" s="10">
         <v>117589.60745430055</v>
       </c>
-      <c r="CP45" s="11"/>
+      <c r="CP45" s="10">
+        <v>92926.010044813185</v>
+      </c>
       <c r="CQ45" s="11"/>
       <c r="CR45" s="11"/>
       <c r="CS45" s="11"/>
@@ -8625,7 +8677,9 @@
       <c r="CO46" s="10">
         <v>170571.3236135242</v>
       </c>
-      <c r="CP46" s="11"/>
+      <c r="CP46" s="10">
+        <v>162487.36802897765</v>
+      </c>
       <c r="CQ46" s="11"/>
       <c r="CR46" s="11"/>
       <c r="CS46" s="11"/>
@@ -8966,7 +9020,9 @@
       <c r="CO47" s="10">
         <v>297223.06230146147</v>
       </c>
-      <c r="CP47" s="11"/>
+      <c r="CP47" s="10">
+        <v>357420.88236659684</v>
+      </c>
       <c r="CQ47" s="11"/>
       <c r="CR47" s="11"/>
       <c r="CS47" s="11"/>
@@ -9307,7 +9363,9 @@
       <c r="CO48" s="10">
         <v>129857.71281263117</v>
       </c>
-      <c r="CP48" s="11"/>
+      <c r="CP48" s="10">
+        <v>120902.5534112626</v>
+      </c>
       <c r="CQ48" s="11"/>
       <c r="CR48" s="11"/>
       <c r="CS48" s="11"/>
@@ -9648,7 +9706,9 @@
       <c r="CO49" s="10">
         <v>78882.706678140559</v>
       </c>
-      <c r="CP49" s="11"/>
+      <c r="CP49" s="10">
+        <v>69175.785647688186</v>
+      </c>
       <c r="CQ49" s="11"/>
       <c r="CR49" s="11"/>
       <c r="CS49" s="11"/>
@@ -9989,7 +10049,9 @@
       <c r="CO50" s="10">
         <v>215143.7332874873</v>
       </c>
-      <c r="CP50" s="11"/>
+      <c r="CP50" s="10">
+        <v>209692.33830165802</v>
+      </c>
       <c r="CQ50" s="11"/>
       <c r="CR50" s="11"/>
       <c r="CS50" s="11"/>
@@ -10330,7 +10392,9 @@
       <c r="CO51" s="10">
         <v>320329.20075240469</v>
       </c>
-      <c r="CP51" s="11"/>
+      <c r="CP51" s="10">
+        <v>350704.87869647751</v>
+      </c>
       <c r="CQ51" s="11"/>
       <c r="CR51" s="11"/>
       <c r="CS51" s="11"/>
@@ -10671,7 +10735,9 @@
       <c r="CO52" s="10">
         <v>638740.87639105879</v>
       </c>
-      <c r="CP52" s="11"/>
+      <c r="CP52" s="10">
+        <v>518109.67157395935</v>
+      </c>
       <c r="CQ52" s="11"/>
       <c r="CR52" s="11"/>
       <c r="CS52" s="11"/>
@@ -11130,43 +11196,45 @@
       <c r="CC54" s="15">
         <v>3935758.6177309696</v>
       </c>
-      <c r="CD54" s="15">
+      <c r="CD54" s="31">
         <v>3314612.1320124432</v>
       </c>
-      <c r="CE54" s="15">
+      <c r="CE54" s="31">
         <v>2917736.7328303363</v>
       </c>
-      <c r="CF54" s="15">
+      <c r="CF54" s="31">
         <v>3030086.4136792915</v>
       </c>
-      <c r="CG54" s="15">
+      <c r="CG54" s="31">
         <v>3648921.6749099772</v>
       </c>
-      <c r="CH54" s="15">
+      <c r="CH54" s="31">
         <v>3156809.3523885403</v>
       </c>
-      <c r="CI54" s="15">
+      <c r="CI54" s="31">
         <v>3130131.1633264814</v>
       </c>
-      <c r="CJ54" s="15">
+      <c r="CJ54" s="31">
         <v>3245552.8170434618</v>
       </c>
-      <c r="CK54" s="15">
+      <c r="CK54" s="31">
         <v>3922623.7313984605</v>
       </c>
-      <c r="CL54" s="15">
+      <c r="CL54" s="31">
         <v>3471756.5527950469</v>
       </c>
-      <c r="CM54" s="15">
+      <c r="CM54" s="31">
         <v>3396881.5167516316</v>
       </c>
-      <c r="CN54" s="15">
+      <c r="CN54" s="31">
         <v>3505506.6774791162</v>
       </c>
-      <c r="CO54" s="15">
+      <c r="CO54" s="31">
         <v>4196072.3544278946</v>
       </c>
-      <c r="CP54" s="11"/>
+      <c r="CP54" s="31">
+        <v>3691935.3735019211</v>
+      </c>
       <c r="CQ54" s="11"/>
       <c r="CR54" s="11"/>
       <c r="CS54" s="11"/>
@@ -11321,6 +11389,7 @@
       <c r="CM55" s="16"/>
       <c r="CN55" s="16"/>
       <c r="CO55" s="16"/>
+      <c r="CP55" s="16"/>
     </row>
     <row r="56" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
@@ -11562,19 +11631,19 @@
       <c r="CA58" s="24"/>
       <c r="CB58" s="24"/>
       <c r="CC58" s="24"/>
-      <c r="CD58" s="24"/>
-      <c r="CE58" s="24"/>
-      <c r="CF58" s="24"/>
-      <c r="CG58" s="24"/>
-      <c r="CH58" s="24"/>
-      <c r="CI58" s="24"/>
-      <c r="CJ58" s="24"/>
-      <c r="CK58" s="24"/>
-      <c r="CL58" s="24"/>
-      <c r="CM58" s="24"/>
-      <c r="CN58" s="24"/>
-      <c r="CO58" s="24"/>
-      <c r="CP58" s="11"/>
+      <c r="CD58" s="33"/>
+      <c r="CE58" s="33"/>
+      <c r="CF58" s="33"/>
+      <c r="CG58" s="33"/>
+      <c r="CH58" s="33"/>
+      <c r="CI58" s="33"/>
+      <c r="CJ58" s="33"/>
+      <c r="CK58" s="33"/>
+      <c r="CL58" s="33"/>
+      <c r="CM58" s="33"/>
+      <c r="CN58" s="33"/>
+      <c r="CO58" s="33"/>
+      <c r="CP58" s="33"/>
       <c r="CQ58" s="11"/>
       <c r="CR58" s="11"/>
       <c r="CS58" s="11"/>
@@ -11647,7 +11716,7 @@
     </row>
     <row r="61" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:153" x14ac:dyDescent="0.2">
@@ -11657,7 +11726,7 @@
     </row>
     <row r="64" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:149" x14ac:dyDescent="0.2">
@@ -11667,142 +11736,145 @@
     </row>
     <row r="67" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30" t="s">
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G67" s="30"/>
-      <c r="H67" s="30"/>
-      <c r="I67" s="30"/>
-      <c r="J67" s="30" t="s">
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="K67" s="30"/>
-      <c r="L67" s="30"/>
-      <c r="M67" s="30"/>
-      <c r="N67" s="30" t="s">
+      <c r="K67" s="35"/>
+      <c r="L67" s="35"/>
+      <c r="M67" s="35"/>
+      <c r="N67" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="O67" s="30"/>
-      <c r="P67" s="30"/>
-      <c r="Q67" s="30"/>
-      <c r="R67" s="30" t="s">
+      <c r="O67" s="35"/>
+      <c r="P67" s="35"/>
+      <c r="Q67" s="35"/>
+      <c r="R67" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="S67" s="30"/>
-      <c r="T67" s="30"/>
-      <c r="U67" s="30"/>
-      <c r="V67" s="30" t="s">
+      <c r="S67" s="35"/>
+      <c r="T67" s="35"/>
+      <c r="U67" s="35"/>
+      <c r="V67" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="W67" s="30"/>
-      <c r="X67" s="30"/>
-      <c r="Y67" s="30"/>
-      <c r="Z67" s="30" t="s">
+      <c r="W67" s="35"/>
+      <c r="X67" s="35"/>
+      <c r="Y67" s="35"/>
+      <c r="Z67" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AA67" s="30"/>
-      <c r="AB67" s="30"/>
-      <c r="AC67" s="30"/>
-      <c r="AD67" s="30" t="s">
+      <c r="AA67" s="35"/>
+      <c r="AB67" s="35"/>
+      <c r="AC67" s="35"/>
+      <c r="AD67" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="AE67" s="30"/>
-      <c r="AF67" s="30"/>
-      <c r="AG67" s="30"/>
-      <c r="AH67" s="30" t="s">
+      <c r="AE67" s="35"/>
+      <c r="AF67" s="35"/>
+      <c r="AG67" s="35"/>
+      <c r="AH67" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="AI67" s="30"/>
-      <c r="AJ67" s="30"/>
-      <c r="AK67" s="30"/>
-      <c r="AL67" s="30" t="s">
+      <c r="AI67" s="35"/>
+      <c r="AJ67" s="35"/>
+      <c r="AK67" s="35"/>
+      <c r="AL67" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="AM67" s="30"/>
-      <c r="AN67" s="30"/>
-      <c r="AO67" s="30"/>
-      <c r="AP67" s="30" t="s">
+      <c r="AM67" s="35"/>
+      <c r="AN67" s="35"/>
+      <c r="AO67" s="35"/>
+      <c r="AP67" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="AQ67" s="30"/>
-      <c r="AR67" s="30"/>
-      <c r="AS67" s="30"/>
-      <c r="AT67" s="30" t="s">
+      <c r="AQ67" s="35"/>
+      <c r="AR67" s="35"/>
+      <c r="AS67" s="35"/>
+      <c r="AT67" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="AU67" s="30"/>
-      <c r="AV67" s="30"/>
-      <c r="AW67" s="30"/>
-      <c r="AX67" s="30" t="s">
+      <c r="AU67" s="35"/>
+      <c r="AV67" s="35"/>
+      <c r="AW67" s="35"/>
+      <c r="AX67" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="AY67" s="30"/>
-      <c r="AZ67" s="30"/>
-      <c r="BA67" s="30"/>
-      <c r="BB67" s="30" t="s">
+      <c r="AY67" s="35"/>
+      <c r="AZ67" s="35"/>
+      <c r="BA67" s="35"/>
+      <c r="BB67" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="BC67" s="30"/>
-      <c r="BD67" s="30"/>
-      <c r="BE67" s="30"/>
-      <c r="BF67" s="30" t="s">
+      <c r="BC67" s="35"/>
+      <c r="BD67" s="35"/>
+      <c r="BE67" s="35"/>
+      <c r="BF67" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="BG67" s="30"/>
-      <c r="BH67" s="30"/>
-      <c r="BI67" s="30"/>
-      <c r="BJ67" s="30" t="s">
+      <c r="BG67" s="35"/>
+      <c r="BH67" s="35"/>
+      <c r="BI67" s="35"/>
+      <c r="BJ67" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="BK67" s="30"/>
-      <c r="BL67" s="30"/>
-      <c r="BM67" s="30"/>
-      <c r="BN67" s="30" t="s">
+      <c r="BK67" s="35"/>
+      <c r="BL67" s="35"/>
+      <c r="BM67" s="35"/>
+      <c r="BN67" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="BO67" s="30"/>
-      <c r="BP67" s="30"/>
-      <c r="BQ67" s="30"/>
-      <c r="BR67" s="31" t="s">
+      <c r="BO67" s="35"/>
+      <c r="BP67" s="35"/>
+      <c r="BQ67" s="35"/>
+      <c r="BR67" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="BS67" s="31"/>
-      <c r="BT67" s="31"/>
-      <c r="BU67" s="31"/>
-      <c r="BV67" s="31" t="s">
+      <c r="BS67" s="34"/>
+      <c r="BT67" s="34"/>
+      <c r="BU67" s="34"/>
+      <c r="BV67" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="BW67" s="31"/>
-      <c r="BX67" s="31"/>
-      <c r="BY67" s="31"/>
-      <c r="BZ67" s="31" t="s">
+      <c r="BW67" s="34"/>
+      <c r="BX67" s="34"/>
+      <c r="BY67" s="34"/>
+      <c r="BZ67" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="CA67" s="31"/>
-      <c r="CB67" s="31"/>
-      <c r="CC67" s="31"/>
-      <c r="CD67" s="31" t="s">
+      <c r="CA67" s="34"/>
+      <c r="CB67" s="34"/>
+      <c r="CC67" s="34"/>
+      <c r="CD67" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="CE67" s="31"/>
-      <c r="CF67" s="31"/>
-      <c r="CG67" s="31"/>
-      <c r="CH67" s="31" t="s">
+      <c r="CE67" s="34"/>
+      <c r="CF67" s="34"/>
+      <c r="CG67" s="34"/>
+      <c r="CH67" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="CI67" s="31"/>
-      <c r="CJ67" s="31"/>
-      <c r="CK67" s="31"/>
-      <c r="CL67" s="31"/>
-      <c r="CM67" s="31"/>
-      <c r="CN67" s="31"/>
-      <c r="CO67" s="31"/>
+      <c r="CI67" s="34"/>
+      <c r="CJ67" s="34"/>
+      <c r="CK67" s="34"/>
+      <c r="CL67" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="CM67" s="30"/>
+      <c r="CN67" s="30"/>
+      <c r="CO67" s="30"/>
+      <c r="CP67" s="30"/>
     </row>
     <row r="68" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
@@ -12072,10 +12144,13 @@
       <c r="CK68" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="CL68" s="7"/>
+      <c r="CL68" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="CM68" s="7"/>
       <c r="CN68" s="7"/>
       <c r="CO68" s="7"/>
+      <c r="CP68" s="7"/>
     </row>
     <row r="69" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
@@ -12348,11 +12423,13 @@
       <c r="CK70" s="26">
         <v>14.230451250859005</v>
       </c>
-      <c r="CL70" s="26"/>
+      <c r="CL70" s="26">
+        <v>11.100941746754089</v>
+      </c>
       <c r="CM70" s="26"/>
       <c r="CN70" s="26"/>
       <c r="CO70" s="26"/>
-      <c r="CP70" s="11"/>
+      <c r="CP70" s="26"/>
       <c r="CQ70" s="11"/>
       <c r="CR70" s="11"/>
       <c r="CS70" s="11"/>
@@ -12677,11 +12754,13 @@
       <c r="CK71" s="26">
         <v>14.879767765446744</v>
       </c>
-      <c r="CL71" s="26"/>
+      <c r="CL71" s="26">
+        <v>11.774547348526255</v>
+      </c>
       <c r="CM71" s="26"/>
       <c r="CN71" s="26"/>
       <c r="CO71" s="26"/>
-      <c r="CP71" s="11"/>
+      <c r="CP71" s="26"/>
       <c r="CQ71" s="11"/>
       <c r="CR71" s="11"/>
       <c r="CS71" s="11"/>
@@ -13006,11 +13085,13 @@
       <c r="CK72" s="26">
         <v>14.085116924879742</v>
       </c>
-      <c r="CL72" s="26"/>
+      <c r="CL72" s="26">
+        <v>0.69553047416124514</v>
+      </c>
       <c r="CM72" s="26"/>
       <c r="CN72" s="26"/>
       <c r="CO72" s="26"/>
-      <c r="CP72" s="11"/>
+      <c r="CP72" s="26"/>
       <c r="CQ72" s="11"/>
       <c r="CR72" s="11"/>
       <c r="CS72" s="11"/>
@@ -13335,11 +13416,13 @@
       <c r="CK73" s="26">
         <v>11.921201320286116</v>
       </c>
-      <c r="CL73" s="26"/>
+      <c r="CL73" s="26">
+        <v>12.28702678557238</v>
+      </c>
       <c r="CM73" s="26"/>
       <c r="CN73" s="26"/>
       <c r="CO73" s="26"/>
-      <c r="CP73" s="11"/>
+      <c r="CP73" s="26"/>
       <c r="CQ73" s="11"/>
       <c r="CR73" s="11"/>
       <c r="CS73" s="11"/>
@@ -13664,11 +13747,13 @@
       <c r="CK74" s="26">
         <v>14.127928224150992</v>
       </c>
-      <c r="CL74" s="26"/>
+      <c r="CL74" s="26">
+        <v>2.5539136197363774</v>
+      </c>
       <c r="CM74" s="26"/>
       <c r="CN74" s="26"/>
       <c r="CO74" s="26"/>
-      <c r="CP74" s="11"/>
+      <c r="CP74" s="26"/>
       <c r="CQ74" s="11"/>
       <c r="CR74" s="11"/>
       <c r="CS74" s="11"/>
@@ -13993,11 +14078,13 @@
       <c r="CK75" s="26">
         <v>8.2225014081690233</v>
       </c>
-      <c r="CL75" s="26"/>
+      <c r="CL75" s="26">
+        <v>11.235877389531382</v>
+      </c>
       <c r="CM75" s="26"/>
       <c r="CN75" s="26"/>
       <c r="CO75" s="26"/>
-      <c r="CP75" s="11"/>
+      <c r="CP75" s="26"/>
       <c r="CQ75" s="11"/>
       <c r="CR75" s="11"/>
       <c r="CS75" s="11"/>
@@ -14322,11 +14409,13 @@
       <c r="CK76" s="26">
         <v>20.962940351693334</v>
       </c>
-      <c r="CL76" s="26"/>
+      <c r="CL76" s="26">
+        <v>24.01244022729054</v>
+      </c>
       <c r="CM76" s="26"/>
       <c r="CN76" s="26"/>
       <c r="CO76" s="26"/>
-      <c r="CP76" s="11"/>
+      <c r="CP76" s="26"/>
       <c r="CQ76" s="11"/>
       <c r="CR76" s="11"/>
       <c r="CS76" s="11"/>
@@ -14651,11 +14740,13 @@
       <c r="CK77" s="26">
         <v>6.6924732388451673</v>
       </c>
-      <c r="CL77" s="26"/>
+      <c r="CL77" s="26">
+        <v>5.3987829377145573</v>
+      </c>
       <c r="CM77" s="26"/>
       <c r="CN77" s="26"/>
       <c r="CO77" s="26"/>
-      <c r="CP77" s="11"/>
+      <c r="CP77" s="26"/>
       <c r="CQ77" s="11"/>
       <c r="CR77" s="11"/>
       <c r="CS77" s="11"/>
@@ -14980,11 +15071,13 @@
       <c r="CK78" s="26">
         <v>19.43592958964993</v>
       </c>
-      <c r="CL78" s="26"/>
+      <c r="CL78" s="26">
+        <v>33.748171644300612</v>
+      </c>
       <c r="CM78" s="26"/>
       <c r="CN78" s="26"/>
       <c r="CO78" s="26"/>
-      <c r="CP78" s="11"/>
+      <c r="CP78" s="26"/>
       <c r="CQ78" s="11"/>
       <c r="CR78" s="11"/>
       <c r="CS78" s="11"/>
@@ -15309,11 +15402,13 @@
       <c r="CK79" s="26">
         <v>14.183716365607538</v>
       </c>
-      <c r="CL79" s="26"/>
+      <c r="CL79" s="26">
+        <v>10.116023254301069</v>
+      </c>
       <c r="CM79" s="26"/>
       <c r="CN79" s="26"/>
       <c r="CO79" s="26"/>
-      <c r="CP79" s="11"/>
+      <c r="CP79" s="26"/>
       <c r="CQ79" s="11"/>
       <c r="CR79" s="11"/>
       <c r="CS79" s="11"/>
@@ -15638,11 +15733,13 @@
       <c r="CK80" s="26">
         <v>32.771002893752922</v>
       </c>
-      <c r="CL80" s="26"/>
+      <c r="CL80" s="26">
+        <v>33.75672181980184</v>
+      </c>
       <c r="CM80" s="26"/>
       <c r="CN80" s="26"/>
       <c r="CO80" s="26"/>
-      <c r="CP80" s="11"/>
+      <c r="CP80" s="26"/>
       <c r="CQ80" s="11"/>
       <c r="CR80" s="11"/>
       <c r="CS80" s="11"/>
@@ -15967,11 +16064,13 @@
       <c r="CK81" s="26">
         <v>11.443585383216643</v>
       </c>
-      <c r="CL81" s="26"/>
+      <c r="CL81" s="26">
+        <v>14.794359879300913</v>
+      </c>
       <c r="CM81" s="26"/>
       <c r="CN81" s="26"/>
       <c r="CO81" s="26"/>
-      <c r="CP81" s="11"/>
+      <c r="CP81" s="26"/>
       <c r="CQ81" s="11"/>
       <c r="CR81" s="11"/>
       <c r="CS81" s="11"/>
@@ -16446,11 +16545,13 @@
       <c r="CK83" s="26">
         <v>14.90946448783501</v>
       </c>
-      <c r="CL83" s="26"/>
+      <c r="CL83" s="26">
+        <v>14.623240348397886</v>
+      </c>
       <c r="CM83" s="26"/>
       <c r="CN83" s="26"/>
       <c r="CO83" s="26"/>
-      <c r="CP83" s="11"/>
+      <c r="CP83" s="26"/>
       <c r="CQ83" s="11"/>
       <c r="CR83" s="11"/>
       <c r="CS83" s="11"/>
@@ -16601,6 +16702,7 @@
       <c r="CM84" s="16"/>
       <c r="CN84" s="16"/>
       <c r="CO84" s="16"/>
+      <c r="CP84" s="16"/>
     </row>
     <row r="85" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
@@ -16919,7 +17021,7 @@
     </row>
     <row r="90" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:149" x14ac:dyDescent="0.2">
@@ -16929,7 +17031,7 @@
     </row>
     <row r="93" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:149" x14ac:dyDescent="0.2">
@@ -16939,142 +17041,145 @@
     </row>
     <row r="96" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
-      <c r="B96" s="30" t="s">
+      <c r="B96" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="30" t="s">
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
+      <c r="E96" s="35"/>
+      <c r="F96" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G96" s="30"/>
-      <c r="H96" s="30"/>
-      <c r="I96" s="30"/>
-      <c r="J96" s="30" t="s">
+      <c r="G96" s="35"/>
+      <c r="H96" s="35"/>
+      <c r="I96" s="35"/>
+      <c r="J96" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="K96" s="30"/>
-      <c r="L96" s="30"/>
-      <c r="M96" s="30"/>
-      <c r="N96" s="30" t="s">
+      <c r="K96" s="35"/>
+      <c r="L96" s="35"/>
+      <c r="M96" s="35"/>
+      <c r="N96" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="O96" s="30"/>
-      <c r="P96" s="30"/>
-      <c r="Q96" s="30"/>
-      <c r="R96" s="30" t="s">
+      <c r="O96" s="35"/>
+      <c r="P96" s="35"/>
+      <c r="Q96" s="35"/>
+      <c r="R96" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="S96" s="30"/>
-      <c r="T96" s="30"/>
-      <c r="U96" s="30"/>
-      <c r="V96" s="30" t="s">
+      <c r="S96" s="35"/>
+      <c r="T96" s="35"/>
+      <c r="U96" s="35"/>
+      <c r="V96" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="W96" s="30"/>
-      <c r="X96" s="30"/>
-      <c r="Y96" s="30"/>
-      <c r="Z96" s="30" t="s">
+      <c r="W96" s="35"/>
+      <c r="X96" s="35"/>
+      <c r="Y96" s="35"/>
+      <c r="Z96" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AA96" s="30"/>
-      <c r="AB96" s="30"/>
-      <c r="AC96" s="30"/>
-      <c r="AD96" s="30" t="s">
+      <c r="AA96" s="35"/>
+      <c r="AB96" s="35"/>
+      <c r="AC96" s="35"/>
+      <c r="AD96" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="AE96" s="30"/>
-      <c r="AF96" s="30"/>
-      <c r="AG96" s="30"/>
-      <c r="AH96" s="30" t="s">
+      <c r="AE96" s="35"/>
+      <c r="AF96" s="35"/>
+      <c r="AG96" s="35"/>
+      <c r="AH96" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="AI96" s="30"/>
-      <c r="AJ96" s="30"/>
-      <c r="AK96" s="30"/>
-      <c r="AL96" s="30" t="s">
+      <c r="AI96" s="35"/>
+      <c r="AJ96" s="35"/>
+      <c r="AK96" s="35"/>
+      <c r="AL96" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="AM96" s="30"/>
-      <c r="AN96" s="30"/>
-      <c r="AO96" s="30"/>
-      <c r="AP96" s="30" t="s">
+      <c r="AM96" s="35"/>
+      <c r="AN96" s="35"/>
+      <c r="AO96" s="35"/>
+      <c r="AP96" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="AQ96" s="30"/>
-      <c r="AR96" s="30"/>
-      <c r="AS96" s="30"/>
-      <c r="AT96" s="30" t="s">
+      <c r="AQ96" s="35"/>
+      <c r="AR96" s="35"/>
+      <c r="AS96" s="35"/>
+      <c r="AT96" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="AU96" s="30"/>
-      <c r="AV96" s="30"/>
-      <c r="AW96" s="30"/>
-      <c r="AX96" s="30" t="s">
+      <c r="AU96" s="35"/>
+      <c r="AV96" s="35"/>
+      <c r="AW96" s="35"/>
+      <c r="AX96" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="AY96" s="30"/>
-      <c r="AZ96" s="30"/>
-      <c r="BA96" s="30"/>
-      <c r="BB96" s="30" t="s">
+      <c r="AY96" s="35"/>
+      <c r="AZ96" s="35"/>
+      <c r="BA96" s="35"/>
+      <c r="BB96" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="BC96" s="30"/>
-      <c r="BD96" s="30"/>
-      <c r="BE96" s="30"/>
-      <c r="BF96" s="30" t="s">
+      <c r="BC96" s="35"/>
+      <c r="BD96" s="35"/>
+      <c r="BE96" s="35"/>
+      <c r="BF96" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="BG96" s="30"/>
-      <c r="BH96" s="30"/>
-      <c r="BI96" s="30"/>
-      <c r="BJ96" s="30" t="s">
+      <c r="BG96" s="35"/>
+      <c r="BH96" s="35"/>
+      <c r="BI96" s="35"/>
+      <c r="BJ96" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="BK96" s="30"/>
-      <c r="BL96" s="30"/>
-      <c r="BM96" s="30"/>
-      <c r="BN96" s="30" t="s">
+      <c r="BK96" s="35"/>
+      <c r="BL96" s="35"/>
+      <c r="BM96" s="35"/>
+      <c r="BN96" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="BO96" s="30"/>
-      <c r="BP96" s="30"/>
-      <c r="BQ96" s="30"/>
-      <c r="BR96" s="31" t="s">
+      <c r="BO96" s="35"/>
+      <c r="BP96" s="35"/>
+      <c r="BQ96" s="35"/>
+      <c r="BR96" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="BS96" s="31"/>
-      <c r="BT96" s="31"/>
-      <c r="BU96" s="31"/>
-      <c r="BV96" s="31" t="s">
+      <c r="BS96" s="34"/>
+      <c r="BT96" s="34"/>
+      <c r="BU96" s="34"/>
+      <c r="BV96" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="BW96" s="31"/>
-      <c r="BX96" s="31"/>
-      <c r="BY96" s="31"/>
-      <c r="BZ96" s="31" t="s">
+      <c r="BW96" s="34"/>
+      <c r="BX96" s="34"/>
+      <c r="BY96" s="34"/>
+      <c r="BZ96" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="CA96" s="31"/>
-      <c r="CB96" s="31"/>
-      <c r="CC96" s="31"/>
-      <c r="CD96" s="31" t="s">
+      <c r="CA96" s="34"/>
+      <c r="CB96" s="34"/>
+      <c r="CC96" s="34"/>
+      <c r="CD96" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="CE96" s="31"/>
-      <c r="CF96" s="31"/>
-      <c r="CG96" s="31"/>
-      <c r="CH96" s="31" t="s">
+      <c r="CE96" s="34"/>
+      <c r="CF96" s="34"/>
+      <c r="CG96" s="34"/>
+      <c r="CH96" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="CI96" s="31"/>
-      <c r="CJ96" s="31"/>
-      <c r="CK96" s="31"/>
-      <c r="CL96" s="31"/>
-      <c r="CM96" s="31"/>
-      <c r="CN96" s="31"/>
-      <c r="CO96" s="31"/>
+      <c r="CI96" s="34"/>
+      <c r="CJ96" s="34"/>
+      <c r="CK96" s="34"/>
+      <c r="CL96" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="CM96" s="30"/>
+      <c r="CN96" s="30"/>
+      <c r="CO96" s="30"/>
+      <c r="CP96" s="30"/>
     </row>
     <row r="97" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
@@ -17344,10 +17449,13 @@
       <c r="CK97" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="CL97" s="7"/>
+      <c r="CL97" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="CM97" s="7"/>
       <c r="CN97" s="7"/>
       <c r="CO97" s="7"/>
+      <c r="CP97" s="7"/>
     </row>
     <row r="98" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
@@ -17620,11 +17728,13 @@
       <c r="CK99" s="26">
         <v>3.9785935809430555</v>
       </c>
-      <c r="CL99" s="26"/>
+      <c r="CL99" s="26">
+        <v>0.77992528418768359</v>
+      </c>
       <c r="CM99" s="26"/>
       <c r="CN99" s="26"/>
       <c r="CO99" s="26"/>
-      <c r="CP99" s="11"/>
+      <c r="CP99" s="26"/>
       <c r="CQ99" s="11"/>
       <c r="CR99" s="11"/>
       <c r="CS99" s="11"/>
@@ -17949,11 +18059,13 @@
       <c r="CK100" s="26">
         <v>3.9147385367330259</v>
       </c>
-      <c r="CL100" s="26"/>
+      <c r="CL100" s="26">
+        <v>0.33161662079015741</v>
+      </c>
       <c r="CM100" s="26"/>
       <c r="CN100" s="26"/>
       <c r="CO100" s="26"/>
-      <c r="CP100" s="11"/>
+      <c r="CP100" s="26"/>
       <c r="CQ100" s="11"/>
       <c r="CR100" s="11"/>
       <c r="CS100" s="11"/>
@@ -18278,11 +18390,13 @@
       <c r="CK101" s="26">
         <v>10.193524067478094</v>
       </c>
-      <c r="CL101" s="26"/>
+      <c r="CL101" s="26">
+        <v>-3.8384354359466784</v>
+      </c>
       <c r="CM101" s="26"/>
       <c r="CN101" s="26"/>
       <c r="CO101" s="26"/>
-      <c r="CP101" s="11"/>
+      <c r="CP101" s="26"/>
       <c r="CQ101" s="11"/>
       <c r="CR101" s="11"/>
       <c r="CS101" s="11"/>
@@ -18607,11 +18721,13 @@
       <c r="CK102" s="26">
         <v>4.4963740045475049</v>
       </c>
-      <c r="CL102" s="26"/>
+      <c r="CL102" s="26">
+        <v>3.7369328662439187</v>
+      </c>
       <c r="CM102" s="26"/>
       <c r="CN102" s="26"/>
       <c r="CO102" s="26"/>
-      <c r="CP102" s="11"/>
+      <c r="CP102" s="26"/>
       <c r="CQ102" s="11"/>
       <c r="CR102" s="11"/>
       <c r="CS102" s="11"/>
@@ -18936,11 +19052,13 @@
       <c r="CK103" s="26">
         <v>9.3573074302153856</v>
       </c>
-      <c r="CL103" s="26"/>
+      <c r="CL103" s="26">
+        <v>-3.1028183975854517</v>
+      </c>
       <c r="CM103" s="26"/>
       <c r="CN103" s="26"/>
       <c r="CO103" s="26"/>
-      <c r="CP103" s="11"/>
+      <c r="CP103" s="26"/>
       <c r="CQ103" s="11"/>
       <c r="CR103" s="11"/>
       <c r="CS103" s="11"/>
@@ -19265,11 +19383,13 @@
       <c r="CK104" s="26">
         <v>5.2490153935198265</v>
       </c>
-      <c r="CL104" s="26"/>
+      <c r="CL104" s="26">
+        <v>7.2205947313644288</v>
+      </c>
       <c r="CM104" s="26"/>
       <c r="CN104" s="26"/>
       <c r="CO104" s="26"/>
-      <c r="CP104" s="11"/>
+      <c r="CP104" s="26"/>
       <c r="CQ104" s="11"/>
       <c r="CR104" s="11"/>
       <c r="CS104" s="11"/>
@@ -19594,11 +19714,13 @@
       <c r="CK105" s="26">
         <v>7.8682121727108552</v>
       </c>
-      <c r="CL105" s="26"/>
+      <c r="CL105" s="26">
+        <v>14.418722341660555</v>
+      </c>
       <c r="CM105" s="26"/>
       <c r="CN105" s="26"/>
       <c r="CO105" s="26"/>
-      <c r="CP105" s="11"/>
+      <c r="CP105" s="26"/>
       <c r="CQ105" s="11"/>
       <c r="CR105" s="11"/>
       <c r="CS105" s="11"/>
@@ -19923,11 +20045,13 @@
       <c r="CK106" s="26">
         <v>6.0323765304316055</v>
       </c>
-      <c r="CL106" s="26"/>
+      <c r="CL106" s="26">
+        <v>4.6459344881594831</v>
+      </c>
       <c r="CM106" s="26"/>
       <c r="CN106" s="26"/>
       <c r="CO106" s="26"/>
-      <c r="CP106" s="11"/>
+      <c r="CP106" s="26"/>
       <c r="CQ106" s="11"/>
       <c r="CR106" s="11"/>
       <c r="CS106" s="11"/>
@@ -20252,11 +20376,13 @@
       <c r="CK107" s="26">
         <v>15.49125668577156</v>
       </c>
-      <c r="CL107" s="26"/>
+      <c r="CL107" s="26">
+        <v>28.103087523045843</v>
+      </c>
       <c r="CM107" s="26"/>
       <c r="CN107" s="26"/>
       <c r="CO107" s="26"/>
-      <c r="CP107" s="11"/>
+      <c r="CP107" s="26"/>
       <c r="CQ107" s="11"/>
       <c r="CR107" s="11"/>
       <c r="CS107" s="11"/>
@@ -20581,11 +20707,13 @@
       <c r="CK108" s="26">
         <v>10.278242718539033</v>
       </c>
-      <c r="CL108" s="26"/>
+      <c r="CL108" s="26">
+        <v>6.254040424339081</v>
+      </c>
       <c r="CM108" s="26"/>
       <c r="CN108" s="26"/>
       <c r="CO108" s="26"/>
-      <c r="CP108" s="11"/>
+      <c r="CP108" s="26"/>
       <c r="CQ108" s="11"/>
       <c r="CR108" s="11"/>
       <c r="CS108" s="11"/>
@@ -20910,11 +21038,13 @@
       <c r="CK109" s="26">
         <v>24.779108341374851</v>
       </c>
-      <c r="CL109" s="26"/>
+      <c r="CL109" s="26">
+        <v>23.833675216332239</v>
+      </c>
       <c r="CM109" s="26"/>
       <c r="CN109" s="26"/>
       <c r="CO109" s="26"/>
-      <c r="CP109" s="11"/>
+      <c r="CP109" s="26"/>
       <c r="CQ109" s="11"/>
       <c r="CR109" s="11"/>
       <c r="CS109" s="11"/>
@@ -21239,11 +21369,13 @@
       <c r="CK110" s="26">
         <v>6.6439501425235221</v>
       </c>
-      <c r="CL110" s="26"/>
+      <c r="CL110" s="26">
+        <v>9.0559330265029558</v>
+      </c>
       <c r="CM110" s="26"/>
       <c r="CN110" s="26"/>
       <c r="CO110" s="26"/>
-      <c r="CP110" s="11"/>
+      <c r="CP110" s="26"/>
       <c r="CQ110" s="11"/>
       <c r="CR110" s="11"/>
       <c r="CS110" s="11"/>
@@ -21718,11 +21850,13 @@
       <c r="CK112" s="26">
         <v>6.971064311894807</v>
       </c>
-      <c r="CL112" s="26"/>
+      <c r="CL112" s="26">
+        <v>6.3420005797817822</v>
+      </c>
       <c r="CM112" s="26"/>
       <c r="CN112" s="26"/>
       <c r="CO112" s="26"/>
-      <c r="CP112" s="11"/>
+      <c r="CP112" s="26"/>
       <c r="CQ112" s="11"/>
       <c r="CR112" s="11"/>
       <c r="CS112" s="11"/>
@@ -21873,6 +22007,7 @@
       <c r="CM113" s="16"/>
       <c r="CN113" s="16"/>
       <c r="CO113" s="16"/>
+      <c r="CP113" s="16"/>
     </row>
     <row r="114" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
@@ -22186,7 +22321,7 @@
     </row>
     <row r="118" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="120" spans="1:153" x14ac:dyDescent="0.2">
@@ -22196,7 +22331,7 @@
     </row>
     <row r="121" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="122" spans="1:153" x14ac:dyDescent="0.2">
@@ -22206,144 +22341,147 @@
     </row>
     <row r="124" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
-      <c r="B124" s="30">
+      <c r="B124" s="35">
         <v>2000</v>
       </c>
-      <c r="C124" s="30"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="30"/>
-      <c r="F124" s="30">
+      <c r="C124" s="35"/>
+      <c r="D124" s="35"/>
+      <c r="E124" s="35"/>
+      <c r="F124" s="35">
         <v>2001</v>
       </c>
-      <c r="G124" s="30"/>
-      <c r="H124" s="30"/>
-      <c r="I124" s="30"/>
-      <c r="J124" s="30">
+      <c r="G124" s="35"/>
+      <c r="H124" s="35"/>
+      <c r="I124" s="35"/>
+      <c r="J124" s="35">
         <v>2002</v>
       </c>
-      <c r="K124" s="30"/>
-      <c r="L124" s="30"/>
-      <c r="M124" s="30"/>
-      <c r="N124" s="30">
+      <c r="K124" s="35"/>
+      <c r="L124" s="35"/>
+      <c r="M124" s="35"/>
+      <c r="N124" s="35">
         <v>2003</v>
       </c>
-      <c r="O124" s="30"/>
-      <c r="P124" s="30"/>
-      <c r="Q124" s="30"/>
-      <c r="R124" s="30">
+      <c r="O124" s="35"/>
+      <c r="P124" s="35"/>
+      <c r="Q124" s="35"/>
+      <c r="R124" s="35">
         <v>2004</v>
       </c>
-      <c r="S124" s="30"/>
-      <c r="T124" s="30"/>
-      <c r="U124" s="30"/>
-      <c r="V124" s="30">
+      <c r="S124" s="35"/>
+      <c r="T124" s="35"/>
+      <c r="U124" s="35"/>
+      <c r="V124" s="35">
         <v>2005</v>
       </c>
-      <c r="W124" s="30"/>
-      <c r="X124" s="30"/>
-      <c r="Y124" s="30"/>
-      <c r="Z124" s="30">
+      <c r="W124" s="35"/>
+      <c r="X124" s="35"/>
+      <c r="Y124" s="35"/>
+      <c r="Z124" s="35">
         <v>2006</v>
       </c>
-      <c r="AA124" s="30"/>
-      <c r="AB124" s="30"/>
-      <c r="AC124" s="30"/>
-      <c r="AD124" s="30">
+      <c r="AA124" s="35"/>
+      <c r="AB124" s="35"/>
+      <c r="AC124" s="35"/>
+      <c r="AD124" s="35">
         <v>2007</v>
       </c>
-      <c r="AE124" s="30"/>
-      <c r="AF124" s="30"/>
-      <c r="AG124" s="30"/>
-      <c r="AH124" s="30">
+      <c r="AE124" s="35"/>
+      <c r="AF124" s="35"/>
+      <c r="AG124" s="35"/>
+      <c r="AH124" s="35">
         <v>2008</v>
       </c>
-      <c r="AI124" s="30"/>
-      <c r="AJ124" s="30"/>
-      <c r="AK124" s="30"/>
-      <c r="AL124" s="30">
+      <c r="AI124" s="35"/>
+      <c r="AJ124" s="35"/>
+      <c r="AK124" s="35"/>
+      <c r="AL124" s="35">
         <v>2009</v>
       </c>
-      <c r="AM124" s="30"/>
-      <c r="AN124" s="30"/>
-      <c r="AO124" s="30"/>
-      <c r="AP124" s="30">
+      <c r="AM124" s="35"/>
+      <c r="AN124" s="35"/>
+      <c r="AO124" s="35"/>
+      <c r="AP124" s="35">
         <v>2010</v>
       </c>
-      <c r="AQ124" s="30"/>
-      <c r="AR124" s="30"/>
-      <c r="AS124" s="30"/>
-      <c r="AT124" s="30">
+      <c r="AQ124" s="35"/>
+      <c r="AR124" s="35"/>
+      <c r="AS124" s="35"/>
+      <c r="AT124" s="35">
         <v>2011</v>
       </c>
-      <c r="AU124" s="30"/>
-      <c r="AV124" s="30"/>
-      <c r="AW124" s="30"/>
-      <c r="AX124" s="30">
+      <c r="AU124" s="35"/>
+      <c r="AV124" s="35"/>
+      <c r="AW124" s="35"/>
+      <c r="AX124" s="35">
         <v>2012</v>
       </c>
-      <c r="AY124" s="30"/>
-      <c r="AZ124" s="30"/>
-      <c r="BA124" s="30"/>
-      <c r="BB124" s="30">
+      <c r="AY124" s="35"/>
+      <c r="AZ124" s="35"/>
+      <c r="BA124" s="35"/>
+      <c r="BB124" s="35">
         <v>2013</v>
       </c>
-      <c r="BC124" s="30"/>
-      <c r="BD124" s="30"/>
-      <c r="BE124" s="30"/>
-      <c r="BF124" s="30">
+      <c r="BC124" s="35"/>
+      <c r="BD124" s="35"/>
+      <c r="BE124" s="35"/>
+      <c r="BF124" s="35">
         <v>2014</v>
       </c>
-      <c r="BG124" s="30"/>
-      <c r="BH124" s="30"/>
-      <c r="BI124" s="30"/>
-      <c r="BJ124" s="30">
+      <c r="BG124" s="35"/>
+      <c r="BH124" s="35"/>
+      <c r="BI124" s="35"/>
+      <c r="BJ124" s="35">
         <v>2015</v>
       </c>
-      <c r="BK124" s="30"/>
-      <c r="BL124" s="30"/>
-      <c r="BM124" s="30"/>
-      <c r="BN124" s="30">
+      <c r="BK124" s="35"/>
+      <c r="BL124" s="35"/>
+      <c r="BM124" s="35"/>
+      <c r="BN124" s="35">
         <v>2016</v>
       </c>
-      <c r="BO124" s="30"/>
-      <c r="BP124" s="30"/>
-      <c r="BQ124" s="30"/>
-      <c r="BR124" s="31">
+      <c r="BO124" s="35"/>
+      <c r="BP124" s="35"/>
+      <c r="BQ124" s="35"/>
+      <c r="BR124" s="34">
         <v>2017</v>
       </c>
-      <c r="BS124" s="31"/>
-      <c r="BT124" s="31"/>
-      <c r="BU124" s="31"/>
-      <c r="BV124" s="31">
+      <c r="BS124" s="34"/>
+      <c r="BT124" s="34"/>
+      <c r="BU124" s="34"/>
+      <c r="BV124" s="34">
         <v>2018</v>
       </c>
-      <c r="BW124" s="31"/>
-      <c r="BX124" s="31"/>
-      <c r="BY124" s="31"/>
-      <c r="BZ124" s="31">
+      <c r="BW124" s="34"/>
+      <c r="BX124" s="34"/>
+      <c r="BY124" s="34"/>
+      <c r="BZ124" s="34">
         <v>2019</v>
       </c>
-      <c r="CA124" s="31"/>
-      <c r="CB124" s="31"/>
-      <c r="CC124" s="31"/>
-      <c r="CD124" s="31">
+      <c r="CA124" s="34"/>
+      <c r="CB124" s="34"/>
+      <c r="CC124" s="34"/>
+      <c r="CD124" s="34">
         <v>2020</v>
       </c>
-      <c r="CE124" s="31"/>
-      <c r="CF124" s="31"/>
-      <c r="CG124" s="31"/>
-      <c r="CH124" s="31">
+      <c r="CE124" s="34"/>
+      <c r="CF124" s="34"/>
+      <c r="CG124" s="34"/>
+      <c r="CH124" s="34">
         <v>2021</v>
       </c>
-      <c r="CI124" s="31"/>
-      <c r="CJ124" s="31"/>
-      <c r="CK124" s="31"/>
-      <c r="CL124" s="31">
+      <c r="CI124" s="34"/>
+      <c r="CJ124" s="34"/>
+      <c r="CK124" s="34"/>
+      <c r="CL124" s="34">
         <v>2022</v>
       </c>
-      <c r="CM124" s="31"/>
-      <c r="CN124" s="31"/>
-      <c r="CO124" s="31"/>
+      <c r="CM124" s="34"/>
+      <c r="CN124" s="34"/>
+      <c r="CO124" s="34"/>
+      <c r="CP124" s="30">
+        <v>2023</v>
+      </c>
     </row>
     <row r="125" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
@@ -22624,6 +22762,9 @@
       </c>
       <c r="CO125" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="CP125" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="126" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -22909,7 +23050,9 @@
       <c r="CO127" s="26">
         <v>119.63502738941952</v>
       </c>
-      <c r="CP127" s="11"/>
+      <c r="CP127" s="26">
+        <v>121.40993984588135</v>
+      </c>
       <c r="CQ127" s="11"/>
       <c r="CR127" s="11"/>
       <c r="CS127" s="11"/>
@@ -23250,7 +23393,9 @@
       <c r="CO128" s="26">
         <v>157.85711271445632</v>
       </c>
-      <c r="CP128" s="11"/>
+      <c r="CP128" s="26">
+        <v>155.8613031242264</v>
+      </c>
       <c r="CQ128" s="11"/>
       <c r="CR128" s="11"/>
       <c r="CS128" s="11"/>
@@ -23591,7 +23736,9 @@
       <c r="CO129" s="26">
         <v>107.88943773035248</v>
       </c>
-      <c r="CP129" s="11"/>
+      <c r="CP129" s="26">
+        <v>110.80516327271272</v>
+      </c>
       <c r="CQ129" s="11"/>
       <c r="CR129" s="11"/>
       <c r="CS129" s="11"/>
@@ -23932,7 +24079,9 @@
       <c r="CO130" s="26">
         <v>117.1180284754346</v>
       </c>
-      <c r="CP130" s="11"/>
+      <c r="CP130" s="26">
+        <v>112.94682454743001</v>
+      </c>
       <c r="CQ130" s="11"/>
       <c r="CR130" s="11"/>
       <c r="CS130" s="11"/>
@@ -24273,7 +24422,9 @@
       <c r="CO131" s="26">
         <v>111.84049601763029</v>
       </c>
-      <c r="CP131" s="11"/>
+      <c r="CP131" s="26">
+        <v>118.43763277423901</v>
+      </c>
       <c r="CQ131" s="11"/>
       <c r="CR131" s="11"/>
       <c r="CS131" s="11"/>
@@ -24614,7 +24765,9 @@
       <c r="CO132" s="26">
         <v>114.33049868938599</v>
       </c>
-      <c r="CP132" s="11"/>
+      <c r="CP132" s="26">
+        <v>112.67232134559868</v>
+      </c>
       <c r="CQ132" s="11"/>
       <c r="CR132" s="11"/>
       <c r="CS132" s="11"/>
@@ -24955,7 +25108,9 @@
       <c r="CO133" s="26">
         <v>126.45166811592503</v>
       </c>
-      <c r="CP133" s="11"/>
+      <c r="CP133" s="26">
+        <v>132.39182950639261</v>
+      </c>
       <c r="CQ133" s="11"/>
       <c r="CR133" s="11"/>
       <c r="CS133" s="11"/>
@@ -25296,7 +25451,9 @@
       <c r="CO134" s="26">
         <v>97.770891822858133</v>
       </c>
-      <c r="CP134" s="11"/>
+      <c r="CP134" s="26">
+        <v>105.67435954176283</v>
+      </c>
       <c r="CQ134" s="11"/>
       <c r="CR134" s="11"/>
       <c r="CS134" s="11"/>
@@ -25637,7 +25794,9 @@
       <c r="CO135" s="26">
         <v>107.41817077769586</v>
       </c>
-      <c r="CP135" s="11"/>
+      <c r="CP135" s="26">
+        <v>109.01624515776258</v>
+      </c>
       <c r="CQ135" s="11"/>
       <c r="CR135" s="11"/>
       <c r="CS135" s="11"/>
@@ -25978,7 +26137,9 @@
       <c r="CO136" s="26">
         <v>102.55628118766403</v>
       </c>
-      <c r="CP136" s="11"/>
+      <c r="CP136" s="26">
+        <v>108.12715026223094</v>
+      </c>
       <c r="CQ136" s="11"/>
       <c r="CR136" s="11"/>
       <c r="CS136" s="11"/>
@@ -26319,7 +26480,9 @@
       <c r="CO137" s="26">
         <v>116.21057920620589</v>
       </c>
-      <c r="CP137" s="11"/>
+      <c r="CP137" s="26">
+        <v>120.83454632830689</v>
+      </c>
       <c r="CQ137" s="11"/>
       <c r="CR137" s="11"/>
       <c r="CS137" s="11"/>
@@ -26660,7 +26823,9 @@
       <c r="CO138" s="26">
         <v>107.40108882700197</v>
       </c>
-      <c r="CP138" s="11"/>
+      <c r="CP138" s="26">
+        <v>120.37521199573725</v>
+      </c>
       <c r="CQ138" s="11"/>
       <c r="CR138" s="11"/>
       <c r="CS138" s="11"/>
@@ -27155,7 +27320,9 @@
       <c r="CO140" s="26">
         <v>115.90512482879622</v>
       </c>
-      <c r="CP140" s="11"/>
+      <c r="CP140" s="26">
+        <v>119.62262414822237</v>
+      </c>
       <c r="CQ140" s="11"/>
       <c r="CR140" s="11"/>
       <c r="CS140" s="11"/>
@@ -27310,6 +27477,7 @@
       <c r="CM141" s="16"/>
       <c r="CN141" s="16"/>
       <c r="CO141" s="16"/>
+      <c r="CP141" s="16"/>
     </row>
     <row r="142" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
@@ -27328,7 +27496,7 @@
     </row>
     <row r="147" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="149" spans="1:153" x14ac:dyDescent="0.2">
@@ -27338,7 +27506,7 @@
     </row>
     <row r="150" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="151" spans="1:153" x14ac:dyDescent="0.2">
@@ -27348,144 +27516,147 @@
     </row>
     <row r="153" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
-      <c r="B153" s="30">
+      <c r="B153" s="35">
         <v>2000</v>
       </c>
-      <c r="C153" s="30"/>
-      <c r="D153" s="30"/>
-      <c r="E153" s="30"/>
-      <c r="F153" s="30">
+      <c r="C153" s="35"/>
+      <c r="D153" s="35"/>
+      <c r="E153" s="35"/>
+      <c r="F153" s="35">
         <v>2001</v>
       </c>
-      <c r="G153" s="30"/>
-      <c r="H153" s="30"/>
-      <c r="I153" s="30"/>
-      <c r="J153" s="30">
+      <c r="G153" s="35"/>
+      <c r="H153" s="35"/>
+      <c r="I153" s="35"/>
+      <c r="J153" s="35">
         <v>2002</v>
       </c>
-      <c r="K153" s="30"/>
-      <c r="L153" s="30"/>
-      <c r="M153" s="30"/>
-      <c r="N153" s="30">
+      <c r="K153" s="35"/>
+      <c r="L153" s="35"/>
+      <c r="M153" s="35"/>
+      <c r="N153" s="35">
         <v>2003</v>
       </c>
-      <c r="O153" s="30"/>
-      <c r="P153" s="30"/>
-      <c r="Q153" s="30"/>
-      <c r="R153" s="30">
+      <c r="O153" s="35"/>
+      <c r="P153" s="35"/>
+      <c r="Q153" s="35"/>
+      <c r="R153" s="35">
         <v>2004</v>
       </c>
-      <c r="S153" s="30"/>
-      <c r="T153" s="30"/>
-      <c r="U153" s="30"/>
-      <c r="V153" s="30">
+      <c r="S153" s="35"/>
+      <c r="T153" s="35"/>
+      <c r="U153" s="35"/>
+      <c r="V153" s="35">
         <v>2005</v>
       </c>
-      <c r="W153" s="30"/>
-      <c r="X153" s="30"/>
-      <c r="Y153" s="30"/>
-      <c r="Z153" s="30">
+      <c r="W153" s="35"/>
+      <c r="X153" s="35"/>
+      <c r="Y153" s="35"/>
+      <c r="Z153" s="35">
         <v>2006</v>
       </c>
-      <c r="AA153" s="30"/>
-      <c r="AB153" s="30"/>
-      <c r="AC153" s="30"/>
-      <c r="AD153" s="30">
+      <c r="AA153" s="35"/>
+      <c r="AB153" s="35"/>
+      <c r="AC153" s="35"/>
+      <c r="AD153" s="35">
         <v>2007</v>
       </c>
-      <c r="AE153" s="30"/>
-      <c r="AF153" s="30"/>
-      <c r="AG153" s="30"/>
-      <c r="AH153" s="30">
+      <c r="AE153" s="35"/>
+      <c r="AF153" s="35"/>
+      <c r="AG153" s="35"/>
+      <c r="AH153" s="35">
         <v>2008</v>
       </c>
-      <c r="AI153" s="30"/>
-      <c r="AJ153" s="30"/>
-      <c r="AK153" s="30"/>
-      <c r="AL153" s="30">
+      <c r="AI153" s="35"/>
+      <c r="AJ153" s="35"/>
+      <c r="AK153" s="35"/>
+      <c r="AL153" s="35">
         <v>2009</v>
       </c>
-      <c r="AM153" s="30"/>
-      <c r="AN153" s="30"/>
-      <c r="AO153" s="30"/>
-      <c r="AP153" s="30">
+      <c r="AM153" s="35"/>
+      <c r="AN153" s="35"/>
+      <c r="AO153" s="35"/>
+      <c r="AP153" s="35">
         <v>2010</v>
       </c>
-      <c r="AQ153" s="30"/>
-      <c r="AR153" s="30"/>
-      <c r="AS153" s="30"/>
-      <c r="AT153" s="30">
+      <c r="AQ153" s="35"/>
+      <c r="AR153" s="35"/>
+      <c r="AS153" s="35"/>
+      <c r="AT153" s="35">
         <v>2011</v>
       </c>
-      <c r="AU153" s="30"/>
-      <c r="AV153" s="30"/>
-      <c r="AW153" s="30"/>
-      <c r="AX153" s="30">
+      <c r="AU153" s="35"/>
+      <c r="AV153" s="35"/>
+      <c r="AW153" s="35"/>
+      <c r="AX153" s="35">
         <v>2012</v>
       </c>
-      <c r="AY153" s="30"/>
-      <c r="AZ153" s="30"/>
-      <c r="BA153" s="30"/>
-      <c r="BB153" s="30">
+      <c r="AY153" s="35"/>
+      <c r="AZ153" s="35"/>
+      <c r="BA153" s="35"/>
+      <c r="BB153" s="35">
         <v>2013</v>
       </c>
-      <c r="BC153" s="30"/>
-      <c r="BD153" s="30"/>
-      <c r="BE153" s="30"/>
-      <c r="BF153" s="30">
+      <c r="BC153" s="35"/>
+      <c r="BD153" s="35"/>
+      <c r="BE153" s="35"/>
+      <c r="BF153" s="35">
         <v>2014</v>
       </c>
-      <c r="BG153" s="30"/>
-      <c r="BH153" s="30"/>
-      <c r="BI153" s="30"/>
-      <c r="BJ153" s="30">
+      <c r="BG153" s="35"/>
+      <c r="BH153" s="35"/>
+      <c r="BI153" s="35"/>
+      <c r="BJ153" s="35">
         <v>2015</v>
       </c>
-      <c r="BK153" s="30"/>
-      <c r="BL153" s="30"/>
-      <c r="BM153" s="30"/>
-      <c r="BN153" s="30">
+      <c r="BK153" s="35"/>
+      <c r="BL153" s="35"/>
+      <c r="BM153" s="35"/>
+      <c r="BN153" s="35">
         <v>2016</v>
       </c>
-      <c r="BO153" s="30"/>
-      <c r="BP153" s="30"/>
-      <c r="BQ153" s="30"/>
-      <c r="BR153" s="31">
+      <c r="BO153" s="35"/>
+      <c r="BP153" s="35"/>
+      <c r="BQ153" s="35"/>
+      <c r="BR153" s="34">
         <v>2017</v>
       </c>
-      <c r="BS153" s="31"/>
-      <c r="BT153" s="31"/>
-      <c r="BU153" s="31"/>
-      <c r="BV153" s="31">
+      <c r="BS153" s="34"/>
+      <c r="BT153" s="34"/>
+      <c r="BU153" s="34"/>
+      <c r="BV153" s="34">
         <v>2018</v>
       </c>
-      <c r="BW153" s="31"/>
-      <c r="BX153" s="31"/>
-      <c r="BY153" s="31"/>
-      <c r="BZ153" s="31">
+      <c r="BW153" s="34"/>
+      <c r="BX153" s="34"/>
+      <c r="BY153" s="34"/>
+      <c r="BZ153" s="34">
         <v>2019</v>
       </c>
-      <c r="CA153" s="31"/>
-      <c r="CB153" s="31"/>
-      <c r="CC153" s="31"/>
-      <c r="CD153" s="31">
+      <c r="CA153" s="34"/>
+      <c r="CB153" s="34"/>
+      <c r="CC153" s="34"/>
+      <c r="CD153" s="34">
         <v>2020</v>
       </c>
-      <c r="CE153" s="31"/>
-      <c r="CF153" s="31"/>
-      <c r="CG153" s="31"/>
-      <c r="CH153" s="31">
+      <c r="CE153" s="34"/>
+      <c r="CF153" s="34"/>
+      <c r="CG153" s="34"/>
+      <c r="CH153" s="34">
         <v>2021</v>
       </c>
-      <c r="CI153" s="31"/>
-      <c r="CJ153" s="31"/>
-      <c r="CK153" s="31"/>
-      <c r="CL153" s="31">
+      <c r="CI153" s="34"/>
+      <c r="CJ153" s="34"/>
+      <c r="CK153" s="34"/>
+      <c r="CL153" s="34">
         <v>2022</v>
       </c>
-      <c r="CM153" s="31"/>
-      <c r="CN153" s="31"/>
-      <c r="CO153" s="31"/>
+      <c r="CM153" s="34"/>
+      <c r="CN153" s="34"/>
+      <c r="CO153" s="34"/>
+      <c r="CP153" s="30">
+        <v>2023</v>
+      </c>
     </row>
     <row r="154" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
@@ -27766,6 +27937,9 @@
       </c>
       <c r="CO154" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="CP154" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="155" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -28051,7 +28225,9 @@
       <c r="CO156" s="26">
         <v>39.714505651846942</v>
       </c>
-      <c r="CP156" s="11"/>
+      <c r="CP156" s="26">
+        <v>34.801309530293437</v>
+      </c>
       <c r="CQ156" s="11"/>
       <c r="CR156" s="11"/>
       <c r="CS156" s="11"/>
@@ -28392,7 +28568,9 @@
       <c r="CO157" s="26">
         <v>2.2458821519621286</v>
       </c>
-      <c r="CP157" s="11"/>
+      <c r="CP157" s="26">
+        <v>1.7900164915719372</v>
+      </c>
       <c r="CQ157" s="11"/>
       <c r="CR157" s="11"/>
       <c r="CS157" s="11"/>
@@ -28733,7 +28911,9 @@
       <c r="CO158" s="26">
         <v>1.784686817842867</v>
       </c>
-      <c r="CP158" s="11"/>
+      <c r="CP158" s="26">
+        <v>1.3189175864749361</v>
+      </c>
       <c r="CQ158" s="11"/>
       <c r="CR158" s="11"/>
       <c r="CS158" s="11"/>
@@ -29074,7 +29254,9 @@
       <c r="CO159" s="26">
         <v>11.163941802320894</v>
       </c>
-      <c r="CP159" s="11"/>
+      <c r="CP159" s="26">
+        <v>11.285996511002963</v>
+      </c>
       <c r="CQ159" s="11"/>
       <c r="CR159" s="11"/>
       <c r="CS159" s="11"/>
@@ -29415,7 +29597,9 @@
       <c r="CO160" s="26">
         <v>2.7040979429244238</v>
       </c>
-      <c r="CP160" s="11"/>
+      <c r="CP160" s="26">
+        <v>2.4920663060940895</v>
+      </c>
       <c r="CQ160" s="11"/>
       <c r="CR160" s="11"/>
       <c r="CS160" s="11"/>
@@ -29756,7 +29940,9 @@
       <c r="CO161" s="26">
         <v>4.0097981398428715</v>
       </c>
-      <c r="CP161" s="11"/>
+      <c r="CP161" s="26">
+        <v>4.1454285165364357</v>
+      </c>
       <c r="CQ161" s="11"/>
       <c r="CR161" s="11"/>
       <c r="CS161" s="11"/>
@@ -30097,7 +30283,9 @@
       <c r="CO162" s="26">
         <v>7.7278994002764083</v>
       </c>
-      <c r="CP162" s="11"/>
+      <c r="CP162" s="26">
+        <v>10.71454395588135</v>
+      </c>
       <c r="CQ162" s="11"/>
       <c r="CR162" s="11"/>
       <c r="CS162" s="11"/>
@@ -30438,7 +30626,9 @@
       <c r="CO163" s="26">
         <v>2.6105482147233063</v>
       </c>
-      <c r="CP163" s="11"/>
+      <c r="CP163" s="26">
+        <v>2.8929283802318659</v>
+      </c>
       <c r="CQ163" s="11"/>
       <c r="CR163" s="11"/>
       <c r="CS163" s="11"/>
@@ -30779,7 +30969,9 @@
       <c r="CO164" s="26">
         <v>1.742263944652648</v>
       </c>
-      <c r="CP164" s="11"/>
+      <c r="CP164" s="26">
+        <v>1.7075675945164392</v>
+      </c>
       <c r="CQ164" s="11"/>
       <c r="CR164" s="11"/>
       <c r="CS164" s="11"/>
@@ -31120,7 +31312,9 @@
       <c r="CO165" s="26">
         <v>4.5367553241551217</v>
       </c>
-      <c r="CP165" s="11"/>
+      <c r="CP165" s="26">
+        <v>5.1339295436877572</v>
+      </c>
       <c r="CQ165" s="11"/>
       <c r="CR165" s="11"/>
       <c r="CS165" s="11"/>
@@ -31461,7 +31655,9 @@
       <c r="CO166" s="26">
         <v>7.6541432964881455</v>
       </c>
-      <c r="CP166" s="11"/>
+      <c r="CP166" s="26">
+        <v>9.5954535596183916</v>
+      </c>
       <c r="CQ166" s="11"/>
       <c r="CR166" s="11"/>
       <c r="CS166" s="11"/>
@@ -31802,7 +31998,9 @@
       <c r="CO167" s="26">
         <v>14.105477312964235</v>
       </c>
-      <c r="CP167" s="11"/>
+      <c r="CP167" s="26">
+        <v>14.121842024090418</v>
+      </c>
       <c r="CQ167" s="11"/>
       <c r="CR167" s="11"/>
       <c r="CS167" s="11"/>
@@ -32297,7 +32495,9 @@
       <c r="CO169" s="26">
         <v>100</v>
       </c>
-      <c r="CP169" s="11"/>
+      <c r="CP169" s="26">
+        <v>100</v>
+      </c>
       <c r="CQ169" s="11"/>
       <c r="CR169" s="11"/>
       <c r="CS169" s="11"/>
@@ -32452,6 +32652,7 @@
       <c r="CM170" s="16"/>
       <c r="CN170" s="16"/>
       <c r="CO170" s="16"/>
+      <c r="CP170" s="16"/>
     </row>
     <row r="171" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
@@ -32778,7 +32979,7 @@
     </row>
     <row r="176" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="178" spans="1:153" x14ac:dyDescent="0.2">
@@ -32788,7 +32989,7 @@
     </row>
     <row r="179" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="180" spans="1:153" x14ac:dyDescent="0.2">
@@ -32798,144 +32999,147 @@
     </row>
     <row r="182" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A182" s="4"/>
-      <c r="B182" s="30">
+      <c r="B182" s="35">
         <v>2000</v>
       </c>
-      <c r="C182" s="30"/>
-      <c r="D182" s="30"/>
-      <c r="E182" s="30"/>
-      <c r="F182" s="30">
+      <c r="C182" s="35"/>
+      <c r="D182" s="35"/>
+      <c r="E182" s="35"/>
+      <c r="F182" s="35">
         <v>2001</v>
       </c>
-      <c r="G182" s="30"/>
-      <c r="H182" s="30"/>
-      <c r="I182" s="30"/>
-      <c r="J182" s="30">
+      <c r="G182" s="35"/>
+      <c r="H182" s="35"/>
+      <c r="I182" s="35"/>
+      <c r="J182" s="35">
         <v>2002</v>
       </c>
-      <c r="K182" s="30"/>
-      <c r="L182" s="30"/>
-      <c r="M182" s="30"/>
-      <c r="N182" s="30">
+      <c r="K182" s="35"/>
+      <c r="L182" s="35"/>
+      <c r="M182" s="35"/>
+      <c r="N182" s="35">
         <v>2003</v>
       </c>
-      <c r="O182" s="30"/>
-      <c r="P182" s="30"/>
-      <c r="Q182" s="30"/>
-      <c r="R182" s="30">
+      <c r="O182" s="35"/>
+      <c r="P182" s="35"/>
+      <c r="Q182" s="35"/>
+      <c r="R182" s="35">
         <v>2004</v>
       </c>
-      <c r="S182" s="30"/>
-      <c r="T182" s="30"/>
-      <c r="U182" s="30"/>
-      <c r="V182" s="30">
+      <c r="S182" s="35"/>
+      <c r="T182" s="35"/>
+      <c r="U182" s="35"/>
+      <c r="V182" s="35">
         <v>2005</v>
       </c>
-      <c r="W182" s="30"/>
-      <c r="X182" s="30"/>
-      <c r="Y182" s="30"/>
-      <c r="Z182" s="30">
+      <c r="W182" s="35"/>
+      <c r="X182" s="35"/>
+      <c r="Y182" s="35"/>
+      <c r="Z182" s="35">
         <v>2006</v>
       </c>
-      <c r="AA182" s="30"/>
-      <c r="AB182" s="30"/>
-      <c r="AC182" s="30"/>
-      <c r="AD182" s="30">
+      <c r="AA182" s="35"/>
+      <c r="AB182" s="35"/>
+      <c r="AC182" s="35"/>
+      <c r="AD182" s="35">
         <v>2007</v>
       </c>
-      <c r="AE182" s="30"/>
-      <c r="AF182" s="30"/>
-      <c r="AG182" s="30"/>
-      <c r="AH182" s="30">
+      <c r="AE182" s="35"/>
+      <c r="AF182" s="35"/>
+      <c r="AG182" s="35"/>
+      <c r="AH182" s="35">
         <v>2008</v>
       </c>
-      <c r="AI182" s="30"/>
-      <c r="AJ182" s="30"/>
-      <c r="AK182" s="30"/>
-      <c r="AL182" s="30">
+      <c r="AI182" s="35"/>
+      <c r="AJ182" s="35"/>
+      <c r="AK182" s="35"/>
+      <c r="AL182" s="35">
         <v>2009</v>
       </c>
-      <c r="AM182" s="30"/>
-      <c r="AN182" s="30"/>
-      <c r="AO182" s="30"/>
-      <c r="AP182" s="30">
+      <c r="AM182" s="35"/>
+      <c r="AN182" s="35"/>
+      <c r="AO182" s="35"/>
+      <c r="AP182" s="35">
         <v>2010</v>
       </c>
-      <c r="AQ182" s="30"/>
-      <c r="AR182" s="30"/>
-      <c r="AS182" s="30"/>
-      <c r="AT182" s="30">
+      <c r="AQ182" s="35"/>
+      <c r="AR182" s="35"/>
+      <c r="AS182" s="35"/>
+      <c r="AT182" s="35">
         <v>2011</v>
       </c>
-      <c r="AU182" s="30"/>
-      <c r="AV182" s="30"/>
-      <c r="AW182" s="30"/>
-      <c r="AX182" s="30">
+      <c r="AU182" s="35"/>
+      <c r="AV182" s="35"/>
+      <c r="AW182" s="35"/>
+      <c r="AX182" s="35">
         <v>2012</v>
       </c>
-      <c r="AY182" s="30"/>
-      <c r="AZ182" s="30"/>
-      <c r="BA182" s="30"/>
-      <c r="BB182" s="30">
+      <c r="AY182" s="35"/>
+      <c r="AZ182" s="35"/>
+      <c r="BA182" s="35"/>
+      <c r="BB182" s="35">
         <v>2013</v>
       </c>
-      <c r="BC182" s="30"/>
-      <c r="BD182" s="30"/>
-      <c r="BE182" s="30"/>
-      <c r="BF182" s="30">
+      <c r="BC182" s="35"/>
+      <c r="BD182" s="35"/>
+      <c r="BE182" s="35"/>
+      <c r="BF182" s="35">
         <v>2014</v>
       </c>
-      <c r="BG182" s="30"/>
-      <c r="BH182" s="30"/>
-      <c r="BI182" s="30"/>
-      <c r="BJ182" s="30">
+      <c r="BG182" s="35"/>
+      <c r="BH182" s="35"/>
+      <c r="BI182" s="35"/>
+      <c r="BJ182" s="35">
         <v>2015</v>
       </c>
-      <c r="BK182" s="30"/>
-      <c r="BL182" s="30"/>
-      <c r="BM182" s="30"/>
-      <c r="BN182" s="30">
+      <c r="BK182" s="35"/>
+      <c r="BL182" s="35"/>
+      <c r="BM182" s="35"/>
+      <c r="BN182" s="35">
         <v>2016</v>
       </c>
-      <c r="BO182" s="30"/>
-      <c r="BP182" s="30"/>
-      <c r="BQ182" s="30"/>
-      <c r="BR182" s="31">
+      <c r="BO182" s="35"/>
+      <c r="BP182" s="35"/>
+      <c r="BQ182" s="35"/>
+      <c r="BR182" s="34">
         <v>2017</v>
       </c>
-      <c r="BS182" s="31"/>
-      <c r="BT182" s="31"/>
-      <c r="BU182" s="31"/>
-      <c r="BV182" s="31">
+      <c r="BS182" s="34"/>
+      <c r="BT182" s="34"/>
+      <c r="BU182" s="34"/>
+      <c r="BV182" s="34">
         <v>2018</v>
       </c>
-      <c r="BW182" s="31"/>
-      <c r="BX182" s="31"/>
-      <c r="BY182" s="31"/>
-      <c r="BZ182" s="31">
+      <c r="BW182" s="34"/>
+      <c r="BX182" s="34"/>
+      <c r="BY182" s="34"/>
+      <c r="BZ182" s="34">
         <v>2019</v>
       </c>
-      <c r="CA182" s="31"/>
-      <c r="CB182" s="31"/>
-      <c r="CC182" s="31"/>
-      <c r="CD182" s="31">
+      <c r="CA182" s="34"/>
+      <c r="CB182" s="34"/>
+      <c r="CC182" s="34"/>
+      <c r="CD182" s="34">
         <v>2020</v>
       </c>
-      <c r="CE182" s="31"/>
-      <c r="CF182" s="31"/>
-      <c r="CG182" s="31"/>
-      <c r="CH182" s="31">
+      <c r="CE182" s="34"/>
+      <c r="CF182" s="34"/>
+      <c r="CG182" s="34"/>
+      <c r="CH182" s="34">
         <v>2021</v>
       </c>
-      <c r="CI182" s="31"/>
-      <c r="CJ182" s="31"/>
-      <c r="CK182" s="31"/>
-      <c r="CL182" s="31">
+      <c r="CI182" s="34"/>
+      <c r="CJ182" s="34"/>
+      <c r="CK182" s="34"/>
+      <c r="CL182" s="34">
         <v>2022</v>
       </c>
-      <c r="CM182" s="31"/>
-      <c r="CN182" s="31"/>
-      <c r="CO182" s="31"/>
+      <c r="CM182" s="34"/>
+      <c r="CN182" s="34"/>
+      <c r="CO182" s="34"/>
+      <c r="CP182" s="30">
+        <v>2023</v>
+      </c>
     </row>
     <row r="183" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
@@ -33216,6 +33420,9 @@
       </c>
       <c r="CO183" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="CP183" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="184" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -33501,7 +33708,9 @@
       <c r="CO185" s="26">
         <v>38.476312795146747</v>
       </c>
-      <c r="CP185" s="11"/>
+      <c r="CP185" s="26">
+        <v>34.288987994663479</v>
+      </c>
       <c r="CQ185" s="11"/>
       <c r="CR185" s="11"/>
       <c r="CS185" s="11"/>
@@ -33842,7 +34051,9 @@
       <c r="CO186" s="26">
         <v>1.6490181956184811</v>
       </c>
-      <c r="CP186" s="11"/>
+      <c r="CP186" s="26">
+        <v>1.3738270224762841</v>
+      </c>
       <c r="CQ186" s="11"/>
       <c r="CR186" s="11"/>
       <c r="CS186" s="11"/>
@@ -34183,7 +34394,9 @@
       <c r="CO187" s="26">
         <v>1.9172808085196866</v>
       </c>
-      <c r="CP187" s="11"/>
+      <c r="CP187" s="26">
+        <v>1.4238721199396078</v>
+      </c>
       <c r="CQ187" s="11"/>
       <c r="CR187" s="11"/>
       <c r="CS187" s="11"/>
@@ -34524,7 +34737,9 @@
       <c r="CO188" s="26">
         <v>11.048325223907147</v>
       </c>
-      <c r="CP188" s="11"/>
+      <c r="CP188" s="26">
+        <v>11.953063082414705</v>
+      </c>
       <c r="CQ188" s="11"/>
       <c r="CR188" s="11"/>
       <c r="CS188" s="11"/>
@@ -34865,7 +35080,9 @@
       <c r="CO189" s="26">
         <v>2.802373208131514</v>
       </c>
-      <c r="CP189" s="11"/>
+      <c r="CP189" s="26">
+        <v>2.516999910447236</v>
+      </c>
       <c r="CQ189" s="11"/>
       <c r="CR189" s="11"/>
       <c r="CS189" s="11"/>
@@ -35206,7 +35423,9 @@
       <c r="CO190" s="26">
         <v>4.0650234125140683</v>
       </c>
-      <c r="CP190" s="11"/>
+      <c r="CP190" s="26">
+        <v>4.40114334598585</v>
+      </c>
       <c r="CQ190" s="11"/>
       <c r="CR190" s="11"/>
       <c r="CS190" s="11"/>
@@ -35547,7 +35766,9 @@
       <c r="CO191" s="26">
         <v>7.0833636123509072</v>
       </c>
-      <c r="CP191" s="11"/>
+      <c r="CP191" s="26">
+        <v>9.6811251066827708</v>
+      </c>
       <c r="CQ191" s="11"/>
       <c r="CR191" s="11"/>
       <c r="CS191" s="11"/>
@@ -35888,7 +36109,9 @@
       <c r="CO192" s="26">
         <v>3.0947443667314065</v>
       </c>
-      <c r="CP192" s="11"/>
+      <c r="CP192" s="26">
+        <v>3.2747743711608526</v>
+      </c>
       <c r="CQ192" s="11"/>
       <c r="CR192" s="11"/>
       <c r="CS192" s="11"/>
@@ -36229,7 +36452,9 @@
       <c r="CO193" s="26">
         <v>1.879917694815243</v>
       </c>
-      <c r="CP193" s="11"/>
+      <c r="CP193" s="26">
+        <v>1.8736997983275285</v>
+      </c>
       <c r="CQ193" s="11"/>
       <c r="CR193" s="11"/>
       <c r="CS193" s="11"/>
@@ -36570,7 +36795,9 @@
       <c r="CO194" s="26">
         <v>5.1272646206983881</v>
       </c>
-      <c r="CP194" s="11"/>
+      <c r="CP194" s="26">
+        <v>5.6797402199041747</v>
+      </c>
       <c r="CQ194" s="11"/>
       <c r="CR194" s="11"/>
       <c r="CS194" s="11"/>
@@ -36911,7 +37138,9 @@
       <c r="CO195" s="26">
         <v>7.6340247187200703</v>
       </c>
-      <c r="CP195" s="11"/>
+      <c r="CP195" s="26">
+        <v>9.4992149974668294</v>
+      </c>
       <c r="CQ195" s="11"/>
       <c r="CR195" s="11"/>
       <c r="CS195" s="11"/>
@@ -37252,7 +37481,9 @@
       <c r="CO196" s="26">
         <v>15.222351342846343</v>
       </c>
-      <c r="CP196" s="11"/>
+      <c r="CP196" s="26">
+        <v>14.033552030530682</v>
+      </c>
       <c r="CQ196" s="11"/>
       <c r="CR196" s="11"/>
       <c r="CS196" s="11"/>
@@ -37747,7 +37978,9 @@
       <c r="CO198" s="26">
         <v>100</v>
       </c>
-      <c r="CP198" s="11"/>
+      <c r="CP198" s="26">
+        <v>100</v>
+      </c>
       <c r="CQ198" s="11"/>
       <c r="CR198" s="11"/>
       <c r="CS198" s="11"/>
@@ -37902,6 +38135,7 @@
       <c r="CM199" s="16"/>
       <c r="CN199" s="16"/>
       <c r="CO199" s="16"/>
+      <c r="CP199" s="16"/>
     </row>
     <row r="200" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
@@ -38002,7 +38236,7 @@
       <c r="CM201" s="1"/>
       <c r="CN201" s="1"/>
       <c r="CO201" s="1"/>
-      <c r="CP201" s="28"/>
+      <c r="CP201" s="1"/>
       <c r="CQ201" s="28"/>
       <c r="CR201" s="28"/>
       <c r="CS201" s="28"/>
@@ -38157,7 +38391,7 @@
       <c r="CM202" s="1"/>
       <c r="CN202" s="1"/>
       <c r="CO202" s="1"/>
-      <c r="CP202" s="28"/>
+      <c r="CP202" s="1"/>
       <c r="CQ202" s="28"/>
       <c r="CR202" s="28"/>
       <c r="CS202" s="28"/>
@@ -38219,7 +38453,7 @@
       <c r="EW202" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="161">
+  <mergeCells count="159">
     <mergeCell ref="CL182:CO182"/>
     <mergeCell ref="B182:E182"/>
     <mergeCell ref="F182:I182"/>
@@ -38230,6 +38464,12 @@
     <mergeCell ref="Z182:AC182"/>
     <mergeCell ref="AD182:AG182"/>
     <mergeCell ref="AH182:AK182"/>
+    <mergeCell ref="AP182:AS182"/>
+    <mergeCell ref="AT182:AW182"/>
+    <mergeCell ref="BF182:BI182"/>
+    <mergeCell ref="BJ182:BM182"/>
+    <mergeCell ref="CH182:CK182"/>
+    <mergeCell ref="CD182:CG182"/>
     <mergeCell ref="V153:Y153"/>
     <mergeCell ref="Z153:AC153"/>
     <mergeCell ref="AD153:AG153"/>
@@ -38254,6 +38494,13 @@
     <mergeCell ref="J153:M153"/>
     <mergeCell ref="N153:Q153"/>
     <mergeCell ref="R153:U153"/>
+    <mergeCell ref="BN67:BQ67"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="R38:U38"/>
+    <mergeCell ref="V38:Y38"/>
     <mergeCell ref="AH96:AK96"/>
     <mergeCell ref="B67:E67"/>
     <mergeCell ref="F67:I67"/>
@@ -38264,17 +38511,6 @@
     <mergeCell ref="Z67:AC67"/>
     <mergeCell ref="AD67:AG67"/>
     <mergeCell ref="AH67:AK67"/>
-    <mergeCell ref="AX67:BA67"/>
-    <mergeCell ref="BB67:BE67"/>
-    <mergeCell ref="BF67:BI67"/>
-    <mergeCell ref="BJ67:BM67"/>
-    <mergeCell ref="BN67:BQ67"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="N38:Q38"/>
-    <mergeCell ref="R38:U38"/>
-    <mergeCell ref="V38:Y38"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="J9:M9"/>
@@ -38285,9 +38521,6 @@
     <mergeCell ref="AL67:AO67"/>
     <mergeCell ref="AP67:AS67"/>
     <mergeCell ref="AT67:AW67"/>
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="BB9:BE9"/>
-    <mergeCell ref="BF9:BI9"/>
     <mergeCell ref="Z38:AC38"/>
     <mergeCell ref="AD38:AG38"/>
     <mergeCell ref="AH38:AK38"/>
@@ -38300,11 +38533,6 @@
     <mergeCell ref="AX38:BA38"/>
     <mergeCell ref="AH9:AK9"/>
     <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="AP182:AS182"/>
-    <mergeCell ref="AT182:AW182"/>
-    <mergeCell ref="BF124:BI124"/>
-    <mergeCell ref="BJ124:BM124"/>
-    <mergeCell ref="BN124:BQ124"/>
     <mergeCell ref="BJ9:BM9"/>
     <mergeCell ref="BN9:BQ9"/>
     <mergeCell ref="AL153:AO153"/>
@@ -38313,8 +38541,6 @@
     <mergeCell ref="AT124:AW124"/>
     <mergeCell ref="AX124:BA124"/>
     <mergeCell ref="BB124:BE124"/>
-    <mergeCell ref="BF182:BI182"/>
-    <mergeCell ref="BJ182:BM182"/>
     <mergeCell ref="BN38:BQ38"/>
     <mergeCell ref="BN96:BQ96"/>
     <mergeCell ref="AL96:AO96"/>
@@ -38324,6 +38550,13 @@
     <mergeCell ref="BB96:BE96"/>
     <mergeCell ref="BF96:BI96"/>
     <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="BB9:BE9"/>
+    <mergeCell ref="BF9:BI9"/>
+    <mergeCell ref="AX67:BA67"/>
+    <mergeCell ref="BB67:BE67"/>
+    <mergeCell ref="BF67:BI67"/>
+    <mergeCell ref="BJ67:BM67"/>
     <mergeCell ref="BV38:BY38"/>
     <mergeCell ref="BZ67:CC67"/>
     <mergeCell ref="BZ96:CC96"/>
@@ -38345,7 +38578,9 @@
     <mergeCell ref="CD96:CG96"/>
     <mergeCell ref="BJ38:BM38"/>
     <mergeCell ref="BR38:BU38"/>
-    <mergeCell ref="CH182:CK182"/>
+    <mergeCell ref="BF124:BI124"/>
+    <mergeCell ref="BJ124:BM124"/>
+    <mergeCell ref="BN124:BQ124"/>
     <mergeCell ref="AH124:AK124"/>
     <mergeCell ref="BR182:BU182"/>
     <mergeCell ref="BV182:BY182"/>
@@ -38367,7 +38602,6 @@
     <mergeCell ref="AX182:BA182"/>
     <mergeCell ref="BB182:BE182"/>
     <mergeCell ref="BZ182:CC182"/>
-    <mergeCell ref="CD182:CG182"/>
     <mergeCell ref="AL182:AO182"/>
     <mergeCell ref="CH9:CK9"/>
     <mergeCell ref="CH38:CK38"/>
@@ -38379,16 +38613,14 @@
     <mergeCell ref="CH124:CK124"/>
     <mergeCell ref="CH153:CK153"/>
     <mergeCell ref="CL153:CO153"/>
-    <mergeCell ref="CL67:CO67"/>
-    <mergeCell ref="CL96:CO96"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="58" max="92" man="1"/>
-    <brk id="116" max="92" man="1"/>
-    <brk id="144" max="92" man="1"/>
+    <brk id="58" max="93" man="1"/>
+    <brk id="116" max="93" man="1"/>
+    <brk id="144" max="93" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q2 2023 SNA Update + Script for New PSA Website
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of May 2023\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2023\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B859DD5E-24AD-4784-9ACF-E38A8CF73368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8535EF9B-B114-443D-A2D2-CF5D8FA4E22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="390" windowWidth="28770" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="PCE_Per_Anl">#REF!</definedName>
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CP$202</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$CQ$202</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="62">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -223,13 +223,13 @@
     <t>2022 - 2023</t>
   </si>
   <si>
-    <t>As of May 2023</t>
+    <t>As of August 2023</t>
   </si>
   <si>
-    <t>Q1 2000 to Q1 2023</t>
+    <t>Q1 2000 to Q2 2023</t>
   </si>
   <si>
-    <t>Q1 2001 to Q1 2023</t>
+    <t>Q1 2001 to Q2 2023</t>
   </si>
 </sst>
 </file>
@@ -359,16 +359,16 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -707,8 +707,8 @@
   </sheetPr>
   <dimension ref="A1:EW202"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BX158" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="CD2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="CA66" sqref="CA66"/>
       <selection pane="topRight" activeCell="CA66" sqref="CA66"/>
       <selection pane="bottomLeft" activeCell="CA66" sqref="CA66"/>
@@ -734,8 +734,8 @@
     <col min="74" max="74" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="75" max="77" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="79" max="94" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="95" max="16384" width="7.77734375" style="1"/>
+    <col min="79" max="95" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="96" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:153" x14ac:dyDescent="0.2">
@@ -770,108 +770,108 @@
     </row>
     <row r="9" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="35">
+      <c r="B9" s="33">
         <v>2000</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33">
         <v>2001</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35">
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33">
         <v>2002</v>
       </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35">
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33">
         <v>2003</v>
       </c>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35">
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33">
         <v>2004</v>
       </c>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35">
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33">
         <v>2005</v>
       </c>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="35">
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
+      <c r="Z9" s="33">
         <v>2006</v>
       </c>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="35"/>
-      <c r="AD9" s="35">
+      <c r="AA9" s="33"/>
+      <c r="AB9" s="33"/>
+      <c r="AC9" s="33"/>
+      <c r="AD9" s="33">
         <v>2007</v>
       </c>
-      <c r="AE9" s="35"/>
-      <c r="AF9" s="35"/>
-      <c r="AG9" s="35"/>
-      <c r="AH9" s="35">
+      <c r="AE9" s="33"/>
+      <c r="AF9" s="33"/>
+      <c r="AG9" s="33"/>
+      <c r="AH9" s="33">
         <v>2008</v>
       </c>
-      <c r="AI9" s="35"/>
-      <c r="AJ9" s="35"/>
-      <c r="AK9" s="35"/>
-      <c r="AL9" s="35">
+      <c r="AI9" s="33"/>
+      <c r="AJ9" s="33"/>
+      <c r="AK9" s="33"/>
+      <c r="AL9" s="33">
         <v>2009</v>
       </c>
-      <c r="AM9" s="35"/>
-      <c r="AN9" s="35"/>
-      <c r="AO9" s="35"/>
-      <c r="AP9" s="35">
+      <c r="AM9" s="33"/>
+      <c r="AN9" s="33"/>
+      <c r="AO9" s="33"/>
+      <c r="AP9" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="35"/>
-      <c r="AR9" s="35"/>
-      <c r="AS9" s="35"/>
-      <c r="AT9" s="35">
+      <c r="AQ9" s="33"/>
+      <c r="AR9" s="33"/>
+      <c r="AS9" s="33"/>
+      <c r="AT9" s="33">
         <v>2011</v>
       </c>
-      <c r="AU9" s="35"/>
-      <c r="AV9" s="35"/>
-      <c r="AW9" s="35"/>
-      <c r="AX9" s="35">
+      <c r="AU9" s="33"/>
+      <c r="AV9" s="33"/>
+      <c r="AW9" s="33"/>
+      <c r="AX9" s="33">
         <v>2012</v>
       </c>
-      <c r="AY9" s="35"/>
-      <c r="AZ9" s="35"/>
-      <c r="BA9" s="35"/>
-      <c r="BB9" s="35">
+      <c r="AY9" s="33"/>
+      <c r="AZ9" s="33"/>
+      <c r="BA9" s="33"/>
+      <c r="BB9" s="33">
         <v>2013</v>
       </c>
-      <c r="BC9" s="35"/>
-      <c r="BD9" s="35"/>
-      <c r="BE9" s="35"/>
-      <c r="BF9" s="35">
+      <c r="BC9" s="33"/>
+      <c r="BD9" s="33"/>
+      <c r="BE9" s="33"/>
+      <c r="BF9" s="33">
         <v>2014</v>
       </c>
-      <c r="BG9" s="35"/>
-      <c r="BH9" s="35"/>
-      <c r="BI9" s="35"/>
-      <c r="BJ9" s="35">
+      <c r="BG9" s="33"/>
+      <c r="BH9" s="33"/>
+      <c r="BI9" s="33"/>
+      <c r="BJ9" s="33">
         <v>2015</v>
       </c>
-      <c r="BK9" s="35"/>
-      <c r="BL9" s="35"/>
-      <c r="BM9" s="35"/>
-      <c r="BN9" s="35">
+      <c r="BK9" s="33"/>
+      <c r="BL9" s="33"/>
+      <c r="BM9" s="33"/>
+      <c r="BN9" s="33">
         <v>2016</v>
       </c>
-      <c r="BO9" s="35"/>
-      <c r="BP9" s="35"/>
-      <c r="BQ9" s="35"/>
+      <c r="BO9" s="33"/>
+      <c r="BP9" s="33"/>
+      <c r="BQ9" s="33"/>
       <c r="BR9" s="34">
         <v>2017</v>
       </c>
@@ -908,9 +908,10 @@
       <c r="CM9" s="34"/>
       <c r="CN9" s="34"/>
       <c r="CO9" s="34"/>
-      <c r="CP9" s="30">
+      <c r="CP9" s="34">
         <v>2023</v>
       </c>
+      <c r="CQ9" s="35"/>
     </row>
     <row r="10" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -1194,6 +1195,9 @@
       </c>
       <c r="CP10" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="CQ10" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1480,9 +1484,11 @@
         <v>1931500.2484176089</v>
       </c>
       <c r="CP12" s="10">
-        <v>1536961.5454871436</v>
-      </c>
-      <c r="CQ12" s="11"/>
+        <v>1534902.7290848328</v>
+      </c>
+      <c r="CQ12" s="10">
+        <v>1686600.4695069194</v>
+      </c>
       <c r="CR12" s="11"/>
       <c r="CS12" s="11"/>
       <c r="CT12" s="11"/>
@@ -1823,9 +1829,11 @@
         <v>109227.64524527798</v>
       </c>
       <c r="CP13" s="10">
-        <v>79054.108896076417</v>
-      </c>
-      <c r="CQ13" s="11"/>
+        <v>78577.262359796136</v>
+      </c>
+      <c r="CQ13" s="10">
+        <v>76717.762177284254</v>
+      </c>
       <c r="CR13" s="11"/>
       <c r="CS13" s="11"/>
       <c r="CT13" s="11"/>
@@ -2166,9 +2174,11 @@
         <v>86797.581272444193</v>
       </c>
       <c r="CP14" s="10">
-        <v>58248.544076025151</v>
-      </c>
-      <c r="CQ14" s="11"/>
+        <v>59142.699532093626</v>
+      </c>
+      <c r="CQ14" s="10">
+        <v>49734.51545580048</v>
+      </c>
       <c r="CR14" s="11"/>
       <c r="CS14" s="11"/>
       <c r="CT14" s="11"/>
@@ -2509,9 +2519,11 @@
         <v>542954.16776765871</v>
       </c>
       <c r="CP15" s="10">
-        <v>498433.61856295553</v>
-      </c>
-      <c r="CQ15" s="11"/>
+        <v>499104.71244148072</v>
+      </c>
+      <c r="CQ15" s="10">
+        <v>648697.61821689364</v>
+      </c>
       <c r="CR15" s="11"/>
       <c r="CS15" s="11"/>
       <c r="CT15" s="11"/>
@@ -2852,9 +2864,11 @@
         <v>131512.8002420741</v>
       </c>
       <c r="CP16" s="10">
-        <v>110059.36652862828</v>
-      </c>
-      <c r="CQ16" s="11"/>
+        <v>110439.07435267864</v>
+      </c>
+      <c r="CQ16" s="10">
+        <v>105970.07916830956</v>
+      </c>
       <c r="CR16" s="11"/>
       <c r="CS16" s="11"/>
       <c r="CT16" s="11"/>
@@ -3195,9 +3209,11 @@
         <v>195015.04490842862</v>
       </c>
       <c r="CP17" s="10">
-        <v>183078.28945161527</v>
-      </c>
-      <c r="CQ17" s="11"/>
+        <v>184071.27892650483</v>
+      </c>
+      <c r="CQ17" s="10">
+        <v>156483.14364244594</v>
+      </c>
       <c r="CR17" s="11"/>
       <c r="CS17" s="11"/>
       <c r="CT17" s="11"/>
@@ -3538,9 +3554,11 @@
         <v>375843.52030543314</v>
       </c>
       <c r="CP18" s="10">
-        <v>473196.04520302895</v>
-      </c>
-      <c r="CQ18" s="11"/>
+        <v>472851.25966836378</v>
+      </c>
+      <c r="CQ18" s="10">
+        <v>384048.71192407014</v>
+      </c>
       <c r="CR18" s="11"/>
       <c r="CS18" s="11"/>
       <c r="CT18" s="11"/>
@@ -3881,9 +3899,11 @@
         <v>126963.0439176754</v>
       </c>
       <c r="CP19" s="10">
-        <v>127762.99898698949</v>
-      </c>
-      <c r="CQ19" s="11"/>
+        <v>128102.85613251821</v>
+      </c>
+      <c r="CQ19" s="10">
+        <v>134586.0823199171</v>
+      </c>
       <c r="CR19" s="11"/>
       <c r="CS19" s="11"/>
       <c r="CT19" s="11"/>
@@ -4224,9 +4244,11 @@
         <v>84734.360573593935</v>
       </c>
       <c r="CP20" s="10">
-        <v>75412.844071492102</v>
-      </c>
-      <c r="CQ20" s="11"/>
+        <v>76403.305244792777</v>
+      </c>
+      <c r="CQ20" s="10">
+        <v>53071.762457292527</v>
+      </c>
       <c r="CR20" s="11"/>
       <c r="CS20" s="11"/>
       <c r="CT20" s="11"/>
@@ -4567,9 +4589,11 @@
         <v>220643.41206795338</v>
       </c>
       <c r="CP21" s="10">
-        <v>226734.34972381941</v>
-      </c>
-      <c r="CQ21" s="11"/>
+        <v>227528.12153380137</v>
+      </c>
+      <c r="CQ21" s="10">
+        <v>207245.97407203735</v>
+      </c>
       <c r="CR21" s="11"/>
       <c r="CS21" s="11"/>
       <c r="CT21" s="11"/>
@@ -4910,9 +4934,11 @@
         <v>372256.41956097959</v>
       </c>
       <c r="CP22" s="10">
-        <v>423772.64912412758</v>
-      </c>
-      <c r="CQ22" s="11"/>
+        <v>424434.51070063253</v>
+      </c>
+      <c r="CQ22" s="10">
+        <v>243802.91132714995</v>
+      </c>
       <c r="CR22" s="11"/>
       <c r="CS22" s="11"/>
       <c r="CT22" s="11"/>
@@ -5253,9 +5279,11 @@
         <v>686014.65602713195</v>
       </c>
       <c r="CP23" s="10">
-        <v>623675.61552757153</v>
-      </c>
-      <c r="CQ23" s="11"/>
+        <v>623919.99372991757</v>
+      </c>
+      <c r="CQ23" s="10">
+        <v>579210.37901549623</v>
+      </c>
       <c r="CR23" s="11"/>
       <c r="CS23" s="11"/>
       <c r="CT23" s="11"/>
@@ -5713,46 +5741,48 @@
       <c r="CC25" s="15">
         <v>3985148.1660785396</v>
       </c>
-      <c r="CD25" s="31">
+      <c r="CD25" s="30">
         <v>3422615.4261275791</v>
       </c>
-      <c r="CE25" s="31">
+      <c r="CE25" s="30">
         <v>3042127.6382782664</v>
       </c>
-      <c r="CF25" s="31">
+      <c r="CF25" s="30">
         <v>3210324.7745829187</v>
       </c>
-      <c r="CG25" s="31">
+      <c r="CG25" s="30">
         <v>3801007.5529332561</v>
       </c>
-      <c r="CH25" s="31">
+      <c r="CH25" s="30">
         <v>3397749.5102690379</v>
       </c>
-      <c r="CI25" s="31">
+      <c r="CI25" s="30">
         <v>3395239.9625219679</v>
       </c>
-      <c r="CJ25" s="31">
+      <c r="CJ25" s="30">
         <v>3583126.8104622592</v>
       </c>
-      <c r="CK25" s="31">
+      <c r="CK25" s="30">
         <v>4232430.2197240982</v>
       </c>
-      <c r="CL25" s="31">
+      <c r="CL25" s="30">
         <v>3852962.0714052701</v>
       </c>
-      <c r="CM25" s="31">
+      <c r="CM25" s="30">
         <v>3877423.6981095998</v>
       </c>
-      <c r="CN25" s="31">
+      <c r="CN25" s="30">
         <v>4130910.5601173565</v>
       </c>
-      <c r="CO25" s="31">
+      <c r="CO25" s="30">
         <v>4863462.9003062602</v>
       </c>
-      <c r="CP25" s="31">
-        <v>4416389.9756394727</v>
-      </c>
-      <c r="CQ25" s="11"/>
+      <c r="CP25" s="30">
+        <v>4419477.8037074124</v>
+      </c>
+      <c r="CQ25" s="30">
+        <v>4326169.4092836166</v>
+      </c>
       <c r="CR25" s="11"/>
       <c r="CS25" s="11"/>
       <c r="CT25" s="11"/>
@@ -5907,6 +5937,7 @@
       <c r="CN26" s="16"/>
       <c r="CO26" s="16"/>
       <c r="CP26" s="16"/>
+      <c r="CQ26" s="16"/>
     </row>
     <row r="27" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -5994,20 +6025,20 @@
       <c r="CA28" s="21"/>
       <c r="CB28" s="21"/>
       <c r="CC28" s="21"/>
-      <c r="CD28" s="32"/>
-      <c r="CE28" s="32"/>
-      <c r="CF28" s="32"/>
-      <c r="CG28" s="32"/>
-      <c r="CH28" s="32"/>
-      <c r="CI28" s="32"/>
-      <c r="CJ28" s="32"/>
-      <c r="CK28" s="32"/>
-      <c r="CL28" s="32"/>
-      <c r="CM28" s="32"/>
-      <c r="CN28" s="32"/>
-      <c r="CO28" s="32"/>
-      <c r="CP28" s="32"/>
-      <c r="CQ28" s="11"/>
+      <c r="CD28" s="31"/>
+      <c r="CE28" s="31"/>
+      <c r="CF28" s="31"/>
+      <c r="CG28" s="31"/>
+      <c r="CH28" s="31"/>
+      <c r="CI28" s="31"/>
+      <c r="CJ28" s="31"/>
+      <c r="CK28" s="31"/>
+      <c r="CL28" s="31"/>
+      <c r="CM28" s="31"/>
+      <c r="CN28" s="31"/>
+      <c r="CO28" s="31"/>
+      <c r="CP28" s="31"/>
+      <c r="CQ28" s="31"/>
       <c r="CR28" s="11"/>
       <c r="CS28" s="11"/>
       <c r="CT28" s="11"/>
@@ -6148,20 +6179,20 @@
       <c r="CA29" s="24"/>
       <c r="CB29" s="24"/>
       <c r="CC29" s="24"/>
-      <c r="CD29" s="33"/>
-      <c r="CE29" s="33"/>
-      <c r="CF29" s="33"/>
-      <c r="CG29" s="33"/>
-      <c r="CH29" s="33"/>
-      <c r="CI29" s="33"/>
-      <c r="CJ29" s="33"/>
-      <c r="CK29" s="33"/>
-      <c r="CL29" s="33"/>
-      <c r="CM29" s="33"/>
-      <c r="CN29" s="33"/>
-      <c r="CO29" s="33"/>
-      <c r="CP29" s="33"/>
-      <c r="CQ29" s="11"/>
+      <c r="CD29" s="32"/>
+      <c r="CE29" s="32"/>
+      <c r="CF29" s="32"/>
+      <c r="CG29" s="32"/>
+      <c r="CH29" s="32"/>
+      <c r="CI29" s="32"/>
+      <c r="CJ29" s="32"/>
+      <c r="CK29" s="32"/>
+      <c r="CL29" s="32"/>
+      <c r="CM29" s="32"/>
+      <c r="CN29" s="32"/>
+      <c r="CO29" s="32"/>
+      <c r="CP29" s="32"/>
+      <c r="CQ29" s="32"/>
       <c r="CR29" s="11"/>
       <c r="CS29" s="11"/>
       <c r="CT29" s="11"/>
@@ -6253,108 +6284,108 @@
     </row>
     <row r="38" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="35">
+      <c r="B38" s="33">
         <v>2000</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35">
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33">
         <v>2001</v>
       </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35">
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33">
         <v>2002</v>
       </c>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35">
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33">
         <v>2003</v>
       </c>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="35">
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="33">
         <v>2004</v>
       </c>
-      <c r="S38" s="35"/>
-      <c r="T38" s="35"/>
-      <c r="U38" s="35"/>
-      <c r="V38" s="35">
+      <c r="S38" s="33"/>
+      <c r="T38" s="33"/>
+      <c r="U38" s="33"/>
+      <c r="V38" s="33">
         <v>2005</v>
       </c>
-      <c r="W38" s="35"/>
-      <c r="X38" s="35"/>
-      <c r="Y38" s="35"/>
-      <c r="Z38" s="35">
+      <c r="W38" s="33"/>
+      <c r="X38" s="33"/>
+      <c r="Y38" s="33"/>
+      <c r="Z38" s="33">
         <v>2006</v>
       </c>
-      <c r="AA38" s="35"/>
-      <c r="AB38" s="35"/>
-      <c r="AC38" s="35"/>
-      <c r="AD38" s="35">
+      <c r="AA38" s="33"/>
+      <c r="AB38" s="33"/>
+      <c r="AC38" s="33"/>
+      <c r="AD38" s="33">
         <v>2007</v>
       </c>
-      <c r="AE38" s="35"/>
-      <c r="AF38" s="35"/>
-      <c r="AG38" s="35"/>
-      <c r="AH38" s="35">
+      <c r="AE38" s="33"/>
+      <c r="AF38" s="33"/>
+      <c r="AG38" s="33"/>
+      <c r="AH38" s="33">
         <v>2008</v>
       </c>
-      <c r="AI38" s="35"/>
-      <c r="AJ38" s="35"/>
-      <c r="AK38" s="35"/>
-      <c r="AL38" s="35">
+      <c r="AI38" s="33"/>
+      <c r="AJ38" s="33"/>
+      <c r="AK38" s="33"/>
+      <c r="AL38" s="33">
         <v>2009</v>
       </c>
-      <c r="AM38" s="35"/>
-      <c r="AN38" s="35"/>
-      <c r="AO38" s="35"/>
-      <c r="AP38" s="35">
+      <c r="AM38" s="33"/>
+      <c r="AN38" s="33"/>
+      <c r="AO38" s="33"/>
+      <c r="AP38" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ38" s="35"/>
-      <c r="AR38" s="35"/>
-      <c r="AS38" s="35"/>
-      <c r="AT38" s="35">
+      <c r="AQ38" s="33"/>
+      <c r="AR38" s="33"/>
+      <c r="AS38" s="33"/>
+      <c r="AT38" s="33">
         <v>2011</v>
       </c>
-      <c r="AU38" s="35"/>
-      <c r="AV38" s="35"/>
-      <c r="AW38" s="35"/>
-      <c r="AX38" s="35">
+      <c r="AU38" s="33"/>
+      <c r="AV38" s="33"/>
+      <c r="AW38" s="33"/>
+      <c r="AX38" s="33">
         <v>2012</v>
       </c>
-      <c r="AY38" s="35"/>
-      <c r="AZ38" s="35"/>
-      <c r="BA38" s="35"/>
-      <c r="BB38" s="35">
+      <c r="AY38" s="33"/>
+      <c r="AZ38" s="33"/>
+      <c r="BA38" s="33"/>
+      <c r="BB38" s="33">
         <v>2013</v>
       </c>
-      <c r="BC38" s="35"/>
-      <c r="BD38" s="35"/>
-      <c r="BE38" s="35"/>
-      <c r="BF38" s="35">
+      <c r="BC38" s="33"/>
+      <c r="BD38" s="33"/>
+      <c r="BE38" s="33"/>
+      <c r="BF38" s="33">
         <v>2014</v>
       </c>
-      <c r="BG38" s="35"/>
-      <c r="BH38" s="35"/>
-      <c r="BI38" s="35"/>
-      <c r="BJ38" s="35">
+      <c r="BG38" s="33"/>
+      <c r="BH38" s="33"/>
+      <c r="BI38" s="33"/>
+      <c r="BJ38" s="33">
         <v>2015</v>
       </c>
-      <c r="BK38" s="35"/>
-      <c r="BL38" s="35"/>
-      <c r="BM38" s="35"/>
-      <c r="BN38" s="35">
+      <c r="BK38" s="33"/>
+      <c r="BL38" s="33"/>
+      <c r="BM38" s="33"/>
+      <c r="BN38" s="33">
         <v>2016</v>
       </c>
-      <c r="BO38" s="35"/>
-      <c r="BP38" s="35"/>
-      <c r="BQ38" s="35"/>
+      <c r="BO38" s="33"/>
+      <c r="BP38" s="33"/>
+      <c r="BQ38" s="33"/>
       <c r="BR38" s="34">
         <v>2017</v>
       </c>
@@ -6391,9 +6422,10 @@
       <c r="CM38" s="34"/>
       <c r="CN38" s="34"/>
       <c r="CO38" s="34"/>
-      <c r="CP38" s="30">
+      <c r="CP38" s="34">
         <v>2023</v>
       </c>
+      <c r="CQ38" s="35"/>
     </row>
     <row r="39" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -6677,6 +6709,9 @@
       </c>
       <c r="CP39" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="CQ39" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -6963,9 +6998,11 @@
         <v>1614493.9242003553</v>
       </c>
       <c r="CP41" s="10">
-        <v>1265927.2769908078</v>
-      </c>
-      <c r="CQ41" s="11"/>
+        <v>1264231.5209391005</v>
+      </c>
+      <c r="CQ41" s="10">
+        <v>1363465.7767932732</v>
+      </c>
       <c r="CR41" s="11"/>
       <c r="CS41" s="11"/>
       <c r="CT41" s="11"/>
@@ -7306,9 +7343,11 @@
         <v>69193.996625832791</v>
       </c>
       <c r="CP42" s="10">
-        <v>50720.805813530118</v>
-      </c>
-      <c r="CQ42" s="11"/>
+        <v>50414.862948481554</v>
+      </c>
+      <c r="CQ42" s="10">
+        <v>44004.9556167056</v>
+      </c>
       <c r="CR42" s="11"/>
       <c r="CS42" s="11"/>
       <c r="CT42" s="11"/>
@@ -7649,9 +7688,11 @@
         <v>80450.489963046188</v>
       </c>
       <c r="CP43" s="10">
-        <v>52568.438469482084</v>
-      </c>
-      <c r="CQ43" s="11"/>
+        <v>53375.400374197467</v>
+      </c>
+      <c r="CQ43" s="10">
+        <v>40796.371071060545</v>
+      </c>
       <c r="CR43" s="11"/>
       <c r="CS43" s="11"/>
       <c r="CT43" s="11"/>
@@ -7992,9 +8033,11 @@
         <v>463595.72034765157</v>
       </c>
       <c r="CP44" s="10">
-        <v>441299.36415666755</v>
-      </c>
-      <c r="CQ44" s="11"/>
+        <v>441893.53214785649</v>
+      </c>
+      <c r="CQ44" s="10">
+        <v>553860.6279826106</v>
+      </c>
       <c r="CR44" s="11"/>
       <c r="CS44" s="11"/>
       <c r="CT44" s="11"/>
@@ -8335,9 +8378,11 @@
         <v>117589.60745430055</v>
       </c>
       <c r="CP45" s="10">
-        <v>92926.010044813185</v>
-      </c>
-      <c r="CQ45" s="11"/>
+        <v>93246.607320490031</v>
+      </c>
+      <c r="CQ45" s="10">
+        <v>89130.130115700318</v>
+      </c>
       <c r="CR45" s="11"/>
       <c r="CS45" s="11"/>
       <c r="CT45" s="11"/>
@@ -8678,9 +8723,11 @@
         <v>170571.3236135242</v>
       </c>
       <c r="CP46" s="10">
-        <v>162487.36802897765</v>
-      </c>
-      <c r="CQ46" s="11"/>
+        <v>163368.67540156987</v>
+      </c>
+      <c r="CQ46" s="10">
+        <v>137776.18394928213</v>
+      </c>
       <c r="CR46" s="11"/>
       <c r="CS46" s="11"/>
       <c r="CT46" s="11"/>
@@ -9021,9 +9068,11 @@
         <v>297223.06230146147</v>
       </c>
       <c r="CP47" s="10">
-        <v>357420.88236659684</v>
-      </c>
-      <c r="CQ47" s="11"/>
+        <v>357160.45426015649</v>
+      </c>
+      <c r="CQ47" s="10">
+        <v>308694.02552574786</v>
+      </c>
       <c r="CR47" s="11"/>
       <c r="CS47" s="11"/>
       <c r="CT47" s="11"/>
@@ -9364,9 +9413,11 @@
         <v>129857.71281263117</v>
       </c>
       <c r="CP48" s="10">
-        <v>120902.5534112626</v>
-      </c>
-      <c r="CQ48" s="11"/>
+        <v>121224.16136517162</v>
+      </c>
+      <c r="CQ48" s="10">
+        <v>130951.60152593734</v>
+      </c>
       <c r="CR48" s="11"/>
       <c r="CS48" s="11"/>
       <c r="CT48" s="11"/>
@@ -9707,9 +9758,11 @@
         <v>78882.706678140559</v>
       </c>
       <c r="CP49" s="10">
-        <v>69175.785647688186</v>
-      </c>
-      <c r="CQ49" s="11"/>
+        <v>70084.330215396738</v>
+      </c>
+      <c r="CQ49" s="10">
+        <v>49066.258476514893</v>
+      </c>
       <c r="CR49" s="11"/>
       <c r="CS49" s="11"/>
       <c r="CT49" s="11"/>
@@ -10050,9 +10103,11 @@
         <v>215143.7332874873</v>
       </c>
       <c r="CP50" s="10">
-        <v>209692.33830165802</v>
-      </c>
-      <c r="CQ50" s="11"/>
+        <v>210426.44791987777</v>
+      </c>
+      <c r="CQ50" s="10">
+        <v>187607.80648436726</v>
+      </c>
       <c r="CR50" s="11"/>
       <c r="CS50" s="11"/>
       <c r="CT50" s="11"/>
@@ -10393,9 +10448,11 @@
         <v>320329.20075240469</v>
       </c>
       <c r="CP51" s="10">
-        <v>350704.87869647751</v>
-      </c>
-      <c r="CQ51" s="11"/>
+        <v>351252.62070951628</v>
+      </c>
+      <c r="CQ51" s="10">
+        <v>207366.46693099246</v>
+      </c>
       <c r="CR51" s="11"/>
       <c r="CS51" s="11"/>
       <c r="CT51" s="11"/>
@@ -10736,9 +10793,11 @@
         <v>638740.87639105879</v>
       </c>
       <c r="CP52" s="10">
-        <v>518109.67157395935</v>
-      </c>
-      <c r="CQ52" s="11"/>
+        <v>518312.68529937207</v>
+      </c>
+      <c r="CQ52" s="10">
+        <v>471235.84364824608</v>
+      </c>
       <c r="CR52" s="11"/>
       <c r="CS52" s="11"/>
       <c r="CT52" s="11"/>
@@ -11196,46 +11255,48 @@
       <c r="CC54" s="15">
         <v>3935758.6177309696</v>
       </c>
-      <c r="CD54" s="31">
+      <c r="CD54" s="30">
         <v>3314612.1320124432</v>
       </c>
-      <c r="CE54" s="31">
+      <c r="CE54" s="30">
         <v>2917736.7328303363</v>
       </c>
-      <c r="CF54" s="31">
+      <c r="CF54" s="30">
         <v>3030086.4136792915</v>
       </c>
-      <c r="CG54" s="31">
+      <c r="CG54" s="30">
         <v>3648921.6749099772</v>
       </c>
-      <c r="CH54" s="31">
+      <c r="CH54" s="30">
         <v>3156809.3523885403</v>
       </c>
-      <c r="CI54" s="31">
+      <c r="CI54" s="30">
         <v>3130131.1633264814</v>
       </c>
-      <c r="CJ54" s="31">
+      <c r="CJ54" s="30">
         <v>3245552.8170434618</v>
       </c>
-      <c r="CK54" s="31">
+      <c r="CK54" s="30">
         <v>3922623.7313984605</v>
       </c>
-      <c r="CL54" s="31">
+      <c r="CL54" s="30">
         <v>3471756.5527950469</v>
       </c>
-      <c r="CM54" s="31">
+      <c r="CM54" s="30">
         <v>3396881.5167516316</v>
       </c>
-      <c r="CN54" s="31">
+      <c r="CN54" s="30">
         <v>3505506.6774791162</v>
       </c>
-      <c r="CO54" s="31">
+      <c r="CO54" s="30">
         <v>4196072.3544278946</v>
       </c>
-      <c r="CP54" s="31">
-        <v>3691935.3735019211</v>
-      </c>
-      <c r="CQ54" s="11"/>
+      <c r="CP54" s="30">
+        <v>3694991.2989011863</v>
+      </c>
+      <c r="CQ54" s="30">
+        <v>3583956.0481204381</v>
+      </c>
       <c r="CR54" s="11"/>
       <c r="CS54" s="11"/>
       <c r="CT54" s="11"/>
@@ -11390,6 +11451,7 @@
       <c r="CN55" s="16"/>
       <c r="CO55" s="16"/>
       <c r="CP55" s="16"/>
+      <c r="CQ55" s="16"/>
     </row>
     <row r="56" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
@@ -11631,20 +11693,20 @@
       <c r="CA58" s="24"/>
       <c r="CB58" s="24"/>
       <c r="CC58" s="24"/>
-      <c r="CD58" s="33"/>
-      <c r="CE58" s="33"/>
-      <c r="CF58" s="33"/>
-      <c r="CG58" s="33"/>
-      <c r="CH58" s="33"/>
-      <c r="CI58" s="33"/>
-      <c r="CJ58" s="33"/>
-      <c r="CK58" s="33"/>
-      <c r="CL58" s="33"/>
-      <c r="CM58" s="33"/>
-      <c r="CN58" s="33"/>
-      <c r="CO58" s="33"/>
-      <c r="CP58" s="33"/>
-      <c r="CQ58" s="11"/>
+      <c r="CD58" s="32"/>
+      <c r="CE58" s="32"/>
+      <c r="CF58" s="32"/>
+      <c r="CG58" s="32"/>
+      <c r="CH58" s="32"/>
+      <c r="CI58" s="32"/>
+      <c r="CJ58" s="32"/>
+      <c r="CK58" s="32"/>
+      <c r="CL58" s="32"/>
+      <c r="CM58" s="32"/>
+      <c r="CN58" s="32"/>
+      <c r="CO58" s="32"/>
+      <c r="CP58" s="32"/>
+      <c r="CQ58" s="32"/>
       <c r="CR58" s="11"/>
       <c r="CS58" s="11"/>
       <c r="CT58" s="11"/>
@@ -11736,108 +11798,108 @@
     </row>
     <row r="67" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35" t="s">
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35" t="s">
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K67" s="35"/>
-      <c r="L67" s="35"/>
-      <c r="M67" s="35"/>
-      <c r="N67" s="35" t="s">
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="O67" s="35"/>
-      <c r="P67" s="35"/>
-      <c r="Q67" s="35"/>
-      <c r="R67" s="35" t="s">
+      <c r="O67" s="33"/>
+      <c r="P67" s="33"/>
+      <c r="Q67" s="33"/>
+      <c r="R67" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="S67" s="35"/>
-      <c r="T67" s="35"/>
-      <c r="U67" s="35"/>
-      <c r="V67" s="35" t="s">
+      <c r="S67" s="33"/>
+      <c r="T67" s="33"/>
+      <c r="U67" s="33"/>
+      <c r="V67" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="W67" s="35"/>
-      <c r="X67" s="35"/>
-      <c r="Y67" s="35"/>
-      <c r="Z67" s="35" t="s">
+      <c r="W67" s="33"/>
+      <c r="X67" s="33"/>
+      <c r="Y67" s="33"/>
+      <c r="Z67" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AA67" s="35"/>
-      <c r="AB67" s="35"/>
-      <c r="AC67" s="35"/>
-      <c r="AD67" s="35" t="s">
+      <c r="AA67" s="33"/>
+      <c r="AB67" s="33"/>
+      <c r="AC67" s="33"/>
+      <c r="AD67" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="AE67" s="35"/>
-      <c r="AF67" s="35"/>
-      <c r="AG67" s="35"/>
-      <c r="AH67" s="35" t="s">
+      <c r="AE67" s="33"/>
+      <c r="AF67" s="33"/>
+      <c r="AG67" s="33"/>
+      <c r="AH67" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="AI67" s="35"/>
-      <c r="AJ67" s="35"/>
-      <c r="AK67" s="35"/>
-      <c r="AL67" s="35" t="s">
+      <c r="AI67" s="33"/>
+      <c r="AJ67" s="33"/>
+      <c r="AK67" s="33"/>
+      <c r="AL67" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="AM67" s="35"/>
-      <c r="AN67" s="35"/>
-      <c r="AO67" s="35"/>
-      <c r="AP67" s="35" t="s">
+      <c r="AM67" s="33"/>
+      <c r="AN67" s="33"/>
+      <c r="AO67" s="33"/>
+      <c r="AP67" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="AQ67" s="35"/>
-      <c r="AR67" s="35"/>
-      <c r="AS67" s="35"/>
-      <c r="AT67" s="35" t="s">
+      <c r="AQ67" s="33"/>
+      <c r="AR67" s="33"/>
+      <c r="AS67" s="33"/>
+      <c r="AT67" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AU67" s="35"/>
-      <c r="AV67" s="35"/>
-      <c r="AW67" s="35"/>
-      <c r="AX67" s="35" t="s">
+      <c r="AU67" s="33"/>
+      <c r="AV67" s="33"/>
+      <c r="AW67" s="33"/>
+      <c r="AX67" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="AY67" s="35"/>
-      <c r="AZ67" s="35"/>
-      <c r="BA67" s="35"/>
-      <c r="BB67" s="35" t="s">
+      <c r="AY67" s="33"/>
+      <c r="AZ67" s="33"/>
+      <c r="BA67" s="33"/>
+      <c r="BB67" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="BC67" s="35"/>
-      <c r="BD67" s="35"/>
-      <c r="BE67" s="35"/>
-      <c r="BF67" s="35" t="s">
+      <c r="BC67" s="33"/>
+      <c r="BD67" s="33"/>
+      <c r="BE67" s="33"/>
+      <c r="BF67" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="BG67" s="35"/>
-      <c r="BH67" s="35"/>
-      <c r="BI67" s="35"/>
-      <c r="BJ67" s="35" t="s">
+      <c r="BG67" s="33"/>
+      <c r="BH67" s="33"/>
+      <c r="BI67" s="33"/>
+      <c r="BJ67" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="BK67" s="35"/>
-      <c r="BL67" s="35"/>
-      <c r="BM67" s="35"/>
-      <c r="BN67" s="35" t="s">
+      <c r="BK67" s="33"/>
+      <c r="BL67" s="33"/>
+      <c r="BM67" s="33"/>
+      <c r="BN67" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="BO67" s="35"/>
-      <c r="BP67" s="35"/>
-      <c r="BQ67" s="35"/>
+      <c r="BO67" s="33"/>
+      <c r="BP67" s="33"/>
+      <c r="BQ67" s="33"/>
       <c r="BR67" s="34" t="s">
         <v>34</v>
       </c>
@@ -11868,13 +11930,14 @@
       <c r="CI67" s="34"/>
       <c r="CJ67" s="34"/>
       <c r="CK67" s="34"/>
-      <c r="CL67" s="30" t="s">
+      <c r="CL67" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="CM67" s="30"/>
-      <c r="CN67" s="30"/>
-      <c r="CO67" s="30"/>
-      <c r="CP67" s="30"/>
+      <c r="CM67" s="34"/>
+      <c r="CN67" s="34"/>
+      <c r="CO67" s="34"/>
+      <c r="CP67" s="34"/>
+      <c r="CQ67" s="35"/>
     </row>
     <row r="68" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
@@ -12147,10 +12210,13 @@
       <c r="CL68" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="CM68" s="7"/>
+      <c r="CM68" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="CN68" s="7"/>
       <c r="CO68" s="7"/>
       <c r="CP68" s="7"/>
+      <c r="CQ68" s="7"/>
     </row>
     <row r="69" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
@@ -12424,13 +12490,15 @@
         <v>14.230451250859005</v>
       </c>
       <c r="CL70" s="26">
-        <v>11.100941746754089</v>
-      </c>
-      <c r="CM70" s="26"/>
+        <v>10.952117957471913</v>
+      </c>
+      <c r="CM70" s="26">
+        <v>7.8199556815264089</v>
+      </c>
       <c r="CN70" s="26"/>
       <c r="CO70" s="26"/>
       <c r="CP70" s="26"/>
-      <c r="CQ70" s="11"/>
+      <c r="CQ70" s="26"/>
       <c r="CR70" s="11"/>
       <c r="CS70" s="11"/>
       <c r="CT70" s="11"/>
@@ -12755,13 +12823,15 @@
         <v>14.879767765446744</v>
       </c>
       <c r="CL71" s="26">
-        <v>11.774547348526255</v>
-      </c>
-      <c r="CM71" s="26"/>
+        <v>11.100334376022715</v>
+      </c>
+      <c r="CM71" s="26">
+        <v>1.984713329214415</v>
+      </c>
       <c r="CN71" s="26"/>
       <c r="CO71" s="26"/>
       <c r="CP71" s="26"/>
-      <c r="CQ71" s="11"/>
+      <c r="CQ71" s="26"/>
       <c r="CR71" s="11"/>
       <c r="CS71" s="11"/>
       <c r="CT71" s="11"/>
@@ -13086,13 +13156,15 @@
         <v>14.085116924879742</v>
       </c>
       <c r="CL72" s="26">
-        <v>0.69553047416124514</v>
-      </c>
-      <c r="CM72" s="26"/>
+        <v>2.2412765422117076</v>
+      </c>
+      <c r="CM72" s="26">
+        <v>-23.592930158396769</v>
+      </c>
       <c r="CN72" s="26"/>
       <c r="CO72" s="26"/>
       <c r="CP72" s="26"/>
-      <c r="CQ72" s="11"/>
+      <c r="CQ72" s="26"/>
       <c r="CR72" s="11"/>
       <c r="CS72" s="11"/>
       <c r="CT72" s="11"/>
@@ -13417,13 +13489,15 @@
         <v>11.921201320286116</v>
       </c>
       <c r="CL73" s="26">
-        <v>12.28702678557238</v>
-      </c>
-      <c r="CM73" s="26"/>
+        <v>12.438210681495889</v>
+      </c>
+      <c r="CM73" s="26">
+        <v>12.636766068427875</v>
+      </c>
       <c r="CN73" s="26"/>
       <c r="CO73" s="26"/>
       <c r="CP73" s="26"/>
-      <c r="CQ73" s="11"/>
+      <c r="CQ73" s="26"/>
       <c r="CR73" s="11"/>
       <c r="CS73" s="11"/>
       <c r="CT73" s="11"/>
@@ -13748,13 +13822,15 @@
         <v>14.127928224150992</v>
       </c>
       <c r="CL74" s="26">
-        <v>2.5539136197363774</v>
-      </c>
-      <c r="CM74" s="26"/>
+        <v>2.9077274260176296</v>
+      </c>
+      <c r="CM74" s="26">
+        <v>3.2294590743144056</v>
+      </c>
       <c r="CN74" s="26"/>
       <c r="CO74" s="26"/>
       <c r="CP74" s="26"/>
-      <c r="CQ74" s="11"/>
+      <c r="CQ74" s="26"/>
       <c r="CR74" s="11"/>
       <c r="CS74" s="11"/>
       <c r="CT74" s="11"/>
@@ -14079,13 +14155,15 @@
         <v>8.2225014081690233</v>
       </c>
       <c r="CL75" s="26">
-        <v>11.235877389531382</v>
-      </c>
-      <c r="CM75" s="26"/>
+        <v>11.839204282134361</v>
+      </c>
+      <c r="CM75" s="26">
+        <v>13.06079368861927</v>
+      </c>
       <c r="CN75" s="26"/>
       <c r="CO75" s="26"/>
       <c r="CP75" s="26"/>
-      <c r="CQ75" s="11"/>
+      <c r="CQ75" s="26"/>
       <c r="CR75" s="11"/>
       <c r="CS75" s="11"/>
       <c r="CT75" s="11"/>
@@ -14410,13 +14488,15 @@
         <v>20.962940351693334</v>
       </c>
       <c r="CL76" s="26">
-        <v>24.01244022729054</v>
-      </c>
-      <c r="CM76" s="26"/>
+        <v>23.922080859450617</v>
+      </c>
+      <c r="CM76" s="26">
+        <v>29.643917481861763</v>
+      </c>
       <c r="CN76" s="26"/>
       <c r="CO76" s="26"/>
       <c r="CP76" s="26"/>
-      <c r="CQ76" s="11"/>
+      <c r="CQ76" s="26"/>
       <c r="CR76" s="11"/>
       <c r="CS76" s="11"/>
       <c r="CT76" s="11"/>
@@ -14741,13 +14821,15 @@
         <v>6.6924732388451673</v>
       </c>
       <c r="CL77" s="26">
-        <v>5.3987829377145573</v>
-      </c>
-      <c r="CM77" s="26"/>
+        <v>5.6791499437760109</v>
+      </c>
+      <c r="CM77" s="26">
+        <v>5.7492260133699062</v>
+      </c>
       <c r="CN77" s="26"/>
       <c r="CO77" s="26"/>
       <c r="CP77" s="26"/>
-      <c r="CQ77" s="11"/>
+      <c r="CQ77" s="26"/>
       <c r="CR77" s="11"/>
       <c r="CS77" s="11"/>
       <c r="CT77" s="11"/>
@@ -15072,13 +15154,15 @@
         <v>19.43592958964993</v>
       </c>
       <c r="CL78" s="26">
-        <v>33.748171644300612</v>
-      </c>
-      <c r="CM78" s="26"/>
+        <v>35.504800407539534</v>
+      </c>
+      <c r="CM78" s="26">
+        <v>25.812468153670665</v>
+      </c>
       <c r="CN78" s="26"/>
       <c r="CO78" s="26"/>
       <c r="CP78" s="26"/>
-      <c r="CQ78" s="11"/>
+      <c r="CQ78" s="26"/>
       <c r="CR78" s="11"/>
       <c r="CS78" s="11"/>
       <c r="CT78" s="11"/>
@@ -15403,13 +15487,15 @@
         <v>14.183716365607538</v>
       </c>
       <c r="CL79" s="26">
-        <v>10.116023254301069</v>
-      </c>
-      <c r="CM79" s="26"/>
+        <v>10.501527238117617</v>
+      </c>
+      <c r="CM79" s="26">
+        <v>10.875820548340712</v>
+      </c>
       <c r="CN79" s="26"/>
       <c r="CO79" s="26"/>
       <c r="CP79" s="26"/>
-      <c r="CQ79" s="11"/>
+      <c r="CQ79" s="26"/>
       <c r="CR79" s="11"/>
       <c r="CS79" s="11"/>
       <c r="CT79" s="11"/>
@@ -15734,13 +15820,15 @@
         <v>32.771002893752922</v>
       </c>
       <c r="CL80" s="26">
-        <v>33.75672181980184</v>
-      </c>
-      <c r="CM80" s="26"/>
+        <v>33.965627314186065</v>
+      </c>
+      <c r="CM80" s="26">
+        <v>33.620865500350476</v>
+      </c>
       <c r="CN80" s="26"/>
       <c r="CO80" s="26"/>
       <c r="CP80" s="26"/>
-      <c r="CQ80" s="11"/>
+      <c r="CQ80" s="26"/>
       <c r="CR80" s="11"/>
       <c r="CS80" s="11"/>
       <c r="CT80" s="11"/>
@@ -16065,13 +16153,15 @@
         <v>11.443585383216643</v>
       </c>
       <c r="CL81" s="26">
-        <v>14.794359879300913</v>
-      </c>
-      <c r="CM81" s="26"/>
+        <v>14.839340376547128</v>
+      </c>
+      <c r="CM81" s="26">
+        <v>11.217691884866184</v>
+      </c>
       <c r="CN81" s="26"/>
       <c r="CO81" s="26"/>
       <c r="CP81" s="26"/>
-      <c r="CQ81" s="11"/>
+      <c r="CQ81" s="26"/>
       <c r="CR81" s="11"/>
       <c r="CS81" s="11"/>
       <c r="CT81" s="11"/>
@@ -16546,13 +16636,15 @@
         <v>14.90946448783501</v>
       </c>
       <c r="CL83" s="26">
-        <v>14.623240348397886</v>
-      </c>
-      <c r="CM83" s="26"/>
+        <v>14.703382016307259</v>
+      </c>
+      <c r="CM83" s="26">
+        <v>11.573295727077706</v>
+      </c>
       <c r="CN83" s="26"/>
       <c r="CO83" s="26"/>
       <c r="CP83" s="26"/>
-      <c r="CQ83" s="11"/>
+      <c r="CQ83" s="26"/>
       <c r="CR83" s="11"/>
       <c r="CS83" s="11"/>
       <c r="CT83" s="11"/>
@@ -16703,6 +16795,7 @@
       <c r="CN84" s="16"/>
       <c r="CO84" s="16"/>
       <c r="CP84" s="16"/>
+      <c r="CQ84" s="16"/>
     </row>
     <row r="85" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
@@ -17041,108 +17134,108 @@
     </row>
     <row r="96" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
-      <c r="B96" s="35" t="s">
+      <c r="B96" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C96" s="35"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="35"/>
-      <c r="F96" s="35" t="s">
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G96" s="35"/>
-      <c r="H96" s="35"/>
-      <c r="I96" s="35"/>
-      <c r="J96" s="35" t="s">
+      <c r="G96" s="33"/>
+      <c r="H96" s="33"/>
+      <c r="I96" s="33"/>
+      <c r="J96" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K96" s="35"/>
-      <c r="L96" s="35"/>
-      <c r="M96" s="35"/>
-      <c r="N96" s="35" t="s">
+      <c r="K96" s="33"/>
+      <c r="L96" s="33"/>
+      <c r="M96" s="33"/>
+      <c r="N96" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="O96" s="35"/>
-      <c r="P96" s="35"/>
-      <c r="Q96" s="35"/>
-      <c r="R96" s="35" t="s">
+      <c r="O96" s="33"/>
+      <c r="P96" s="33"/>
+      <c r="Q96" s="33"/>
+      <c r="R96" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="S96" s="35"/>
-      <c r="T96" s="35"/>
-      <c r="U96" s="35"/>
-      <c r="V96" s="35" t="s">
+      <c r="S96" s="33"/>
+      <c r="T96" s="33"/>
+      <c r="U96" s="33"/>
+      <c r="V96" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="W96" s="35"/>
-      <c r="X96" s="35"/>
-      <c r="Y96" s="35"/>
-      <c r="Z96" s="35" t="s">
+      <c r="W96" s="33"/>
+      <c r="X96" s="33"/>
+      <c r="Y96" s="33"/>
+      <c r="Z96" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AA96" s="35"/>
-      <c r="AB96" s="35"/>
-      <c r="AC96" s="35"/>
-      <c r="AD96" s="35" t="s">
+      <c r="AA96" s="33"/>
+      <c r="AB96" s="33"/>
+      <c r="AC96" s="33"/>
+      <c r="AD96" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="AE96" s="35"/>
-      <c r="AF96" s="35"/>
-      <c r="AG96" s="35"/>
-      <c r="AH96" s="35" t="s">
+      <c r="AE96" s="33"/>
+      <c r="AF96" s="33"/>
+      <c r="AG96" s="33"/>
+      <c r="AH96" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="AI96" s="35"/>
-      <c r="AJ96" s="35"/>
-      <c r="AK96" s="35"/>
-      <c r="AL96" s="35" t="s">
+      <c r="AI96" s="33"/>
+      <c r="AJ96" s="33"/>
+      <c r="AK96" s="33"/>
+      <c r="AL96" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="AM96" s="35"/>
-      <c r="AN96" s="35"/>
-      <c r="AO96" s="35"/>
-      <c r="AP96" s="35" t="s">
+      <c r="AM96" s="33"/>
+      <c r="AN96" s="33"/>
+      <c r="AO96" s="33"/>
+      <c r="AP96" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="AQ96" s="35"/>
-      <c r="AR96" s="35"/>
-      <c r="AS96" s="35"/>
-      <c r="AT96" s="35" t="s">
+      <c r="AQ96" s="33"/>
+      <c r="AR96" s="33"/>
+      <c r="AS96" s="33"/>
+      <c r="AT96" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AU96" s="35"/>
-      <c r="AV96" s="35"/>
-      <c r="AW96" s="35"/>
-      <c r="AX96" s="35" t="s">
+      <c r="AU96" s="33"/>
+      <c r="AV96" s="33"/>
+      <c r="AW96" s="33"/>
+      <c r="AX96" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="AY96" s="35"/>
-      <c r="AZ96" s="35"/>
-      <c r="BA96" s="35"/>
-      <c r="BB96" s="35" t="s">
+      <c r="AY96" s="33"/>
+      <c r="AZ96" s="33"/>
+      <c r="BA96" s="33"/>
+      <c r="BB96" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="BC96" s="35"/>
-      <c r="BD96" s="35"/>
-      <c r="BE96" s="35"/>
-      <c r="BF96" s="35" t="s">
+      <c r="BC96" s="33"/>
+      <c r="BD96" s="33"/>
+      <c r="BE96" s="33"/>
+      <c r="BF96" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="BG96" s="35"/>
-      <c r="BH96" s="35"/>
-      <c r="BI96" s="35"/>
-      <c r="BJ96" s="35" t="s">
+      <c r="BG96" s="33"/>
+      <c r="BH96" s="33"/>
+      <c r="BI96" s="33"/>
+      <c r="BJ96" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="BK96" s="35"/>
-      <c r="BL96" s="35"/>
-      <c r="BM96" s="35"/>
-      <c r="BN96" s="35" t="s">
+      <c r="BK96" s="33"/>
+      <c r="BL96" s="33"/>
+      <c r="BM96" s="33"/>
+      <c r="BN96" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="BO96" s="35"/>
-      <c r="BP96" s="35"/>
-      <c r="BQ96" s="35"/>
+      <c r="BO96" s="33"/>
+      <c r="BP96" s="33"/>
+      <c r="BQ96" s="33"/>
       <c r="BR96" s="34" t="s">
         <v>34</v>
       </c>
@@ -17173,13 +17266,16 @@
       <c r="CI96" s="34"/>
       <c r="CJ96" s="34"/>
       <c r="CK96" s="34"/>
-      <c r="CL96" s="30" t="s">
+      <c r="CL96" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="CM96" s="30"/>
-      <c r="CN96" s="30"/>
-      <c r="CO96" s="30"/>
-      <c r="CP96" s="30"/>
+      <c r="CM96" s="34">
+        <v>0</v>
+      </c>
+      <c r="CN96" s="34"/>
+      <c r="CO96" s="34"/>
+      <c r="CP96" s="34"/>
+      <c r="CQ96" s="35"/>
     </row>
     <row r="97" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
@@ -17452,10 +17548,13 @@
       <c r="CL97" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="CM97" s="7"/>
+      <c r="CM97" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="CN97" s="7"/>
       <c r="CO97" s="7"/>
       <c r="CP97" s="7"/>
+      <c r="CQ97" s="7"/>
     </row>
     <row r="98" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
@@ -17729,13 +17828,15 @@
         <v>3.9785935809430555</v>
       </c>
       <c r="CL99" s="26">
-        <v>0.77992528418768359</v>
-      </c>
-      <c r="CM99" s="26"/>
+        <v>0.64492687527631176</v>
+      </c>
+      <c r="CM99" s="26">
+        <v>0.43502721018897716</v>
+      </c>
       <c r="CN99" s="26"/>
       <c r="CO99" s="26"/>
       <c r="CP99" s="26"/>
-      <c r="CQ99" s="11"/>
+      <c r="CQ99" s="26"/>
       <c r="CR99" s="11"/>
       <c r="CS99" s="11"/>
       <c r="CT99" s="11"/>
@@ -18060,13 +18161,15 @@
         <v>3.9147385367330259</v>
       </c>
       <c r="CL100" s="26">
-        <v>0.33161662079015741</v>
-      </c>
-      <c r="CM100" s="26"/>
+        <v>-0.27357372963069793</v>
+      </c>
+      <c r="CM100" s="26">
+        <v>-9.110613538984552</v>
+      </c>
       <c r="CN100" s="26"/>
       <c r="CO100" s="26"/>
       <c r="CP100" s="26"/>
-      <c r="CQ100" s="11"/>
+      <c r="CQ100" s="26"/>
       <c r="CR100" s="11"/>
       <c r="CS100" s="11"/>
       <c r="CT100" s="11"/>
@@ -18391,13 +18494,15 @@
         <v>10.193524067478094</v>
       </c>
       <c r="CL101" s="26">
-        <v>-3.8384354359466784</v>
-      </c>
-      <c r="CM101" s="26"/>
+        <v>-2.3622888818490395</v>
+      </c>
+      <c r="CM101" s="26">
+        <v>-27.308707870553945</v>
+      </c>
       <c r="CN101" s="26"/>
       <c r="CO101" s="26"/>
       <c r="CP101" s="26"/>
-      <c r="CQ101" s="11"/>
+      <c r="CQ101" s="26"/>
       <c r="CR101" s="11"/>
       <c r="CS101" s="11"/>
       <c r="CT101" s="11"/>
@@ -18722,13 +18827,15 @@
         <v>4.4963740045475049</v>
       </c>
       <c r="CL102" s="26">
-        <v>3.7369328662439187</v>
-      </c>
-      <c r="CM102" s="26"/>
+        <v>3.8766048667486785</v>
+      </c>
+      <c r="CM102" s="26">
+        <v>6.0818572755786846</v>
+      </c>
       <c r="CN102" s="26"/>
       <c r="CO102" s="26"/>
       <c r="CP102" s="26"/>
-      <c r="CQ102" s="11"/>
+      <c r="CQ102" s="26"/>
       <c r="CR102" s="11"/>
       <c r="CS102" s="11"/>
       <c r="CT102" s="11"/>
@@ -19053,13 +19160,15 @@
         <v>9.3573074302153856</v>
       </c>
       <c r="CL103" s="26">
-        <v>-3.1028183975854517</v>
-      </c>
-      <c r="CM103" s="26"/>
+        <v>-2.768520471444873</v>
+      </c>
+      <c r="CM103" s="26">
+        <v>-2.7227200243741549</v>
+      </c>
       <c r="CN103" s="26"/>
       <c r="CO103" s="26"/>
       <c r="CP103" s="26"/>
-      <c r="CQ103" s="11"/>
+      <c r="CQ103" s="26"/>
       <c r="CR103" s="11"/>
       <c r="CS103" s="11"/>
       <c r="CT103" s="11"/>
@@ -19384,13 +19493,15 @@
         <v>5.2490153935198265</v>
       </c>
       <c r="CL104" s="26">
-        <v>7.2205947313644288</v>
-      </c>
-      <c r="CM104" s="26"/>
+        <v>7.8021433266596745</v>
+      </c>
+      <c r="CM104" s="26">
+        <v>8.6648635284183939</v>
+      </c>
       <c r="CN104" s="26"/>
       <c r="CO104" s="26"/>
       <c r="CP104" s="26"/>
-      <c r="CQ104" s="11"/>
+      <c r="CQ104" s="26"/>
       <c r="CR104" s="11"/>
       <c r="CS104" s="11"/>
       <c r="CT104" s="11"/>
@@ -19715,13 +19826,15 @@
         <v>7.8682121727108552</v>
       </c>
       <c r="CL105" s="26">
-        <v>14.418722341660555</v>
-      </c>
-      <c r="CM105" s="26"/>
+        <v>14.335353258680669</v>
+      </c>
+      <c r="CM105" s="26">
+        <v>30.085229586408559</v>
+      </c>
       <c r="CN105" s="26"/>
       <c r="CO105" s="26"/>
       <c r="CP105" s="26"/>
-      <c r="CQ105" s="11"/>
+      <c r="CQ105" s="26"/>
       <c r="CR105" s="11"/>
       <c r="CS105" s="11"/>
       <c r="CT105" s="11"/>
@@ -20046,13 +20159,15 @@
         <v>6.0323765304316055</v>
       </c>
       <c r="CL106" s="26">
-        <v>4.6459344881594831</v>
-      </c>
-      <c r="CM106" s="26"/>
+        <v>4.9242988727490626</v>
+      </c>
+      <c r="CM106" s="26">
+        <v>5.02844258387276</v>
+      </c>
       <c r="CN106" s="26"/>
       <c r="CO106" s="26"/>
       <c r="CP106" s="26"/>
-      <c r="CQ106" s="11"/>
+      <c r="CQ106" s="26"/>
       <c r="CR106" s="11"/>
       <c r="CS106" s="11"/>
       <c r="CT106" s="11"/>
@@ -20377,13 +20492,15 @@
         <v>15.49125668577156</v>
       </c>
       <c r="CL107" s="26">
-        <v>28.103087523045843</v>
-      </c>
-      <c r="CM107" s="26"/>
+        <v>29.785574583887012</v>
+      </c>
+      <c r="CM107" s="26">
+        <v>20.059537003786716</v>
+      </c>
       <c r="CN107" s="26"/>
       <c r="CO107" s="26"/>
       <c r="CP107" s="26"/>
-      <c r="CQ107" s="11"/>
+      <c r="CQ107" s="26"/>
       <c r="CR107" s="11"/>
       <c r="CS107" s="11"/>
       <c r="CT107" s="11"/>
@@ -20708,13 +20825,15 @@
         <v>10.278242718539033</v>
       </c>
       <c r="CL108" s="26">
-        <v>6.254040424339081</v>
-      </c>
-      <c r="CM108" s="26"/>
+        <v>6.6260240346224748</v>
+      </c>
+      <c r="CM108" s="26">
+        <v>6.9871901514114683</v>
+      </c>
       <c r="CN108" s="26"/>
       <c r="CO108" s="26"/>
       <c r="CP108" s="26"/>
-      <c r="CQ108" s="11"/>
+      <c r="CQ108" s="26"/>
       <c r="CR108" s="11"/>
       <c r="CS108" s="11"/>
       <c r="CT108" s="11"/>
@@ -21039,13 +21158,15 @@
         <v>24.779108341374851</v>
       </c>
       <c r="CL109" s="26">
-        <v>23.833675216332239</v>
-      </c>
-      <c r="CM109" s="26"/>
+        <v>24.027082581513739</v>
+      </c>
+      <c r="CM109" s="26">
+        <v>23.302934484167892</v>
+      </c>
       <c r="CN109" s="26"/>
       <c r="CO109" s="26"/>
       <c r="CP109" s="26"/>
-      <c r="CQ109" s="11"/>
+      <c r="CQ109" s="26"/>
       <c r="CR109" s="11"/>
       <c r="CS109" s="11"/>
       <c r="CT109" s="11"/>
@@ -21370,13 +21491,15 @@
         <v>6.6439501425235221</v>
       </c>
       <c r="CL110" s="26">
-        <v>9.0559330265029558</v>
-      </c>
-      <c r="CM110" s="26"/>
+        <v>9.0986650048017168</v>
+      </c>
+      <c r="CM110" s="26">
+        <v>5.2153121611257234</v>
+      </c>
       <c r="CN110" s="26"/>
       <c r="CO110" s="26"/>
       <c r="CP110" s="26"/>
-      <c r="CQ110" s="11"/>
+      <c r="CQ110" s="26"/>
       <c r="CR110" s="11"/>
       <c r="CS110" s="11"/>
       <c r="CT110" s="11"/>
@@ -21851,13 +21974,15 @@
         <v>6.971064311894807</v>
       </c>
       <c r="CL112" s="26">
-        <v>6.3420005797817822</v>
-      </c>
-      <c r="CM112" s="26"/>
+        <v>6.4300230362182873</v>
+      </c>
+      <c r="CM112" s="26">
+        <v>5.5072433479429037</v>
+      </c>
       <c r="CN112" s="26"/>
       <c r="CO112" s="26"/>
       <c r="CP112" s="26"/>
-      <c r="CQ112" s="11"/>
+      <c r="CQ112" s="26"/>
       <c r="CR112" s="11"/>
       <c r="CS112" s="11"/>
       <c r="CT112" s="11"/>
@@ -22008,6 +22133,7 @@
       <c r="CN113" s="16"/>
       <c r="CO113" s="16"/>
       <c r="CP113" s="16"/>
+      <c r="CQ113" s="16"/>
     </row>
     <row r="114" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
@@ -22341,108 +22467,108 @@
     </row>
     <row r="124" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
-      <c r="B124" s="35">
+      <c r="B124" s="33">
         <v>2000</v>
       </c>
-      <c r="C124" s="35"/>
-      <c r="D124" s="35"/>
-      <c r="E124" s="35"/>
-      <c r="F124" s="35">
+      <c r="C124" s="33"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="33"/>
+      <c r="F124" s="33">
         <v>2001</v>
       </c>
-      <c r="G124" s="35"/>
-      <c r="H124" s="35"/>
-      <c r="I124" s="35"/>
-      <c r="J124" s="35">
+      <c r="G124" s="33"/>
+      <c r="H124" s="33"/>
+      <c r="I124" s="33"/>
+      <c r="J124" s="33">
         <v>2002</v>
       </c>
-      <c r="K124" s="35"/>
-      <c r="L124" s="35"/>
-      <c r="M124" s="35"/>
-      <c r="N124" s="35">
+      <c r="K124" s="33"/>
+      <c r="L124" s="33"/>
+      <c r="M124" s="33"/>
+      <c r="N124" s="33">
         <v>2003</v>
       </c>
-      <c r="O124" s="35"/>
-      <c r="P124" s="35"/>
-      <c r="Q124" s="35"/>
-      <c r="R124" s="35">
+      <c r="O124" s="33"/>
+      <c r="P124" s="33"/>
+      <c r="Q124" s="33"/>
+      <c r="R124" s="33">
         <v>2004</v>
       </c>
-      <c r="S124" s="35"/>
-      <c r="T124" s="35"/>
-      <c r="U124" s="35"/>
-      <c r="V124" s="35">
+      <c r="S124" s="33"/>
+      <c r="T124" s="33"/>
+      <c r="U124" s="33"/>
+      <c r="V124" s="33">
         <v>2005</v>
       </c>
-      <c r="W124" s="35"/>
-      <c r="X124" s="35"/>
-      <c r="Y124" s="35"/>
-      <c r="Z124" s="35">
+      <c r="W124" s="33"/>
+      <c r="X124" s="33"/>
+      <c r="Y124" s="33"/>
+      <c r="Z124" s="33">
         <v>2006</v>
       </c>
-      <c r="AA124" s="35"/>
-      <c r="AB124" s="35"/>
-      <c r="AC124" s="35"/>
-      <c r="AD124" s="35">
+      <c r="AA124" s="33"/>
+      <c r="AB124" s="33"/>
+      <c r="AC124" s="33"/>
+      <c r="AD124" s="33">
         <v>2007</v>
       </c>
-      <c r="AE124" s="35"/>
-      <c r="AF124" s="35"/>
-      <c r="AG124" s="35"/>
-      <c r="AH124" s="35">
+      <c r="AE124" s="33"/>
+      <c r="AF124" s="33"/>
+      <c r="AG124" s="33"/>
+      <c r="AH124" s="33">
         <v>2008</v>
       </c>
-      <c r="AI124" s="35"/>
-      <c r="AJ124" s="35"/>
-      <c r="AK124" s="35"/>
-      <c r="AL124" s="35">
+      <c r="AI124" s="33"/>
+      <c r="AJ124" s="33"/>
+      <c r="AK124" s="33"/>
+      <c r="AL124" s="33">
         <v>2009</v>
       </c>
-      <c r="AM124" s="35"/>
-      <c r="AN124" s="35"/>
-      <c r="AO124" s="35"/>
-      <c r="AP124" s="35">
+      <c r="AM124" s="33"/>
+      <c r="AN124" s="33"/>
+      <c r="AO124" s="33"/>
+      <c r="AP124" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ124" s="35"/>
-      <c r="AR124" s="35"/>
-      <c r="AS124" s="35"/>
-      <c r="AT124" s="35">
+      <c r="AQ124" s="33"/>
+      <c r="AR124" s="33"/>
+      <c r="AS124" s="33"/>
+      <c r="AT124" s="33">
         <v>2011</v>
       </c>
-      <c r="AU124" s="35"/>
-      <c r="AV124" s="35"/>
-      <c r="AW124" s="35"/>
-      <c r="AX124" s="35">
+      <c r="AU124" s="33"/>
+      <c r="AV124" s="33"/>
+      <c r="AW124" s="33"/>
+      <c r="AX124" s="33">
         <v>2012</v>
       </c>
-      <c r="AY124" s="35"/>
-      <c r="AZ124" s="35"/>
-      <c r="BA124" s="35"/>
-      <c r="BB124" s="35">
+      <c r="AY124" s="33"/>
+      <c r="AZ124" s="33"/>
+      <c r="BA124" s="33"/>
+      <c r="BB124" s="33">
         <v>2013</v>
       </c>
-      <c r="BC124" s="35"/>
-      <c r="BD124" s="35"/>
-      <c r="BE124" s="35"/>
-      <c r="BF124" s="35">
+      <c r="BC124" s="33"/>
+      <c r="BD124" s="33"/>
+      <c r="BE124" s="33"/>
+      <c r="BF124" s="33">
         <v>2014</v>
       </c>
-      <c r="BG124" s="35"/>
-      <c r="BH124" s="35"/>
-      <c r="BI124" s="35"/>
-      <c r="BJ124" s="35">
+      <c r="BG124" s="33"/>
+      <c r="BH124" s="33"/>
+      <c r="BI124" s="33"/>
+      <c r="BJ124" s="33">
         <v>2015</v>
       </c>
-      <c r="BK124" s="35"/>
-      <c r="BL124" s="35"/>
-      <c r="BM124" s="35"/>
-      <c r="BN124" s="35">
+      <c r="BK124" s="33"/>
+      <c r="BL124" s="33"/>
+      <c r="BM124" s="33"/>
+      <c r="BN124" s="33">
         <v>2016</v>
       </c>
-      <c r="BO124" s="35"/>
-      <c r="BP124" s="35"/>
-      <c r="BQ124" s="35"/>
+      <c r="BO124" s="33"/>
+      <c r="BP124" s="33"/>
+      <c r="BQ124" s="33"/>
       <c r="BR124" s="34">
         <v>2017</v>
       </c>
@@ -22479,9 +22605,10 @@
       <c r="CM124" s="34"/>
       <c r="CN124" s="34"/>
       <c r="CO124" s="34"/>
-      <c r="CP124" s="30">
+      <c r="CP124" s="34">
         <v>2023</v>
       </c>
+      <c r="CQ124" s="35"/>
     </row>
     <row r="125" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
@@ -22765,6 +22892,9 @@
       </c>
       <c r="CP125" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="CQ125" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -23053,7 +23183,9 @@
       <c r="CP127" s="26">
         <v>121.40993984588135</v>
       </c>
-      <c r="CQ127" s="11"/>
+      <c r="CQ127" s="26">
+        <v>123.69950887022809</v>
+      </c>
       <c r="CR127" s="11"/>
       <c r="CS127" s="11"/>
       <c r="CT127" s="11"/>
@@ -23396,7 +23528,9 @@
       <c r="CP128" s="26">
         <v>155.8613031242264</v>
       </c>
-      <c r="CQ128" s="11"/>
+      <c r="CQ128" s="26">
+        <v>174.33891502019807</v>
+      </c>
       <c r="CR128" s="11"/>
       <c r="CS128" s="11"/>
       <c r="CT128" s="11"/>
@@ -23739,7 +23873,9 @@
       <c r="CP129" s="26">
         <v>110.80516327271272</v>
       </c>
-      <c r="CQ129" s="11"/>
+      <c r="CQ129" s="26">
+        <v>121.9091653254432</v>
+      </c>
       <c r="CR129" s="11"/>
       <c r="CS129" s="11"/>
       <c r="CT129" s="11"/>
@@ -24082,7 +24218,9 @@
       <c r="CP130" s="26">
         <v>112.94682454743001</v>
       </c>
-      <c r="CQ130" s="11"/>
+      <c r="CQ130" s="26">
+        <v>117.12289797159234</v>
+      </c>
       <c r="CR130" s="11"/>
       <c r="CS130" s="11"/>
       <c r="CT130" s="11"/>
@@ -24425,7 +24563,9 @@
       <c r="CP131" s="26">
         <v>118.43763277423901</v>
       </c>
-      <c r="CQ131" s="11"/>
+      <c r="CQ131" s="26">
+        <v>118.89366595869345</v>
+      </c>
       <c r="CR131" s="11"/>
       <c r="CS131" s="11"/>
       <c r="CT131" s="11"/>
@@ -24768,7 +24908,9 @@
       <c r="CP132" s="26">
         <v>112.67232134559868</v>
       </c>
-      <c r="CQ132" s="11"/>
+      <c r="CQ132" s="26">
+        <v>113.5777891047194</v>
+      </c>
       <c r="CR132" s="11"/>
       <c r="CS132" s="11"/>
       <c r="CT132" s="11"/>
@@ -25111,7 +25253,9 @@
       <c r="CP133" s="26">
         <v>132.39182950639261</v>
       </c>
-      <c r="CQ133" s="11"/>
+      <c r="CQ133" s="26">
+        <v>124.41080168946679</v>
+      </c>
       <c r="CR133" s="11"/>
       <c r="CS133" s="11"/>
       <c r="CT133" s="11"/>
@@ -25454,7 +25598,9 @@
       <c r="CP134" s="26">
         <v>105.67435954176283</v>
       </c>
-      <c r="CQ134" s="11"/>
+      <c r="CQ134" s="26">
+        <v>102.77543821658408</v>
+      </c>
       <c r="CR134" s="11"/>
       <c r="CS134" s="11"/>
       <c r="CT134" s="11"/>
@@ -25797,7 +25943,9 @@
       <c r="CP135" s="26">
         <v>109.01624515776258</v>
       </c>
-      <c r="CQ135" s="11"/>
+      <c r="CQ135" s="26">
+        <v>108.16345917774601</v>
+      </c>
       <c r="CR135" s="11"/>
       <c r="CS135" s="11"/>
       <c r="CT135" s="11"/>
@@ -26140,7 +26288,9 @@
       <c r="CP136" s="26">
         <v>108.12715026223094</v>
       </c>
-      <c r="CQ136" s="11"/>
+      <c r="CQ136" s="26">
+        <v>110.46767080521592</v>
+      </c>
       <c r="CR136" s="11"/>
       <c r="CS136" s="11"/>
       <c r="CT136" s="11"/>
@@ -26483,7 +26633,9 @@
       <c r="CP137" s="26">
         <v>120.83454632830689</v>
       </c>
-      <c r="CQ137" s="11"/>
+      <c r="CQ137" s="26">
+        <v>117.57103978064248</v>
+      </c>
       <c r="CR137" s="11"/>
       <c r="CS137" s="11"/>
       <c r="CT137" s="11"/>
@@ -26826,7 +26978,9 @@
       <c r="CP138" s="26">
         <v>120.37521199573725</v>
       </c>
-      <c r="CQ138" s="11"/>
+      <c r="CQ138" s="26">
+        <v>122.91305655599656</v>
+      </c>
       <c r="CR138" s="11"/>
       <c r="CS138" s="11"/>
       <c r="CT138" s="11"/>
@@ -27321,9 +27475,11 @@
         <v>115.90512482879622</v>
       </c>
       <c r="CP140" s="26">
-        <v>119.62262414822237</v>
-      </c>
-      <c r="CQ140" s="11"/>
+        <v>119.60725875110107</v>
+      </c>
+      <c r="CQ140" s="26">
+        <v>120.70933212343446</v>
+      </c>
       <c r="CR140" s="11"/>
       <c r="CS140" s="11"/>
       <c r="CT140" s="11"/>
@@ -27478,6 +27634,7 @@
       <c r="CN141" s="16"/>
       <c r="CO141" s="16"/>
       <c r="CP141" s="16"/>
+      <c r="CQ141" s="16"/>
     </row>
     <row r="142" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
@@ -27516,108 +27673,108 @@
     </row>
     <row r="153" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
-      <c r="B153" s="35">
+      <c r="B153" s="33">
         <v>2000</v>
       </c>
-      <c r="C153" s="35"/>
-      <c r="D153" s="35"/>
-      <c r="E153" s="35"/>
-      <c r="F153" s="35">
+      <c r="C153" s="33"/>
+      <c r="D153" s="33"/>
+      <c r="E153" s="33"/>
+      <c r="F153" s="33">
         <v>2001</v>
       </c>
-      <c r="G153" s="35"/>
-      <c r="H153" s="35"/>
-      <c r="I153" s="35"/>
-      <c r="J153" s="35">
+      <c r="G153" s="33"/>
+      <c r="H153" s="33"/>
+      <c r="I153" s="33"/>
+      <c r="J153" s="33">
         <v>2002</v>
       </c>
-      <c r="K153" s="35"/>
-      <c r="L153" s="35"/>
-      <c r="M153" s="35"/>
-      <c r="N153" s="35">
+      <c r="K153" s="33"/>
+      <c r="L153" s="33"/>
+      <c r="M153" s="33"/>
+      <c r="N153" s="33">
         <v>2003</v>
       </c>
-      <c r="O153" s="35"/>
-      <c r="P153" s="35"/>
-      <c r="Q153" s="35"/>
-      <c r="R153" s="35">
+      <c r="O153" s="33"/>
+      <c r="P153" s="33"/>
+      <c r="Q153" s="33"/>
+      <c r="R153" s="33">
         <v>2004</v>
       </c>
-      <c r="S153" s="35"/>
-      <c r="T153" s="35"/>
-      <c r="U153" s="35"/>
-      <c r="V153" s="35">
+      <c r="S153" s="33"/>
+      <c r="T153" s="33"/>
+      <c r="U153" s="33"/>
+      <c r="V153" s="33">
         <v>2005</v>
       </c>
-      <c r="W153" s="35"/>
-      <c r="X153" s="35"/>
-      <c r="Y153" s="35"/>
-      <c r="Z153" s="35">
+      <c r="W153" s="33"/>
+      <c r="X153" s="33"/>
+      <c r="Y153" s="33"/>
+      <c r="Z153" s="33">
         <v>2006</v>
       </c>
-      <c r="AA153" s="35"/>
-      <c r="AB153" s="35"/>
-      <c r="AC153" s="35"/>
-      <c r="AD153" s="35">
+      <c r="AA153" s="33"/>
+      <c r="AB153" s="33"/>
+      <c r="AC153" s="33"/>
+      <c r="AD153" s="33">
         <v>2007</v>
       </c>
-      <c r="AE153" s="35"/>
-      <c r="AF153" s="35"/>
-      <c r="AG153" s="35"/>
-      <c r="AH153" s="35">
+      <c r="AE153" s="33"/>
+      <c r="AF153" s="33"/>
+      <c r="AG153" s="33"/>
+      <c r="AH153" s="33">
         <v>2008</v>
       </c>
-      <c r="AI153" s="35"/>
-      <c r="AJ153" s="35"/>
-      <c r="AK153" s="35"/>
-      <c r="AL153" s="35">
+      <c r="AI153" s="33"/>
+      <c r="AJ153" s="33"/>
+      <c r="AK153" s="33"/>
+      <c r="AL153" s="33">
         <v>2009</v>
       </c>
-      <c r="AM153" s="35"/>
-      <c r="AN153" s="35"/>
-      <c r="AO153" s="35"/>
-      <c r="AP153" s="35">
+      <c r="AM153" s="33"/>
+      <c r="AN153" s="33"/>
+      <c r="AO153" s="33"/>
+      <c r="AP153" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ153" s="35"/>
-      <c r="AR153" s="35"/>
-      <c r="AS153" s="35"/>
-      <c r="AT153" s="35">
+      <c r="AQ153" s="33"/>
+      <c r="AR153" s="33"/>
+      <c r="AS153" s="33"/>
+      <c r="AT153" s="33">
         <v>2011</v>
       </c>
-      <c r="AU153" s="35"/>
-      <c r="AV153" s="35"/>
-      <c r="AW153" s="35"/>
-      <c r="AX153" s="35">
+      <c r="AU153" s="33"/>
+      <c r="AV153" s="33"/>
+      <c r="AW153" s="33"/>
+      <c r="AX153" s="33">
         <v>2012</v>
       </c>
-      <c r="AY153" s="35"/>
-      <c r="AZ153" s="35"/>
-      <c r="BA153" s="35"/>
-      <c r="BB153" s="35">
+      <c r="AY153" s="33"/>
+      <c r="AZ153" s="33"/>
+      <c r="BA153" s="33"/>
+      <c r="BB153" s="33">
         <v>2013</v>
       </c>
-      <c r="BC153" s="35"/>
-      <c r="BD153" s="35"/>
-      <c r="BE153" s="35"/>
-      <c r="BF153" s="35">
+      <c r="BC153" s="33"/>
+      <c r="BD153" s="33"/>
+      <c r="BE153" s="33"/>
+      <c r="BF153" s="33">
         <v>2014</v>
       </c>
-      <c r="BG153" s="35"/>
-      <c r="BH153" s="35"/>
-      <c r="BI153" s="35"/>
-      <c r="BJ153" s="35">
+      <c r="BG153" s="33"/>
+      <c r="BH153" s="33"/>
+      <c r="BI153" s="33"/>
+      <c r="BJ153" s="33">
         <v>2015</v>
       </c>
-      <c r="BK153" s="35"/>
-      <c r="BL153" s="35"/>
-      <c r="BM153" s="35"/>
-      <c r="BN153" s="35">
+      <c r="BK153" s="33"/>
+      <c r="BL153" s="33"/>
+      <c r="BM153" s="33"/>
+      <c r="BN153" s="33">
         <v>2016</v>
       </c>
-      <c r="BO153" s="35"/>
-      <c r="BP153" s="35"/>
-      <c r="BQ153" s="35"/>
+      <c r="BO153" s="33"/>
+      <c r="BP153" s="33"/>
+      <c r="BQ153" s="33"/>
       <c r="BR153" s="34">
         <v>2017</v>
       </c>
@@ -27654,9 +27811,10 @@
       <c r="CM153" s="34"/>
       <c r="CN153" s="34"/>
       <c r="CO153" s="34"/>
-      <c r="CP153" s="30">
+      <c r="CP153" s="34">
         <v>2023</v>
       </c>
+      <c r="CQ153" s="35"/>
     </row>
     <row r="154" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
@@ -27940,6 +28098,9 @@
       </c>
       <c r="CP154" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="CQ154" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="155" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -28226,9 +28387,11 @@
         <v>39.714505651846942</v>
       </c>
       <c r="CP156" s="26">
-        <v>34.801309530293437</v>
-      </c>
-      <c r="CQ156" s="11"/>
+        <v>34.730409275893031</v>
+      </c>
+      <c r="CQ156" s="26">
+        <v>38.986001470206148</v>
+      </c>
       <c r="CR156" s="11"/>
       <c r="CS156" s="11"/>
       <c r="CT156" s="11"/>
@@ -28569,9 +28732,11 @@
         <v>2.2458821519621286</v>
       </c>
       <c r="CP157" s="26">
-        <v>1.7900164915719372</v>
-      </c>
-      <c r="CQ157" s="11"/>
+        <v>1.777976173879168</v>
+      </c>
+      <c r="CQ157" s="26">
+        <v>1.7733416082286104</v>
+      </c>
       <c r="CR157" s="11"/>
       <c r="CS157" s="11"/>
       <c r="CT157" s="11"/>
@@ -28912,9 +29077,11 @@
         <v>1.784686817842867</v>
       </c>
       <c r="CP158" s="26">
-        <v>1.3189175864749361</v>
-      </c>
-      <c r="CQ158" s="11"/>
+        <v>1.3382282287396032</v>
+      </c>
+      <c r="CQ158" s="26">
+        <v>1.1496201547048561</v>
+      </c>
       <c r="CR158" s="11"/>
       <c r="CS158" s="11"/>
       <c r="CT158" s="11"/>
@@ -29255,9 +29422,11 @@
         <v>11.163941802320894</v>
       </c>
       <c r="CP159" s="26">
-        <v>11.285996511002963</v>
-      </c>
-      <c r="CQ159" s="11"/>
+        <v>11.293296054633235</v>
+      </c>
+      <c r="CQ159" s="26">
+        <v>14.994734529462484</v>
+      </c>
       <c r="CR159" s="11"/>
       <c r="CS159" s="11"/>
       <c r="CT159" s="11"/>
@@ -29598,9 +29767,11 @@
         <v>2.7040979429244238</v>
       </c>
       <c r="CP160" s="26">
-        <v>2.4920663060940895</v>
-      </c>
-      <c r="CQ160" s="11"/>
+        <v>2.4989168236128143</v>
+      </c>
+      <c r="CQ160" s="26">
+        <v>2.449512932639812</v>
+      </c>
       <c r="CR160" s="11"/>
       <c r="CS160" s="11"/>
       <c r="CT160" s="11"/>
@@ -29941,9 +30112,11 @@
         <v>4.0097981398428715</v>
       </c>
       <c r="CP161" s="26">
-        <v>4.1454285165364357</v>
-      </c>
-      <c r="CQ161" s="11"/>
+        <v>4.1650006426571728</v>
+      </c>
+      <c r="CQ161" s="26">
+        <v>3.6171293548201215</v>
+      </c>
       <c r="CR161" s="11"/>
       <c r="CS161" s="11"/>
       <c r="CT161" s="11"/>
@@ -30284,9 +30457,11 @@
         <v>7.7278994002764083</v>
       </c>
       <c r="CP162" s="26">
-        <v>10.71454395588135</v>
-      </c>
-      <c r="CQ162" s="11"/>
+        <v>10.699256352678098</v>
+      </c>
+      <c r="CQ162" s="26">
+        <v>8.8773387167856175</v>
+      </c>
       <c r="CR162" s="11"/>
       <c r="CS162" s="11"/>
       <c r="CT162" s="11"/>
@@ -30627,9 +30802,11 @@
         <v>2.6105482147233063</v>
       </c>
       <c r="CP163" s="26">
-        <v>2.8929283802318659</v>
-      </c>
-      <c r="CQ163" s="11"/>
+        <v>2.8985971153663281</v>
+      </c>
+      <c r="CQ163" s="26">
+        <v>3.1109757752691336</v>
+      </c>
       <c r="CR163" s="11"/>
       <c r="CS163" s="11"/>
       <c r="CT163" s="11"/>
@@ -30970,9 +31147,11 @@
         <v>1.742263944652648</v>
       </c>
       <c r="CP164" s="26">
-        <v>1.7075675945164392</v>
-      </c>
-      <c r="CQ164" s="11"/>
+        <v>1.7287858122219679</v>
+      </c>
+      <c r="CQ164" s="26">
+        <v>1.2267610774419684</v>
+      </c>
       <c r="CR164" s="11"/>
       <c r="CS164" s="11"/>
       <c r="CT164" s="11"/>
@@ -31313,9 +31492,11 @@
         <v>4.5367553241551217</v>
       </c>
       <c r="CP165" s="26">
-        <v>5.1339295436877572</v>
-      </c>
-      <c r="CQ165" s="11"/>
+        <v>5.1483032982523982</v>
+      </c>
+      <c r="CQ165" s="26">
+        <v>4.7905191513606455</v>
+      </c>
       <c r="CR165" s="11"/>
       <c r="CS165" s="11"/>
       <c r="CT165" s="11"/>
@@ -31656,9 +31837,11 @@
         <v>7.6541432964881455</v>
       </c>
       <c r="CP166" s="26">
-        <v>9.5954535596183916</v>
-      </c>
-      <c r="CQ166" s="11"/>
+        <v>9.60372536195527</v>
+      </c>
+      <c r="CQ166" s="26">
+        <v>5.6355377763054824</v>
+      </c>
       <c r="CR166" s="11"/>
       <c r="CS166" s="11"/>
       <c r="CT166" s="11"/>
@@ -31999,9 +32182,11 @@
         <v>14.105477312964235</v>
       </c>
       <c r="CP167" s="26">
-        <v>14.121842024090418</v>
-      </c>
-      <c r="CQ167" s="11"/>
+        <v>14.117504860110927</v>
+      </c>
+      <c r="CQ167" s="26">
+        <v>13.38852745277512</v>
+      </c>
       <c r="CR167" s="11"/>
       <c r="CS167" s="11"/>
       <c r="CT167" s="11"/>
@@ -32498,7 +32683,9 @@
       <c r="CP169" s="26">
         <v>100</v>
       </c>
-      <c r="CQ169" s="11"/>
+      <c r="CQ169" s="26">
+        <v>100</v>
+      </c>
       <c r="CR169" s="11"/>
       <c r="CS169" s="11"/>
       <c r="CT169" s="11"/>
@@ -32653,6 +32840,7 @@
       <c r="CN170" s="16"/>
       <c r="CO170" s="16"/>
       <c r="CP170" s="16"/>
+      <c r="CQ170" s="16"/>
     </row>
     <row r="171" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
@@ -32999,108 +33187,108 @@
     </row>
     <row r="182" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A182" s="4"/>
-      <c r="B182" s="35">
+      <c r="B182" s="33">
         <v>2000</v>
       </c>
-      <c r="C182" s="35"/>
-      <c r="D182" s="35"/>
-      <c r="E182" s="35"/>
-      <c r="F182" s="35">
+      <c r="C182" s="33"/>
+      <c r="D182" s="33"/>
+      <c r="E182" s="33"/>
+      <c r="F182" s="33">
         <v>2001</v>
       </c>
-      <c r="G182" s="35"/>
-      <c r="H182" s="35"/>
-      <c r="I182" s="35"/>
-      <c r="J182" s="35">
+      <c r="G182" s="33"/>
+      <c r="H182" s="33"/>
+      <c r="I182" s="33"/>
+      <c r="J182" s="33">
         <v>2002</v>
       </c>
-      <c r="K182" s="35"/>
-      <c r="L182" s="35"/>
-      <c r="M182" s="35"/>
-      <c r="N182" s="35">
+      <c r="K182" s="33"/>
+      <c r="L182" s="33"/>
+      <c r="M182" s="33"/>
+      <c r="N182" s="33">
         <v>2003</v>
       </c>
-      <c r="O182" s="35"/>
-      <c r="P182" s="35"/>
-      <c r="Q182" s="35"/>
-      <c r="R182" s="35">
+      <c r="O182" s="33"/>
+      <c r="P182" s="33"/>
+      <c r="Q182" s="33"/>
+      <c r="R182" s="33">
         <v>2004</v>
       </c>
-      <c r="S182" s="35"/>
-      <c r="T182" s="35"/>
-      <c r="U182" s="35"/>
-      <c r="V182" s="35">
+      <c r="S182" s="33"/>
+      <c r="T182" s="33"/>
+      <c r="U182" s="33"/>
+      <c r="V182" s="33">
         <v>2005</v>
       </c>
-      <c r="W182" s="35"/>
-      <c r="X182" s="35"/>
-      <c r="Y182" s="35"/>
-      <c r="Z182" s="35">
+      <c r="W182" s="33"/>
+      <c r="X182" s="33"/>
+      <c r="Y182" s="33"/>
+      <c r="Z182" s="33">
         <v>2006</v>
       </c>
-      <c r="AA182" s="35"/>
-      <c r="AB182" s="35"/>
-      <c r="AC182" s="35"/>
-      <c r="AD182" s="35">
+      <c r="AA182" s="33"/>
+      <c r="AB182" s="33"/>
+      <c r="AC182" s="33"/>
+      <c r="AD182" s="33">
         <v>2007</v>
       </c>
-      <c r="AE182" s="35"/>
-      <c r="AF182" s="35"/>
-      <c r="AG182" s="35"/>
-      <c r="AH182" s="35">
+      <c r="AE182" s="33"/>
+      <c r="AF182" s="33"/>
+      <c r="AG182" s="33"/>
+      <c r="AH182" s="33">
         <v>2008</v>
       </c>
-      <c r="AI182" s="35"/>
-      <c r="AJ182" s="35"/>
-      <c r="AK182" s="35"/>
-      <c r="AL182" s="35">
+      <c r="AI182" s="33"/>
+      <c r="AJ182" s="33"/>
+      <c r="AK182" s="33"/>
+      <c r="AL182" s="33">
         <v>2009</v>
       </c>
-      <c r="AM182" s="35"/>
-      <c r="AN182" s="35"/>
-      <c r="AO182" s="35"/>
-      <c r="AP182" s="35">
+      <c r="AM182" s="33"/>
+      <c r="AN182" s="33"/>
+      <c r="AO182" s="33"/>
+      <c r="AP182" s="33">
         <v>2010</v>
       </c>
-      <c r="AQ182" s="35"/>
-      <c r="AR182" s="35"/>
-      <c r="AS182" s="35"/>
-      <c r="AT182" s="35">
+      <c r="AQ182" s="33"/>
+      <c r="AR182" s="33"/>
+      <c r="AS182" s="33"/>
+      <c r="AT182" s="33">
         <v>2011</v>
       </c>
-      <c r="AU182" s="35"/>
-      <c r="AV182" s="35"/>
-      <c r="AW182" s="35"/>
-      <c r="AX182" s="35">
+      <c r="AU182" s="33"/>
+      <c r="AV182" s="33"/>
+      <c r="AW182" s="33"/>
+      <c r="AX182" s="33">
         <v>2012</v>
       </c>
-      <c r="AY182" s="35"/>
-      <c r="AZ182" s="35"/>
-      <c r="BA182" s="35"/>
-      <c r="BB182" s="35">
+      <c r="AY182" s="33"/>
+      <c r="AZ182" s="33"/>
+      <c r="BA182" s="33"/>
+      <c r="BB182" s="33">
         <v>2013</v>
       </c>
-      <c r="BC182" s="35"/>
-      <c r="BD182" s="35"/>
-      <c r="BE182" s="35"/>
-      <c r="BF182" s="35">
+      <c r="BC182" s="33"/>
+      <c r="BD182" s="33"/>
+      <c r="BE182" s="33"/>
+      <c r="BF182" s="33">
         <v>2014</v>
       </c>
-      <c r="BG182" s="35"/>
-      <c r="BH182" s="35"/>
-      <c r="BI182" s="35"/>
-      <c r="BJ182" s="35">
+      <c r="BG182" s="33"/>
+      <c r="BH182" s="33"/>
+      <c r="BI182" s="33"/>
+      <c r="BJ182" s="33">
         <v>2015</v>
       </c>
-      <c r="BK182" s="35"/>
-      <c r="BL182" s="35"/>
-      <c r="BM182" s="35"/>
-      <c r="BN182" s="35">
+      <c r="BK182" s="33"/>
+      <c r="BL182" s="33"/>
+      <c r="BM182" s="33"/>
+      <c r="BN182" s="33">
         <v>2016</v>
       </c>
-      <c r="BO182" s="35"/>
-      <c r="BP182" s="35"/>
-      <c r="BQ182" s="35"/>
+      <c r="BO182" s="33"/>
+      <c r="BP182" s="33"/>
+      <c r="BQ182" s="33"/>
       <c r="BR182" s="34">
         <v>2017</v>
       </c>
@@ -33137,9 +33325,10 @@
       <c r="CM182" s="34"/>
       <c r="CN182" s="34"/>
       <c r="CO182" s="34"/>
-      <c r="CP182" s="30">
+      <c r="CP182" s="34">
         <v>2023</v>
       </c>
+      <c r="CQ182" s="35"/>
     </row>
     <row r="183" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
@@ -33423,6 +33612,9 @@
       </c>
       <c r="CP183" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="CQ183" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="184" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -33709,9 +33901,11 @@
         <v>38.476312795146747</v>
       </c>
       <c r="CP185" s="26">
-        <v>34.288987994663479</v>
-      </c>
-      <c r="CQ185" s="11"/>
+        <v>34.21473607569947</v>
+      </c>
+      <c r="CQ185" s="26">
+        <v>38.043596475138862</v>
+      </c>
       <c r="CR185" s="11"/>
       <c r="CS185" s="11"/>
       <c r="CT185" s="11"/>
@@ -34052,9 +34246,11 @@
         <v>1.6490181956184811</v>
       </c>
       <c r="CP186" s="26">
-        <v>1.3738270224762841</v>
-      </c>
-      <c r="CQ186" s="11"/>
+        <v>1.3644108705607478</v>
+      </c>
+      <c r="CQ186" s="26">
+        <v>1.2278318993276567</v>
+      </c>
       <c r="CR186" s="11"/>
       <c r="CS186" s="11"/>
       <c r="CT186" s="11"/>
@@ -34395,9 +34591,11 @@
         <v>1.9172808085196866</v>
       </c>
       <c r="CP187" s="26">
-        <v>1.4238721199396078</v>
-      </c>
-      <c r="CQ187" s="11"/>
+        <v>1.4445338583089546</v>
+      </c>
+      <c r="CQ187" s="26">
+        <v>1.1383055629952745</v>
+      </c>
       <c r="CR187" s="11"/>
       <c r="CS187" s="11"/>
       <c r="CT187" s="11"/>
@@ -34738,9 +34936,11 @@
         <v>11.048325223907147</v>
       </c>
       <c r="CP188" s="26">
-        <v>11.953063082414705</v>
-      </c>
-      <c r="CQ188" s="11"/>
+        <v>11.95925771947735</v>
+      </c>
+      <c r="CQ188" s="26">
+        <v>15.453890074156352</v>
+      </c>
       <c r="CR188" s="11"/>
       <c r="CS188" s="11"/>
       <c r="CT188" s="11"/>
@@ -35081,9 +35281,11 @@
         <v>2.802373208131514</v>
       </c>
       <c r="CP189" s="26">
-        <v>2.516999910447236</v>
-      </c>
-      <c r="CQ189" s="11"/>
+        <v>2.5235947740450602</v>
+      </c>
+      <c r="CQ189" s="26">
+        <v>2.4869202891716133</v>
+      </c>
       <c r="CR189" s="11"/>
       <c r="CS189" s="11"/>
       <c r="CT189" s="11"/>
@@ -35424,9 +35626,11 @@
         <v>4.0650234125140683</v>
       </c>
       <c r="CP190" s="26">
-        <v>4.40114334598585</v>
-      </c>
-      <c r="CQ190" s="11"/>
+        <v>4.4213548067123281</v>
+      </c>
+      <c r="CQ190" s="26">
+        <v>3.8442487044878009</v>
+      </c>
       <c r="CR190" s="11"/>
       <c r="CS190" s="11"/>
       <c r="CT190" s="11"/>
@@ -35767,9 +35971,11 @@
         <v>7.0833636123509072</v>
       </c>
       <c r="CP191" s="26">
-        <v>9.6811251066827708</v>
-      </c>
-      <c r="CQ191" s="11"/>
+        <v>9.6660702385515389</v>
+      </c>
+      <c r="CQ191" s="26">
+        <v>8.613220178513032</v>
+      </c>
       <c r="CR191" s="11"/>
       <c r="CS191" s="11"/>
       <c r="CT191" s="11"/>
@@ -36110,9 +36316,11 @@
         <v>3.0947443667314065</v>
       </c>
       <c r="CP192" s="26">
-        <v>3.2747743711608526</v>
-      </c>
-      <c r="CQ192" s="11"/>
+        <v>3.2807698735642807</v>
+      </c>
+      <c r="CQ192" s="26">
+        <v>3.6538283329287284</v>
+      </c>
       <c r="CR192" s="11"/>
       <c r="CS192" s="11"/>
       <c r="CT192" s="11"/>
@@ -36453,9 +36661,11 @@
         <v>1.879917694815243</v>
       </c>
       <c r="CP193" s="26">
-        <v>1.8736997983275285</v>
-      </c>
-      <c r="CQ193" s="11"/>
+        <v>1.8967387077809454</v>
+      </c>
+      <c r="CQ193" s="26">
+        <v>1.3690530190024817</v>
+      </c>
       <c r="CR193" s="11"/>
       <c r="CS193" s="11"/>
       <c r="CT193" s="11"/>
@@ -36796,9 +37006,11 @@
         <v>5.1272646206983881</v>
       </c>
       <c r="CP194" s="26">
-        <v>5.6797402199041747</v>
-      </c>
-      <c r="CQ194" s="11"/>
+        <v>5.6949105125756105</v>
+      </c>
+      <c r="CQ194" s="26">
+        <v>5.2346570093334677</v>
+      </c>
       <c r="CR194" s="11"/>
       <c r="CS194" s="11"/>
       <c r="CT194" s="11"/>
@@ -37139,9 +37351,11 @@
         <v>7.6340247187200703</v>
       </c>
       <c r="CP195" s="26">
-        <v>9.4992149974668294</v>
-      </c>
-      <c r="CQ195" s="11"/>
+        <v>9.5061826211599332</v>
+      </c>
+      <c r="CQ195" s="26">
+        <v>5.7859656800128247</v>
+      </c>
       <c r="CR195" s="11"/>
       <c r="CS195" s="11"/>
       <c r="CT195" s="11"/>
@@ -37482,9 +37696,11 @@
         <v>15.222351342846343</v>
       </c>
       <c r="CP196" s="26">
-        <v>14.033552030530682</v>
-      </c>
-      <c r="CQ196" s="11"/>
+        <v>14.027439941563799</v>
+      </c>
+      <c r="CQ196" s="26">
+        <v>13.148482774931908</v>
+      </c>
       <c r="CR196" s="11"/>
       <c r="CS196" s="11"/>
       <c r="CT196" s="11"/>
@@ -37981,7 +38197,9 @@
       <c r="CP198" s="26">
         <v>100</v>
       </c>
-      <c r="CQ198" s="11"/>
+      <c r="CQ198" s="26">
+        <v>100</v>
+      </c>
       <c r="CR198" s="11"/>
       <c r="CS198" s="11"/>
       <c r="CT198" s="11"/>
@@ -38136,6 +38354,7 @@
       <c r="CN199" s="16"/>
       <c r="CO199" s="16"/>
       <c r="CP199" s="16"/>
+      <c r="CQ199" s="16"/>
     </row>
     <row r="200" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
@@ -38237,7 +38456,7 @@
       <c r="CN201" s="1"/>
       <c r="CO201" s="1"/>
       <c r="CP201" s="1"/>
-      <c r="CQ201" s="28"/>
+      <c r="CQ201" s="1"/>
       <c r="CR201" s="28"/>
       <c r="CS201" s="28"/>
       <c r="CT201" s="28"/>
@@ -38392,7 +38611,7 @@
       <c r="CN202" s="1"/>
       <c r="CO202" s="1"/>
       <c r="CP202" s="1"/>
-      <c r="CQ202" s="28"/>
+      <c r="CQ202" s="1"/>
       <c r="CR202" s="28"/>
       <c r="CS202" s="28"/>
       <c r="CT202" s="28"/>
@@ -38453,23 +38672,138 @@
       <c r="EW202" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="159">
+  <mergeCells count="168">
+    <mergeCell ref="CP9:CQ9"/>
+    <mergeCell ref="CP38:CQ38"/>
+    <mergeCell ref="CP124:CQ124"/>
+    <mergeCell ref="CP153:CQ153"/>
+    <mergeCell ref="CP182:CQ182"/>
+    <mergeCell ref="CL67:CO67"/>
+    <mergeCell ref="CP67:CQ67"/>
+    <mergeCell ref="CL96:CO96"/>
+    <mergeCell ref="CP96:CQ96"/>
     <mergeCell ref="CL182:CO182"/>
-    <mergeCell ref="B182:E182"/>
-    <mergeCell ref="F182:I182"/>
-    <mergeCell ref="J182:M182"/>
-    <mergeCell ref="N182:Q182"/>
-    <mergeCell ref="R182:U182"/>
-    <mergeCell ref="V182:Y182"/>
-    <mergeCell ref="Z182:AC182"/>
-    <mergeCell ref="AD182:AG182"/>
-    <mergeCell ref="AH182:AK182"/>
+    <mergeCell ref="CH9:CK9"/>
+    <mergeCell ref="CH38:CK38"/>
+    <mergeCell ref="CL9:CO9"/>
+    <mergeCell ref="CL38:CO38"/>
+    <mergeCell ref="CH67:CK67"/>
+    <mergeCell ref="CH96:CK96"/>
+    <mergeCell ref="CL124:CO124"/>
+    <mergeCell ref="CH124:CK124"/>
+    <mergeCell ref="CH153:CK153"/>
+    <mergeCell ref="CL153:CO153"/>
+    <mergeCell ref="AH124:AK124"/>
+    <mergeCell ref="BR182:BU182"/>
+    <mergeCell ref="BV182:BY182"/>
+    <mergeCell ref="BZ124:CC124"/>
+    <mergeCell ref="BR124:BU124"/>
+    <mergeCell ref="BV124:BY124"/>
+    <mergeCell ref="BR153:BU153"/>
+    <mergeCell ref="BV153:BY153"/>
+    <mergeCell ref="BZ153:CC153"/>
+    <mergeCell ref="AH153:AK153"/>
+    <mergeCell ref="BN182:BQ182"/>
+    <mergeCell ref="BB153:BE153"/>
+    <mergeCell ref="BF153:BI153"/>
+    <mergeCell ref="BJ153:BM153"/>
+    <mergeCell ref="BN153:BQ153"/>
+    <mergeCell ref="AP153:AS153"/>
+    <mergeCell ref="AT153:AW153"/>
+    <mergeCell ref="AX153:BA153"/>
+    <mergeCell ref="AX182:BA182"/>
+    <mergeCell ref="BB182:BE182"/>
+    <mergeCell ref="BZ182:CC182"/>
+    <mergeCell ref="AL182:AO182"/>
     <mergeCell ref="AP182:AS182"/>
     <mergeCell ref="AT182:AW182"/>
-    <mergeCell ref="BF182:BI182"/>
-    <mergeCell ref="BJ182:BM182"/>
-    <mergeCell ref="CH182:CK182"/>
-    <mergeCell ref="CD182:CG182"/>
+    <mergeCell ref="BV38:BY38"/>
+    <mergeCell ref="BZ67:CC67"/>
+    <mergeCell ref="BZ96:CC96"/>
+    <mergeCell ref="BJ96:BM96"/>
+    <mergeCell ref="BB38:BE38"/>
+    <mergeCell ref="CD9:CG9"/>
+    <mergeCell ref="CD38:CG38"/>
+    <mergeCell ref="CD124:CG124"/>
+    <mergeCell ref="CD153:CG153"/>
+    <mergeCell ref="BV9:BY9"/>
+    <mergeCell ref="BZ9:CC9"/>
+    <mergeCell ref="BR9:BU9"/>
+    <mergeCell ref="BR67:BU67"/>
+    <mergeCell ref="BV67:BY67"/>
+    <mergeCell ref="BR96:BU96"/>
+    <mergeCell ref="BV96:BY96"/>
+    <mergeCell ref="BZ38:CC38"/>
+    <mergeCell ref="CD67:CG67"/>
+    <mergeCell ref="CD96:CG96"/>
+    <mergeCell ref="BJ38:BM38"/>
+    <mergeCell ref="BR38:BU38"/>
+    <mergeCell ref="BF124:BI124"/>
+    <mergeCell ref="BJ124:BM124"/>
+    <mergeCell ref="BN124:BQ124"/>
+    <mergeCell ref="BJ9:BM9"/>
+    <mergeCell ref="BN9:BQ9"/>
+    <mergeCell ref="AL153:AO153"/>
+    <mergeCell ref="AL124:AO124"/>
+    <mergeCell ref="AP124:AS124"/>
+    <mergeCell ref="AT124:AW124"/>
+    <mergeCell ref="AX124:BA124"/>
+    <mergeCell ref="BB124:BE124"/>
+    <mergeCell ref="BN38:BQ38"/>
+    <mergeCell ref="BN96:BQ96"/>
+    <mergeCell ref="AL96:AO96"/>
+    <mergeCell ref="AP96:AS96"/>
+    <mergeCell ref="AT96:AW96"/>
+    <mergeCell ref="AX96:BA96"/>
+    <mergeCell ref="BB96:BE96"/>
+    <mergeCell ref="BF96:BI96"/>
+    <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="BB9:BE9"/>
+    <mergeCell ref="BF9:BI9"/>
+    <mergeCell ref="AX67:BA67"/>
+    <mergeCell ref="BB67:BE67"/>
+    <mergeCell ref="BF67:BI67"/>
+    <mergeCell ref="BJ67:BM67"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="AL67:AO67"/>
+    <mergeCell ref="AP67:AS67"/>
+    <mergeCell ref="AT67:AW67"/>
+    <mergeCell ref="Z38:AC38"/>
+    <mergeCell ref="AD38:AG38"/>
+    <mergeCell ref="AH38:AK38"/>
+    <mergeCell ref="AL38:AO38"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="AD9:AG9"/>
+    <mergeCell ref="AP38:AS38"/>
+    <mergeCell ref="AT38:AW38"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="BN67:BQ67"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="R38:U38"/>
+    <mergeCell ref="V38:Y38"/>
+    <mergeCell ref="AH96:AK96"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="J67:M67"/>
+    <mergeCell ref="N67:Q67"/>
+    <mergeCell ref="R67:U67"/>
+    <mergeCell ref="V67:Y67"/>
+    <mergeCell ref="Z67:AC67"/>
+    <mergeCell ref="AD67:AG67"/>
+    <mergeCell ref="AH67:AK67"/>
+    <mergeCell ref="BF38:BI38"/>
+    <mergeCell ref="AX38:BA38"/>
     <mergeCell ref="V153:Y153"/>
     <mergeCell ref="Z153:AC153"/>
     <mergeCell ref="AD153:AG153"/>
@@ -38494,133 +38828,27 @@
     <mergeCell ref="J153:M153"/>
     <mergeCell ref="N153:Q153"/>
     <mergeCell ref="R153:U153"/>
-    <mergeCell ref="BN67:BQ67"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="N38:Q38"/>
-    <mergeCell ref="R38:U38"/>
-    <mergeCell ref="V38:Y38"/>
-    <mergeCell ref="AH96:AK96"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="J67:M67"/>
-    <mergeCell ref="N67:Q67"/>
-    <mergeCell ref="R67:U67"/>
-    <mergeCell ref="V67:Y67"/>
-    <mergeCell ref="Z67:AC67"/>
-    <mergeCell ref="AD67:AG67"/>
-    <mergeCell ref="AH67:AK67"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="AT9:AW9"/>
-    <mergeCell ref="AL67:AO67"/>
-    <mergeCell ref="AP67:AS67"/>
-    <mergeCell ref="AT67:AW67"/>
-    <mergeCell ref="Z38:AC38"/>
-    <mergeCell ref="AD38:AG38"/>
-    <mergeCell ref="AH38:AK38"/>
-    <mergeCell ref="AL38:AO38"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="AD9:AG9"/>
-    <mergeCell ref="BF38:BI38"/>
-    <mergeCell ref="AP38:AS38"/>
-    <mergeCell ref="AT38:AW38"/>
-    <mergeCell ref="AX38:BA38"/>
-    <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="BJ9:BM9"/>
-    <mergeCell ref="BN9:BQ9"/>
-    <mergeCell ref="AL153:AO153"/>
-    <mergeCell ref="AL124:AO124"/>
-    <mergeCell ref="AP124:AS124"/>
-    <mergeCell ref="AT124:AW124"/>
-    <mergeCell ref="AX124:BA124"/>
-    <mergeCell ref="BB124:BE124"/>
-    <mergeCell ref="BN38:BQ38"/>
-    <mergeCell ref="BN96:BQ96"/>
-    <mergeCell ref="AL96:AO96"/>
-    <mergeCell ref="AP96:AS96"/>
-    <mergeCell ref="AT96:AW96"/>
-    <mergeCell ref="AX96:BA96"/>
-    <mergeCell ref="BB96:BE96"/>
-    <mergeCell ref="BF96:BI96"/>
-    <mergeCell ref="AP9:AS9"/>
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="BB9:BE9"/>
-    <mergeCell ref="BF9:BI9"/>
-    <mergeCell ref="AX67:BA67"/>
-    <mergeCell ref="BB67:BE67"/>
-    <mergeCell ref="BF67:BI67"/>
-    <mergeCell ref="BJ67:BM67"/>
-    <mergeCell ref="BV38:BY38"/>
-    <mergeCell ref="BZ67:CC67"/>
-    <mergeCell ref="BZ96:CC96"/>
-    <mergeCell ref="BJ96:BM96"/>
-    <mergeCell ref="BB38:BE38"/>
-    <mergeCell ref="CD9:CG9"/>
-    <mergeCell ref="CD38:CG38"/>
-    <mergeCell ref="CD124:CG124"/>
-    <mergeCell ref="CD153:CG153"/>
-    <mergeCell ref="BV9:BY9"/>
-    <mergeCell ref="BZ9:CC9"/>
-    <mergeCell ref="BR9:BU9"/>
-    <mergeCell ref="BR67:BU67"/>
-    <mergeCell ref="BV67:BY67"/>
-    <mergeCell ref="BR96:BU96"/>
-    <mergeCell ref="BV96:BY96"/>
-    <mergeCell ref="BZ38:CC38"/>
-    <mergeCell ref="CD67:CG67"/>
-    <mergeCell ref="CD96:CG96"/>
-    <mergeCell ref="BJ38:BM38"/>
-    <mergeCell ref="BR38:BU38"/>
-    <mergeCell ref="BF124:BI124"/>
-    <mergeCell ref="BJ124:BM124"/>
-    <mergeCell ref="BN124:BQ124"/>
-    <mergeCell ref="AH124:AK124"/>
-    <mergeCell ref="BR182:BU182"/>
-    <mergeCell ref="BV182:BY182"/>
-    <mergeCell ref="BZ124:CC124"/>
-    <mergeCell ref="BR124:BU124"/>
-    <mergeCell ref="BV124:BY124"/>
-    <mergeCell ref="BR153:BU153"/>
-    <mergeCell ref="BV153:BY153"/>
-    <mergeCell ref="BZ153:CC153"/>
-    <mergeCell ref="AH153:AK153"/>
-    <mergeCell ref="BN182:BQ182"/>
-    <mergeCell ref="BB153:BE153"/>
-    <mergeCell ref="BF153:BI153"/>
-    <mergeCell ref="BJ153:BM153"/>
-    <mergeCell ref="BN153:BQ153"/>
-    <mergeCell ref="AP153:AS153"/>
-    <mergeCell ref="AT153:AW153"/>
-    <mergeCell ref="AX153:BA153"/>
-    <mergeCell ref="AX182:BA182"/>
-    <mergeCell ref="BB182:BE182"/>
-    <mergeCell ref="BZ182:CC182"/>
-    <mergeCell ref="AL182:AO182"/>
-    <mergeCell ref="CH9:CK9"/>
-    <mergeCell ref="CH38:CK38"/>
-    <mergeCell ref="CL9:CO9"/>
-    <mergeCell ref="CL38:CO38"/>
-    <mergeCell ref="CH67:CK67"/>
-    <mergeCell ref="CH96:CK96"/>
-    <mergeCell ref="CL124:CO124"/>
-    <mergeCell ref="CH124:CK124"/>
-    <mergeCell ref="CH153:CK153"/>
-    <mergeCell ref="CL153:CO153"/>
+    <mergeCell ref="BF182:BI182"/>
+    <mergeCell ref="BJ182:BM182"/>
+    <mergeCell ref="CH182:CK182"/>
+    <mergeCell ref="CD182:CG182"/>
+    <mergeCell ref="B182:E182"/>
+    <mergeCell ref="F182:I182"/>
+    <mergeCell ref="J182:M182"/>
+    <mergeCell ref="N182:Q182"/>
+    <mergeCell ref="R182:U182"/>
+    <mergeCell ref="V182:Y182"/>
+    <mergeCell ref="Z182:AC182"/>
+    <mergeCell ref="AD182:AG182"/>
+    <mergeCell ref="AH182:AK182"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="58" max="93" man="1"/>
-    <brk id="116" max="93" man="1"/>
-    <brk id="144" max="93" man="1"/>
+    <brk id="58" max="94" man="1"/>
+    <brk id="116" max="94" man="1"/>
+    <brk id="144" max="94" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q2 2025 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Qrt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of May 2025\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2025\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF267F3-59E0-46DB-A32D-826935E4C703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC3E591-8FF2-4D3B-AC45-85066F4677B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="64">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -229,13 +229,13 @@
     <t>2024 - 2025</t>
   </si>
   <si>
-    <t>Q1 2000 to Q1 2025</t>
+    <t>As of August 2025</t>
   </si>
   <si>
-    <t>Q1 2001 to Q1 2025</t>
+    <t>Q1 2000 to Q2 2025</t>
   </si>
   <si>
-    <t>As of May 2025</t>
+    <t>Q1 2001 to Q2 2025</t>
   </si>
 </sst>
 </file>
@@ -243,10 +243,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -319,10 +319,10 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -342,32 +342,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -377,13 +377,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -732,11 +732,11 @@
   <dimension ref="A1:EW202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CQ2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="CA66" sqref="CA66"/>
       <selection pane="topRight" activeCell="CA66" sqref="CA66"/>
       <selection pane="bottomLeft" activeCell="CA66" sqref="CA66"/>
-      <selection pane="bottomRight" activeCell="CX1" sqref="CX1"/>
+      <selection pane="bottomRight" activeCell="CY1" sqref="CY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -744,8 +744,8 @@
     <col min="1" max="1" width="38.88671875" style="1" customWidth="1"/>
     <col min="2" max="69" width="11.109375" style="2" customWidth="1"/>
     <col min="70" max="89" width="11.109375" style="1" customWidth="1"/>
-    <col min="90" max="102" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="103" max="16384" width="7.77734375" style="1"/>
+    <col min="90" max="103" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="104" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:153" x14ac:dyDescent="0.2">
@@ -760,7 +760,7 @@
     </row>
     <row r="3" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:153" x14ac:dyDescent="0.2">
@@ -770,7 +770,7 @@
     </row>
     <row r="6" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:153" x14ac:dyDescent="0.2">
@@ -933,6 +933,7 @@
       <c r="CX9" s="35">
         <v>2025</v>
       </c>
+      <c r="CY9" s="35"/>
     </row>
     <row r="10" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -1240,6 +1241,9 @@
       </c>
       <c r="CX10" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="CY10" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1550,9 +1554,11 @@
         <v>2162044.6171398368</v>
       </c>
       <c r="CX12" s="9">
-        <v>1734887.1469660599</v>
-      </c>
-      <c r="CY12" s="11"/>
+        <v>1739032.9216468222</v>
+      </c>
+      <c r="CY12" s="9">
+        <v>1912472.8891737878</v>
+      </c>
       <c r="CZ12" s="11"/>
       <c r="DA12" s="11"/>
       <c r="DB12" s="11"/>
@@ -1909,9 +1915,11 @@
         <v>124543.37838654699</v>
       </c>
       <c r="CX13" s="9">
-        <v>92342.468078674035</v>
-      </c>
-      <c r="CY13" s="11"/>
+        <v>92362.791113174331</v>
+      </c>
+      <c r="CY13" s="9">
+        <v>86552.496906400003</v>
+      </c>
       <c r="CZ13" s="11"/>
       <c r="DA13" s="11"/>
       <c r="DB13" s="11"/>
@@ -2268,9 +2276,11 @@
         <v>93902.795225128575</v>
       </c>
       <c r="CX14" s="9">
-        <v>65317.153480865432</v>
-      </c>
-      <c r="CY14" s="11"/>
+        <v>65079.664639905059</v>
+      </c>
+      <c r="CY14" s="9">
+        <v>52259.712213336432</v>
+      </c>
       <c r="CZ14" s="11"/>
       <c r="DA14" s="11"/>
       <c r="DB14" s="11"/>
@@ -2627,9 +2637,11 @@
         <v>614054.36448713182</v>
       </c>
       <c r="CX15" s="9">
-        <v>561595.47827925475</v>
-      </c>
-      <c r="CY15" s="11"/>
+        <v>560592.39430115058</v>
+      </c>
+      <c r="CY15" s="9">
+        <v>715758.04437039909</v>
+      </c>
       <c r="CZ15" s="11"/>
       <c r="DA15" s="11"/>
       <c r="DB15" s="11"/>
@@ -2986,9 +2998,11 @@
         <v>147767.90231364404</v>
       </c>
       <c r="CX16" s="9">
-        <v>121247.09726119338</v>
-      </c>
-      <c r="CY16" s="11"/>
+        <v>122290.55596765227</v>
+      </c>
+      <c r="CY16" s="9">
+        <v>114693.10285810464</v>
+      </c>
       <c r="CZ16" s="11"/>
       <c r="DA16" s="11"/>
       <c r="DB16" s="11"/>
@@ -3345,9 +3359,11 @@
         <v>247318.81060222766</v>
       </c>
       <c r="CX17" s="9">
-        <v>228972.93731324174</v>
-      </c>
-      <c r="CY17" s="11"/>
+        <v>229434.65337623964</v>
+      </c>
+      <c r="CY17" s="9">
+        <v>199073.01957684947</v>
+      </c>
       <c r="CZ17" s="11"/>
       <c r="DA17" s="11"/>
       <c r="DB17" s="11"/>
@@ -3704,9 +3720,11 @@
         <v>464043.1526550423</v>
       </c>
       <c r="CX18" s="9">
-        <v>557498.6238903926</v>
-      </c>
-      <c r="CY18" s="11"/>
+        <v>557556.77390960406</v>
+      </c>
+      <c r="CY18" s="9">
+        <v>482467.27959665802</v>
+      </c>
       <c r="CZ18" s="11"/>
       <c r="DA18" s="11"/>
       <c r="DB18" s="11"/>
@@ -4063,9 +4081,11 @@
         <v>139247.27733421652</v>
       </c>
       <c r="CX19" s="9">
-        <v>143437.22210288173</v>
-      </c>
-      <c r="CY19" s="11"/>
+        <v>142284.7414504984</v>
+      </c>
+      <c r="CY19" s="9">
+        <v>151091.54245982703</v>
+      </c>
       <c r="CZ19" s="11"/>
       <c r="DA19" s="11"/>
       <c r="DB19" s="11"/>
@@ -4422,9 +4442,11 @@
         <v>106868.69742001814</v>
       </c>
       <c r="CX20" s="9">
-        <v>96321.104570154654</v>
-      </c>
-      <c r="CY20" s="11"/>
+        <v>95832.357670154655</v>
+      </c>
+      <c r="CY20" s="9">
+        <v>69205.522444502625</v>
+      </c>
       <c r="CZ20" s="11"/>
       <c r="DA20" s="11"/>
       <c r="DB20" s="11"/>
@@ -4781,9 +4803,11 @@
         <v>271497.04271244386</v>
       </c>
       <c r="CX21" s="9">
-        <v>275940.3223190729</v>
-      </c>
-      <c r="CY21" s="11"/>
+        <v>274487.10755094176</v>
+      </c>
+      <c r="CY21" s="9">
+        <v>247290.33901176177</v>
+      </c>
       <c r="CZ21" s="11"/>
       <c r="DA21" s="11"/>
       <c r="DB21" s="11"/>
@@ -5140,9 +5164,11 @@
         <v>499380.11673069955</v>
       </c>
       <c r="CX22" s="9">
-        <v>542012.530055949</v>
-      </c>
-      <c r="CY22" s="11"/>
+        <v>543358.73903827975</v>
+      </c>
+      <c r="CY22" s="9">
+        <v>312431.51421393396</v>
+      </c>
       <c r="CZ22" s="11"/>
       <c r="DA22" s="11"/>
       <c r="DB22" s="11"/>
@@ -5499,9 +5525,11 @@
         <v>858697.14329350879</v>
       </c>
       <c r="CX23" s="9">
-        <v>731820.03261882951</v>
-      </c>
-      <c r="CY23" s="11"/>
+        <v>729278.39016381756</v>
+      </c>
+      <c r="CY23" s="9">
+        <v>685188.29995057802</v>
+      </c>
       <c r="CZ23" s="11"/>
       <c r="DA23" s="11"/>
       <c r="DB23" s="11"/>
@@ -5655,7 +5683,7 @@
       <c r="CV24" s="13"/>
       <c r="CW24" s="13"/>
       <c r="CX24" s="13"/>
-      <c r="CY24" s="11"/>
+      <c r="CY24" s="13"/>
       <c r="CZ24" s="11"/>
       <c r="DA24" s="11"/>
       <c r="DB24" s="11"/>
@@ -6012,9 +6040,11 @@
         <v>5729365.2983004451</v>
       </c>
       <c r="CX25" s="36">
-        <v>5151392.11693657</v>
-      </c>
-      <c r="CY25" s="11"/>
+        <v>5151591.0908282408</v>
+      </c>
+      <c r="CY25" s="36">
+        <v>5028483.7627761383</v>
+      </c>
       <c r="CZ25" s="11"/>
       <c r="DA25" s="11"/>
       <c r="DB25" s="11"/>
@@ -6169,6 +6199,7 @@
       <c r="CV26" s="17"/>
       <c r="CW26" s="17"/>
       <c r="CX26" s="17"/>
+      <c r="CY26" s="17"/>
     </row>
     <row r="27" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -6277,7 +6308,7 @@
       <c r="CV28" s="37"/>
       <c r="CW28" s="37"/>
       <c r="CX28" s="37"/>
-      <c r="CY28" s="11"/>
+      <c r="CY28" s="37"/>
       <c r="CZ28" s="11"/>
       <c r="DA28" s="11"/>
       <c r="DB28" s="11"/>
@@ -6431,7 +6462,7 @@
       <c r="CV29" s="38"/>
       <c r="CW29" s="38"/>
       <c r="CX29" s="38"/>
-      <c r="CY29" s="11"/>
+      <c r="CY29" s="38"/>
       <c r="CZ29" s="11"/>
       <c r="DA29" s="11"/>
       <c r="DB29" s="11"/>
@@ -6495,7 +6526,7 @@
     </row>
     <row r="32" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:153" x14ac:dyDescent="0.2">
@@ -6505,7 +6536,7 @@
     </row>
     <row r="35" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:153" x14ac:dyDescent="0.2">
@@ -6668,6 +6699,7 @@
       <c r="CX38" s="35">
         <v>2025</v>
       </c>
+      <c r="CY38" s="35"/>
     </row>
     <row r="39" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -6975,6 +7007,9 @@
       </c>
       <c r="CX39" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="CY39" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -7285,9 +7320,11 @@
         <v>1650790.3578221325</v>
       </c>
       <c r="CX41" s="9">
-        <v>1328830.0540412916</v>
-      </c>
-      <c r="CY41" s="11"/>
+        <v>1332005.494013116</v>
+      </c>
+      <c r="CY41" s="9">
+        <v>1448070.7151311939</v>
+      </c>
       <c r="CZ41" s="11"/>
       <c r="DA41" s="11"/>
       <c r="DB41" s="11"/>
@@ -7644,9 +7681,11 @@
         <v>71876.742738170637</v>
       </c>
       <c r="CX42" s="9">
-        <v>53054.679661728303</v>
-      </c>
-      <c r="CY42" s="11"/>
+        <v>53066.356110361332</v>
+      </c>
+      <c r="CY42" s="9">
+        <v>45848.69161605979</v>
+      </c>
       <c r="CZ42" s="11"/>
       <c r="DA42" s="11"/>
       <c r="DB42" s="11"/>
@@ -8003,9 +8042,11 @@
         <v>81272.634446154829</v>
       </c>
       <c r="CX43" s="9">
-        <v>55702.019808985584</v>
-      </c>
-      <c r="CY43" s="11"/>
+        <v>55499.490956783491</v>
+      </c>
+      <c r="CY43" s="9">
+        <v>40789.094546193111</v>
+      </c>
       <c r="CZ43" s="11"/>
       <c r="DA43" s="11"/>
       <c r="DB43" s="11"/>
@@ -8362,9 +8403,11 @@
         <v>501036.80901641428</v>
       </c>
       <c r="CX44" s="9">
-        <v>484957.52390025562</v>
-      </c>
-      <c r="CY44" s="11"/>
+        <v>484091.32546900056</v>
+      </c>
+      <c r="CY44" s="9">
+        <v>591655.82056751603</v>
+      </c>
       <c r="CZ44" s="11"/>
       <c r="DA44" s="11"/>
       <c r="DB44" s="11"/>
@@ -8721,9 +8764,11 @@
         <v>122824.86039783062</v>
       </c>
       <c r="CX45" s="9">
-        <v>96680.160284199766</v>
-      </c>
-      <c r="CY45" s="11"/>
+        <v>97512.194677345411</v>
+      </c>
+      <c r="CY45" s="9">
+        <v>91772.007948891827</v>
+      </c>
       <c r="CZ45" s="11"/>
       <c r="DA45" s="11"/>
       <c r="DB45" s="11"/>
@@ -9080,9 +9125,11 @@
         <v>203231.85149515138</v>
       </c>
       <c r="CX46" s="9">
-        <v>192472.99514204662</v>
-      </c>
-      <c r="CY46" s="11"/>
+        <v>192861.11032540922</v>
+      </c>
+      <c r="CY46" s="9">
+        <v>166208.67578242454</v>
+      </c>
       <c r="CZ46" s="11"/>
       <c r="DA46" s="11"/>
       <c r="DB46" s="11"/>
@@ -9439,9 +9486,11 @@
         <v>369251.48516124854</v>
       </c>
       <c r="CX47" s="9">
-        <v>417104.47495431098</v>
-      </c>
-      <c r="CY47" s="11"/>
+        <v>417147.98113027698</v>
+      </c>
+      <c r="CY47" s="9">
+        <v>384279.94928777596</v>
+      </c>
       <c r="CZ47" s="11"/>
       <c r="DA47" s="11"/>
       <c r="DB47" s="11"/>
@@ -9798,9 +9847,11 @@
         <v>141271.96959121188</v>
       </c>
       <c r="CX48" s="9">
-        <v>134772.4627405534</v>
-      </c>
-      <c r="CY48" s="11"/>
+        <v>133689.60116874235</v>
+      </c>
+      <c r="CY48" s="9">
+        <v>145781.11335515749</v>
+      </c>
       <c r="CZ48" s="11"/>
       <c r="DA48" s="11"/>
       <c r="DB48" s="11"/>
@@ -10157,9 +10208,11 @@
         <v>92738.684566163356</v>
       </c>
       <c r="CX49" s="9">
-        <v>83094.111142448994</v>
-      </c>
-      <c r="CY49" s="11"/>
+        <v>82672.47987679478</v>
+      </c>
+      <c r="CY49" s="9">
+        <v>60458.893337978079</v>
+      </c>
       <c r="CZ49" s="11"/>
       <c r="DA49" s="11"/>
       <c r="DB49" s="11"/>
@@ -10516,9 +10569,11 @@
         <v>244891.60101847848</v>
       </c>
       <c r="CX50" s="9">
-        <v>235895.45316415778</v>
-      </c>
-      <c r="CY50" s="11"/>
+        <v>234653.13108019371</v>
+      </c>
+      <c r="CY50" s="9">
+        <v>206181.4306886688</v>
+      </c>
       <c r="CZ50" s="11"/>
       <c r="DA50" s="11"/>
       <c r="DB50" s="11"/>
@@ -10875,9 +10930,11 @@
         <v>390876.52060471731</v>
       </c>
       <c r="CX51" s="9">
-        <v>416825.83700790745</v>
-      </c>
-      <c r="CY51" s="11"/>
+        <v>417861.11692254274</v>
+      </c>
+      <c r="CY51" s="9">
+        <v>247192.30556426576</v>
+      </c>
       <c r="CZ51" s="11"/>
       <c r="DA51" s="11"/>
       <c r="DB51" s="11"/>
@@ -11234,9 +11291,11 @@
         <v>758934.00048357504</v>
       </c>
       <c r="CX52" s="9">
-        <v>570725.12599211966</v>
-      </c>
-      <c r="CY52" s="11"/>
+        <v>568742.97307786741</v>
+      </c>
+      <c r="CY52" s="9">
+        <v>530413.6727475028</v>
+      </c>
       <c r="CZ52" s="11"/>
       <c r="DA52" s="11"/>
       <c r="DB52" s="11"/>
@@ -11390,7 +11449,7 @@
       <c r="CV53" s="13"/>
       <c r="CW53" s="13"/>
       <c r="CX53" s="13"/>
-      <c r="CY53" s="11"/>
+      <c r="CY53" s="13"/>
       <c r="CZ53" s="11"/>
       <c r="DA53" s="11"/>
       <c r="DB53" s="11"/>
@@ -11747,9 +11806,11 @@
         <v>4628997.5173412496</v>
       </c>
       <c r="CX54" s="36">
-        <v>4070114.8978400058</v>
-      </c>
-      <c r="CY54" s="11"/>
+        <v>4069803.2548084343</v>
+      </c>
+      <c r="CY54" s="36">
+        <v>3958652.3705736278</v>
+      </c>
       <c r="CZ54" s="11"/>
       <c r="DA54" s="11"/>
       <c r="DB54" s="11"/>
@@ -11904,6 +11965,7 @@
       <c r="CV55" s="17"/>
       <c r="CW55" s="17"/>
       <c r="CX55" s="17"/>
+      <c r="CY55" s="17"/>
     </row>
     <row r="56" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
@@ -12012,7 +12074,7 @@
       <c r="CV57" s="13"/>
       <c r="CW57" s="13"/>
       <c r="CX57" s="13"/>
-      <c r="CY57" s="11"/>
+      <c r="CY57" s="13"/>
       <c r="CZ57" s="11"/>
       <c r="DA57" s="11"/>
       <c r="DB57" s="11"/>
@@ -12166,7 +12228,7 @@
       <c r="CV58" s="38"/>
       <c r="CW58" s="38"/>
       <c r="CX58" s="38"/>
-      <c r="CY58" s="11"/>
+      <c r="CY58" s="38"/>
       <c r="CZ58" s="11"/>
       <c r="DA58" s="11"/>
       <c r="DB58" s="11"/>
@@ -12230,18 +12292,20 @@
     </row>
     <row r="61" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="CT61" s="39"/>
       <c r="CU61" s="39"/>
       <c r="CV61" s="39"/>
       <c r="CX61" s="39"/>
+      <c r="CY61" s="39"/>
     </row>
     <row r="62" spans="1:153" x14ac:dyDescent="0.2">
       <c r="CT62" s="39"/>
       <c r="CU62" s="39"/>
       <c r="CV62" s="39"/>
       <c r="CX62" s="39"/>
+      <c r="CY62" s="39"/>
     </row>
     <row r="63" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
@@ -12251,15 +12315,17 @@
       <c r="CU63" s="39"/>
       <c r="CV63" s="39"/>
       <c r="CX63" s="39"/>
+      <c r="CY63" s="39"/>
     </row>
     <row r="64" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="CT64" s="39"/>
       <c r="CU64" s="39"/>
       <c r="CV64" s="39"/>
       <c r="CX64" s="39"/>
+      <c r="CY64" s="39"/>
     </row>
     <row r="65" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
@@ -12268,12 +12334,13 @@
       <c r="CU65" s="39"/>
       <c r="CV65" s="39"/>
       <c r="CX65" s="39"/>
+      <c r="CY65" s="39"/>
     </row>
     <row r="66" spans="1:149" x14ac:dyDescent="0.2">
-      <c r="CU66" s="39"/>
       <c r="CV66" s="39"/>
       <c r="CW66" s="39"/>
       <c r="CX66" s="39"/>
+      <c r="CY66" s="39"/>
     </row>
     <row r="67" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
@@ -12424,10 +12491,11 @@
       <c r="CT67" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="CU67" s="34"/>
+      <c r="CU67" s="35"/>
       <c r="CV67" s="34"/>
       <c r="CW67" s="34"/>
       <c r="CX67" s="34"/>
+      <c r="CY67" s="34"/>
     </row>
     <row r="68" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
@@ -12724,17 +12792,20 @@
       <c r="CT68" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="CU68" s="6"/>
+      <c r="CU68" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="CV68" s="6"/>
       <c r="CW68" s="6"/>
       <c r="CX68" s="6"/>
+      <c r="CY68" s="6"/>
     </row>
     <row r="69" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
-      <c r="CU69" s="39"/>
       <c r="CV69" s="39"/>
       <c r="CW69" s="39"/>
       <c r="CX69" s="39"/>
+      <c r="CY69" s="39"/>
     </row>
     <row r="70" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
@@ -13029,13 +13100,15 @@
         <v>4.7717007129400457</v>
       </c>
       <c r="CT70" s="25">
-        <v>7.511269368093366</v>
-      </c>
-      <c r="CU70" s="40"/>
+        <v>7.7681837727117369</v>
+      </c>
+      <c r="CU70" s="25">
+        <v>6.4427003777558554</v>
+      </c>
       <c r="CV70" s="40"/>
       <c r="CW70" s="40"/>
       <c r="CX70" s="40"/>
-      <c r="CY70" s="11"/>
+      <c r="CY70" s="40"/>
       <c r="CZ70" s="11"/>
       <c r="DA70" s="11"/>
       <c r="DB70" s="11"/>
@@ -13376,13 +13449,15 @@
         <v>6.7352233138463475</v>
       </c>
       <c r="CT71" s="25">
-        <v>10.988612572857974</v>
-      </c>
-      <c r="CU71" s="40"/>
+        <v>11.013039312248736</v>
+      </c>
+      <c r="CU71" s="25">
+        <v>2.2174251884260201</v>
+      </c>
       <c r="CV71" s="40"/>
       <c r="CW71" s="40"/>
       <c r="CX71" s="40"/>
-      <c r="CY71" s="11"/>
+      <c r="CY71" s="40"/>
       <c r="CZ71" s="11"/>
       <c r="DA71" s="11"/>
       <c r="DB71" s="11"/>
@@ -13723,13 +13798,15 @@
         <v>5.6974487057801042</v>
       </c>
       <c r="CT72" s="25">
-        <v>6.4514218706507904</v>
-      </c>
-      <c r="CU72" s="40"/>
+        <v>6.0643715561258205</v>
+      </c>
+      <c r="CU72" s="25">
+        <v>5.5834306756110266</v>
+      </c>
       <c r="CV72" s="40"/>
       <c r="CW72" s="40"/>
       <c r="CX72" s="40"/>
-      <c r="CY72" s="11"/>
+      <c r="CY72" s="40"/>
       <c r="CZ72" s="11"/>
       <c r="DA72" s="11"/>
       <c r="DB72" s="11"/>
@@ -14070,13 +14147,15 @@
         <v>6.146743608712967</v>
       </c>
       <c r="CT73" s="25">
-        <v>4.2068212362639485</v>
-      </c>
-      <c r="CU73" s="40"/>
+        <v>4.0206940382467167</v>
+      </c>
+      <c r="CU73" s="25">
+        <v>3.5790718590346557</v>
+      </c>
       <c r="CV73" s="40"/>
       <c r="CW73" s="40"/>
       <c r="CX73" s="40"/>
-      <c r="CY73" s="11"/>
+      <c r="CY73" s="40"/>
       <c r="CZ73" s="11"/>
       <c r="DA73" s="11"/>
       <c r="DB73" s="11"/>
@@ -14417,13 +14496,15 @@
         <v>7.1903482061526489</v>
       </c>
       <c r="CT74" s="25">
-        <v>2.6699349130941243</v>
-      </c>
-      <c r="CU74" s="40"/>
+        <v>3.5535176123636205</v>
+      </c>
+      <c r="CU74" s="25">
+        <v>2.4943130170342158</v>
+      </c>
       <c r="CV74" s="40"/>
       <c r="CW74" s="40"/>
       <c r="CX74" s="40"/>
-      <c r="CY74" s="11"/>
+      <c r="CY74" s="40"/>
       <c r="CZ74" s="11"/>
       <c r="DA74" s="11"/>
       <c r="DB74" s="11"/>
@@ -14764,13 +14845,15 @@
         <v>14.271742994448289</v>
       </c>
       <c r="CT75" s="25">
-        <v>12.351783713119445</v>
-      </c>
-      <c r="CU75" s="40"/>
+        <v>12.578337225755078</v>
+      </c>
+      <c r="CU75" s="25">
+        <v>12.70418946555381</v>
+      </c>
       <c r="CV75" s="40"/>
       <c r="CW75" s="40"/>
       <c r="CX75" s="40"/>
-      <c r="CY75" s="11"/>
+      <c r="CY75" s="40"/>
       <c r="CZ75" s="11"/>
       <c r="DA75" s="11"/>
       <c r="DB75" s="11"/>
@@ -15111,13 +15194,15 @@
         <v>9.7737540474051912</v>
       </c>
       <c r="CT76" s="25">
-        <v>8.4393707905875033</v>
-      </c>
-      <c r="CU76" s="40"/>
+        <v>8.4506815835195823</v>
+      </c>
+      <c r="CU76" s="25">
+        <v>8.8715826222831424</v>
+      </c>
       <c r="CV76" s="40"/>
       <c r="CW76" s="40"/>
       <c r="CX76" s="40"/>
-      <c r="CY76" s="11"/>
+      <c r="CY76" s="40"/>
       <c r="CZ76" s="11"/>
       <c r="DA76" s="11"/>
       <c r="DB76" s="11"/>
@@ -15458,13 +15543,15 @@
         <v>4.0205603380900641</v>
       </c>
       <c r="CT77" s="25">
-        <v>6.677223061604451</v>
-      </c>
-      <c r="CU77" s="40"/>
+        <v>5.8200994096956151</v>
+      </c>
+      <c r="CU77" s="25">
+        <v>5.0379054472316369</v>
+      </c>
       <c r="CV77" s="40"/>
       <c r="CW77" s="40"/>
       <c r="CX77" s="40"/>
-      <c r="CY77" s="11"/>
+      <c r="CY77" s="40"/>
       <c r="CZ77" s="11"/>
       <c r="DA77" s="11"/>
       <c r="DB77" s="11"/>
@@ -15805,13 +15892,15 @@
         <v>11.841800107850958</v>
       </c>
       <c r="CT78" s="25">
-        <v>12.316577147252559</v>
-      </c>
-      <c r="CU78" s="40"/>
+        <v>11.746666958366106</v>
+      </c>
+      <c r="CU78" s="25">
+        <v>8.8885360460055836</v>
+      </c>
       <c r="CV78" s="40"/>
       <c r="CW78" s="40"/>
       <c r="CX78" s="40"/>
-      <c r="CY78" s="11"/>
+      <c r="CY78" s="40"/>
       <c r="CZ78" s="11"/>
       <c r="DA78" s="11"/>
       <c r="DB78" s="11"/>
@@ -16152,13 +16241,15 @@
         <v>10.657442008195119</v>
       </c>
       <c r="CT79" s="25">
-        <v>11.79317307091226</v>
-      </c>
-      <c r="CU79" s="40"/>
+        <v>11.204424428751025</v>
+      </c>
+      <c r="CU79" s="25">
+        <v>14.79076164097286</v>
+      </c>
       <c r="CV79" s="40"/>
       <c r="CW79" s="40"/>
       <c r="CX79" s="40"/>
-      <c r="CY79" s="11"/>
+      <c r="CY79" s="40"/>
       <c r="CZ79" s="11"/>
       <c r="DA79" s="11"/>
       <c r="DB79" s="11"/>
@@ -16499,13 +16590,15 @@
         <v>9.6724702139006098</v>
       </c>
       <c r="CT80" s="25">
-        <v>8.1082364877808004</v>
-      </c>
-      <c r="CU80" s="40"/>
+        <v>8.3767474002661118</v>
+      </c>
+      <c r="CU80" s="25">
+        <v>9.6563018331089552</v>
+      </c>
       <c r="CV80" s="40"/>
       <c r="CW80" s="40"/>
       <c r="CX80" s="40"/>
-      <c r="CY80" s="11"/>
+      <c r="CY80" s="40"/>
       <c r="CZ80" s="11"/>
       <c r="DA80" s="11"/>
       <c r="DB80" s="11"/>
@@ -16846,13 +16939,15 @@
         <v>10.63374262686736</v>
       </c>
       <c r="CT81" s="25">
-        <v>7.457419687550896</v>
-      </c>
-      <c r="CU81" s="40"/>
+        <v>7.0842154463297788</v>
+      </c>
+      <c r="CU81" s="25">
+        <v>6.1060646695225955</v>
+      </c>
       <c r="CV81" s="40"/>
       <c r="CW81" s="40"/>
       <c r="CX81" s="40"/>
-      <c r="CY81" s="11"/>
+      <c r="CY81" s="40"/>
       <c r="CZ81" s="11"/>
       <c r="DA81" s="11"/>
       <c r="DB81" s="11"/>
@@ -16998,11 +17093,11 @@
       <c r="CR82" s="13"/>
       <c r="CS82" s="13"/>
       <c r="CT82" s="13"/>
-      <c r="CU82" s="41"/>
+      <c r="CU82" s="13"/>
       <c r="CV82" s="41"/>
       <c r="CW82" s="41"/>
       <c r="CX82" s="41"/>
-      <c r="CY82" s="11"/>
+      <c r="CY82" s="41"/>
       <c r="CZ82" s="11"/>
       <c r="DA82" s="11"/>
       <c r="DB82" s="11"/>
@@ -17343,13 +17438,15 @@
         <v>7.4750674956280534</v>
       </c>
       <c r="CT83" s="25">
-        <v>7.7109155831550709</v>
-      </c>
-      <c r="CU83" s="40"/>
+        <v>7.7150759459390343</v>
+      </c>
+      <c r="CU83" s="25">
+        <v>6.8275183225073164</v>
+      </c>
       <c r="CV83" s="40"/>
       <c r="CW83" s="40"/>
       <c r="CX83" s="40"/>
-      <c r="CY83" s="11"/>
+      <c r="CY83" s="40"/>
       <c r="CZ83" s="11"/>
       <c r="DA83" s="11"/>
       <c r="DB83" s="11"/>
@@ -17496,19 +17593,20 @@
       <c r="CR84" s="17"/>
       <c r="CS84" s="17"/>
       <c r="CT84" s="17"/>
-      <c r="CU84" s="6"/>
+      <c r="CU84" s="17"/>
       <c r="CV84" s="6"/>
       <c r="CW84" s="6"/>
       <c r="CX84" s="6"/>
+      <c r="CY84" s="6"/>
     </row>
     <row r="85" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="CU85" s="39"/>
       <c r="CV85" s="39"/>
       <c r="CW85" s="39"/>
       <c r="CX85" s="39"/>
+      <c r="CY85" s="39"/>
     </row>
     <row r="86" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="13"/>
@@ -17608,11 +17706,11 @@
       <c r="CR86" s="13"/>
       <c r="CS86" s="13"/>
       <c r="CT86" s="13"/>
-      <c r="CU86" s="41"/>
+      <c r="CU86" s="13"/>
       <c r="CV86" s="41"/>
       <c r="CW86" s="41"/>
       <c r="CX86" s="41"/>
-      <c r="CY86" s="11"/>
+      <c r="CY86" s="41"/>
       <c r="CZ86" s="11"/>
       <c r="DA86" s="11"/>
       <c r="DB86" s="11"/>
@@ -17758,11 +17856,11 @@
       <c r="CR87" s="13"/>
       <c r="CS87" s="13"/>
       <c r="CT87" s="13"/>
-      <c r="CU87" s="41"/>
+      <c r="CU87" s="13"/>
       <c r="CV87" s="41"/>
       <c r="CW87" s="41"/>
       <c r="CX87" s="41"/>
-      <c r="CY87" s="11"/>
+      <c r="CY87" s="41"/>
       <c r="CZ87" s="11"/>
       <c r="DA87" s="11"/>
       <c r="DB87" s="11"/>
@@ -17814,67 +17912,67 @@
       <c r="A88" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="CU88" s="39"/>
       <c r="CV88" s="39"/>
       <c r="CW88" s="39"/>
       <c r="CX88" s="39"/>
+      <c r="CY88" s="39"/>
     </row>
     <row r="89" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="CU89" s="39"/>
       <c r="CV89" s="39"/>
       <c r="CW89" s="39"/>
       <c r="CX89" s="39"/>
+      <c r="CY89" s="39"/>
     </row>
     <row r="90" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="CU90" s="39"/>
+        <v>61</v>
+      </c>
       <c r="CV90" s="39"/>
       <c r="CW90" s="39"/>
       <c r="CX90" s="39"/>
+      <c r="CY90" s="39"/>
     </row>
     <row r="91" spans="1:149" x14ac:dyDescent="0.2">
-      <c r="CU91" s="39"/>
       <c r="CV91" s="39"/>
       <c r="CW91" s="39"/>
       <c r="CX91" s="39"/>
+      <c r="CY91" s="39"/>
     </row>
     <row r="92" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="CU92" s="39"/>
       <c r="CV92" s="39"/>
       <c r="CW92" s="39"/>
       <c r="CX92" s="39"/>
+      <c r="CY92" s="39"/>
     </row>
     <row r="93" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="CU93" s="39"/>
+        <v>63</v>
+      </c>
       <c r="CV93" s="39"/>
       <c r="CW93" s="39"/>
       <c r="CX93" s="39"/>
+      <c r="CY93" s="39"/>
     </row>
     <row r="94" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="CU94" s="39"/>
       <c r="CV94" s="39"/>
       <c r="CW94" s="39"/>
       <c r="CX94" s="39"/>
+      <c r="CY94" s="39"/>
     </row>
     <row r="95" spans="1:149" x14ac:dyDescent="0.2">
-      <c r="CU95" s="39"/>
       <c r="CV95" s="39"/>
       <c r="CW95" s="39"/>
       <c r="CX95" s="39"/>
+      <c r="CY95" s="39"/>
     </row>
     <row r="96" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
@@ -18025,10 +18123,11 @@
       <c r="CT96" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="CU96" s="34"/>
+      <c r="CU96" s="35"/>
       <c r="CV96" s="34"/>
       <c r="CW96" s="34"/>
       <c r="CX96" s="34"/>
+      <c r="CY96" s="34"/>
     </row>
     <row r="97" spans="1:149" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
@@ -18325,17 +18424,20 @@
       <c r="CT97" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="CU97" s="6"/>
+      <c r="CU97" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="CV97" s="6"/>
       <c r="CW97" s="6"/>
       <c r="CX97" s="6"/>
+      <c r="CY97" s="6"/>
     </row>
     <row r="98" spans="1:149" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
-      <c r="CU98" s="39"/>
       <c r="CV98" s="39"/>
       <c r="CW98" s="39"/>
       <c r="CX98" s="39"/>
+      <c r="CY98" s="39"/>
     </row>
     <row r="99" spans="1:149" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
@@ -18630,13 +18732,15 @@
         <v>1.4743172387257033</v>
       </c>
       <c r="CT99" s="25">
-        <v>4.5143454856577847</v>
-      </c>
-      <c r="CU99" s="40"/>
+        <v>4.7640982883392979</v>
+      </c>
+      <c r="CU99" s="25">
+        <v>5.6779080732710696</v>
+      </c>
       <c r="CV99" s="40"/>
       <c r="CW99" s="40"/>
       <c r="CX99" s="40"/>
-      <c r="CY99" s="11"/>
+      <c r="CY99" s="40"/>
       <c r="CZ99" s="11"/>
       <c r="DA99" s="11"/>
       <c r="DB99" s="11"/>
@@ -18977,13 +19081,15 @@
         <v>3.569010532707992</v>
       </c>
       <c r="CT100" s="25">
-        <v>7.2238723224035084</v>
-      </c>
-      <c r="CU100" s="40"/>
+        <v>7.2474705053609796</v>
+      </c>
+      <c r="CU100" s="25">
+        <v>-1.5154422648577395</v>
+      </c>
       <c r="CV100" s="40"/>
       <c r="CW100" s="40"/>
       <c r="CX100" s="40"/>
-      <c r="CY100" s="11"/>
+      <c r="CY100" s="40"/>
       <c r="CZ100" s="11"/>
       <c r="DA100" s="11"/>
       <c r="DB100" s="11"/>
@@ -19324,13 +19430,15 @@
         <v>3.0690405094083673</v>
       </c>
       <c r="CT101" s="25">
-        <v>4.2904224833989986</v>
-      </c>
-      <c r="CU101" s="40"/>
+        <v>3.9112294194191719</v>
+      </c>
+      <c r="CU101" s="25">
+        <v>3.8866063533097019</v>
+      </c>
       <c r="CV101" s="40"/>
       <c r="CW101" s="40"/>
       <c r="CX101" s="40"/>
-      <c r="CY101" s="11"/>
+      <c r="CY101" s="40"/>
       <c r="CZ101" s="11"/>
       <c r="DA101" s="11"/>
       <c r="DB101" s="11"/>
@@ -19671,13 +19779,15 @@
         <v>3.6598436068550342</v>
       </c>
       <c r="CT102" s="25">
-        <v>2.3505747631597416</v>
-      </c>
-      <c r="CU102" s="40"/>
+        <v>2.1677630674365957</v>
+      </c>
+      <c r="CU102" s="25">
+        <v>0.75982657163579859</v>
+      </c>
       <c r="CV102" s="40"/>
       <c r="CW102" s="40"/>
       <c r="CX102" s="40"/>
-      <c r="CY102" s="11"/>
+      <c r="CY102" s="40"/>
       <c r="CZ102" s="11"/>
       <c r="DA102" s="11"/>
       <c r="DB102" s="11"/>
@@ -20018,13 +20128,15 @@
         <v>4.4814616889862862</v>
       </c>
       <c r="CT103" s="25">
-        <v>0.31448431454809622</v>
-      </c>
-      <c r="CU103" s="40"/>
+        <v>1.1777958857641693</v>
+      </c>
+      <c r="CU103" s="25">
+        <v>0.39978013472861562</v>
+      </c>
       <c r="CV103" s="40"/>
       <c r="CW103" s="40"/>
       <c r="CX103" s="40"/>
-      <c r="CY103" s="11"/>
+      <c r="CY103" s="40"/>
       <c r="CZ103" s="11"/>
       <c r="DA103" s="11"/>
       <c r="DB103" s="11"/>
@@ -20365,13 +20477,15 @@
         <v>11.444907728116149</v>
       </c>
       <c r="CT104" s="25">
-        <v>9.8010621277521324</v>
-      </c>
-      <c r="CU104" s="40"/>
+        <v>10.02247219792676</v>
+      </c>
+      <c r="CU104" s="25">
+        <v>10.043533533873614</v>
+      </c>
       <c r="CV104" s="40"/>
       <c r="CW104" s="40"/>
       <c r="CX104" s="40"/>
-      <c r="CY104" s="11"/>
+      <c r="CY104" s="40"/>
       <c r="CZ104" s="11"/>
       <c r="DA104" s="11"/>
       <c r="DB104" s="11"/>
@@ -20712,13 +20826,15 @@
         <v>10.682618246504006</v>
       </c>
       <c r="CT105" s="25">
-        <v>8.4949522210285693</v>
-      </c>
-      <c r="CU105" s="40"/>
+        <v>8.50626881139425</v>
+      </c>
+      <c r="CU105" s="25">
+        <v>11.159750290265748</v>
+      </c>
       <c r="CV105" s="40"/>
       <c r="CW105" s="40"/>
       <c r="CX105" s="40"/>
-      <c r="CY105" s="11"/>
+      <c r="CY105" s="40"/>
       <c r="CZ105" s="11"/>
       <c r="DA105" s="11"/>
       <c r="DB105" s="11"/>
@@ -21059,13 +21175,15 @@
         <v>3.818970104876712</v>
       </c>
       <c r="CT106" s="25">
-        <v>6.3677146774798246</v>
-      </c>
-      <c r="CU106" s="40"/>
+        <v>5.5130778446771416</v>
+      </c>
+      <c r="CU106" s="25">
+        <v>4.6660300175826137</v>
+      </c>
       <c r="CV106" s="40"/>
       <c r="CW106" s="40"/>
       <c r="CX106" s="40"/>
-      <c r="CY106" s="11"/>
+      <c r="CY106" s="40"/>
       <c r="CZ106" s="11"/>
       <c r="DA106" s="11"/>
       <c r="DB106" s="11"/>
@@ -21406,13 +21524,15 @@
         <v>9.1318363082023524</v>
       </c>
       <c r="CT107" s="25">
-        <v>9.7371490925524142</v>
-      </c>
-      <c r="CU107" s="40"/>
+        <v>9.1803272862289731</v>
+      </c>
+      <c r="CU107" s="25">
+        <v>6.5822270362766062</v>
+      </c>
       <c r="CV107" s="40"/>
       <c r="CW107" s="40"/>
       <c r="CX107" s="40"/>
-      <c r="CY107" s="11"/>
+      <c r="CY107" s="40"/>
       <c r="CZ107" s="11"/>
       <c r="DA107" s="11"/>
       <c r="DB107" s="11"/>
@@ -21753,13 +21873,15 @@
         <v>6.0505543309180609</v>
       </c>
       <c r="CT108" s="25">
-        <v>7.2396689308668272</v>
-      </c>
-      <c r="CU108" s="40"/>
+        <v>6.6749009067154788</v>
+      </c>
+      <c r="CU108" s="25">
+        <v>9.7199383768768968</v>
+      </c>
       <c r="CV108" s="40"/>
       <c r="CW108" s="40"/>
       <c r="CX108" s="40"/>
-      <c r="CY108" s="11"/>
+      <c r="CY108" s="40"/>
       <c r="CZ108" s="11"/>
       <c r="DA108" s="11"/>
       <c r="DB108" s="11"/>
@@ -22100,13 +22222,15 @@
         <v>5.5937419828051134</v>
       </c>
       <c r="CT109" s="25">
-        <v>5.9594170655046668</v>
-      </c>
-      <c r="CU109" s="40"/>
+        <v>6.2225909057872713</v>
+      </c>
+      <c r="CU109" s="25">
+        <v>7.3659766292589808</v>
+      </c>
       <c r="CV109" s="40"/>
       <c r="CW109" s="40"/>
       <c r="CX109" s="40"/>
-      <c r="CY109" s="11"/>
+      <c r="CY109" s="40"/>
       <c r="CZ109" s="11"/>
       <c r="DA109" s="11"/>
       <c r="DB109" s="11"/>
@@ -22447,13 +22571,15 @@
         <v>7.5880575725243915</v>
       </c>
       <c r="CT110" s="25">
-        <v>4.6902160799810417</v>
-      </c>
-      <c r="CU110" s="40"/>
+        <v>4.3266224559296944</v>
+      </c>
+      <c r="CU110" s="25">
+        <v>4.3253671278139905</v>
+      </c>
       <c r="CV110" s="40"/>
       <c r="CW110" s="40"/>
       <c r="CX110" s="40"/>
-      <c r="CY110" s="11"/>
+      <c r="CY110" s="40"/>
       <c r="CZ110" s="11"/>
       <c r="DA110" s="11"/>
       <c r="DB110" s="11"/>
@@ -22599,11 +22725,11 @@
       <c r="CR111" s="13"/>
       <c r="CS111" s="13"/>
       <c r="CT111" s="13"/>
-      <c r="CU111" s="41"/>
+      <c r="CU111" s="13"/>
       <c r="CV111" s="41"/>
       <c r="CW111" s="41"/>
       <c r="CX111" s="41"/>
-      <c r="CY111" s="11"/>
+      <c r="CY111" s="41"/>
       <c r="CZ111" s="11"/>
       <c r="DA111" s="11"/>
       <c r="DB111" s="11"/>
@@ -22944,13 +23070,15 @@
         <v>4.740608766315674</v>
       </c>
       <c r="CT112" s="25">
-        <v>5.301702917474131</v>
-      </c>
-      <c r="CU112" s="40"/>
+        <v>5.2936401126761012</v>
+      </c>
+      <c r="CU112" s="25">
+        <v>5.4514379593826305</v>
+      </c>
       <c r="CV112" s="40"/>
       <c r="CW112" s="40"/>
       <c r="CX112" s="40"/>
-      <c r="CY112" s="11"/>
+      <c r="CY112" s="40"/>
       <c r="CZ112" s="11"/>
       <c r="DA112" s="11"/>
       <c r="DB112" s="11"/>
@@ -23097,19 +23225,20 @@
       <c r="CR113" s="17"/>
       <c r="CS113" s="17"/>
       <c r="CT113" s="17"/>
-      <c r="CU113" s="6"/>
+      <c r="CU113" s="17"/>
       <c r="CV113" s="6"/>
       <c r="CW113" s="6"/>
       <c r="CX113" s="6"/>
+      <c r="CY113" s="6"/>
     </row>
     <row r="114" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="CU114" s="39"/>
       <c r="CV114" s="39"/>
       <c r="CW114" s="39"/>
       <c r="CX114" s="39"/>
+      <c r="CY114" s="39"/>
     </row>
     <row r="115" spans="1:153" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="13"/>
@@ -23209,11 +23338,11 @@
       <c r="CR115" s="13"/>
       <c r="CS115" s="13"/>
       <c r="CT115" s="13"/>
-      <c r="CU115" s="41"/>
+      <c r="CU115" s="13"/>
       <c r="CV115" s="41"/>
       <c r="CW115" s="41"/>
       <c r="CX115" s="41"/>
-      <c r="CY115" s="11"/>
+      <c r="CY115" s="41"/>
       <c r="CZ115" s="11"/>
       <c r="DA115" s="11"/>
       <c r="DB115" s="11"/>
@@ -23359,11 +23488,11 @@
       <c r="CR116" s="13"/>
       <c r="CS116" s="13"/>
       <c r="CT116" s="13"/>
-      <c r="CU116" s="41"/>
+      <c r="CU116" s="13"/>
       <c r="CV116" s="41"/>
       <c r="CW116" s="41"/>
       <c r="CX116" s="41"/>
-      <c r="CY116" s="11"/>
+      <c r="CY116" s="41"/>
       <c r="CZ116" s="11"/>
       <c r="DA116" s="11"/>
       <c r="DB116" s="11"/>
@@ -23418,7 +23547,7 @@
     </row>
     <row r="118" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="120" spans="1:153" x14ac:dyDescent="0.2">
@@ -23428,7 +23557,7 @@
     </row>
     <row r="121" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="122" spans="1:153" x14ac:dyDescent="0.2">
@@ -23591,6 +23720,7 @@
       <c r="CX124" s="35">
         <v>2025</v>
       </c>
+      <c r="CY124" s="35"/>
     </row>
     <row r="125" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
@@ -23898,6 +24028,9 @@
       </c>
       <c r="CX125" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="CY125" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -24210,7 +24343,9 @@
       <c r="CX127" s="25">
         <v>130.55748864874414</v>
       </c>
-      <c r="CY127" s="11"/>
+      <c r="CY127" s="25">
+        <v>132.07040714172024</v>
+      </c>
       <c r="CZ127" s="11"/>
       <c r="DA127" s="11"/>
       <c r="DB127" s="11"/>
@@ -24569,7 +24704,9 @@
       <c r="CX128" s="25">
         <v>174.05150434879829</v>
       </c>
-      <c r="CY128" s="11"/>
+      <c r="CY128" s="25">
+        <v>188.77855366342135</v>
+      </c>
       <c r="CZ128" s="11"/>
       <c r="DA128" s="11"/>
       <c r="DB128" s="11"/>
@@ -24928,7 +25065,9 @@
       <c r="CX129" s="25">
         <v>117.26173252756766</v>
       </c>
-      <c r="CY129" s="11"/>
+      <c r="CY129" s="25">
+        <v>128.12177567254648</v>
+      </c>
       <c r="CZ129" s="11"/>
       <c r="DA129" s="11"/>
       <c r="DB129" s="11"/>
@@ -25287,7 +25426,9 @@
       <c r="CX130" s="25">
         <v>115.80302410046983</v>
       </c>
-      <c r="CY130" s="11"/>
+      <c r="CY130" s="25">
+        <v>120.97540825066915</v>
+      </c>
       <c r="CZ130" s="11"/>
       <c r="DA130" s="11"/>
       <c r="DB130" s="11"/>
@@ -25646,7 +25787,9 @@
       <c r="CX131" s="25">
         <v>125.41052570121623</v>
       </c>
-      <c r="CY131" s="11"/>
+      <c r="CY131" s="25">
+        <v>124.97612880169045</v>
+      </c>
       <c r="CZ131" s="11"/>
       <c r="DA131" s="11"/>
       <c r="DB131" s="11"/>
@@ -26005,7 +26148,9 @@
       <c r="CX132" s="25">
         <v>118.96366923799251</v>
       </c>
-      <c r="CY132" s="11"/>
+      <c r="CY132" s="25">
+        <v>119.7729412377041</v>
+      </c>
       <c r="CZ132" s="11"/>
       <c r="DA132" s="11"/>
       <c r="DB132" s="11"/>
@@ -26364,7 +26509,9 @@
       <c r="CX133" s="25">
         <v>133.65922865043828</v>
       </c>
-      <c r="CY133" s="11"/>
+      <c r="CY133" s="25">
+        <v>125.55098971228198</v>
+      </c>
       <c r="CZ133" s="11"/>
       <c r="DA133" s="11"/>
       <c r="DB133" s="11"/>
@@ -26723,7 +26870,9 @@
       <c r="CX134" s="25">
         <v>106.42917639563254</v>
       </c>
-      <c r="CY134" s="11"/>
+      <c r="CY134" s="25">
+        <v>103.64274149267338</v>
+      </c>
       <c r="CZ134" s="11"/>
       <c r="DA134" s="11"/>
       <c r="DB134" s="11"/>
@@ -27082,7 +27231,9 @@
       <c r="CX135" s="25">
         <v>115.91808763081958</v>
       </c>
-      <c r="CY135" s="11"/>
+      <c r="CY135" s="25">
+        <v>114.46706782677782</v>
+      </c>
       <c r="CZ135" s="11"/>
       <c r="DA135" s="11"/>
       <c r="DB135" s="11"/>
@@ -27441,7 +27592,9 @@
       <c r="CX136" s="25">
         <v>116.97568504088471</v>
       </c>
-      <c r="CY136" s="11"/>
+      <c r="CY136" s="25">
+        <v>119.9382205205312</v>
+      </c>
       <c r="CZ136" s="11"/>
       <c r="DA136" s="11"/>
       <c r="DB136" s="11"/>
@@ -27800,7 +27953,9 @@
       <c r="CX137" s="25">
         <v>130.03333333333333</v>
       </c>
-      <c r="CY137" s="11"/>
+      <c r="CY137" s="25">
+        <v>126.39208712453515</v>
+      </c>
       <c r="CZ137" s="11"/>
       <c r="DA137" s="11"/>
       <c r="DB137" s="11"/>
@@ -28159,7 +28314,9 @@
       <c r="CX138" s="25">
         <v>128.22635613714581</v>
       </c>
-      <c r="CY138" s="11"/>
+      <c r="CY138" s="25">
+        <v>129.17998444522635</v>
+      </c>
       <c r="CZ138" s="11"/>
       <c r="DA138" s="11"/>
       <c r="DB138" s="11"/>
@@ -28313,7 +28470,7 @@
       <c r="CV139" s="13"/>
       <c r="CW139" s="13"/>
       <c r="CX139" s="13"/>
-      <c r="CY139" s="11"/>
+      <c r="CY139" s="13"/>
       <c r="CZ139" s="11"/>
       <c r="DA139" s="11"/>
       <c r="DB139" s="11"/>
@@ -28670,9 +28827,11 @@
         <v>123.77118969792001</v>
       </c>
       <c r="CX140" s="25">
-        <v>126.56625786339333</v>
-      </c>
-      <c r="CY140" s="11"/>
+        <v>126.5808386373883</v>
+      </c>
+      <c r="CY140" s="25">
+        <v>127.02514118579921</v>
+      </c>
       <c r="CZ140" s="11"/>
       <c r="DA140" s="11"/>
       <c r="DB140" s="11"/>
@@ -28827,6 +28986,7 @@
       <c r="CV141" s="17"/>
       <c r="CW141" s="17"/>
       <c r="CX141" s="17"/>
+      <c r="CY141" s="17"/>
     </row>
     <row r="142" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A142" s="18" t="s">
@@ -28845,7 +29005,7 @@
     </row>
     <row r="147" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="149" spans="1:153" x14ac:dyDescent="0.2">
@@ -28855,7 +29015,7 @@
     </row>
     <row r="150" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="151" spans="1:153" x14ac:dyDescent="0.2">
@@ -29018,6 +29178,7 @@
       <c r="CX153" s="35">
         <v>2025</v>
       </c>
+      <c r="CY153" s="35"/>
     </row>
     <row r="154" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
@@ -29325,6 +29486,9 @@
       </c>
       <c r="CX154" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="CY154" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="155" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -29635,9 +29799,11 @@
         <v>37.736197721258655</v>
       </c>
       <c r="CX156" s="25">
-        <v>33.678025426605707</v>
-      </c>
-      <c r="CY156" s="11"/>
+        <v>33.757200270474712</v>
+      </c>
+      <c r="CY156" s="25">
+        <v>38.03279436499453</v>
+      </c>
       <c r="CZ156" s="11"/>
       <c r="DA156" s="11"/>
       <c r="DB156" s="11"/>
@@ -29994,9 +30160,11 @@
         <v>2.1737726938704962</v>
       </c>
       <c r="CX157" s="25">
-        <v>1.7925730750542874</v>
-      </c>
-      <c r="CY157" s="11"/>
+        <v>1.7928983392648274</v>
+      </c>
+      <c r="CY157" s="25">
+        <v>1.7212444344976046</v>
+      </c>
       <c r="CZ157" s="11"/>
       <c r="DA157" s="11"/>
       <c r="DB157" s="11"/>
@@ -30353,9 +30521,11 @@
         <v>1.6389737839370069</v>
       </c>
       <c r="CX158" s="25">
-        <v>1.267951497346085</v>
-      </c>
-      <c r="CY158" s="11"/>
+        <v>1.2632925147295018</v>
+      </c>
+      <c r="CY158" s="25">
+        <v>1.0392737588255581</v>
+      </c>
       <c r="CZ158" s="11"/>
       <c r="DA158" s="11"/>
       <c r="DB158" s="11"/>
@@ -30712,9 +30882,11 @@
         <v>10.717668232278442</v>
       </c>
       <c r="CX159" s="25">
-        <v>10.901819654397118</v>
-      </c>
-      <c r="CY159" s="11"/>
+        <v>10.881927241842131</v>
+      </c>
+      <c r="CY159" s="25">
+        <v>14.234072896264887</v>
+      </c>
       <c r="CZ159" s="11"/>
       <c r="DA159" s="11"/>
       <c r="DB159" s="11"/>
@@ -31071,9 +31243,11 @@
         <v>2.5791321485030427</v>
       </c>
       <c r="CX160" s="25">
-        <v>2.3536763365879554</v>
-      </c>
-      <c r="CY160" s="11"/>
+        <v>2.3738405050310609</v>
+      </c>
+      <c r="CY160" s="25">
+        <v>2.2808685136289388</v>
+      </c>
       <c r="CZ160" s="11"/>
       <c r="DA160" s="11"/>
       <c r="DB160" s="11"/>
@@ -31430,9 +31604,11 @@
         <v>4.3166877607820213</v>
       </c>
       <c r="CX161" s="25">
-        <v>4.4448749409005845</v>
-      </c>
-      <c r="CY161" s="11"/>
+        <v>4.4536658545108354</v>
+      </c>
+      <c r="CY161" s="25">
+        <v>3.958907475261384</v>
+      </c>
       <c r="CZ161" s="11"/>
       <c r="DA161" s="11"/>
       <c r="DB161" s="11"/>
@@ -31789,9 +31965,11 @@
         <v>8.0993814933164714</v>
       </c>
       <c r="CX162" s="25">
-        <v>10.822290581558871</v>
-      </c>
-      <c r="CY162" s="11"/>
+        <v>10.823001361700925</v>
+      </c>
+      <c r="CY162" s="25">
+        <v>9.5946870340552959</v>
+      </c>
       <c r="CZ162" s="11"/>
       <c r="DA162" s="11"/>
       <c r="DB162" s="11"/>
@@ -32148,9 +32326,11 @@
         <v>2.4304136686051896</v>
       </c>
       <c r="CX163" s="25">
-        <v>2.7844361067233412</v>
-      </c>
-      <c r="CY163" s="11"/>
+        <v>2.7619572078191235</v>
+      </c>
+      <c r="CY163" s="25">
+        <v>3.0047137385288485</v>
+      </c>
       <c r="CZ163" s="11"/>
       <c r="DA163" s="11"/>
       <c r="DB163" s="11"/>
@@ -32507,9 +32687,11 @@
         <v>1.865279867068689</v>
       </c>
       <c r="CX164" s="25">
-        <v>1.869807275075672</v>
-      </c>
-      <c r="CY164" s="11"/>
+        <v>1.8602477560917461</v>
+      </c>
+      <c r="CY164" s="25">
+        <v>1.3762701782355058</v>
+      </c>
       <c r="CZ164" s="11"/>
       <c r="DA164" s="11"/>
       <c r="DB164" s="11"/>
@@ -32866,9 +33048,11 @@
         <v>4.7386931811274202</v>
       </c>
       <c r="CX165" s="25">
-        <v>5.3566165427758019</v>
-      </c>
-      <c r="CY165" s="11"/>
+        <v>5.3282006027153725</v>
+      </c>
+      <c r="CY165" s="25">
+        <v>4.9177913398538466</v>
+      </c>
       <c r="CZ165" s="11"/>
       <c r="DA165" s="11"/>
       <c r="DB165" s="11"/>
@@ -33225,9 +33409,11 @@
         <v>8.7161507554568978</v>
       </c>
       <c r="CX166" s="25">
-        <v>10.521670992078798</v>
-      </c>
-      <c r="CY166" s="11"/>
+        <v>10.547396512228262</v>
+      </c>
+      <c r="CY166" s="25">
+        <v>6.2132350217920553</v>
+      </c>
       <c r="CZ166" s="11"/>
       <c r="DA166" s="11"/>
       <c r="DB166" s="11"/>
@@ -33584,9 +33770,11 @@
         <v>14.987648693795666</v>
       </c>
       <c r="CX167" s="25">
-        <v>14.206257570895772</v>
-      </c>
-      <c r="CY167" s="11"/>
+        <v>14.156371833591489</v>
+      </c>
+      <c r="CY167" s="25">
+        <v>13.626141244061559</v>
+      </c>
       <c r="CZ167" s="11"/>
       <c r="DA167" s="11"/>
       <c r="DB167" s="11"/>
@@ -33740,7 +33928,7 @@
       <c r="CV168" s="13"/>
       <c r="CW168" s="13"/>
       <c r="CX168" s="13"/>
-      <c r="CY168" s="11"/>
+      <c r="CY168" s="13"/>
       <c r="CZ168" s="11"/>
       <c r="DA168" s="11"/>
       <c r="DB168" s="11"/>
@@ -34099,7 +34287,9 @@
       <c r="CX169" s="25">
         <v>100</v>
       </c>
-      <c r="CY169" s="11"/>
+      <c r="CY169" s="25">
+        <v>100</v>
+      </c>
       <c r="CZ169" s="11"/>
       <c r="DA169" s="11"/>
       <c r="DB169" s="11"/>
@@ -34254,6 +34444,7 @@
       <c r="CV170" s="17"/>
       <c r="CW170" s="17"/>
       <c r="CX170" s="17"/>
+      <c r="CY170" s="17"/>
     </row>
     <row r="171" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A171" s="18" t="s">
@@ -34362,7 +34553,7 @@
       <c r="CV172" s="13"/>
       <c r="CW172" s="13"/>
       <c r="CX172" s="13"/>
-      <c r="CY172" s="11"/>
+      <c r="CY172" s="13"/>
       <c r="CZ172" s="11"/>
       <c r="DA172" s="11"/>
       <c r="DB172" s="11"/>
@@ -34516,7 +34707,7 @@
       <c r="CV173" s="13"/>
       <c r="CW173" s="13"/>
       <c r="CX173" s="13"/>
-      <c r="CY173" s="11"/>
+      <c r="CY173" s="13"/>
       <c r="CZ173" s="11"/>
       <c r="DA173" s="11"/>
       <c r="DB173" s="11"/>
@@ -34580,7 +34771,7 @@
     </row>
     <row r="176" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="178" spans="1:153" x14ac:dyDescent="0.2">
@@ -34590,7 +34781,7 @@
     </row>
     <row r="179" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="180" spans="1:153" x14ac:dyDescent="0.2">
@@ -34753,6 +34944,7 @@
       <c r="CX182" s="35">
         <v>2025</v>
       </c>
+      <c r="CY182" s="35"/>
     </row>
     <row r="183" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
@@ -35060,6 +35252,9 @@
       </c>
       <c r="CX183" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="CY183" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="184" spans="1:153" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -35370,9 +35565,11 @@
         <v>35.66194087678609</v>
       </c>
       <c r="CX185" s="25">
-        <v>32.648465397045584</v>
-      </c>
-      <c r="CY185" s="11"/>
+        <v>32.728989845869428</v>
+      </c>
+      <c r="CY185" s="25">
+        <v>36.579890820808835</v>
+      </c>
       <c r="CZ185" s="11"/>
       <c r="DA185" s="11"/>
       <c r="DB185" s="11"/>
@@ -35729,9 +35926,11 @@
         <v>1.5527496497655149</v>
       </c>
       <c r="CX186" s="25">
-        <v>1.3035179839734798</v>
-      </c>
-      <c r="CY186" s="11"/>
+        <v>1.3039047046724908</v>
+      </c>
+      <c r="CY186" s="25">
+        <v>1.1581893867941755</v>
+      </c>
       <c r="CZ186" s="11"/>
       <c r="DA186" s="11"/>
       <c r="DB186" s="11"/>
@@ -36088,9 +36287,11 @@
         <v>1.7557286246469035</v>
       </c>
       <c r="CX187" s="25">
-        <v>1.3685613602344846</v>
-      </c>
-      <c r="CY187" s="11"/>
+        <v>1.3636897776621355</v>
+      </c>
+      <c r="CY187" s="25">
+        <v>1.0303782885659794</v>
+      </c>
       <c r="CZ187" s="11"/>
       <c r="DA187" s="11"/>
       <c r="DB187" s="11"/>
@@ -36447,9 +36648,11 @@
         <v>10.823872925820751</v>
       </c>
       <c r="CX188" s="25">
-        <v>11.915081909791311</v>
-      </c>
-      <c r="CY188" s="11"/>
+        <v>11.894710755293913</v>
+      </c>
+      <c r="CY188" s="25">
+        <v>14.945889792333098</v>
+      </c>
       <c r="CZ188" s="11"/>
       <c r="DA188" s="11"/>
       <c r="DB188" s="11"/>
@@ -36806,9 +37009,11 @@
         <v>2.6533792670594769</v>
       </c>
       <c r="CX189" s="25">
-        <v>2.3753668559948404</v>
-      </c>
-      <c r="CY189" s="11"/>
+        <v>2.3959928422125976</v>
+      </c>
+      <c r="CY189" s="25">
+        <v>2.3182638776537385</v>
+      </c>
       <c r="CZ189" s="11"/>
       <c r="DA189" s="11"/>
       <c r="DB189" s="11"/>
@@ -37165,9 +37370,11 @@
         <v>4.3904074420822194</v>
       </c>
       <c r="CX190" s="25">
-        <v>4.7289327199139093</v>
-      </c>
-      <c r="CY190" s="11"/>
+        <v>4.7388312960226182</v>
+      </c>
+      <c r="CY190" s="25">
+        <v>4.1986176158817425</v>
+      </c>
       <c r="CZ190" s="11"/>
       <c r="DA190" s="11"/>
       <c r="DB190" s="11"/>
@@ -37524,9 +37731,11 @@
         <v>7.9769212184268996</v>
       </c>
       <c r="CX191" s="25">
-        <v>10.247977893097481</v>
-      </c>
-      <c r="CY191" s="11"/>
+        <v>10.249831626072355</v>
+      </c>
+      <c r="CY191" s="25">
+        <v>9.7073426336774293</v>
+      </c>
       <c r="CZ191" s="11"/>
       <c r="DA191" s="11"/>
       <c r="DB191" s="11"/>
@@ -37883,9 +38092,11 @@
         <v>3.051891236968173</v>
       </c>
       <c r="CX192" s="25">
-        <v>3.3112692423517727</v>
-      </c>
-      <c r="CY192" s="11"/>
+        <v>3.2849155794150326</v>
+      </c>
+      <c r="CY192" s="25">
+        <v>3.682594471765479</v>
+      </c>
       <c r="CZ192" s="11"/>
       <c r="DA192" s="11"/>
       <c r="DB192" s="11"/>
@@ -38242,9 +38453,11 @@
         <v>2.003429127337911</v>
       </c>
       <c r="CX193" s="25">
-        <v>2.0415667180930619</v>
-      </c>
-      <c r="CY193" s="11"/>
+        <v>2.0313630586225027</v>
+      </c>
+      <c r="CY193" s="25">
+        <v>1.5272594731327038</v>
+      </c>
       <c r="CZ193" s="11"/>
       <c r="DA193" s="11"/>
       <c r="DB193" s="11"/>
@@ -38601,9 +38814,11 @@
         <v>5.2903809107924626</v>
       </c>
       <c r="CX194" s="25">
-        <v>5.7957934624731742</v>
-      </c>
-      <c r="CY194" s="11"/>
+        <v>5.7657119125587517</v>
+      </c>
+      <c r="CY194" s="25">
+        <v>5.2083742493103058</v>
+      </c>
       <c r="CZ194" s="11"/>
       <c r="DA194" s="11"/>
       <c r="DB194" s="11"/>
@@ -38960,9 +39175,11 @@
         <v>8.4440857689036832</v>
       </c>
       <c r="CX195" s="25">
-        <v>10.241131945172244</v>
-      </c>
-      <c r="CY195" s="11"/>
+        <v>10.267354237059095</v>
+      </c>
+      <c r="CY195" s="25">
+        <v>6.2443549578071789</v>
+      </c>
       <c r="CZ195" s="11"/>
       <c r="DA195" s="11"/>
       <c r="DB195" s="11"/>
@@ -39319,9 +39536,11 @@
         <v>16.395212951409896</v>
       </c>
       <c r="CX196" s="25">
-        <v>14.022334511858652</v>
-      </c>
-      <c r="CY196" s="11"/>
+        <v>13.97470436453907</v>
+      </c>
+      <c r="CY196" s="25">
+        <v>13.398844432269341</v>
+      </c>
       <c r="CZ196" s="11"/>
       <c r="DA196" s="11"/>
       <c r="DB196" s="11"/>
@@ -39475,7 +39694,7 @@
       <c r="CV197" s="13"/>
       <c r="CW197" s="13"/>
       <c r="CX197" s="13"/>
-      <c r="CY197" s="11"/>
+      <c r="CY197" s="13"/>
       <c r="CZ197" s="11"/>
       <c r="DA197" s="11"/>
       <c r="DB197" s="11"/>
@@ -39834,7 +40053,9 @@
       <c r="CX198" s="25">
         <v>100</v>
       </c>
-      <c r="CY198" s="11"/>
+      <c r="CY198" s="25">
+        <v>100</v>
+      </c>
       <c r="CZ198" s="11"/>
       <c r="DA198" s="11"/>
       <c r="DB198" s="11"/>
@@ -39989,6 +40210,7 @@
       <c r="CV199" s="17"/>
       <c r="CW199" s="17"/>
       <c r="CX199" s="17"/>
+      <c r="CY199" s="17"/>
     </row>
     <row r="200" spans="1:153" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
@@ -40093,12 +40315,12 @@
       <c r="CQ201" s="2"/>
       <c r="CR201" s="2"/>
       <c r="CS201" s="2"/>
-      <c r="CT201" s="2"/>
-      <c r="CU201" s="2"/>
-      <c r="CV201" s="2"/>
+      <c r="CT201" s="39"/>
+      <c r="CU201" s="39"/>
+      <c r="CV201" s="39"/>
       <c r="CW201" s="2"/>
-      <c r="CX201" s="2"/>
-      <c r="CY201" s="28"/>
+      <c r="CX201" s="39"/>
+      <c r="CY201" s="39"/>
       <c r="CZ201" s="28"/>
       <c r="DA201" s="28"/>
       <c r="DB201" s="28"/>
@@ -40253,7 +40475,7 @@
       <c r="CV202" s="2"/>
       <c r="CW202" s="2"/>
       <c r="CX202" s="2"/>
-      <c r="CY202" s="28"/>
+      <c r="CY202" s="2"/>
       <c r="CZ202" s="28"/>
       <c r="DA202" s="28"/>
       <c r="DB202" s="28"/>

</xml_diff>